<commit_message>
Added achievements and leaderboards up to the beginning of Traverse Town
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Locations" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="158">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -410,6 +411,90 @@
   </si>
   <si>
     <t xml:space="preserve">0x195bba </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somewhere in the datascape...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SoA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Station of Awakening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SoA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Station of Awakening or Destiny Islands System Sector, Floor 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destiny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destiny Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DestinySecret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destiny Islands: Secret Place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISectorF2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destiny Islands System Sector, Floor 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DestinyStorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destiny Islands: Storm-tossed Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraverseFirst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First District</t>
   </si>
 </sst>
 </file>
@@ -419,11 +504,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -444,6 +530,14 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -488,7 +582,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -498,6 +592,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -520,11 +618,11 @@
   </sheetPr>
   <dimension ref="A1:D681"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A642" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A642" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -10074,4 +10172,261 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A2,": { ""worldId"": ",B2,", ""name"": """,C2,""", ""display"": """,D2,""", ""areaId"": ",A2,", },")</f>
+        <v>0x0: { "worldId": 0x0, "name": "Null", "display": "Somewhere in the datascape...", "areaId": 0x0, },</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A3,": { ""worldId"": ",B3,", ""name"": """,C3,""", ""display"": """,D3,""", ""areaId"": ",A3,", },")</f>
+        <v>0x1: { "worldId": 0x0, "name": "SoA1", "display": "Station of Awakening", "areaId": 0x1, },</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A4,": { ""worldId"": ",B4,", ""name"": """,C4,""", ""display"": """,D4,""", ""areaId"": ",A4,", },")</f>
+        <v>0x2: { "worldId": 0x0, "name": "SoA2", "display": "Station of Awakening or Destiny Islands System Sector, Floor 1", "areaId": 0x2, },</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A5,": { ""worldId"": ",B5,", ""name"": """,C5,""", ""display"": """,D5,""", ""areaId"": ",A5,", },")</f>
+        <v>0x3: { "worldId": 0x0, "name": "Destiny", "display": "Destiny Islands", "areaId": 0x3, },</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A6,": { ""worldId"": ",B6,", ""name"": """,C6,""", ""display"": """,D6,""", ""areaId"": ",A6,", },")</f>
+        <v>0x5: { "worldId": 0x0, "name": "DestinySecret", "display": "Destiny Islands: Secret Place", "areaId": 0x5, },</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A7,": { ""worldId"": ",B7,", ""name"": """,C7,""", ""display"": """,D7,""", ""areaId"": ",A7,", },")</f>
+        <v>0x12: { "worldId": 0x0, "name": "DISectorF2", "display": "Destiny Islands System Sector, Floor 2", "areaId": 0x12, },</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A8,": { ""worldId"": ",B8,", ""name"": """,C8,""", ""display"": """,D8,""", ""areaId"": ",A8,", },")</f>
+        <v>0x4: { "worldId": 0x0, "name": "DestinyStorm", "display": "Destiny Islands: Storm-tossed Island", "areaId": 0x4, },</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A9,": { ""worldId"": ",B9,", ""name"": """,C9,""", ""display"": """,D9,""", ""areaId"": ",A9,", },")</f>
+        <v>0x1: { "worldId": 0x1, "name": "TraverseFirst", "display": "First District", "areaId": 0x1, },</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A10,": { ""worldId"": ",B10,", ""name"": """,C10,""", ""display"": """,D10,""", ""areaId"": ",A10,", },")</f>
+        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A11,": { ""worldId"": ",B11,", ""name"": """,C11,""", ""display"": """,D11,""", ""areaId"": ",A11,", },")</f>
+        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A12,": { ""worldId"": ",B12,", ""name"": """,C12,""", ""display"": """,D12,""", ""areaId"": ",A12,", },")</f>
+        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A13,": { ""worldId"": ",B13,", ""name"": """,C13,""", ""display"": """,D13,""", ""areaId"": ",A13,", },")</f>
+        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A14,": { ""worldId"": ",B14,", ""name"": """,C14,""", ""display"": """,D14,""", ""areaId"": ",A14,", },")</f>
+        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A15,": { ""worldId"": ",B15,", ""name"": """,C15,""", ""display"": """,D15,""", ""areaId"": ",A15,", },")</f>
+        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A16,": { ""worldId"": ",B16,", ""name"": """,C16,""", ""display"": """,D16,""", ""areaId"": ",A16,", },")</f>
+        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A17,": { ""worldId"": ",B17,", ""name"": """,C17,""", ""display"": """,D17,""", ""areaId"": ",A17,", },")</f>
+        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A18,": { ""worldId"": ",B18,", ""name"": """,C18,""", ""display"": """,D18,""", ""areaId"": ",A18,", },")</f>
+        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A19,": { ""worldId"": ",B19,", ""name"": """,C19,""", ""display"": """,D19,""", ""areaId"": ",A19,", },")</f>
+        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A20,": { ""worldId"": ",B20,", ""name"": """,C20,""", ""display"": """,D20,""", ""areaId"": ",A20,", },")</f>
+        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A21,": { ""worldId"": ",B21,", ""name"": """,C21,""", ""display"": """,D21,""", ""areaId"": ",A21,", },")</f>
+        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored Rich Presence and added sector reward addresses
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="172">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -413,6 +413,9 @@
     <t xml:space="preserve">0x195bba </t>
   </si>
   <si>
+    <t xml:space="preserve">Key</t>
+  </si>
+  <si>
     <t xml:space="preserve">Area ID</t>
   </si>
   <si>
@@ -495,6 +498,45 @@
   </si>
   <si>
     <t xml:space="preserve">First District</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraverseSecond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second District</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraverseAlley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alleyway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraverseSector2F1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traverse Town System Sector 2, Floor 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraverseSector2F2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traverse Town System Sector 2, Floor 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraverseSector2F3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traverse Town System Sector 2, Floor 3</t>
   </si>
 </sst>
 </file>
@@ -622,7 +664,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -10179,13 +10221,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -10203,13 +10248,16 @@
       <c r="E1" s="3" t="s">
         <v>134</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>135</v>
+      <c r="A2" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>136</v>
@@ -10217,207 +10265,327 @@
       <c r="D2" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A2,": { ""worldId"": ",B2,", ""name"": """,C2,""", ""display"": """,D2,""", ""areaId"": ",A2,", },")</f>
-        <v>0x0: { "worldId": 0x0, "name": "Null", "display": "Somewhere in the datascape...", "areaId": 0x0, },</v>
+      <c r="E2" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A2,": { ""worldId"": ",C2,", ""name"": """,D2,""", ""display"": """,E2,""", ""areaId"": ",B2,", },")</f>
+        <v>0: { "worldId": 0x0, "name": "Null", "display": "Somewhere in the datascape...", "areaId": 0x0, },</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>138</v>
+      <c r="A3" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A3,": { ""worldId"": ",B3,", ""name"": """,C3,""", ""display"": """,D3,""", ""areaId"": ",A3,", },")</f>
-        <v>0x1: { "worldId": 0x0, "name": "SoA1", "display": "Station of Awakening", "areaId": 0x1, },</v>
+      <c r="E3" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A3,": { ""worldId"": ",C3,", ""name"": """,D3,""", ""display"": """,E3,""", ""areaId"": ",B3,", },")</f>
+        <v>1: { "worldId": 0x0, "name": "SoA1", "display": "Station of Awakening", "areaId": 0x1, },</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>141</v>
+      <c r="A4" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="E4" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A4,": { ""worldId"": ",B4,", ""name"": """,C4,""", ""display"": """,D4,""", ""areaId"": ",A4,", },")</f>
-        <v>0x2: { "worldId": 0x0, "name": "SoA2", "display": "Station of Awakening or Destiny Islands System Sector, Floor 1", "areaId": 0x2, },</v>
+      <c r="E4" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A4,": { ""worldId"": ",C4,", ""name"": """,D4,""", ""display"": """,E4,""", ""areaId"": ",B4,", },")</f>
+        <v>2: { "worldId": 0x0, "name": "SoA2", "display": "Station of Awakening or Destiny Islands System Sector, Floor 1", "areaId": 0x2, },</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>144</v>
+      <c r="A5" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="E5" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A5,": { ""worldId"": ",B5,", ""name"": """,C5,""", ""display"": """,D5,""", ""areaId"": ",A5,", },")</f>
-        <v>0x3: { "worldId": 0x0, "name": "Destiny", "display": "Destiny Islands", "areaId": 0x3, },</v>
+      <c r="E5" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A5,": { ""worldId"": ",C5,", ""name"": """,D5,""", ""display"": """,E5,""", ""areaId"": ",B5,", },")</f>
+        <v>3: { "worldId": 0x0, "name": "Destiny", "display": "Destiny Islands", "areaId": 0x3, },</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>147</v>
+      <c r="A6" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A6,": { ""worldId"": ",B6,", ""name"": """,C6,""", ""display"": """,D6,""", ""areaId"": ",A6,", },")</f>
-        <v>0x5: { "worldId": 0x0, "name": "DestinySecret", "display": "Destiny Islands: Secret Place", "areaId": 0x5, },</v>
+      <c r="E6" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A6,": { ""worldId"": ",C6,", ""name"": """,D6,""", ""display"": """,E6,""", ""areaId"": ",B6,", },")</f>
+        <v>4: { "worldId": 0x0, "name": "DestinySecret", "display": "Destiny Islands: Secret Place", "areaId": 0x5, },</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>150</v>
+      <c r="A7" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="E7" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A7,": { ""worldId"": ",B7,", ""name"": """,C7,""", ""display"": """,D7,""", ""areaId"": ",A7,", },")</f>
-        <v>0x12: { "worldId": 0x0, "name": "DISectorF2", "display": "Destiny Islands System Sector, Floor 2", "areaId": 0x12, },</v>
+      <c r="E7" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A7,": { ""worldId"": ",C7,", ""name"": """,D7,""", ""display"": """,E7,""", ""areaId"": ",B7,", },")</f>
+        <v>5: { "worldId": 0x0, "name": "DISectorF2", "display": "Destiny Islands System Sector, Floor 2", "areaId": 0x12, },</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>153</v>
+      <c r="A8" s="0" t="n">
+        <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="E8" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A8,": { ""worldId"": ",B8,", ""name"": """,C8,""", ""display"": """,D8,""", ""areaId"": ",A8,", },")</f>
-        <v>0x4: { "worldId": 0x0, "name": "DestinyStorm", "display": "Destiny Islands: Storm-tossed Island", "areaId": 0x4, },</v>
+      <c r="E8" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A8,": { ""worldId"": ",C8,", ""name"": """,D8,""", ""display"": """,E8,""", ""areaId"": ",B8,", },")</f>
+        <v>6: { "worldId": 0x0, "name": "DestinyStorm", "display": "Destiny Islands: Storm-tossed Island", "areaId": 0x4, },</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>138</v>
+      <c r="A9" s="0" t="n">
+        <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="E9" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A9,": { ""worldId"": ",B9,", ""name"": """,C9,""", ""display"": """,D9,""", ""areaId"": ",A9,", },")</f>
-        <v>0x1: { "worldId": 0x1, "name": "TraverseFirst", "display": "First District", "areaId": 0x1, },</v>
+      <c r="E9" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A9,": { ""worldId"": ",C9,", ""name"": """,D9,""", ""display"": """,E9,""", ""areaId"": ",B9,", },")</f>
+        <v>7: { "worldId": 0x1, "name": "TraverseFirst", "display": "First District", "areaId": 0x1, },</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A10,": { ""worldId"": ",B10,", ""name"": """,C10,""", ""display"": """,D10,""", ""areaId"": ",A10,", },")</f>
-        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      <c r="A10" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A10,": { ""worldId"": ",C10,", ""name"": """,D10,""", ""display"": """,E10,""", ""areaId"": ",B10,", },")</f>
+        <v>8: { "worldId": 0x1, "name": "TraverseSecond", "display": "Second District", "areaId": 0x2, },</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E11" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A11,": { ""worldId"": ",B11,", ""name"": """,C11,""", ""display"": """,D11,""", ""areaId"": ",A11,", },")</f>
-        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      <c r="A11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F11" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A11,": { ""worldId"": ",C11,", ""name"": """,D11,""", ""display"": """,E11,""", ""areaId"": ",B11,", },")</f>
+        <v>9: { "worldId": 0x1, "name": "TraverseAlley", "display": "Alleyway", "areaId": 0x4, },</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A12,": { ""worldId"": ",B12,", ""name"": """,C12,""", ""display"": """,D12,""", ""areaId"": ",A12,", },")</f>
-        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      <c r="A12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A12,": { ""worldId"": ",C12,", ""name"": """,D12,""", ""display"": """,E12,""", ""areaId"": ",B12,", },")</f>
+        <v>10: { "worldId": 0x1, "name": "TraverseSector2F1", "display": "Traverse Town System Sector 2, Floor 1", "areaId": 0x6, },</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E13" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A13,": { ""worldId"": ",B13,", ""name"": """,C13,""", ""display"": """,D13,""", ""areaId"": ",A13,", },")</f>
-        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      <c r="A13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="F13" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A13,": { ""worldId"": ",C13,", ""name"": """,D13,""", ""display"": """,E13,""", ""areaId"": ",B13,", },")</f>
+        <v>11: { "worldId": 0x1, "name": "TraverseSector2F2", "display": "Traverse Town System Sector 2, Floor 2", "areaId": 0x7, },</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A14,": { ""worldId"": ",B14,", ""name"": """,C14,""", ""display"": """,D14,""", ""areaId"": ",A14,", },")</f>
-        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      <c r="A14" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="F14" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A14,": { ""worldId"": ",C14,", ""name"": """,D14,""", ""display"": """,E14,""", ""areaId"": ",B14,", },")</f>
+        <v>12: { "worldId": 0x1, "name": "TraverseSector2F3", "display": "Traverse Town System Sector 2, Floor 3", "areaId": 0xd, },</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A15,": { ""worldId"": ",B15,", ""name"": """,C15,""", ""display"": """,D15,""", ""areaId"": ",A15,", },")</f>
-        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      <c r="A15" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F15" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A15,": { ""worldId"": ",C15,", ""name"": """,D15,""", ""display"": """,E15,""", ""areaId"": ",B15,", },")</f>
+        <v>13: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A16,": { ""worldId"": ",B16,", ""name"": """,C16,""", ""display"": """,D16,""", ""areaId"": ",A16,", },")</f>
-        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      <c r="A16" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F16" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A16,": { ""worldId"": ",C16,", ""name"": """,D16,""", ""display"": """,E16,""", ""areaId"": ",B16,", },")</f>
+        <v>14: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E17" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A17,": { ""worldId"": ",B17,", ""name"": """,C17,""", ""display"": """,D17,""", ""areaId"": ",A17,", },")</f>
-        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      <c r="A17" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F17" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A17,": { ""worldId"": ",C17,", ""name"": """,D17,""", ""display"": """,E17,""", ""areaId"": ",B17,", },")</f>
+        <v>15: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A18,": { ""worldId"": ",B18,", ""name"": """,C18,""", ""display"": """,D18,""", ""areaId"": ",A18,", },")</f>
-        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      <c r="A18" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F18" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A18,": { ""worldId"": ",C18,", ""name"": """,D18,""", ""display"": """,E18,""", ""areaId"": ",B18,", },")</f>
+        <v>16: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E19" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A19,": { ""worldId"": ",B19,", ""name"": """,C19,""", ""display"": """,D19,""", ""areaId"": ",A19,", },")</f>
-        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      <c r="A19" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="F19" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A19,": { ""worldId"": ",C19,", ""name"": """,D19,""", ""display"": """,E19,""", ""areaId"": ",B19,", },")</f>
+        <v>17: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A20,": { ""worldId"": ",B20,", ""name"": """,C20,""", ""display"": """,D20,""", ""areaId"": ",A20,", },")</f>
-        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      <c r="A20" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F20" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A20,": { ""worldId"": ",C20,", ""name"": """,D20,""", ""display"": """,E20,""", ""areaId"": ",B20,", },")</f>
+        <v>18: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E21" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A21,": { ""worldId"": ",B21,", ""name"": """,C21,""", ""display"": """,D21,""", ""areaId"": ",A21,", },")</f>
-        <v>: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      <c r="A21" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="F21" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A21,": { ""worldId"": ",C21,", ""name"": """,D21,""", ""display"": """,E21,""", ""areaId"": ",B21,", },")</f>
+        <v>19: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added cheevos up to the end of the Traverse Town keyhole (still needs testing)
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="183">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -515,19 +515,19 @@
     <t xml:space="preserve">0x6</t>
   </si>
   <si>
-    <t xml:space="preserve">TraverseSector2F1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Traverse Town System Sector 2, Floor 1</t>
+    <t xml:space="preserve">TraverseKeyholeSecond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyhole / Second District</t>
   </si>
   <si>
     <t xml:space="preserve">0x7</t>
   </si>
   <si>
-    <t xml:space="preserve">TraverseSector2F2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Traverse Town System Sector 2, Floor 2</t>
+    <t xml:space="preserve">TraverseKeyholeThird</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyhole / Third District</t>
   </si>
   <si>
     <t xml:space="preserve">0xd</t>
@@ -537,6 +537,39 @@
   </si>
   <si>
     <t xml:space="preserve">Traverse Town System Sector 2, Floor 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraverseThird</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third District</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraverseSecondCorrupted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraverseKeyholeFirst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyhole / First District</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraverseKeyholeFall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyhole / Terminus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TraverseKeyholeTerminus</t>
   </si>
 </sst>
 </file>
@@ -664,7 +697,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -10224,10 +10257,10 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -10480,7 +10513,7 @@
       </c>
       <c r="F12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""worldId"": ",C12,", ""name"": """,D12,""", ""display"": """,E12,""", ""areaId"": ",B12,", },")</f>
-        <v>10: { "worldId": 0x1, "name": "TraverseSector2F1", "display": "Traverse Town System Sector 2, Floor 1", "areaId": 0x6, },</v>
+        <v>10: { "worldId": 0x1, "name": "TraverseKeyholeSecond", "display": "Keyhole / Second District", "areaId": 0x6, },</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10501,7 +10534,7 @@
       </c>
       <c r="F13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A13,": { ""worldId"": ",C13,", ""name"": """,D13,""", ""display"": """,E13,""", ""areaId"": ",B13,", },")</f>
-        <v>11: { "worldId": 0x1, "name": "TraverseSector2F2", "display": "Traverse Town System Sector 2, Floor 2", "areaId": 0x7, },</v>
+        <v>11: { "worldId": 0x1, "name": "TraverseKeyholeThird", "display": "Keyhole / Third District", "areaId": 0x7, },</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10529,45 +10562,105 @@
       <c r="A15" s="0" t="n">
         <v>13</v>
       </c>
+      <c r="B15" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>173</v>
+      </c>
       <c r="F15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A15,": { ""worldId"": ",C15,", ""name"": """,D15,""", ""display"": """,E15,""", ""areaId"": ",B15,", },")</f>
-        <v>13: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>13: { "worldId": 0x1, "name": "TraverseThird", "display": "Third District", "areaId": 0x3, },</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="B16" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>160</v>
+      </c>
       <c r="F16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A16,": { ""worldId"": ",C16,", ""name"": """,D16,""", ""display"": """,E16,""", ""areaId"": ",B16,", },")</f>
-        <v>14: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>14: { "worldId": 0x1, "name": "TraverseSecondCorrupted", "display": "Second District", "areaId": 0xa, },</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>15</v>
       </c>
+      <c r="B17" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>177</v>
+      </c>
       <c r="F17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A17,": { ""worldId"": ",C17,", ""name"": """,D17,""", ""display"": """,E17,""", ""areaId"": ",B17,", },")</f>
-        <v>15: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>15: { "worldId": 0x1, "name": "TraverseKeyholeFirst", "display": "Keyhole / First District", "areaId": 0x5, },</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="B18" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>180</v>
+      </c>
       <c r="F18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A18,": { ""worldId"": ",C18,", ""name"": """,D18,""", ""display"": """,E18,""", ""areaId"": ",B18,", },")</f>
-        <v>16: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>16: { "worldId": 0x1, "name": "TraverseKeyholeFall", "display": "Keyhole / Terminus", "areaId": 0x8, },</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>17</v>
       </c>
+      <c r="B19" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>180</v>
+      </c>
       <c r="F19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A19,": { ""worldId"": ",C19,", ""name"": """,D19,""", ""display"": """,E19,""", ""areaId"": ",B19,", },")</f>
-        <v>17: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>17: { "worldId": 0x1, "name": "TraverseKeyholeTerminus", "display": "Keyhole / Terminus", "areaId": 0x9, },</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added cheevos up to the end of Traverse Town
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="185">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -570,6 +570,12 @@
   </si>
   <si>
     <t xml:space="preserve">TraverseKeyholeTerminus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WonderlandClearing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clearing</t>
   </si>
 </sst>
 </file>
@@ -697,7 +703,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -10257,10 +10263,10 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -10667,9 +10673,21 @@
       <c r="A20" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="B20" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>184</v>
+      </c>
       <c r="F20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A20,": { ""worldId"": ",C20,", ""name"": """,D20,""", ""display"": """,E20,""", ""areaId"": ",B20,", },")</f>
-        <v>18: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>18: { "worldId": 0x2, "name": "WonderlandClearing", "display": "Clearing", "areaId": 0x6, },</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Initial update for checkpoint code
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="207">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -588,6 +588,60 @@
   </si>
   <si>
     <t xml:space="preserve">Lotus Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WonderlandAimless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aimless Path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WonderlandMaze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hedge Maze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WonderlandBizarreSmall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bizarre Room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WonderlandBizarreBig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WonderlandTea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tea Party Garden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WonderlandQueen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Queen’s Castle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WonderlandKeyholeFirst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyhole / The Falsewood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WonderlandKeyholeSecond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyhole / Fleeting Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WonderlandKeyholeTerminus</t>
   </si>
 </sst>
 </file>
@@ -715,7 +769,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -10272,13 +10326,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -10748,45 +10802,234 @@
       <c r="A23" s="0" t="n">
         <v>21</v>
       </c>
+      <c r="B23" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>190</v>
+      </c>
       <c r="F23" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A23,": { ""worldId"": ",C23,", ""name"": """,D23,""", ""display"": """,E23,""", ""areaId"": ",B23,", },")</f>
-        <v>21: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>21: { "worldId": 0x2, "name": "WonderlandAimless", "display": "Aimless Path", "areaId": 0x5, },</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>22</v>
       </c>
+      <c r="B24" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>192</v>
+      </c>
       <c r="F24" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A24,": { ""worldId"": ",C24,", ""name"": """,D24,""", ""display"": """,E24,""", ""areaId"": ",B24,", },")</f>
-        <v>22: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>22: { "worldId": 0x2, "name": "WonderlandMaze", "display": "Hedge Maze", "areaId": 0x4, },</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>23</v>
       </c>
+      <c r="B25" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>194</v>
+      </c>
       <c r="F25" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A25,": { ""worldId"": ",C25,", ""name"": """,D25,""", ""display"": """,E25,""", ""areaId"": ",B25,", },")</f>
-        <v>23: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>23: { "worldId": 0x2, "name": "WonderlandBizarreSmall", "display": "Bizarre Room", "areaId": 0x7, },</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="B26" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>194</v>
+      </c>
       <c r="F26" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A26,": { ""worldId"": ",C26,", ""name"": """,D26,""", ""display"": """,E26,""", ""areaId"": ",B26,", },")</f>
-        <v>24: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>24: { "worldId": 0x2, "name": "WonderlandBizarreBig", "display": "Bizarre Room", "areaId": 0x1, },</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>25</v>
       </c>
+      <c r="B27" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>197</v>
+      </c>
       <c r="F27" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A27,": { ""worldId"": ",C27,", ""name"": """,D27,""", ""display"": """,E27,""", ""areaId"": ",B27,", },")</f>
-        <v>25: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>25: { "worldId": 0x2, "name": "WonderlandTea", "display": "Tea Party Garden", "areaId": 0x3, },</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F28" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A28,": { ""worldId"": ",C28,", ""name"": """,D28,""", ""display"": """,E28,""", ""areaId"": ",B28,", },")</f>
+        <v>26: { "worldId": 0x2, "name": "WonderlandQueen", "display": "The Queen’s Castle", "areaId": 0x2, },</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="F29" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A29,": { ""worldId"": ",C29,", ""name"": """,D29,""", ""display"": """,E29,""", ""areaId"": ",B29,", },")</f>
+        <v>27: { "worldId": 0x2, "name": "WonderlandKeyholeFirst", "display": "Keyhole / The Falsewood", "areaId": 0xa, },</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="F30" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A30,": { ""worldId"": ",C30,", ""name"": """,D30,""", ""display"": """,E30,""", ""areaId"": ",B30,", },")</f>
+        <v>28: { "worldId": 0x2, "name": "WonderlandKeyholeSecond", "display": "Keyhole / Fleeting Forest", "areaId": 0xb, },</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="F31" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A31,": { ""worldId"": ",C31,", ""name"": """,D31,""", ""display"": """,E31,""", ""areaId"": ",B31,", },")</f>
+        <v>29: { "worldId": 0x2, "name": "WonderlandKeyholeTerminus", "display": "Keyhole / Terminus", "areaId": 0xc, },</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F32" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A32,": { ""worldId"": ",C32,", ""name"": """,D32,""", ""display"": """,E32,""", ""areaId"": ",B32,", },")</f>
+        <v>30: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="F33" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A33,": { ""worldId"": ",C33,", ""name"": """,D33,""", ""display"": """,E33,""", ""areaId"": ",B33,", },")</f>
+        <v>31: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="F34" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A34,": { ""worldId"": ",C34,", ""name"": """,D34,""", ""display"": """,E34,""", ""areaId"": ",B34,", },")</f>
+        <v>32: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="F35" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A35,": { ""worldId"": ",C35,", ""name"": """,D35,""", ""display"": """,E35,""", ""areaId"": ",B35,", },")</f>
+        <v>33: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="F36" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A36,": { ""worldId"": ",C36,", ""name"": """,D36,""", ""display"": """,E36,""", ""areaId"": ",B36,", },")</f>
+        <v>34: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added cheevos up to the end of Wonderland and updated the logic for the leaderboards
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="209">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -455,9 +455,6 @@
     <t xml:space="preserve">SoA2</t>
   </si>
   <si>
-    <t xml:space="preserve">Station of Awakening or Destiny Islands System Sector, Floor 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">0x3</t>
   </si>
   <si>
@@ -473,16 +470,7 @@
     <t xml:space="preserve">DestinySecret</t>
   </si>
   <si>
-    <t xml:space="preserve">Destiny Islands: Secret Place</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISectorF2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destiny Islands System Sector, Floor 2</t>
+    <t xml:space="preserve">Secret Place</t>
   </si>
   <si>
     <t xml:space="preserve">0x4</t>
@@ -491,7 +479,7 @@
     <t xml:space="preserve">DestinyStorm</t>
   </si>
   <si>
-    <t xml:space="preserve">Destiny Islands: Storm-tossed Island</t>
+    <t xml:space="preserve">Storm-tossed Island</t>
   </si>
   <si>
     <t xml:space="preserve">TraverseFirst</t>
@@ -642,6 +630,24 @@
   </si>
   <si>
     <t xml:space="preserve">WonderlandKeyholeTerminus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusOutside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outside the Coliseum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusVestibule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vestibule</t>
   </si>
 </sst>
 </file>
@@ -769,7 +775,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -10326,13 +10332,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
+      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -10413,11 +10419,11 @@
         <v>143</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""worldId"": ",C4,", ""name"": """,D4,""", ""display"": """,E4,""", ""areaId"": ",B4,", },")</f>
-        <v>2: { "worldId": 0x0, "name": "SoA2", "display": "Station of Awakening or Destiny Islands System Sector, Floor 1", "areaId": 0x2, },</v>
+        <v>2: { "worldId": 0x0, "name": "SoA2", "display": "Station of Awakening", "areaId": 0x2, },</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10425,16 +10431,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>136</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>147</v>
       </c>
       <c r="F5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""worldId"": ",C5,", ""name"": """,D5,""", ""display"": """,E5,""", ""areaId"": ",B5,", },")</f>
@@ -10446,589 +10452,592 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>136</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>149</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>150</v>
       </c>
       <c r="F6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""worldId"": ",C6,", ""name"": """,D6,""", ""display"": """,E6,""", ""areaId"": ",B6,", },")</f>
-        <v>4: { "worldId": 0x0, "name": "DestinySecret", "display": "Destiny Islands: Secret Place", "areaId": 0x5, },</v>
+        <v>4: { "worldId": 0x0, "name": "DestinySecret", "display": "Secret Place", "areaId": 0x5, },</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>136</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>152</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>153</v>
       </c>
       <c r="F7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""worldId"": ",C7,", ""name"": """,D7,""", ""display"": """,E7,""", ""areaId"": ",B7,", },")</f>
-        <v>5: { "worldId": 0x0, "name": "DISectorF2", "display": "Destiny Islands System Sector, Floor 2", "areaId": 0x12, },</v>
+        <v>6: { "worldId": 0x0, "name": "DestinyStorm", "display": "Storm-tossed Island", "areaId": 0x4, },</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>156</v>
       </c>
       <c r="F8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""worldId"": ",C8,", ""name"": """,D8,""", ""display"": """,E8,""", ""areaId"": ",B8,", },")</f>
-        <v>6: { "worldId": 0x0, "name": "DestinyStorm", "display": "Destiny Islands: Storm-tossed Island", "areaId": 0x4, },</v>
+        <v>7: { "worldId": 0x1, "name": "TraverseFirst", "display": "First District", "areaId": 0x1, },</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>139</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""worldId"": ",C9,", ""name"": """,D9,""", ""display"": """,E9,""", ""areaId"": ",B9,", },")</f>
-        <v>7: { "worldId": 0x1, "name": "TraverseFirst", "display": "First District", "areaId": 0x1, },</v>
+        <v>8: { "worldId": 0x1, "name": "TraverseSecond", "display": "Second District", "areaId": 0x2, },</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>139</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""worldId"": ",C10,", ""name"": """,D10,""", ""display"": """,E10,""", ""areaId"": ",B10,", },")</f>
-        <v>8: { "worldId": 0x1, "name": "TraverseSecond", "display": "Second District", "areaId": 0x2, },</v>
+        <v>9: { "worldId": 0x1, "name": "TraverseAlley", "display": "Alleyway", "areaId": 0x4, },</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>139</v>
       </c>
       <c r="D11" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="F11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""worldId"": ",C11,", ""name"": """,D11,""", ""display"": """,E11,""", ""areaId"": ",B11,", },")</f>
-        <v>9: { "worldId": 0x1, "name": "TraverseAlley", "display": "Alleyway", "areaId": 0x4, },</v>
+        <v>10: { "worldId": 0x1, "name": "TraverseKeyholeSecond", "display": "Keyhole / Second District", "areaId": 0x6, },</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>139</v>
       </c>
       <c r="D12" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>164</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>165</v>
       </c>
       <c r="F12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""worldId"": ",C12,", ""name"": """,D12,""", ""display"": """,E12,""", ""areaId"": ",B12,", },")</f>
-        <v>10: { "worldId": 0x1, "name": "TraverseKeyholeSecond", "display": "Keyhole / Second District", "areaId": 0x6, },</v>
+        <v>11: { "worldId": 0x1, "name": "TraverseKeyholeThird", "display": "Keyhole / Third District", "areaId": 0x7, },</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>139</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="F13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A13,": { ""worldId"": ",C13,", ""name"": """,D13,""", ""display"": """,E13,""", ""areaId"": ",B13,", },")</f>
-        <v>11: { "worldId": 0x1, "name": "TraverseKeyholeThird", "display": "Keyhole / Third District", "areaId": 0x7, },</v>
+        <v>12: { "worldId": 0x1, "name": "TraverseSector2F3", "display": "Traverse Town System Sector 2, Floor 3", "areaId": 0xd, },</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>139</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A14,": { ""worldId"": ",C14,", ""name"": """,D14,""", ""display"": """,E14,""", ""areaId"": ",B14,", },")</f>
-        <v>12: { "worldId": 0x1, "name": "TraverseSector2F3", "display": "Traverse Town System Sector 2, Floor 3", "areaId": 0xd, },</v>
+        <v>13: { "worldId": 0x1, "name": "TraverseThird", "display": "Third District", "areaId": 0x3, },</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>139</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="F15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A15,": { ""worldId"": ",C15,", ""name"": """,D15,""", ""display"": """,E15,""", ""areaId"": ",B15,", },")</f>
-        <v>13: { "worldId": 0x1, "name": "TraverseThird", "display": "Third District", "areaId": 0x3, },</v>
+        <v>14: { "worldId": 0x1, "name": "TraverseSecondCorrupted", "display": "Second District", "areaId": 0xa, },</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>139</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="F16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A16,": { ""worldId"": ",C16,", ""name"": """,D16,""", ""display"": """,E16,""", ""areaId"": ",B16,", },")</f>
-        <v>14: { "worldId": 0x1, "name": "TraverseSecondCorrupted", "display": "Second District", "areaId": 0xa, },</v>
+        <v>15: { "worldId": 0x1, "name": "TraverseKeyholeFirst", "display": "Keyhole / First District", "areaId": 0x5, },</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>139</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>176</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>177</v>
       </c>
       <c r="F17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A17,": { ""worldId"": ",C17,", ""name"": """,D17,""", ""display"": """,E17,""", ""areaId"": ",B17,", },")</f>
-        <v>15: { "worldId": 0x1, "name": "TraverseKeyholeFirst", "display": "Keyhole / First District", "areaId": 0x5, },</v>
+        <v>16: { "worldId": 0x1, "name": "TraverseKeyholeFall", "display": "Keyhole / Terminus", "areaId": 0x8, },</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>139</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A18,": { ""worldId"": ",C18,", ""name"": """,D18,""", ""display"": """,E18,""", ""areaId"": ",B18,", },")</f>
-        <v>16: { "worldId": 0x1, "name": "TraverseKeyholeFall", "display": "Keyhole / Terminus", "areaId": 0x8, },</v>
+        <v>17: { "worldId": 0x1, "name": "TraverseKeyholeTerminus", "display": "Keyhole / Terminus", "areaId": 0x9, },</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>180</v>
       </c>
       <c r="F19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A19,": { ""worldId"": ",C19,", ""name"": """,D19,""", ""display"": """,E19,""", ""areaId"": ",B19,", },")</f>
-        <v>17: { "worldId": 0x1, "name": "TraverseKeyholeTerminus", "display": "Keyhole / Terminus", "areaId": 0x9, },</v>
+        <v>18: { "worldId": 0x2, "name": "WonderlandClearing", "display": "Clearing", "areaId": 0x6, },</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>142</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A20,": { ""worldId"": ",C20,", ""name"": """,D20,""", ""display"": """,E20,""", ""areaId"": ",B20,", },")</f>
-        <v>18: { "worldId": 0x2, "name": "WonderlandClearing", "display": "Clearing", "areaId": 0x6, },</v>
+        <v>19: { "worldId": 0x2, "name": "WonderlandRoseGarden", "display": "Rose Garden", "areaId": 0x9, },</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>142</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A21,": { ""worldId"": ",C21,", ""name"": """,D21,""", ""display"": """,E21,""", ""areaId"": ",B21,", },")</f>
-        <v>19: { "worldId": 0x2, "name": "WonderlandRoseGarden", "display": "Rose Garden", "areaId": 0x9, },</v>
+        <v>20: { "worldId": 0x2, "name": "WonderlandLotus", "display": "Lotus Forest", "areaId": 0x8, },</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>142</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A22,": { ""worldId"": ",C22,", ""name"": """,D22,""", ""display"": """,E22,""", ""areaId"": ",B22,", },")</f>
-        <v>20: { "worldId": 0x2, "name": "WonderlandLotus", "display": "Lotus Forest", "areaId": 0x8, },</v>
+        <v>21: { "worldId": 0x2, "name": "WonderlandAimless", "display": "Aimless Path", "areaId": 0x5, },</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>142</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F23" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A23,": { ""worldId"": ",C23,", ""name"": """,D23,""", ""display"": """,E23,""", ""areaId"": ",B23,", },")</f>
-        <v>21: { "worldId": 0x2, "name": "WonderlandAimless", "display": "Aimless Path", "areaId": 0x5, },</v>
+        <v>22: { "worldId": 0x2, "name": "WonderlandMaze", "display": "Hedge Maze", "areaId": 0x4, },</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>142</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F24" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A24,": { ""worldId"": ",C24,", ""name"": """,D24,""", ""display"": """,E24,""", ""areaId"": ",B24,", },")</f>
-        <v>22: { "worldId": 0x2, "name": "WonderlandMaze", "display": "Hedge Maze", "areaId": 0x4, },</v>
+        <v>23: { "worldId": 0x2, "name": "WonderlandBizarreSmall", "display": "Bizarre Room", "areaId": 0x7, },</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>142</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F25" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A25,": { ""worldId"": ",C25,", ""name"": """,D25,""", ""display"": """,E25,""", ""areaId"": ",B25,", },")</f>
-        <v>23: { "worldId": 0x2, "name": "WonderlandBizarreSmall", "display": "Bizarre Room", "areaId": 0x7, },</v>
+        <v>24: { "worldId": 0x2, "name": "WonderlandBizarreBig", "display": "Bizarre Room", "areaId": 0x1, },</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>142</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F26" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A26,": { ""worldId"": ",C26,", ""name"": """,D26,""", ""display"": """,E26,""", ""areaId"": ",B26,", },")</f>
-        <v>24: { "worldId": 0x2, "name": "WonderlandBizarreBig", "display": "Bizarre Room", "areaId": 0x1, },</v>
+        <v>25: { "worldId": 0x2, "name": "WonderlandTea", "display": "Tea Party Garden", "areaId": 0x3, },</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>142</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F27" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A27,": { ""worldId"": ",C27,", ""name"": """,D27,""", ""display"": """,E27,""", ""areaId"": ",B27,", },")</f>
-        <v>25: { "worldId": 0x2, "name": "WonderlandTea", "display": "Tea Party Garden", "areaId": 0x3, },</v>
+        <v>26: { "worldId": 0x2, "name": "WonderlandQueen", "display": "The Queen’s Castle", "areaId": 0x2, },</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>142</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F28" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A28,": { ""worldId"": ",C28,", ""name"": """,D28,""", ""display"": """,E28,""", ""areaId"": ",B28,", },")</f>
-        <v>26: { "worldId": 0x2, "name": "WonderlandQueen", "display": "The Queen’s Castle", "areaId": 0x2, },</v>
+        <v>27: { "worldId": 0x2, "name": "WonderlandKeyholeFirst", "display": "Keyhole / The Falsewood", "areaId": 0xa, },</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>142</v>
       </c>
       <c r="D29" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="E29" s="0" t="s">
         <v>200</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>201</v>
       </c>
       <c r="F29" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A29,": { ""worldId"": ",C29,", ""name"": """,D29,""", ""display"": """,E29,""", ""areaId"": ",B29,", },")</f>
-        <v>27: { "worldId": 0x2, "name": "WonderlandKeyholeFirst", "display": "Keyhole / The Falsewood", "areaId": 0xa, },</v>
+        <v>28: { "worldId": 0x2, "name": "WonderlandKeyholeSecond", "display": "Keyhole / Fleeting Forest", "areaId": 0xb, },</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>142</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="F30" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A30,": { ""worldId"": ",C30,", ""name"": """,D30,""", ""display"": """,E30,""", ""areaId"": ",B30,", },")</f>
-        <v>28: { "worldId": 0x2, "name": "WonderlandKeyholeSecond", "display": "Keyhole / Fleeting Forest", "areaId": 0xb, },</v>
+        <v>29: { "worldId": 0x2, "name": "WonderlandKeyholeTerminus", "display": "Keyhole / Terminus", "areaId": 0xc, },</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>205</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>180</v>
       </c>
       <c r="F31" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A31,": { ""worldId"": ",C31,", ""name"": """,D31,""", ""display"": """,E31,""", ""areaId"": ",B31,", },")</f>
-        <v>29: { "worldId": 0x2, "name": "WonderlandKeyholeTerminus", "display": "Keyhole / Terminus", "areaId": 0xc, },</v>
+        <v>30: { "worldId": 0x3, "name": "OlympusOutside", "display": "Outside the Coliseum", "areaId": 0x1d, },</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>208</v>
       </c>
       <c r="F32" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A32,": { ""worldId"": ",C32,", ""name"": """,D32,""", ""display"": """,E32,""", ""areaId"": ",B32,", },")</f>
-        <v>30: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>31: { "worldId": 0x3, "name": "OlympusVestibule", "display": "Vestibule", "areaId": 0x1e, },</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F33" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A33,": { ""worldId"": ",C33,", ""name"": """,D33,""", ""display"": """,E33,""", ""areaId"": ",B33,", },")</f>
-        <v>31: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>32: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F34" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A34,": { ""worldId"": ",C34,", ""name"": """,D34,""", ""display"": """,E34,""", ""areaId"": ",B34,", },")</f>
-        <v>32: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>33: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F35" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A35,": { ""worldId"": ",C35,", ""name"": """,D35,""", ""display"": """,E35,""", ""areaId"": ",B35,", },")</f>
-        <v>33: { "worldId": , "name": "", "display": "", "areaId": , },</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="F36" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A36,": { ""worldId"": ",C36,", ""name"": """,D36,""", ""display"": """,E36,""", ""areaId"": ",B36,", },")</f>
         <v>34: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added utility function for negative pointers
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="211">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -648,6 +648,12 @@
   </si>
   <si>
     <t xml:space="preserve">Vestibule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 1</t>
   </si>
 </sst>
 </file>
@@ -775,7 +781,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -10335,10 +10341,10 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -11018,9 +11024,21 @@
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="B33" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>210</v>
+      </c>
       <c r="F33" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A33,": { ""worldId"": ",C33,", ""name"": """,D33,""", ""display"": """,E33,""", ""areaId"": ",B33,", },")</f>
-        <v>32: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>32: { "worldId": 0x3, "name": "OlympusLayer1", "display": "Layer 1", "areaId": 0x1, },</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added achievements up to Layer 5 of Olympus Coliseum
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="224">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -654,6 +654,45 @@
   </si>
   <si>
     <t xml:space="preserve">Layer 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusSave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save Room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 6</t>
   </si>
 </sst>
 </file>
@@ -781,7 +820,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -10338,13 +10377,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -11045,18 +11084,162 @@
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
+      <c r="B34" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>213</v>
+      </c>
       <c r="F34" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A34,": { ""worldId"": ",C34,", ""name"": """,D34,""", ""display"": """,E34,""", ""areaId"": ",B34,", },")</f>
-        <v>33: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>33: { "worldId": 0x3, "name": "OlympusSave", "display": "Save Room", "areaId": 0x1f, },</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
+      <c r="B35" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>215</v>
+      </c>
       <c r="F35" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A35,": { ""worldId"": ",C35,", ""name"": """,D35,""", ""display"": """,E35,""", ""areaId"": ",B35,", },")</f>
-        <v>34: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>34: { "worldId": 0x3, "name": "OlympusLayer2", "display": "Layer 2", "areaId": 0x2, },</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="F36" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A36,": { ""worldId"": ",C36,", ""name"": """,D36,""", ""display"": """,E36,""", ""areaId"": ",B36,", },")</f>
+        <v>35: { "worldId": 0x3, "name": "OlympusLayer3", "display": "Layer 3", "areaId": 0x3, },</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F37" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A37,": { ""worldId"": ",C37,", ""name"": """,D37,""", ""display"": """,E37,""", ""areaId"": ",B37,", },")</f>
+        <v>36: { "worldId": 0x3, "name": "OlympusLayer4", "display": "Layer 4", "areaId": 0x4, },</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="F38" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A38,": { ""worldId"": ",C38,", ""name"": """,D38,""", ""display"": """,E38,""", ""areaId"": ",B38,", },")</f>
+        <v>37: { "worldId": 0x3, "name": "OlympusLayer5", "display": "Layer 5", "areaId": 0x5, },</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="F39" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A39,": { ""worldId"": ",C39,", ""name"": """,D39,""", ""display"": """,E39,""", ""areaId"": ",B39,", },")</f>
+        <v>38: { "worldId": 0x3, "name": "OlympusLayer6", "display": "Layer 6", "areaId": 0x6, },</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="F40" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A40,": { ""worldId"": ",C40,", ""name"": """,D40,""", ""display"": """,E40,""", ""areaId"": ",B40,", },")</f>
+        <v>39: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="F41" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A41,": { ""worldId"": ",C41,", ""name"": """,D41,""", ""display"": """,E41,""", ""areaId"": ",B41,", },")</f>
+        <v>40: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="F42" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A42,": { ""worldId"": ",C42,", ""name"": """,D42,""", ""display"": """,E42,""", ""areaId"": ",B42,", },")</f>
+        <v>41: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="F43" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A43,": { ""worldId"": ",C43,", ""name"": """,D43,""", ""display"": """,E43,""", ""areaId"": ",B43,", },")</f>
+        <v>42: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added achievements up to the end of Olympus Coliseum, Layer 15.
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="244">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -693,6 +693,66 @@
   </si>
   <si>
     <t xml:space="preserve">Layer 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 15</t>
   </si>
 </sst>
 </file>
@@ -820,7 +880,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -10377,13 +10437,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -11210,36 +11270,207 @@
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
+      <c r="B40" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>225</v>
+      </c>
       <c r="F40" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A40,": { ""worldId"": ",C40,", ""name"": """,D40,""", ""display"": """,E40,""", ""areaId"": ",B40,", },")</f>
-        <v>39: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>39: { "worldId": 0x3, "name": "OlympusLayer7", "display": "Layer 7", "areaId": 0x7, },</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="B41" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>227</v>
+      </c>
       <c r="F41" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A41,": { ""worldId"": ",C41,", ""name"": """,D41,""", ""display"": """,E41,""", ""areaId"": ",B41,", },")</f>
-        <v>40: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>40: { "worldId": 0x3, "name": "OlympusLayer8", "display": "Layer 8", "areaId": 0x8, },</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
+      <c r="B42" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>229</v>
+      </c>
       <c r="F42" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A42,": { ""worldId"": ",C42,", ""name"": """,D42,""", ""display"": """,E42,""", ""areaId"": ",B42,", },")</f>
-        <v>41: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>41: { "worldId": 0x3, "name": "OlympusLayer9", "display": "Layer 9", "areaId": 0x9, },</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
+      <c r="B43" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>231</v>
+      </c>
       <c r="F43" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A43,": { ""worldId"": ",C43,", ""name"": """,D43,""", ""display"": """,E43,""", ""areaId"": ",B43,", },")</f>
-        <v>42: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>42: { "worldId": 0x3, "name": "OlympusLayer10", "display": "Layer 10", "areaId": 0xa, },</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="F44" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A44,": { ""worldId"": ",C44,", ""name"": """,D44,""", ""display"": """,E44,""", ""areaId"": ",B44,", },")</f>
+        <v>43: { "worldId": 0x3, "name": "OlympusLayer11", "display": "Layer 11", "areaId": 0xb, },</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="F45" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A45,": { ""worldId"": ",C45,", ""name"": """,D45,""", ""display"": """,E45,""", ""areaId"": ",B45,", },")</f>
+        <v>44: { "worldId": 0x3, "name": "OlympusLayer12", "display": "Layer 12", "areaId": 0xc, },</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="F46" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A46,": { ""worldId"": ",C46,", ""name"": """,D46,""", ""display"": """,E46,""", ""areaId"": ",B46,", },")</f>
+        <v>45: { "worldId": 0x3, "name": "OlympusLayer13", "display": "Layer 13", "areaId": 0xd, },</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="F47" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A47,": { ""worldId"": ",C47,", ""name"": """,D47,""", ""display"": """,E47,""", ""areaId"": ",B47,", },")</f>
+        <v>46: { "worldId": 0x3, "name": "OlympusLayer14", "display": "Layer 14", "areaId": 0xe, },</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="F48" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A48,": { ""worldId"": ",C48,", ""name"": """,D48,""", ""display"": """,E48,""", ""areaId"": ",B48,", },")</f>
+        <v>47: { "worldId": 0x3, "name": "OlympusLayer15", "display": "Layer 15", "areaId": 0x21, },</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="F49" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A49,": { ""worldId"": ",C49,", ""name"": """,D49,""", ""display"": """,E49,""", ""areaId"": ",B49,", },")</f>
+        <v>48: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="F50" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A50,": { ""worldId"": ",C50,", ""name"": """,D50,""", ""display"": """,E50,""", ""areaId"": ",B50,", },")</f>
+        <v>49: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Locations and prize blox flags
Added locations and prize blox flags, as well as dummied out logic for an achievement idea that I had that probably won't pan out very well.
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="269">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -753,6 +753,81 @@
   </si>
   <si>
     <t xml:space="preserve">Layer 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahPlaza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plaza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahAlley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahStreet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahPalace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palace Gates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahPlazaFrozen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahPalaceFrozen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahStreetFrozen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahAlleyFrozen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahCaveEntranceNoEntry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cave / Entrance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahBazaarFrozen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bazaar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahBazaar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahCaveEntrance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahCaveBeginnings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cave / Hall of Beginnings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahGauntlet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cave / Gauntlet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahGauntletLower</t>
   </si>
 </sst>
 </file>
@@ -880,7 +955,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -10437,13 +10512,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -11459,18 +11534,396 @@
       <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
+      <c r="B49" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>245</v>
+      </c>
       <c r="F49" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A49,": { ""worldId"": ",C49,", ""name"": """,D49,""", ""display"": """,E49,""", ""areaId"": ",B49,", },")</f>
-        <v>48: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>48: { "worldId": 0x4, "name": "AgrabahPlaza", "display": "Plaza", "areaId": 0x6, },</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
+      <c r="B50" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>247</v>
+      </c>
       <c r="F50" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A50,": { ""worldId"": ",C50,", ""name"": """,D50,""", ""display"": """,E50,""", ""areaId"": ",B50,", },")</f>
-        <v>49: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>49: { "worldId": 0x4, "name": "AgrabahAlley", "display": "Alley", "areaId": 0x8, },</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="F51" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A51,": { ""worldId"": ",C51,", ""name"": """,D51,""", ""display"": """,E51,""", ""areaId"": ",B51,", },")</f>
+        <v>50: { "worldId": 0x4, "name": "AgrabahStreet", "display": "Main Street", "areaId": 0x2, },</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="F52" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A52,": { ""worldId"": ",C52,", ""name"": """,D52,""", ""display"": """,E52,""", ""areaId"": ",B52,", },")</f>
+        <v>51: { "worldId": 0x4, "name": "AgrabahPalace", "display": "Palace Gates", "areaId": 0x3, },</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="F53" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A53,": { ""worldId"": ",C53,", ""name"": """,D53,""", ""display"": """,E53,""", ""areaId"": ",B53,", },")</f>
+        <v>52: { "worldId": 0x4, "name": "AgrabahPlazaFrozen", "display": "Plaza", "areaId": 0xa, },</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="F54" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A54,": { ""worldId"": ",C54,", ""name"": """,D54,""", ""display"": """,E54,""", ""areaId"": ",B54,", },")</f>
+        <v>53: { "worldId": 0x4, "name": "AgrabahPalaceFrozen", "display": "Palace Gates", "areaId": 0xc, },</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="F55" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A55,": { ""worldId"": ",C55,", ""name"": """,D55,""", ""display"": """,E55,""", ""areaId"": ",B55,", },")</f>
+        <v>54: { "worldId": 0x4, "name": "AgrabahStreetFrozen", "display": "Main Street", "areaId": 0xb, },</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="F56" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A56,": { ""worldId"": ",C56,", ""name"": """,D56,""", ""display"": """,E56,""", ""areaId"": ",B56,", },")</f>
+        <v>55: { "worldId": 0x4, "name": "AgrabahAlleyFrozen", "display": "Alley", "areaId": 0xd, },</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="F57" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A57,": { ""worldId"": ",C57,", ""name"": """,D57,""", ""display"": """,E57,""", ""areaId"": ",B57,", },")</f>
+        <v>56: { "worldId": 0x4, "name": "AgrabahCaveEntranceNoEntry", "display": "Cave / Entrance", "areaId": 0x12, },</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="F58" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A58,": { ""worldId"": ",C58,", ""name"": """,D58,""", ""display"": """,E58,""", ""areaId"": ",B58,", },")</f>
+        <v>57: { "worldId": 0x4, "name": "AgrabahBazaarFrozen", "display": "Bazaar", "areaId": 0xe, },</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="F59" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A59,": { ""worldId"": ",C59,", ""name"": """,D59,""", ""display"": """,E59,""", ""areaId"": ",B59,", },")</f>
+        <v>58: { "worldId": 0x4, "name": "AgrabahBazaar", "display": "Bazaar", "areaId": 0x9, },</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="F60" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A60,": { ""worldId"": ",C60,", ""name"": """,D60,""", ""display"": """,E60,""", ""areaId"": ",B60,", },")</f>
+        <v>59: { "worldId": 0x4, "name": "AgrabahCaveEntrance", "display": "Cave / Entrance", "areaId": 0x1, },</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="F61" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A61,": { ""worldId"": ",C61,", ""name"": """,D61,""", ""display"": """,E61,""", ""areaId"": ",B61,", },")</f>
+        <v>60: { "worldId": 0x4, "name": "AgrabahCaveBeginnings", "display": "Cave / Hall of Beginnings", "areaId": 0x4, },</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="F62" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A62,": { ""worldId"": ",C62,", ""name"": """,D62,""", ""display"": """,E62,""", ""areaId"": ",B62,", },")</f>
+        <v>61: { "worldId": 0x4, "name": "AgrabahGauntlet", "display": "Cave / Gauntlet", "areaId": 0x5, },</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="F63" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A63,": { ""worldId"": ",C63,", ""name"": """,D63,""", ""display"": """,E63,""", ""areaId"": ",B63,", },")</f>
+        <v>62: { "worldId": 0x4, "name": "AgrabahGauntletLower", "display": "Cave / Gauntlet", "areaId": 0x11, },</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="F64" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A64,": { ""worldId"": ",C64,", ""name"": """,D64,""", ""display"": """,E64,""", ""areaId"": ",B64,", },")</f>
+        <v>63: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="F65" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A65,": { ""worldId"": ",C65,", ""name"": """,D65,""", ""display"": """,E65,""", ""areaId"": ",B65,", },")</f>
+        <v>64: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="F66" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A66,": { ""worldId"": ",C66,", ""name"": """,D66,""", ""display"": """,E66,""", ""areaId"": ",B66,", },")</f>
+        <v>65: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="F67" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A67,": { ""worldId"": ",C67,", ""name"": """,D67,""", ""display"": """,E67,""", ""areaId"": ",B67,", },")</f>
+        <v>66: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="F68" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A68,": { ""worldId"": ",C68,", ""name"": """,D68,""", ""display"": """,E68,""", ""areaId"": ",B68,", },")</f>
+        <v>67: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="F69" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A69,": { ""worldId"": ",C69,", ""name"": """,D69,""", ""display"": """,E69,""", ""areaId"": ",B69,", },")</f>
+        <v>68: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="F70" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A70,": { ""worldId"": ",C70,", ""name"": """,D70,""", ""display"": """,E70,""", ""areaId"": ",B70,", },")</f>
+        <v>69: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="F71" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A71,": { ""worldId"": ",C71,", ""name"": """,D71,""", ""display"": """,E71,""", ""areaId"": ",B71,", },")</f>
+        <v>70: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="F72" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A72,": { ""worldId"": ",C72,", ""name"": """,D72,""", ""display"": """,E72,""", ""areaId"": ",B72,", },")</f>
+        <v>71: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added WIP achievements and leaderboards up to the end of the Agrabah Keyhole
"Keyblade Beats Rock" is unfinished.
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="273">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -828,6 +828,18 @@
   </si>
   <si>
     <t xml:space="preserve">AgrabahGauntletLower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahLamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cave / Lamp Chamber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahKeyholeTerminus</t>
   </si>
 </sst>
 </file>
@@ -955,7 +967,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -10514,11 +10526,11 @@
   </sheetPr>
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E66" activeCellId="0" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -11849,18 +11861,42 @@
       <c r="A64" s="0" t="n">
         <v>63</v>
       </c>
+      <c r="B64" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>270</v>
+      </c>
       <c r="F64" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A64,": { ""worldId"": ",C64,", ""name"": """,D64,""", ""display"": """,E64,""", ""areaId"": ",B64,", },")</f>
-        <v>63: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>63: { "worldId": 0x4, "name": "AgrabahLamp", "display": "Cave / Lamp Chamber", "areaId": 0x7, },</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>64</v>
       </c>
+      <c r="B65" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>176</v>
+      </c>
       <c r="F65" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A65,": { ""worldId"": ",C65,", ""name"": """,D65,""", ""display"": """,E65,""", ""areaId"": ",B65,", },")</f>
-        <v>64: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>64: { "worldId": 0x4, "name": "AgrabahKeyholeTerminus", "display": "Keyhole / Terminus", "areaId": 0xf, },</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
More areas added to RP and updated "Justice for All"
"Justice for All" was just checking for the trophy bit. This update adds Measured functionality.
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="281">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -840,6 +840,30 @@
   </si>
   <si>
     <t xml:space="preserve">AgrabahKeyholeTerminus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionGates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castle Gates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionWaterway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waterway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionEntranceLower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrance Hall (Lower Level)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionLibrary1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library 1</t>
   </si>
 </sst>
 </file>
@@ -967,7 +991,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -10527,10 +10551,10 @@
   <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E66" activeCellId="0" sqref="E66"/>
+      <selection pane="topLeft" activeCell="B70" activeCellId="0" sqref="B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -11903,36 +11927,84 @@
       <c r="A66" s="0" t="n">
         <v>65</v>
       </c>
+      <c r="B66" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>274</v>
+      </c>
       <c r="F66" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A66,": { ""worldId"": ",C66,", ""name"": """,D66,""", ""display"": """,E66,""", ""areaId"": ",B66,", },")</f>
-        <v>65: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>65: { "worldId": 0x5, "name": "HollowBastionGates", "display": "Castle Gates", "areaId": 0x2, },</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>66</v>
       </c>
+      <c r="B67" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>276</v>
+      </c>
       <c r="F67" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A67,": { ""worldId"": ",C67,", ""name"": """,D67,""", ""display"": """,E67,""", ""areaId"": ",B67,", },")</f>
-        <v>66: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>66: { "worldId": 0x5, "name": "HollowBastionWaterway", "display": "Waterway", "areaId": 0x3, },</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>67</v>
       </c>
+      <c r="B68" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>278</v>
+      </c>
       <c r="F68" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A68,": { ""worldId"": ",C68,", ""name"": """,D68,""", ""display"": """,E68,""", ""areaId"": ",B68,", },")</f>
-        <v>67: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>67: { "worldId": 0x5, "name": "HollowBastionEntranceLower", "display": "Entrance Hall (Lower Level)", "areaId": 0x4, },</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>68</v>
       </c>
+      <c r="B69" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>280</v>
+      </c>
       <c r="F69" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A69,": { ""worldId"": ",C69,", ""name"": """,D69,""", ""display"": """,E69,""", ""areaId"": ",B69,", },")</f>
-        <v>68: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>68: { "worldId": 0x5, "name": "HollowBastionLibrary1", "display": "Library 1", "areaId": 0x6, },</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Additional RP locations and sector rewards
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="295">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -864,6 +864,48 @@
   </si>
   <si>
     <t xml:space="preserve">Library 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionLibrary3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionLibrary4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionLibrary2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionEntranceUpper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrance Hall (Upper Level)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionCrest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Crest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionTower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Tower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionGrandHall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Hall(?)</t>
   </si>
 </sst>
 </file>
@@ -10548,10 +10590,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B70" activeCellId="0" sqref="B70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B77" activeCellId="0" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12011,27 +12053,228 @@
       <c r="A70" s="0" t="n">
         <v>69</v>
       </c>
+      <c r="B70" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>282</v>
+      </c>
       <c r="F70" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A70,": { ""worldId"": ",C70,", ""name"": """,D70,""", ""display"": """,E70,""", ""areaId"": ",B70,", },")</f>
-        <v>69: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>69: { "worldId": 0x5, "name": "HollowBastionLibrary3", "display": "Library 3", "areaId": 0x8, },</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>70</v>
       </c>
+      <c r="B71" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>284</v>
+      </c>
       <c r="F71" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A71,": { ""worldId"": ",C71,", ""name"": """,D71,""", ""display"": """,E71,""", ""areaId"": ",B71,", },")</f>
-        <v>70: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>70: { "worldId": 0x5, "name": "HollowBastionLibrary4", "display": "Library 4", "areaId": 0x9, },</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>71</v>
       </c>
+      <c r="B72" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>286</v>
+      </c>
       <c r="F72" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A72,": { ""worldId"": ",C72,", ""name"": """,D72,""", ""display"": """,E72,""", ""areaId"": ",B72,", },")</f>
-        <v>71: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>71: { "worldId": 0x5, "name": "HollowBastionLibrary2", "display": "Library 2", "areaId": 0x7, },</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="F73" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A73,": { ""worldId"": ",C73,", ""name"": """,D73,""", ""display"": """,E73,""", ""areaId"": ",B73,", },")</f>
+        <v>72: { "worldId": 0x5, "name": "HollowBastionEntranceUpper", "display": "Entrance Hall (Upper Level)", "areaId": 0x5, },</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="F74" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A74,": { ""worldId"": ",C74,", ""name"": """,D74,""", ""display"": """,E74,""", ""areaId"": ",B74,", },")</f>
+        <v>73: { "worldId": 0x5, "name": "HollowBastionCrest", "display": "Great Crest", "areaId": 0xa, },</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="F75" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A75,": { ""worldId"": ",C75,", ""name"": """,D75,""", ""display"": """,E75,""", ""areaId"": ",B75,", },")</f>
+        <v>74: { "worldId": 0x5, "name": "HollowBastionTower", "display": "High Tower", "areaId": 0xb, },</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="F76" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A76,": { ""worldId"": ",C76,", ""name"": """,D76,""", ""display"": """,E76,""", ""areaId"": ",B76,", },")</f>
+        <v>75: { "worldId": 0x5, "name": "HollowBastionGrandHall", "display": "Grand Hall(?)", "areaId": 0xd, },</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="F77" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A77,": { ""worldId"": ",C77,", ""name"": """,D77,""", ""display"": """,E77,""", ""areaId"": ",B77,", },")</f>
+        <v>76: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="F78" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A78,": { ""worldId"": ",C78,", ""name"": """,D78,""", ""display"": """,E78,""", ""areaId"": ",B78,", },")</f>
+        <v>77: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="F79" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A79,": { ""worldId"": ",C79,", ""name"": """,D79,""", ""display"": """,E79,""", ""areaId"": ",B79,", },")</f>
+        <v>78: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="F80" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A80,": { ""worldId"": ",C80,", ""name"": """,D80,""", ""display"": """,E80,""", ""areaId"": ",B80,", },")</f>
+        <v>79: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="F81" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A81,": { ""worldId"": ",C81,", ""name"": """,D81,""", ""display"": """,E81,""", ""areaId"": ",B81,", },")</f>
+        <v>80: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="F82" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A82,": { ""worldId"": ",C82,", ""name"": """,D82,""", ""display"": """,E82,""", ""areaId"": ",B82,", },")</f>
+        <v>81: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="F83" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A83,": { ""worldId"": ",C83,", ""name"": """,D83,""", ""display"": """,E83,""", ""areaId"": ",B83,", },")</f>
+        <v>82: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="F84" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A84,": { ""worldId"": ",C84,", ""name"": """,D84,""", ""display"": """,E84,""", ""areaId"": ",B84,", },")</f>
+        <v>83: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="F85" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A85,": { ""worldId"": ",C85,", ""name"": """,D85,""", ""display"": """,E85,""", ""areaId"": ",B85,", },")</f>
+        <v>84: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added "My Friends Are My Power, I Guess"
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="299">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -906,6 +906,18 @@
   </si>
   <si>
     <t xml:space="preserve">Grand Hall(?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionKeyholeEntrance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somewhere in the datascape…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionKeyholeChapel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyhole / Chapel</t>
   </si>
 </sst>
 </file>
@@ -10592,8 +10604,8 @@
   </sheetPr>
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B77" activeCellId="0" sqref="B77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B79" activeCellId="0" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12200,18 +12212,42 @@
       <c r="A77" s="0" t="n">
         <v>76</v>
       </c>
+      <c r="B77" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>296</v>
+      </c>
       <c r="F77" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A77,": { ""worldId"": ",C77,", ""name"": """,D77,""", ""display"": """,E77,""", ""areaId"": ",B77,", },")</f>
-        <v>76: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>76: { "worldId": 0x5, "name": "HollowBastionKeyholeEntrance", "display": "Somewhere in the datascape…", "areaId": 0x0, },</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>77</v>
       </c>
+      <c r="B78" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>298</v>
+      </c>
       <c r="F78" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A78,": { ""worldId"": ",C78,", ""name"": """,D78,""", ""display"": """,E78,""", ""areaId"": ",B78,", },")</f>
-        <v>77: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>77: { "worldId": 0x5, "name": "HollowBastionKeyholeChapel", "display": "Keyhole / Chapel", "areaId": 0xc, },</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Code for "Waste Not, Want Not"
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Locations" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Command Conversion Combinations" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1898" uniqueCount="484">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -918,6 +920,561 @@
   </si>
   <si>
     <t xml:space="preserve">Keyhole / Chapel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick Blitz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sliding Dash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Round Blitz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strike Raid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rising Strike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sliding Rush</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerial Sweep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air Sweep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerial Slam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land Crash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire Edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blizzard Edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thunder Edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aero Edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Dash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Dash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spark Dash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind Dash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire Blast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blizzard Blast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thunder Blast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aero Blast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire Raid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blizzard Raid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thunder Raid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aero Raid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire Buster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blizzard Buster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thunder Buster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aero Buster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Sweep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Sweep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spark Sweep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind Sweep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Storm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Storm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spark Storm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind Storm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire Slam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blizzard Slam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thunder Slam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aero Slam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Dive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Dive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spark Dive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind Dive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stun Impact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x2f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muscle Strike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chain Rave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rising Rush</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zantetsuken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eruption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gravity Drop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shock Fall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judgment Triad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x3a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blizzard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x3b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blizzara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x3c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blizzaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thunder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x3e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thundara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x3f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thundaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aerora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aeroga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x4a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x4b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x4c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firaga Burst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x4d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triple Firaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x4e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triple Burst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x4f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blizzaga Pursuit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triple Blizzaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triple Pursuit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thunder Tracer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulse Tracer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tornado Tracer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind Tracer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnet Grab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esuna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flame Fall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Icicle Mine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x5a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exo Spark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x5b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyclone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x5c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slot A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slot B</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1562,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1019,6 +1576,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1041,11 +1602,11 @@
   </sheetPr>
   <dimension ref="A1:D681"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A642" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -10604,11 +11165,11 @@
   </sheetPr>
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B79" activeCellId="0" sqref="B79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -12312,6 +12873,1553 @@
         <f aca="false">_xlfn.CONCAT( ,A85,": { ""worldId"": ",C85,", ""name"": """,D85,""", ""display"": """,E85,""", ""areaId"": ",B85,", },")</f>
         <v>84: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C95"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""", },")</f>
+        <v>0xFF: { "id": 0xFF, "name": "N/A", },</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="C3" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""", },")</f>
+        <v>0x00: { "id": 0x00, "name": "Quick Blitz", },</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""", },")</f>
+        <v>0x01: { "id": 0x01, "name": "Sliding Dash", },</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""", },")</f>
+        <v>0x02: { "id": 0x02, "name": "Round Blitz", },</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""", },")</f>
+        <v>0x03: { "id": 0x03, "name": "Strike Raid", },</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""", },")</f>
+        <v>0x04: { "id": 0x04, "name": "Rising Strike", },</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="C8" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""", },")</f>
+        <v>0x05: { "id": 0x05, "name": "Sliding Rush", },</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""", },")</f>
+        <v>0x06: { "id": 0x06, "name": "Aerial Sweep", },</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="C10" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""", },")</f>
+        <v>0x07: { "id": 0x07, "name": "Air Sweep", },</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""", },")</f>
+        <v>0x08: { "id": 0x08, "name": "Aerial Slam", },</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="C12" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""", },")</f>
+        <v>0x09: { "id": 0x09, "name": "Land Crash", },</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A13,": { ""id"": ",A13,", ""name"": """,B13,""", },")</f>
+        <v>0x0a: { "id": 0x0a, "name": "Fire Edge", },</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A14,": { ""id"": ",A14,", ""name"": """,B14,""", },")</f>
+        <v>0x0b: { "id": 0x0b, "name": "Blizzard Edge", },</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A15,": { ""id"": ",A15,", ""name"": """,B15,""", },")</f>
+        <v>0x0c: { "id": 0x0c, "name": "Thunder Edge", },</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A16,": { ""id"": ",A16,", ""name"": """,B16,""", },")</f>
+        <v>0x0d: { "id": 0x0d, "name": "Aero Edge", },</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="C17" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A17,": { ""id"": ",A17,", ""name"": """,B17,""", },")</f>
+        <v>0x0e: { "id": 0x0e, "name": "Heat Dash", },</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="C18" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A18,": { ""id"": ",A18,", ""name"": """,B18,""", },")</f>
+        <v>0x0f: { "id": 0x0f, "name": "Ice Dash", },</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="C19" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A19,": { ""id"": ",A19,", ""name"": """,B19,""", },")</f>
+        <v>0x10: { "id": 0x10, "name": "Spark Dash", },</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="C20" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A20,": { ""id"": ",A20,", ""name"": """,B20,""", },")</f>
+        <v>0x11: { "id": 0x11, "name": "Wind Dash", },</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="C21" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A21,": { ""id"": ",A21,", ""name"": """,B21,""", },")</f>
+        <v>0x12: { "id": 0x12, "name": "Fire Blast", },</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="C22" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A22,": { ""id"": ",A22,", ""name"": """,B22,""", },")</f>
+        <v>0x13: { "id": 0x13, "name": "Blizzard Blast", },</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="C23" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A23,": { ""id"": ",A23,", ""name"": """,B23,""", },")</f>
+        <v>0x14: { "id": 0x14, "name": "Thunder Blast", },</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="C24" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A24,": { ""id"": ",A24,", ""name"": """,B24,""", },")</f>
+        <v>0x15: { "id": 0x15, "name": "Aero Blast", },</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="C25" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A25,": { ""id"": ",A25,", ""name"": """,B25,""", },")</f>
+        <v>0x16: { "id": 0x16, "name": "Fire Raid", },</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C26" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A26,": { ""id"": ",A26,", ""name"": """,B26,""", },")</f>
+        <v>0x17: { "id": 0x17, "name": "Blizzard Raid", },</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="C27" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A27,": { ""id"": ",A27,", ""name"": """,B27,""", },")</f>
+        <v>0x18: { "id": 0x18, "name": "Thunder Raid", },</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="C28" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A28,": { ""id"": ",A28,", ""name"": """,B28,""", },")</f>
+        <v>0x19: { "id": 0x19, "name": "Aero Raid", },</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="C29" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A29,": { ""id"": ",A29,", ""name"": """,B29,""", },")</f>
+        <v>0x1a: { "id": 0x1a, "name": "Fire Buster", },</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="C30" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A30,": { ""id"": ",A30,", ""name"": """,B30,""", },")</f>
+        <v>0x1b: { "id": 0x1b, "name": "Blizzard Buster", },</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="C31" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A31,": { ""id"": ",A31,", ""name"": """,B31,""", },")</f>
+        <v>0x1c: { "id": 0x1c, "name": "Thunder Buster", },</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="C32" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A32,": { ""id"": ",A32,", ""name"": """,B32,""", },")</f>
+        <v>0x1d: { "id": 0x1d, "name": "Aero Buster", },</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="C33" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A33,": { ""id"": ",A33,", ""name"": """,B33,""", },")</f>
+        <v>0x1e: { "id": 0x1e, "name": "Heat Sweep", },</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="C34" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A34,": { ""id"": ",A34,", ""name"": """,B34,""", },")</f>
+        <v>0x1f: { "id": 0x1f, "name": "Ice Sweep", },</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="C35" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A35,": { ""id"": ",A35,", ""name"": """,B35,""", },")</f>
+        <v>0x20: { "id": 0x20, "name": "Spark Sweep", },</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="C36" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A36,": { ""id"": ",A36,", ""name"": """,B36,""", },")</f>
+        <v>0x21: { "id": 0x21, "name": "Wind Sweep", },</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="C37" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A37,": { ""id"": ",A37,", ""name"": """,B37,""", },")</f>
+        <v>0x22: { "id": 0x22, "name": "Heat Storm", },</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="C38" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A38,": { ""id"": ",A38,", ""name"": """,B38,""", },")</f>
+        <v>0x23: { "id": 0x23, "name": "Ice Storm", },</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="C39" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A39,": { ""id"": ",A39,", ""name"": """,B39,""", },")</f>
+        <v>0x24: { "id": 0x24, "name": "Spark Storm", },</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="C40" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A40,": { ""id"": ",A40,", ""name"": """,B40,""", },")</f>
+        <v>0x25: { "id": 0x25, "name": "Wind Storm", },</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="C41" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A41,": { ""id"": ",A41,", ""name"": """,B41,""", },")</f>
+        <v>0x26: { "id": 0x26, "name": "Fire Slam", },</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="C42" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A42,": { ""id"": ",A42,", ""name"": """,B42,""", },")</f>
+        <v>0x27: { "id": 0x27, "name": "Blizzard Slam", },</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="C43" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A43,": { ""id"": ",A43,", ""name"": """,B43,""", },")</f>
+        <v>0x28: { "id": 0x28, "name": "Thunder Slam", },</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="C44" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A44,": { ""id"": ",A44,", ""name"": """,B44,""", },")</f>
+        <v>0x29: { "id": 0x29, "name": "Aero Slam", },</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="C45" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A45,": { ""id"": ",A45,", ""name"": """,B45,""", },")</f>
+        <v>0x2a: { "id": 0x2a, "name": "Heat Dive", },</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="C46" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A46,": { ""id"": ",A46,", ""name"": """,B46,""", },")</f>
+        <v>0x2b: { "id": 0x2b, "name": "Ice Dive", },</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="C47" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A47,": { ""id"": ",A47,", ""name"": """,B47,""", },")</f>
+        <v>0x2c: { "id": 0x2c, "name": "Spark Dive", },</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="C48" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A48,": { ""id"": ",A48,", ""name"": """,B48,""", },")</f>
+        <v>0x2d: { "id": 0x2d, "name": "Wind Dive", },</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="C49" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A49,": { ""id"": ",A49,", ""name"": """,B49,""", },")</f>
+        <v>0x2e: { "id": 0x2e, "name": "Stun Impact", },</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="C50" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A50,": { ""id"": ",A50,", ""name"": """,B50,""", },")</f>
+        <v>0x2f: { "id": 0x2f, "name": "Muscle Strike", },</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="C51" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A51,": { ""id"": ",A51,", ""name"": """,B51,""", },")</f>
+        <v>0x30: { "id": 0x30, "name": "Chain Rave", },</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="C52" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A52,": { ""id"": ",A52,", ""name"": """,B52,""", },")</f>
+        <v>0x31: { "id": 0x31, "name": "Rising Rush", },</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="C53" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A53,": { ""id"": ",A53,", ""name"": """,B53,""", },")</f>
+        <v>0x32: { "id": 0x32, "name": "Zantetsuken", },</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="C54" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A54,": { ""id"": ",A54,", ""name"": """,B54,""", },")</f>
+        <v>0x33: { "id": 0x33, "name": "Eruption", },</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="C55" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A55,": { ""id"": ",A55,", ""name"": """,B55,""", },")</f>
+        <v>0x34: { "id": 0x34, "name": "Gravity Drop", },</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="C56" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A56,": { ""id"": ",A56,", ""name"": """,B56,""", },")</f>
+        <v>0x35: { "id": 0x35, "name": "Shock Fall", },</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="C57" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A57,": { ""id"": ",A57,", ""name"": """,B57,""", },")</f>
+        <v>0x36: { "id": 0x36, "name": "Judgment Triad", },</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="C58" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A58,": { ""id"": ",A58,", ""name"": """,B58,""", },")</f>
+        <v>0x37: { "id": 0x37, "name": "Fire", },</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="C59" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A59,": { ""id"": ",A59,", ""name"": """,B59,""", },")</f>
+        <v>0x38: { "id": 0x38, "name": "Fira", },</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="C60" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A60,": { ""id"": ",A60,", ""name"": """,B60,""", },")</f>
+        <v>0x39: { "id": 0x39, "name": "Firaga", },</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="C61" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A61,": { ""id"": ",A61,", ""name"": """,B61,""", },")</f>
+        <v>0x3a: { "id": 0x3a, "name": "Blizzard", },</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="C62" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A62,": { ""id"": ",A62,", ""name"": """,B62,""", },")</f>
+        <v>0x3b: { "id": 0x3b, "name": "Blizzara", },</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="C63" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A63,": { ""id"": ",A63,", ""name"": """,B63,""", },")</f>
+        <v>0x3c: { "id": 0x3c, "name": "Blizzaga", },</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="C64" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A64,": { ""id"": ",A64,", ""name"": """,B64,""", },")</f>
+        <v>0x3d: { "id": 0x3d, "name": "Thunder", },</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="C65" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A65,": { ""id"": ",A65,", ""name"": """,B65,""", },")</f>
+        <v>0x3e: { "id": 0x3e, "name": "Thundara", },</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="C66" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A66,": { ""id"": ",A66,", ""name"": """,B66,""", },")</f>
+        <v>0x3f: { "id": 0x3f, "name": "Thundaga", },</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="C67" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A67,": { ""id"": ",A67,", ""name"": """,B67,""", },")</f>
+        <v>0x40: { "id": 0x40, "name": "Aero", },</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="C68" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A68,": { ""id"": ",A68,", ""name"": """,B68,""", },")</f>
+        <v>0x41: { "id": 0x41, "name": "Aerora", },</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="C69" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A69,": { ""id"": ",A69,", ""name"": """,B69,""", },")</f>
+        <v>0x42: { "id": 0x42, "name": "Aeroga", },</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="C70" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A70,": { ""id"": ",A70,", ""name"": """,B70,""", },")</f>
+        <v>0x43: { "id": 0x43, "name": "Magnet", },</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="C71" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A71,": { ""id"": ",A71,", ""name"": """,B71,""", },")</f>
+        <v>0x44: { "id": 0x44, "name": "Magnera", },</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="C72" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A72,": { ""id"": ",A72,", ""name"": """,B72,""", },")</f>
+        <v>0x45: { "id": 0x45, "name": "Magnega", },</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="C73" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A73,": { ""id"": ",A73,", ""name"": """,B73,""", },")</f>
+        <v>0x46: { "id": 0x46, "name": "Cure", },</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="C74" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A74,": { ""id"": ",A74,", ""name"": """,B74,""", },")</f>
+        <v>0x47: { "id": 0x47, "name": "Cura", },</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="C75" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A75,": { ""id"": ",A75,", ""name"": """,B75,""", },")</f>
+        <v>0x48: { "id": 0x48, "name": "Curaga", },</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="C76" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A76,": { ""id"": ",A76,", ""name"": """,B76,""", },")</f>
+        <v>0x49: { "id": 0x49, "name": "Slow", },</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="C77" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A77,": { ""id"": ",A77,", ""name"": """,B77,""", },")</f>
+        <v>0x4a: { "id": 0x4a, "name": "Stop", },</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="C78" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A78,": { ""id"": ",A78,", ""name"": """,B78,""", },")</f>
+        <v>0x4b: { "id": 0x4b, "name": "Confuse", },</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="C79" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A79,": { ""id"": ",A79,", ""name"": """,B79,""", },")</f>
+        <v>0x4c: { "id": 0x4c, "name": "Firaga Burst", },</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="C80" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A80,": { ""id"": ",A80,", ""name"": """,B80,""", },")</f>
+        <v>0x4d: { "id": 0x4d, "name": "Triple Firaga", },</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="C81" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A81,": { ""id"": ",A81,", ""name"": """,B81,""", },")</f>
+        <v>0x4e: { "id": 0x4e, "name": "Triple Burst", },</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="C82" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A82,": { ""id"": ",A82,", ""name"": """,B82,""", },")</f>
+        <v>0x4f: { "id": 0x4f, "name": "Blizzaga Pursuit", },</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="C83" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A83,": { ""id"": ",A83,", ""name"": """,B83,""", },")</f>
+        <v>0x50: { "id": 0x50, "name": "Triple Blizzaga", },</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="C84" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A84,": { ""id"": ",A84,", ""name"": """,B84,""", },")</f>
+        <v>0x51: { "id": 0x51, "name": "Triple Pursuit", },</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="C85" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A85,": { ""id"": ",A85,", ""name"": """,B85,""", },")</f>
+        <v>0x52: { "id": 0x52, "name": "Thunder Tracer", },</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="C86" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A86,": { ""id"": ",A86,", ""name"": """,B86,""", },")</f>
+        <v>0x53: { "id": 0x53, "name": "Pulse Tracer", },</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="C87" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A87,": { ""id"": ",A87,", ""name"": """,B87,""", },")</f>
+        <v>0x54: { "id": 0x54, "name": "Tornado Tracer", },</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="C88" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A88,": { ""id"": ",A88,", ""name"": """,B88,""", },")</f>
+        <v>0x55: { "id": 0x55, "name": "Wind Tracer", },</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="C89" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A89,": { ""id"": ",A89,", ""name"": """,B89,""", },")</f>
+        <v>0x56: { "id": 0x56, "name": "Magnet Grab", },</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="C90" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A90,": { ""id"": ",A90,", ""name"": """,B90,""", },")</f>
+        <v>0x57: { "id": 0x57, "name": "Esuna", },</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="C91" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A91,": { ""id"": ",A91,", ""name"": """,B91,""", },")</f>
+        <v>0x58: { "id": 0x58, "name": "Flame Fall", },</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C92" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A92,": { ""id"": ",A92,", ""name"": """,B92,""", },")</f>
+        <v>0x59: { "id": 0x59, "name": "Icicle Mine", },</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="C93" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A93,": { ""id"": ",A93,", ""name"": """,B93,""", },")</f>
+        <v>0x5a: { "id": 0x5a, "name": "Exo Spark", },</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="C94" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A94,": { ""id"": ",A94,", ""name"": """,B94,""", },")</f>
+        <v>0x5b: { "id": 0x5b, "name": "Cyclone", },</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="C95" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A95,": { ""id"": ",A95,", ""name"": """,B95,""", },")</f>
+        <v>0x5c: { "id": 0x5c, "name": "Quake", },</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A2,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B2, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C2, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D2, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>0: { "targetId": 0x46, "command1Id": 0x02, "command2Id": 0x49, },</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A3,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B3, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C3, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D3, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>1: { "targetId": 0x47, "command1Id": 0x17, "command2Id": 0x46, },</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A4,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B4, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C4, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D4, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>2: { "targetId": 0x47, "command1Id": 0x44, "command2Id": 0x46, },</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="E5" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A5,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B5, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C5, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D5, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>3: { "targetId": 0x47, "command1Id": 0x49, "command2Id": 0x46, },</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A6,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B6, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C6, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D6, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>4: { "targetId": 0x47, "command1Id": 0x4a, "command2Id": 0x46, },</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A7,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B7, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C7, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D7, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>5: { "targetId": 0x48, "command1Id": 0x2a, "command2Id": 0x47, },</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A8,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B8, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C8, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D8, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>6: { "targetId": 0x48, "command1Id": 0x4b, "command2Id": 0x47, },</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A9,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B9, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C9, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D9, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>7: { "targetId": 0x48, "command1Id": 0x57, "command2Id": 0x47, },</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A10,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B10, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C10, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D10, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A11,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B11, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C11, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D11, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A12,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B12, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C12, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D12, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A13,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B13, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C13, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D13, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E14" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A14,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B14, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C14, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D14, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E15" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A15,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B15, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C15, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D15, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E16" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A16,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B16, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C16, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D16, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E17" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A17,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B17, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C17, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D17, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E18" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A18,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B18, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C18, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D18, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E19" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A19,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B19, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C19, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D19, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="E20" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A20,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B20, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C20, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D20, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E21" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A21,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B21, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C21, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D21, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E22" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A22,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B22, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C22, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D22, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E23" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A23,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B23, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C23, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D23, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E24" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A24,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B24, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C24, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D24, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="E25" s="0" t="e">
+        <f aca="true">_xlfn.CONCAT(A25,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B25, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C25, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D25, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added achievements and leaderboards up to the end of Hollow Bastion I
Also added "High-Stakes Gambler".
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1898" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1902" uniqueCount="486">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -920,6 +920,12 @@
   </si>
   <si>
     <t xml:space="preserve">Keyhole / Chapel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionIIInsideRiku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inside Riku’s Data</t>
   </si>
   <si>
     <t xml:space="preserve">0xFF</t>
@@ -11165,8 +11171,8 @@
   </sheetPr>
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D80" activeCellId="0" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12815,9 +12821,21 @@
       <c r="A79" s="0" t="n">
         <v>78</v>
       </c>
+      <c r="B79" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>300</v>
+      </c>
       <c r="F79" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A79,": { ""worldId"": ",C79,", ""name"": """,D79,""", ""display"": """,E79,""", ""areaId"": ",B79,", },")</f>
-        <v>78: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>78: { "worldId": 0x6, "name": "HollowBastionIIInsideRiku", "display": "Inside Riku’s Data", "areaId": 0x8, },</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12892,8 +12910,8 @@
   </sheetPr>
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F63" activeCellId="0" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12915,10 +12933,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""", },")</f>
@@ -12927,10 +12945,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""", },")</f>
@@ -12939,10 +12957,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""", },")</f>
@@ -12951,10 +12969,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""", },")</f>
@@ -12963,10 +12981,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""", },")</f>
@@ -12975,10 +12993,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""", },")</f>
@@ -12987,10 +13005,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""", },")</f>
@@ -12999,10 +13017,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""", },")</f>
@@ -13011,10 +13029,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""", },")</f>
@@ -13023,10 +13041,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""", },")</f>
@@ -13035,10 +13053,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""", },")</f>
@@ -13047,10 +13065,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A13,": { ""id"": ",A13,", ""name"": """,B13,""", },")</f>
@@ -13059,10 +13077,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A14,": { ""id"": ",A14,", ""name"": """,B14,""", },")</f>
@@ -13071,10 +13089,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A15,": { ""id"": ",A15,", ""name"": """,B15,""", },")</f>
@@ -13083,10 +13101,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A16,": { ""id"": ",A16,", ""name"": """,B16,""", },")</f>
@@ -13095,10 +13113,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A17,": { ""id"": ",A17,", ""name"": """,B17,""", },")</f>
@@ -13107,10 +13125,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A18,": { ""id"": ",A18,", ""name"": """,B18,""", },")</f>
@@ -13119,10 +13137,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A19,": { ""id"": ",A19,", ""name"": """,B19,""", },")</f>
@@ -13134,7 +13152,7 @@
         <v>267</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A20,": { ""id"": ",A20,", ""name"": """,B20,""", },")</f>
@@ -13146,7 +13164,7 @@
         <v>256</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A21,": { ""id"": ",A21,", ""name"": """,B21,""", },")</f>
@@ -13155,10 +13173,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A22,": { ""id"": ",A22,", ""name"": """,B22,""", },")</f>
@@ -13167,10 +13185,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C23" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A23,": { ""id"": ",A23,", ""name"": """,B23,""", },")</f>
@@ -13179,10 +13197,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C24" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A24,": { ""id"": ",A24,", ""name"": """,B24,""", },")</f>
@@ -13191,10 +13209,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C25" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A25,": { ""id"": ",A25,", ""name"": """,B25,""", },")</f>
@@ -13203,10 +13221,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C26" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A26,": { ""id"": ",A26,", ""name"": """,B26,""", },")</f>
@@ -13215,10 +13233,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C27" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A27,": { ""id"": ",A27,", ""name"": """,B27,""", },")</f>
@@ -13227,10 +13245,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C28" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A28,": { ""id"": ",A28,", ""name"": """,B28,""", },")</f>
@@ -13239,10 +13257,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C29" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A29,": { ""id"": ",A29,", ""name"": """,B29,""", },")</f>
@@ -13251,10 +13269,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C30" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A30,": { ""id"": ",A30,", ""name"": """,B30,""", },")</f>
@@ -13263,10 +13281,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C31" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A31,": { ""id"": ",A31,", ""name"": """,B31,""", },")</f>
@@ -13278,7 +13296,7 @@
         <v>203</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C32" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A32,": { ""id"": ",A32,", ""name"": """,B32,""", },")</f>
@@ -13290,7 +13308,7 @@
         <v>206</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C33" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A33,": { ""id"": ",A33,", ""name"": """,B33,""", },")</f>
@@ -13302,7 +13320,7 @@
         <v>211</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C34" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A34,": { ""id"": ",A34,", ""name"": """,B34,""", },")</f>
@@ -13311,10 +13329,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C35" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A35,": { ""id"": ",A35,", ""name"": """,B35,""", },")</f>
@@ -13326,7 +13344,7 @@
         <v>241</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C36" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A36,": { ""id"": ",A36,", ""name"": """,B36,""", },")</f>
@@ -13335,10 +13353,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C37" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A37,": { ""id"": ",A37,", ""name"": """,B37,""", },")</f>
@@ -13347,10 +13365,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C38" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A38,": { ""id"": ",A38,", ""name"": """,B38,""", },")</f>
@@ -13359,10 +13377,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C39" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A39,": { ""id"": ",A39,", ""name"": """,B39,""", },")</f>
@@ -13371,10 +13389,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C40" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A40,": { ""id"": ",A40,", ""name"": """,B40,""", },")</f>
@@ -13383,10 +13401,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C41" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A41,": { ""id"": ",A41,", ""name"": """,B41,""", },")</f>
@@ -13395,10 +13413,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C42" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A42,": { ""id"": ",A42,", ""name"": """,B42,""", },")</f>
@@ -13407,10 +13425,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C43" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A43,": { ""id"": ",A43,", ""name"": """,B43,""", },")</f>
@@ -13419,10 +13437,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C44" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A44,": { ""id"": ",A44,", ""name"": """,B44,""", },")</f>
@@ -13431,10 +13449,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C45" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A45,": { ""id"": ",A45,", ""name"": """,B45,""", },")</f>
@@ -13443,10 +13461,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C46" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A46,": { ""id"": ",A46,", ""name"": """,B46,""", },")</f>
@@ -13455,10 +13473,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C47" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A47,": { ""id"": ",A47,", ""name"": """,B47,""", },")</f>
@@ -13467,10 +13485,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C48" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A48,": { ""id"": ",A48,", ""name"": """,B48,""", },")</f>
@@ -13479,10 +13497,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C49" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A49,": { ""id"": ",A49,", ""name"": """,B49,""", },")</f>
@@ -13491,10 +13509,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C50" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A50,": { ""id"": ",A50,", ""name"": """,B50,""", },")</f>
@@ -13503,10 +13521,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C51" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A51,": { ""id"": ",A51,", ""name"": """,B51,""", },")</f>
@@ -13515,10 +13533,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C52" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A52,": { ""id"": ",A52,", ""name"": """,B52,""", },")</f>
@@ -13527,10 +13545,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C53" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A53,": { ""id"": ",A53,", ""name"": """,B53,""", },")</f>
@@ -13539,10 +13557,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C54" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A54,": { ""id"": ",A54,", ""name"": """,B54,""", },")</f>
@@ -13551,10 +13569,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C55" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A55,": { ""id"": ",A55,", ""name"": """,B55,""", },")</f>
@@ -13563,10 +13581,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C56" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A56,": { ""id"": ",A56,", ""name"": """,B56,""", },")</f>
@@ -13575,10 +13593,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C57" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A57,": { ""id"": ",A57,", ""name"": """,B57,""", },")</f>
@@ -13587,10 +13605,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C58" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A58,": { ""id"": ",A58,", ""name"": """,B58,""", },")</f>
@@ -13599,10 +13617,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C59" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A59,": { ""id"": ",A59,", ""name"": """,B59,""", },")</f>
@@ -13611,10 +13629,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C60" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A60,": { ""id"": ",A60,", ""name"": """,B60,""", },")</f>
@@ -13623,10 +13641,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C61" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A61,": { ""id"": ",A61,", ""name"": """,B61,""", },")</f>
@@ -13635,10 +13653,10 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C62" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A62,": { ""id"": ",A62,", ""name"": """,B62,""", },")</f>
@@ -13647,10 +13665,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C63" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A63,": { ""id"": ",A63,", ""name"": """,B63,""", },")</f>
@@ -13659,10 +13677,10 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C64" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A64,": { ""id"": ",A64,", ""name"": """,B64,""", },")</f>
@@ -13671,10 +13689,10 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C65" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A65,": { ""id"": ",A65,", ""name"": """,B65,""", },")</f>
@@ -13683,10 +13701,10 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C66" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A66,": { ""id"": ",A66,", ""name"": """,B66,""", },")</f>
@@ -13695,10 +13713,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C67" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A67,": { ""id"": ",A67,", ""name"": """,B67,""", },")</f>
@@ -13707,10 +13725,10 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C68" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A68,": { ""id"": ",A68,", ""name"": """,B68,""", },")</f>
@@ -13719,10 +13737,10 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C69" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A69,": { ""id"": ",A69,", ""name"": """,B69,""", },")</f>
@@ -13731,10 +13749,10 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C70" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A70,": { ""id"": ",A70,", ""name"": """,B70,""", },")</f>
@@ -13743,10 +13761,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C71" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A71,": { ""id"": ",A71,", ""name"": """,B71,""", },")</f>
@@ -13755,10 +13773,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C72" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A72,": { ""id"": ",A72,", ""name"": """,B72,""", },")</f>
@@ -13767,10 +13785,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C73" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A73,": { ""id"": ",A73,", ""name"": """,B73,""", },")</f>
@@ -13779,10 +13797,10 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C74" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A74,": { ""id"": ",A74,", ""name"": """,B74,""", },")</f>
@@ -13791,10 +13809,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C75" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A75,": { ""id"": ",A75,", ""name"": """,B75,""", },")</f>
@@ -13803,10 +13821,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C76" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A76,": { ""id"": ",A76,", ""name"": """,B76,""", },")</f>
@@ -13815,10 +13833,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C77" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A77,": { ""id"": ",A77,", ""name"": """,B77,""", },")</f>
@@ -13827,10 +13845,10 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C78" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A78,": { ""id"": ",A78,", ""name"": """,B78,""", },")</f>
@@ -13839,10 +13857,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C79" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A79,": { ""id"": ",A79,", ""name"": """,B79,""", },")</f>
@@ -13851,10 +13869,10 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C80" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A80,": { ""id"": ",A80,", ""name"": """,B80,""", },")</f>
@@ -13863,10 +13881,10 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C81" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A81,": { ""id"": ",A81,", ""name"": """,B81,""", },")</f>
@@ -13875,10 +13893,10 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C82" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A82,": { ""id"": ",A82,", ""name"": """,B82,""", },")</f>
@@ -13887,10 +13905,10 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C83" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A83,": { ""id"": ",A83,", ""name"": """,B83,""", },")</f>
@@ -13899,10 +13917,10 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C84" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A84,": { ""id"": ",A84,", ""name"": """,B84,""", },")</f>
@@ -13911,10 +13929,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C85" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A85,": { ""id"": ",A85,", ""name"": """,B85,""", },")</f>
@@ -13923,10 +13941,10 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C86" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A86,": { ""id"": ",A86,", ""name"": """,B86,""", },")</f>
@@ -13935,10 +13953,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C87" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A87,": { ""id"": ",A87,", ""name"": """,B87,""", },")</f>
@@ -13947,10 +13965,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C88" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A88,": { ""id"": ",A88,", ""name"": """,B88,""", },")</f>
@@ -13959,10 +13977,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C89" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A89,": { ""id"": ",A89,", ""name"": """,B89,""", },")</f>
@@ -13971,10 +13989,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="C90" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A90,": { ""id"": ",A90,", ""name"": """,B90,""", },")</f>
@@ -13983,10 +14001,10 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C91" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A91,": { ""id"": ",A91,", ""name"": """,B91,""", },")</f>
@@ -13995,10 +14013,10 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C92" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A92,": { ""id"": ",A92,", ""name"": """,B92,""", },")</f>
@@ -14007,10 +14025,10 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C93" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A93,": { ""id"": ",A93,", ""name"": """,B93,""", },")</f>
@@ -14019,10 +14037,10 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C94" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A94,": { ""id"": ",A94,", ""name"": """,B94,""", },")</f>
@@ -14031,10 +14049,10 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C95" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A95,": { ""id"": ",A95,", ""name"": """,B95,""", },")</f>
@@ -14059,8 +14077,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I46" activeCellId="0" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14070,16 +14088,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>135</v>
@@ -14090,13 +14108,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E2" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A2,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B2, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C2, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D2, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14110,13 +14128,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>438</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>436</v>
       </c>
       <c r="E3" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A3,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B3, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C3, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D3, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14130,13 +14148,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>438</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>432</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>436</v>
       </c>
       <c r="E4" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A4,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B4, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C4, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D4, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14150,13 +14168,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>438</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>442</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>436</v>
       </c>
       <c r="E5" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A5,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B5, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C5, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D5, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14170,13 +14188,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>438</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>444</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>436</v>
       </c>
       <c r="E6" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A6,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B6, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C6, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D6, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14190,13 +14208,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>440</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>380</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>438</v>
       </c>
       <c r="E7" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A7,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B7, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C7, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D7, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14210,13 +14228,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>440</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>446</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>438</v>
       </c>
       <c r="E8" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A8,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B8, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C8, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D8, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14230,13 +14248,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>440</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>470</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>438</v>
       </c>
       <c r="E9" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A9,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B9, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C9, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D9, Commands!B:B, 0), 1, 1)),", },")</f>

</xml_diff>

<commit_message>
Added quest info and a missed Agrabah location
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1902" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="487">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -928,6 +928,12 @@
     <t xml:space="preserve">Inside Riku’s Data</t>
   </si>
   <si>
+    <t xml:space="preserve">0x10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgrabahCaveGauntletLower2</t>
+  </si>
+  <si>
     <t xml:space="preserve">0xFF</t>
   </si>
   <si>
@@ -1028,9 +1034,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ice Dash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x10</t>
   </si>
   <si>
     <t xml:space="preserve">Spark Dash</t>
@@ -1568,7 +1571,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1582,10 +1585,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1612,7 +1611,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -11175,7 +11174,7 @@
       <selection pane="topLeft" activeCell="D80" activeCellId="0" sqref="D80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -12842,9 +12841,21 @@
       <c r="A80" s="0" t="n">
         <v>79</v>
       </c>
+      <c r="B80" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>266</v>
+      </c>
       <c r="F80" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A80,": { ""worldId"": ",C80,", ""name"": """,D80,""", ""display"": """,E80,""", ""areaId"": ",B80,", },")</f>
-        <v>79: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>79: { "worldId": 0x4, "name": "AgrabahCaveGauntletLower2", "display": "Cave / Gauntlet", "areaId": 0x10, },</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12914,7 +12925,7 @@
       <selection pane="topLeft" activeCell="F63" activeCellId="0" sqref="F63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -12933,10 +12944,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""", },")</f>
@@ -12945,10 +12956,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""", },")</f>
@@ -12957,10 +12968,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""", },")</f>
@@ -12969,10 +12980,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""", },")</f>
@@ -12981,10 +12992,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""", },")</f>
@@ -12993,10 +13004,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""", },")</f>
@@ -13005,10 +13016,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""", },")</f>
@@ -13017,10 +13028,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""", },")</f>
@@ -13029,10 +13040,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""", },")</f>
@@ -13041,10 +13052,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""", },")</f>
@@ -13053,10 +13064,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""", },")</f>
@@ -13065,10 +13076,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A13,": { ""id"": ",A13,", ""name"": """,B13,""", },")</f>
@@ -13077,10 +13088,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A14,": { ""id"": ",A14,", ""name"": """,B14,""", },")</f>
@@ -13089,10 +13100,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A15,": { ""id"": ",A15,", ""name"": """,B15,""", },")</f>
@@ -13101,10 +13112,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A16,": { ""id"": ",A16,", ""name"": """,B16,""", },")</f>
@@ -13113,10 +13124,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A17,": { ""id"": ",A17,", ""name"": """,B17,""", },")</f>
@@ -13125,10 +13136,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A18,": { ""id"": ",A18,", ""name"": """,B18,""", },")</f>
@@ -13137,10 +13148,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>335</v>
+        <v>301</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A19,": { ""id"": ",A19,", ""name"": """,B19,""", },")</f>
@@ -13152,7 +13163,7 @@
         <v>267</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A20,": { ""id"": ",A20,", ""name"": """,B20,""", },")</f>
@@ -13164,7 +13175,7 @@
         <v>256</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A21,": { ""id"": ",A21,", ""name"": """,B21,""", },")</f>
@@ -13173,10 +13184,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A22,": { ""id"": ",A22,", ""name"": """,B22,""", },")</f>
@@ -13185,10 +13196,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C23" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A23,": { ""id"": ",A23,", ""name"": """,B23,""", },")</f>
@@ -13197,10 +13208,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C24" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A24,": { ""id"": ",A24,", ""name"": """,B24,""", },")</f>
@@ -13209,10 +13220,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C25" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A25,": { ""id"": ",A25,", ""name"": """,B25,""", },")</f>
@@ -13221,10 +13232,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C26" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A26,": { ""id"": ",A26,", ""name"": """,B26,""", },")</f>
@@ -13233,10 +13244,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C27" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A27,": { ""id"": ",A27,", ""name"": """,B27,""", },")</f>
@@ -13245,10 +13256,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C28" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A28,": { ""id"": ",A28,", ""name"": """,B28,""", },")</f>
@@ -13257,10 +13268,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C29" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A29,": { ""id"": ",A29,", ""name"": """,B29,""", },")</f>
@@ -13269,10 +13280,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C30" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A30,": { ""id"": ",A30,", ""name"": """,B30,""", },")</f>
@@ -13281,10 +13292,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C31" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A31,": { ""id"": ",A31,", ""name"": """,B31,""", },")</f>
@@ -13296,7 +13307,7 @@
         <v>203</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C32" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A32,": { ""id"": ",A32,", ""name"": """,B32,""", },")</f>
@@ -13308,7 +13319,7 @@
         <v>206</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C33" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A33,": { ""id"": ",A33,", ""name"": """,B33,""", },")</f>
@@ -13320,7 +13331,7 @@
         <v>211</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C34" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A34,": { ""id"": ",A34,", ""name"": """,B34,""", },")</f>
@@ -13329,10 +13340,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C35" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A35,": { ""id"": ",A35,", ""name"": """,B35,""", },")</f>
@@ -13344,7 +13355,7 @@
         <v>241</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C36" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A36,": { ""id"": ",A36,", ""name"": """,B36,""", },")</f>
@@ -13353,10 +13364,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C37" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A37,": { ""id"": ",A37,", ""name"": """,B37,""", },")</f>
@@ -13365,10 +13376,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C38" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A38,": { ""id"": ",A38,", ""name"": """,B38,""", },")</f>
@@ -13377,10 +13388,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C39" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A39,": { ""id"": ",A39,", ""name"": """,B39,""", },")</f>
@@ -13389,10 +13400,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C40" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A40,": { ""id"": ",A40,", ""name"": """,B40,""", },")</f>
@@ -13401,10 +13412,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C41" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A41,": { ""id"": ",A41,", ""name"": """,B41,""", },")</f>
@@ -13413,10 +13424,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C42" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A42,": { ""id"": ",A42,", ""name"": """,B42,""", },")</f>
@@ -13425,10 +13436,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C43" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A43,": { ""id"": ",A43,", ""name"": """,B43,""", },")</f>
@@ -13437,10 +13448,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C44" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A44,": { ""id"": ",A44,", ""name"": """,B44,""", },")</f>
@@ -13449,10 +13460,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C45" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A45,": { ""id"": ",A45,", ""name"": """,B45,""", },")</f>
@@ -13461,10 +13472,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C46" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A46,": { ""id"": ",A46,", ""name"": """,B46,""", },")</f>
@@ -13473,10 +13484,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C47" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A47,": { ""id"": ",A47,", ""name"": """,B47,""", },")</f>
@@ -13485,10 +13496,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C48" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A48,": { ""id"": ",A48,", ""name"": """,B48,""", },")</f>
@@ -13497,10 +13508,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C49" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A49,": { ""id"": ",A49,", ""name"": """,B49,""", },")</f>
@@ -13509,10 +13520,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C50" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A50,": { ""id"": ",A50,", ""name"": """,B50,""", },")</f>
@@ -13521,10 +13532,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C51" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A51,": { ""id"": ",A51,", ""name"": """,B51,""", },")</f>
@@ -13533,10 +13544,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C52" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A52,": { ""id"": ",A52,", ""name"": """,B52,""", },")</f>
@@ -13545,10 +13556,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C53" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A53,": { ""id"": ",A53,", ""name"": """,B53,""", },")</f>
@@ -13557,10 +13568,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C54" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A54,": { ""id"": ",A54,", ""name"": """,B54,""", },")</f>
@@ -13569,10 +13580,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C55" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A55,": { ""id"": ",A55,", ""name"": """,B55,""", },")</f>
@@ -13581,10 +13592,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C56" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A56,": { ""id"": ",A56,", ""name"": """,B56,""", },")</f>
@@ -13593,10 +13604,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C57" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A57,": { ""id"": ",A57,", ""name"": """,B57,""", },")</f>
@@ -13605,10 +13616,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C58" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A58,": { ""id"": ",A58,", ""name"": """,B58,""", },")</f>
@@ -13617,10 +13628,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C59" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A59,": { ""id"": ",A59,", ""name"": """,B59,""", },")</f>
@@ -13629,10 +13640,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C60" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A60,": { ""id"": ",A60,", ""name"": """,B60,""", },")</f>
@@ -13641,10 +13652,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C61" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A61,": { ""id"": ",A61,", ""name"": """,B61,""", },")</f>
@@ -13653,10 +13664,10 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C62" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A62,": { ""id"": ",A62,", ""name"": """,B62,""", },")</f>
@@ -13665,10 +13676,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C63" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A63,": { ""id"": ",A63,", ""name"": """,B63,""", },")</f>
@@ -13677,10 +13688,10 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C64" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A64,": { ""id"": ",A64,", ""name"": """,B64,""", },")</f>
@@ -13689,10 +13700,10 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C65" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A65,": { ""id"": ",A65,", ""name"": """,B65,""", },")</f>
@@ -13701,10 +13712,10 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C66" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A66,": { ""id"": ",A66,", ""name"": """,B66,""", },")</f>
@@ -13713,10 +13724,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C67" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A67,": { ""id"": ",A67,", ""name"": """,B67,""", },")</f>
@@ -13725,10 +13736,10 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C68" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A68,": { ""id"": ",A68,", ""name"": """,B68,""", },")</f>
@@ -13737,10 +13748,10 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C69" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A69,": { ""id"": ",A69,", ""name"": """,B69,""", },")</f>
@@ -13749,10 +13760,10 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C70" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A70,": { ""id"": ",A70,", ""name"": """,B70,""", },")</f>
@@ -13761,10 +13772,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C71" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A71,": { ""id"": ",A71,", ""name"": """,B71,""", },")</f>
@@ -13773,10 +13784,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C72" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A72,": { ""id"": ",A72,", ""name"": """,B72,""", },")</f>
@@ -13785,10 +13796,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C73" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A73,": { ""id"": ",A73,", ""name"": """,B73,""", },")</f>
@@ -13797,10 +13808,10 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C74" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A74,": { ""id"": ",A74,", ""name"": """,B74,""", },")</f>
@@ -13809,10 +13820,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C75" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A75,": { ""id"": ",A75,", ""name"": """,B75,""", },")</f>
@@ -13821,10 +13832,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C76" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A76,": { ""id"": ",A76,", ""name"": """,B76,""", },")</f>
@@ -13833,10 +13844,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C77" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A77,": { ""id"": ",A77,", ""name"": """,B77,""", },")</f>
@@ -13845,10 +13856,10 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C78" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A78,": { ""id"": ",A78,", ""name"": """,B78,""", },")</f>
@@ -13857,10 +13868,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C79" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A79,": { ""id"": ",A79,", ""name"": """,B79,""", },")</f>
@@ -13869,10 +13880,10 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C80" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A80,": { ""id"": ",A80,", ""name"": """,B80,""", },")</f>
@@ -13881,10 +13892,10 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C81" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A81,": { ""id"": ",A81,", ""name"": """,B81,""", },")</f>
@@ -13893,10 +13904,10 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C82" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A82,": { ""id"": ",A82,", ""name"": """,B82,""", },")</f>
@@ -13905,10 +13916,10 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C83" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A83,": { ""id"": ",A83,", ""name"": """,B83,""", },")</f>
@@ -13917,10 +13928,10 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C84" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A84,": { ""id"": ",A84,", ""name"": """,B84,""", },")</f>
@@ -13929,10 +13940,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C85" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A85,": { ""id"": ",A85,", ""name"": """,B85,""", },")</f>
@@ -13941,10 +13952,10 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C86" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A86,": { ""id"": ",A86,", ""name"": """,B86,""", },")</f>
@@ -13953,10 +13964,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C87" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A87,": { ""id"": ",A87,", ""name"": """,B87,""", },")</f>
@@ -13965,10 +13976,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C88" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A88,": { ""id"": ",A88,", ""name"": """,B88,""", },")</f>
@@ -13977,10 +13988,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C89" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A89,": { ""id"": ",A89,", ""name"": """,B89,""", },")</f>
@@ -13989,10 +14000,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C90" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A90,": { ""id"": ",A90,", ""name"": """,B90,""", },")</f>
@@ -14001,10 +14012,10 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C91" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A91,": { ""id"": ",A91,", ""name"": """,B91,""", },")</f>
@@ -14013,10 +14024,10 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C92" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A92,": { ""id"": ",A92,", ""name"": """,B92,""", },")</f>
@@ -14025,10 +14036,10 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C93" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A93,": { ""id"": ",A93,", ""name"": """,B93,""", },")</f>
@@ -14037,10 +14048,10 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C94" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A94,": { ""id"": ",A94,", ""name"": """,B94,""", },")</f>
@@ -14049,10 +14060,10 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C95" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A95,": { ""id"": ",A95,", ""name"": """,B95,""", },")</f>
@@ -14075,29 +14086,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I46" activeCellId="0" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>135</v>
@@ -14108,160 +14119,144 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E2" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A2,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B2, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C2, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D2, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>0: { "targetId": 0x46, "command1Id": 0x02, "command2Id": 0x49, },</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E3" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A3,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B3, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C3, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D3, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>1: { "targetId": 0x47, "command1Id": 0x17, "command2Id": 0x46, },</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E4" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A4,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B4, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C4, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D4, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>2: { "targetId": 0x47, "command1Id": 0x44, "command2Id": 0x46, },</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E5" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A5,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B5, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C5, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D5, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>3: { "targetId": 0x47, "command1Id": 0x49, "command2Id": 0x46, },</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E6" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A6,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B6, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C6, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D6, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>4: { "targetId": 0x47, "command1Id": 0x4a, "command2Id": 0x46, },</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E7" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A7,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B7, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C7, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D7, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>5: { "targetId": 0x48, "command1Id": 0x2a, "command2Id": 0x47, },</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E8" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A8,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B8, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C8, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D8, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>6: { "targetId": 0x48, "command1Id": 0x4b, "command2Id": 0x47, },</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E9" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A9,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B9, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C9, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D9, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>7: { "targetId": 0x48, "command1Id": 0x57, "command2Id": 0x47, },</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -14271,8 +14266,6 @@
         <f aca="true">_xlfn.CONCAT(A10,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B10, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C10, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D10, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -14282,8 +14275,6 @@
         <f aca="true">_xlfn.CONCAT(A11,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B11, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C11, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D11, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -14293,8 +14284,6 @@
         <f aca="true">_xlfn.CONCAT(A12,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B12, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C12, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D12, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -14304,8 +14293,6 @@
         <f aca="true">_xlfn.CONCAT(A13,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B13, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C13, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D13, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -14315,8 +14302,6 @@
         <f aca="true">_xlfn.CONCAT(A14,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B14, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C14, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D14, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -14326,8 +14311,6 @@
         <f aca="true">_xlfn.CONCAT(A15,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B15, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C15, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D15, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -14337,8 +14320,6 @@
         <f aca="true">_xlfn.CONCAT(A16,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B16, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C16, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D16, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -14348,8 +14329,6 @@
         <f aca="true">_xlfn.CONCAT(A17,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B17, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C17, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D17, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -14359,8 +14338,6 @@
         <f aca="true">_xlfn.CONCAT(A18,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B18, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C18, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D18, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -14370,8 +14347,6 @@
         <f aca="true">_xlfn.CONCAT(A19,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B19, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C19, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D19, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -14381,8 +14356,6 @@
         <f aca="true">_xlfn.CONCAT(A20,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B20, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C20, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D20, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -14392,8 +14365,6 @@
         <f aca="true">_xlfn.CONCAT(A21,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B21, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C21, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D21, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -14403,8 +14374,6 @@
         <f aca="true">_xlfn.CONCAT(A22,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B22, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C22, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D22, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -14414,8 +14383,6 @@
         <f aca="true">_xlfn.CONCAT(A23,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B23, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C23, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D23, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -14425,8 +14392,6 @@
         <f aca="true">_xlfn.CONCAT(A24,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B24, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C24, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D24, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -14436,8 +14401,6 @@
         <f aca="true">_xlfn.CONCAT(A25,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B25, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C25, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D25, Commands!B:B, 0), 1, 1)),", },")</f>
         <v>#N/A</v>
       </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Finished quest achievements, and other things
* Quest achievements finalized
* "High-Stakes Gambler" updated with a new threshold of 150,000 points and a value of 50 points
* "Banco" and "High-Stakes Gambler" fixed to not trigger if the player enters the Avatar Menu
* "Quest Bester" refactored to use the same code as "What Am I, a Delivery Boy?" and "A Friend in Need"
* New locations for RP
* Leaderboards (technically) updated with the same fix as the two system sector achievements mentioned above, but they may not need to be updated on the site itself
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="492">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -932,6 +932,21 @@
   </si>
   <si>
     <t xml:space="preserve">AgrabahCaveGauntletLower2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionDestinyIslands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionFirstDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionSecondDistrict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionClearing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionLotusForest</t>
   </si>
   <si>
     <t xml:space="preserve">0xFF</t>
@@ -1611,7 +1626,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -11171,10 +11186,10 @@
   <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D80" activeCellId="0" sqref="D80"/>
+      <selection pane="topLeft" activeCell="F85" activeCellId="0" sqref="F85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -12862,45 +12877,105 @@
       <c r="A81" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="B81" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>146</v>
+      </c>
       <c r="F81" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A81,": { ""worldId"": ",C81,", ""name"": """,D81,""", ""display"": """,E81,""", ""areaId"": ",B81,", },")</f>
-        <v>80: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>80: { "worldId": 0x6, "name": "HollowBastionDestinyIslands", "display": "Destiny Islands", "areaId": 0x9, },</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <v>81</v>
       </c>
+      <c r="B82" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>154</v>
+      </c>
       <c r="F82" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A82,": { ""worldId"": ",C82,", ""name"": """,D82,""", ""display"": """,E82,""", ""areaId"": ",B82,", },")</f>
-        <v>81: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>81: { "worldId": 0x6, "name": "HollowBastionFirstDistrict", "display": "First District", "areaId": 0xa, },</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
         <v>82</v>
       </c>
+      <c r="B83" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>156</v>
+      </c>
       <c r="F83" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A83,": { ""worldId"": ",C83,", ""name"": """,D83,""", ""display"": """,E83,""", ""areaId"": ",B83,", },")</f>
-        <v>82: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>82: { "worldId": 0x6, "name": "HollowBastionSecondDistrict", "display": "Second District", "areaId": 0xb, },</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>83</v>
       </c>
+      <c r="B84" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>180</v>
+      </c>
       <c r="F84" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A84,": { ""worldId"": ",C84,", ""name"": """,D84,""", ""display"": """,E84,""", ""areaId"": ",B84,", },")</f>
-        <v>83: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>83: { "worldId": 0x6, "name": "HollowBastionClearing", "display": "Clearing", "areaId": 0x4, },</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
         <v>84</v>
       </c>
+      <c r="B85" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>184</v>
+      </c>
       <c r="F85" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A85,": { ""worldId"": ",C85,", ""name"": """,D85,""", ""display"": """,E85,""", ""areaId"": ",B85,", },")</f>
-        <v>84: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>84: { "worldId": 0x6, "name": "HollowBastionLotusForest", "display": "Lotus Forest", "areaId": 0x5, },</v>
       </c>
     </row>
   </sheetData>
@@ -12925,7 +13000,7 @@
       <selection pane="topLeft" activeCell="F63" activeCellId="0" sqref="F63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -12944,10 +13019,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""", },")</f>
@@ -12956,10 +13031,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""", },")</f>
@@ -12968,10 +13043,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""", },")</f>
@@ -12980,10 +13055,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="C5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""", },")</f>
@@ -12992,10 +13067,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="C6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""", },")</f>
@@ -13004,10 +13079,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="C7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""", },")</f>
@@ -13016,10 +13091,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""", },")</f>
@@ -13028,10 +13103,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="C9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""", },")</f>
@@ -13040,10 +13115,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""", },")</f>
@@ -13052,10 +13127,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="C11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""", },")</f>
@@ -13064,10 +13139,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="C12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""", },")</f>
@@ -13076,10 +13151,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="C13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A13,": { ""id"": ",A13,", ""name"": """,B13,""", },")</f>
@@ -13088,10 +13163,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="C14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A14,": { ""id"": ",A14,", ""name"": """,B14,""", },")</f>
@@ -13100,10 +13175,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="C15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A15,": { ""id"": ",A15,", ""name"": """,B15,""", },")</f>
@@ -13112,10 +13187,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="C16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A16,": { ""id"": ",A16,", ""name"": """,B16,""", },")</f>
@@ -13124,10 +13199,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="C17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A17,": { ""id"": ",A17,", ""name"": """,B17,""", },")</f>
@@ -13136,10 +13211,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="C18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A18,": { ""id"": ",A18,", ""name"": """,B18,""", },")</f>
@@ -13151,7 +13226,7 @@
         <v>301</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="C19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A19,": { ""id"": ",A19,", ""name"": """,B19,""", },")</f>
@@ -13163,7 +13238,7 @@
         <v>267</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="C20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A20,": { ""id"": ",A20,", ""name"": """,B20,""", },")</f>
@@ -13175,7 +13250,7 @@
         <v>256</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="C21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A21,": { ""id"": ",A21,", ""name"": """,B21,""", },")</f>
@@ -13184,10 +13259,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="C22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A22,": { ""id"": ",A22,", ""name"": """,B22,""", },")</f>
@@ -13196,10 +13271,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="C23" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A23,": { ""id"": ",A23,", ""name"": """,B23,""", },")</f>
@@ -13208,10 +13283,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="C24" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A24,": { ""id"": ",A24,", ""name"": """,B24,""", },")</f>
@@ -13220,10 +13295,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="C25" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A25,": { ""id"": ",A25,", ""name"": """,B25,""", },")</f>
@@ -13232,10 +13307,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="C26" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A26,": { ""id"": ",A26,", ""name"": """,B26,""", },")</f>
@@ -13244,10 +13319,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="C27" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A27,": { ""id"": ",A27,", ""name"": """,B27,""", },")</f>
@@ -13256,10 +13331,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="C28" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A28,": { ""id"": ",A28,", ""name"": """,B28,""", },")</f>
@@ -13268,10 +13343,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="C29" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A29,": { ""id"": ",A29,", ""name"": """,B29,""", },")</f>
@@ -13280,10 +13355,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="C30" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A30,": { ""id"": ",A30,", ""name"": """,B30,""", },")</f>
@@ -13292,10 +13367,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="C31" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A31,": { ""id"": ",A31,", ""name"": """,B31,""", },")</f>
@@ -13307,7 +13382,7 @@
         <v>203</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="C32" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A32,": { ""id"": ",A32,", ""name"": """,B32,""", },")</f>
@@ -13319,7 +13394,7 @@
         <v>206</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="C33" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A33,": { ""id"": ",A33,", ""name"": """,B33,""", },")</f>
@@ -13331,7 +13406,7 @@
         <v>211</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="C34" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A34,": { ""id"": ",A34,", ""name"": """,B34,""", },")</f>
@@ -13340,10 +13415,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="C35" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A35,": { ""id"": ",A35,", ""name"": """,B35,""", },")</f>
@@ -13355,7 +13430,7 @@
         <v>241</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="C36" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A36,": { ""id"": ",A36,", ""name"": """,B36,""", },")</f>
@@ -13364,10 +13439,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="C37" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A37,": { ""id"": ",A37,", ""name"": """,B37,""", },")</f>
@@ -13376,10 +13451,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
       <c r="C38" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A38,": { ""id"": ",A38,", ""name"": """,B38,""", },")</f>
@@ -13388,10 +13463,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="C39" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A39,": { ""id"": ",A39,", ""name"": """,B39,""", },")</f>
@@ -13400,10 +13475,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="C40" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A40,": { ""id"": ",A40,", ""name"": """,B40,""", },")</f>
@@ -13412,10 +13487,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="C41" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A41,": { ""id"": ",A41,", ""name"": """,B41,""", },")</f>
@@ -13424,10 +13499,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="C42" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A42,": { ""id"": ",A42,", ""name"": """,B42,""", },")</f>
@@ -13436,10 +13511,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="C43" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A43,": { ""id"": ",A43,", ""name"": """,B43,""", },")</f>
@@ -13448,10 +13523,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="C44" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A44,": { ""id"": ",A44,", ""name"": """,B44,""", },")</f>
@@ -13460,10 +13535,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="C45" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A45,": { ""id"": ",A45,", ""name"": """,B45,""", },")</f>
@@ -13472,10 +13547,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="C46" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A46,": { ""id"": ",A46,", ""name"": """,B46,""", },")</f>
@@ -13484,10 +13559,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="C47" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A47,": { ""id"": ",A47,", ""name"": """,B47,""", },")</f>
@@ -13496,10 +13571,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="C48" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A48,": { ""id"": ",A48,", ""name"": """,B48,""", },")</f>
@@ -13508,10 +13583,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="C49" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A49,": { ""id"": ",A49,", ""name"": """,B49,""", },")</f>
@@ -13520,10 +13595,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="C50" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A50,": { ""id"": ",A50,", ""name"": """,B50,""", },")</f>
@@ -13532,10 +13607,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="C51" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A51,": { ""id"": ",A51,", ""name"": """,B51,""", },")</f>
@@ -13544,10 +13619,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="C52" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A52,": { ""id"": ",A52,", ""name"": """,B52,""", },")</f>
@@ -13556,10 +13631,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="C53" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A53,": { ""id"": ",A53,", ""name"": """,B53,""", },")</f>
@@ -13568,10 +13643,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="C54" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A54,": { ""id"": ",A54,", ""name"": """,B54,""", },")</f>
@@ -13580,10 +13655,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="C55" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A55,": { ""id"": ",A55,", ""name"": """,B55,""", },")</f>
@@ -13592,10 +13667,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="C56" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A56,": { ""id"": ",A56,", ""name"": """,B56,""", },")</f>
@@ -13604,10 +13679,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="C57" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A57,": { ""id"": ",A57,", ""name"": """,B57,""", },")</f>
@@ -13616,10 +13691,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="C58" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A58,": { ""id"": ",A58,", ""name"": """,B58,""", },")</f>
@@ -13628,10 +13703,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="C59" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A59,": { ""id"": ",A59,", ""name"": """,B59,""", },")</f>
@@ -13640,10 +13715,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="C60" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A60,": { ""id"": ",A60,", ""name"": """,B60,""", },")</f>
@@ -13652,10 +13727,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="C61" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A61,": { ""id"": ",A61,", ""name"": """,B61,""", },")</f>
@@ -13664,10 +13739,10 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="C62" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A62,": { ""id"": ",A62,", ""name"": """,B62,""", },")</f>
@@ -13676,10 +13751,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="C63" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A63,": { ""id"": ",A63,", ""name"": """,B63,""", },")</f>
@@ -13688,10 +13763,10 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="C64" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A64,": { ""id"": ",A64,", ""name"": """,B64,""", },")</f>
@@ -13700,10 +13775,10 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="C65" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A65,": { ""id"": ",A65,", ""name"": """,B65,""", },")</f>
@@ -13712,10 +13787,10 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="C66" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A66,": { ""id"": ",A66,", ""name"": """,B66,""", },")</f>
@@ -13724,10 +13799,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="C67" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A67,": { ""id"": ",A67,", ""name"": """,B67,""", },")</f>
@@ -13736,10 +13811,10 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="C68" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A68,": { ""id"": ",A68,", ""name"": """,B68,""", },")</f>
@@ -13748,10 +13823,10 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="C69" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A69,": { ""id"": ",A69,", ""name"": """,B69,""", },")</f>
@@ -13760,10 +13835,10 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="C70" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A70,": { ""id"": ",A70,", ""name"": """,B70,""", },")</f>
@@ -13772,10 +13847,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="C71" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A71,": { ""id"": ",A71,", ""name"": """,B71,""", },")</f>
@@ -13784,10 +13859,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="C72" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A72,": { ""id"": ",A72,", ""name"": """,B72,""", },")</f>
@@ -13796,10 +13871,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="C73" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A73,": { ""id"": ",A73,", ""name"": """,B73,""", },")</f>
@@ -13808,10 +13883,10 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="C74" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A74,": { ""id"": ",A74,", ""name"": """,B74,""", },")</f>
@@ -13820,10 +13895,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="C75" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A75,": { ""id"": ",A75,", ""name"": """,B75,""", },")</f>
@@ -13832,10 +13907,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="C76" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A76,": { ""id"": ",A76,", ""name"": """,B76,""", },")</f>
@@ -13844,10 +13919,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="C77" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A77,": { ""id"": ",A77,", ""name"": """,B77,""", },")</f>
@@ -13856,10 +13931,10 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="C78" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A78,": { ""id"": ",A78,", ""name"": """,B78,""", },")</f>
@@ -13868,10 +13943,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="C79" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A79,": { ""id"": ",A79,", ""name"": """,B79,""", },")</f>
@@ -13880,10 +13955,10 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="C80" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A80,": { ""id"": ",A80,", ""name"": """,B80,""", },")</f>
@@ -13892,10 +13967,10 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="C81" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A81,": { ""id"": ",A81,", ""name"": """,B81,""", },")</f>
@@ -13904,10 +13979,10 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="C82" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A82,": { ""id"": ",A82,", ""name"": """,B82,""", },")</f>
@@ -13916,10 +13991,10 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="C83" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A83,": { ""id"": ",A83,", ""name"": """,B83,""", },")</f>
@@ -13928,10 +14003,10 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="C84" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A84,": { ""id"": ",A84,", ""name"": """,B84,""", },")</f>
@@ -13940,10 +14015,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="C85" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A85,": { ""id"": ",A85,", ""name"": """,B85,""", },")</f>
@@ -13952,10 +14027,10 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="C86" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A86,": { ""id"": ",A86,", ""name"": """,B86,""", },")</f>
@@ -13964,10 +14039,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="C87" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A87,": { ""id"": ",A87,", ""name"": """,B87,""", },")</f>
@@ -13976,10 +14051,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="C88" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A88,": { ""id"": ",A88,", ""name"": """,B88,""", },")</f>
@@ -13988,10 +14063,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="C89" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A89,": { ""id"": ",A89,", ""name"": """,B89,""", },")</f>
@@ -14000,10 +14075,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="C90" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A90,": { ""id"": ",A90,", ""name"": """,B90,""", },")</f>
@@ -14012,10 +14087,10 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="C91" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A91,": { ""id"": ",A91,", ""name"": """,B91,""", },")</f>
@@ -14024,10 +14099,10 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="C92" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A92,": { ""id"": ",A92,", ""name"": """,B92,""", },")</f>
@@ -14036,10 +14111,10 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="C93" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A93,": { ""id"": ",A93,", ""name"": """,B93,""", },")</f>
@@ -14048,10 +14123,10 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C94" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A94,": { ""id"": ",A94,", ""name"": """,B94,""", },")</f>
@@ -14060,10 +14135,10 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C95" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A95,": { ""id"": ",A95,", ""name"": """,B95,""", },")</f>
@@ -14092,23 +14167,23 @@
       <selection pane="topLeft" activeCell="I46" activeCellId="0" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>135</v>
@@ -14119,13 +14194,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="E2" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A2,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B2, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C2, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D2, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14137,13 +14212,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="E3" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A3,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B3, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C3, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D3, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14155,13 +14230,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="E4" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A4,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B4, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C4, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D4, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14173,13 +14248,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="E5" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A5,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B5, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C5, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D5, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14191,13 +14266,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="E6" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A6,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B6, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C6, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D6, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14209,13 +14284,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="E7" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A7,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B7, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C7, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D7, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14227,13 +14302,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="E8" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A8,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B8, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C8, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D8, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14245,13 +14320,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="E9" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A9,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B9, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C9, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D9, Commands!B:B, 0), 1, 1)),", },")</f>

</xml_diff>

<commit_message>
Added achievements and leaderboards up to the end of Hollow Bastion II
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1946" uniqueCount="499">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -962,6 +962,12 @@
   </si>
   <si>
     <t xml:space="preserve">HollowBastionEscapeRiku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionDragon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chapel (Dragon’s Lair)</t>
   </si>
   <si>
     <t xml:space="preserve">0xFF</t>
@@ -1641,7 +1647,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -11201,10 +11207,10 @@
   <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B90" activeCellId="0" sqref="B90"/>
+      <selection pane="topLeft" activeCell="B91" activeCellId="0" sqref="B91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
   </cols>
@@ -13081,9 +13087,21 @@
       <c r="A90" s="0" t="n">
         <v>89</v>
       </c>
+      <c r="B90" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="E90" s="0" t="s">
+        <v>314</v>
+      </c>
       <c r="F90" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A90,": { ""worldId"": ",C90,", ""name"": """,D90,""", ""display"": """,E90,""", ""areaId"": ",B90,", },")</f>
-        <v>89: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>89: { "worldId": 0x6, "name": "HollowBastionDragon", "display": "Chapel (Dragon’s Lair)", "areaId": 0x2, },</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13189,7 +13207,7 @@
       <selection pane="topLeft" activeCell="F63" activeCellId="0" sqref="F63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -13208,10 +13226,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""", },")</f>
@@ -13220,10 +13238,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""", },")</f>
@@ -13232,10 +13250,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""", },")</f>
@@ -13244,10 +13262,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""", },")</f>
@@ -13256,10 +13274,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""", },")</f>
@@ -13268,10 +13286,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""", },")</f>
@@ -13280,10 +13298,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""", },")</f>
@@ -13292,10 +13310,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""", },")</f>
@@ -13304,10 +13322,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""", },")</f>
@@ -13316,10 +13334,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""", },")</f>
@@ -13328,10 +13346,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""", },")</f>
@@ -13340,10 +13358,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A13,": { ""id"": ",A13,", ""name"": """,B13,""", },")</f>
@@ -13352,10 +13370,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A14,": { ""id"": ",A14,", ""name"": """,B14,""", },")</f>
@@ -13364,10 +13382,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A15,": { ""id"": ",A15,", ""name"": """,B15,""", },")</f>
@@ -13376,10 +13394,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A16,": { ""id"": ",A16,", ""name"": """,B16,""", },")</f>
@@ -13388,10 +13406,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A17,": { ""id"": ",A17,", ""name"": """,B17,""", },")</f>
@@ -13400,10 +13418,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A18,": { ""id"": ",A18,", ""name"": """,B18,""", },")</f>
@@ -13415,7 +13433,7 @@
         <v>301</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A19,": { ""id"": ",A19,", ""name"": """,B19,""", },")</f>
@@ -13427,7 +13445,7 @@
         <v>267</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A20,": { ""id"": ",A20,", ""name"": """,B20,""", },")</f>
@@ -13439,7 +13457,7 @@
         <v>256</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A21,": { ""id"": ",A21,", ""name"": """,B21,""", },")</f>
@@ -13448,10 +13466,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A22,": { ""id"": ",A22,", ""name"": """,B22,""", },")</f>
@@ -13460,10 +13478,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C23" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A23,": { ""id"": ",A23,", ""name"": """,B23,""", },")</f>
@@ -13472,10 +13490,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C24" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A24,": { ""id"": ",A24,", ""name"": """,B24,""", },")</f>
@@ -13484,10 +13502,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C25" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A25,": { ""id"": ",A25,", ""name"": """,B25,""", },")</f>
@@ -13496,10 +13514,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C26" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A26,": { ""id"": ",A26,", ""name"": """,B26,""", },")</f>
@@ -13508,10 +13526,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C27" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A27,": { ""id"": ",A27,", ""name"": """,B27,""", },")</f>
@@ -13520,10 +13538,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C28" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A28,": { ""id"": ",A28,", ""name"": """,B28,""", },")</f>
@@ -13532,10 +13550,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C29" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A29,": { ""id"": ",A29,", ""name"": """,B29,""", },")</f>
@@ -13544,10 +13562,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C30" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A30,": { ""id"": ",A30,", ""name"": """,B30,""", },")</f>
@@ -13556,10 +13574,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C31" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A31,": { ""id"": ",A31,", ""name"": """,B31,""", },")</f>
@@ -13571,7 +13589,7 @@
         <v>203</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C32" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A32,": { ""id"": ",A32,", ""name"": """,B32,""", },")</f>
@@ -13583,7 +13601,7 @@
         <v>206</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C33" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A33,": { ""id"": ",A33,", ""name"": """,B33,""", },")</f>
@@ -13595,7 +13613,7 @@
         <v>211</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C34" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A34,": { ""id"": ",A34,", ""name"": """,B34,""", },")</f>
@@ -13604,10 +13622,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C35" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A35,": { ""id"": ",A35,", ""name"": """,B35,""", },")</f>
@@ -13619,7 +13637,7 @@
         <v>241</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C36" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A36,": { ""id"": ",A36,", ""name"": """,B36,""", },")</f>
@@ -13628,10 +13646,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C37" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A37,": { ""id"": ",A37,", ""name"": """,B37,""", },")</f>
@@ -13640,10 +13658,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C38" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A38,": { ""id"": ",A38,", ""name"": """,B38,""", },")</f>
@@ -13652,10 +13670,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C39" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A39,": { ""id"": ",A39,", ""name"": """,B39,""", },")</f>
@@ -13664,10 +13682,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C40" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A40,": { ""id"": ",A40,", ""name"": """,B40,""", },")</f>
@@ -13676,10 +13694,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C41" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A41,": { ""id"": ",A41,", ""name"": """,B41,""", },")</f>
@@ -13688,10 +13706,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C42" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A42,": { ""id"": ",A42,", ""name"": """,B42,""", },")</f>
@@ -13700,10 +13718,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C43" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A43,": { ""id"": ",A43,", ""name"": """,B43,""", },")</f>
@@ -13712,10 +13730,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C44" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A44,": { ""id"": ",A44,", ""name"": """,B44,""", },")</f>
@@ -13724,10 +13742,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C45" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A45,": { ""id"": ",A45,", ""name"": """,B45,""", },")</f>
@@ -13736,10 +13754,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C46" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A46,": { ""id"": ",A46,", ""name"": """,B46,""", },")</f>
@@ -13748,10 +13766,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C47" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A47,": { ""id"": ",A47,", ""name"": """,B47,""", },")</f>
@@ -13760,10 +13778,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C48" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A48,": { ""id"": ",A48,", ""name"": """,B48,""", },")</f>
@@ -13772,10 +13790,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C49" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A49,": { ""id"": ",A49,", ""name"": """,B49,""", },")</f>
@@ -13784,10 +13802,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C50" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A50,": { ""id"": ",A50,", ""name"": """,B50,""", },")</f>
@@ -13796,10 +13814,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C51" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A51,": { ""id"": ",A51,", ""name"": """,B51,""", },")</f>
@@ -13808,10 +13826,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C52" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A52,": { ""id"": ",A52,", ""name"": """,B52,""", },")</f>
@@ -13820,10 +13838,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C53" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A53,": { ""id"": ",A53,", ""name"": """,B53,""", },")</f>
@@ -13832,10 +13850,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C54" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A54,": { ""id"": ",A54,", ""name"": """,B54,""", },")</f>
@@ -13844,10 +13862,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C55" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A55,": { ""id"": ",A55,", ""name"": """,B55,""", },")</f>
@@ -13856,10 +13874,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C56" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A56,": { ""id"": ",A56,", ""name"": """,B56,""", },")</f>
@@ -13868,10 +13886,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C57" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A57,": { ""id"": ",A57,", ""name"": """,B57,""", },")</f>
@@ -13880,10 +13898,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C58" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A58,": { ""id"": ",A58,", ""name"": """,B58,""", },")</f>
@@ -13892,10 +13910,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C59" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A59,": { ""id"": ",A59,", ""name"": """,B59,""", },")</f>
@@ -13904,10 +13922,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C60" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A60,": { ""id"": ",A60,", ""name"": """,B60,""", },")</f>
@@ -13916,10 +13934,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C61" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A61,": { ""id"": ",A61,", ""name"": """,B61,""", },")</f>
@@ -13928,10 +13946,10 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C62" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A62,": { ""id"": ",A62,", ""name"": """,B62,""", },")</f>
@@ -13940,10 +13958,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C63" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A63,": { ""id"": ",A63,", ""name"": """,B63,""", },")</f>
@@ -13952,10 +13970,10 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C64" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A64,": { ""id"": ",A64,", ""name"": """,B64,""", },")</f>
@@ -13964,10 +13982,10 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C65" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A65,": { ""id"": ",A65,", ""name"": """,B65,""", },")</f>
@@ -13976,10 +13994,10 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C66" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A66,": { ""id"": ",A66,", ""name"": """,B66,""", },")</f>
@@ -13988,10 +14006,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C67" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A67,": { ""id"": ",A67,", ""name"": """,B67,""", },")</f>
@@ -14000,10 +14018,10 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C68" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A68,": { ""id"": ",A68,", ""name"": """,B68,""", },")</f>
@@ -14012,10 +14030,10 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="C69" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A69,": { ""id"": ",A69,", ""name"": """,B69,""", },")</f>
@@ -14024,10 +14042,10 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C70" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A70,": { ""id"": ",A70,", ""name"": """,B70,""", },")</f>
@@ -14036,10 +14054,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C71" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A71,": { ""id"": ",A71,", ""name"": """,B71,""", },")</f>
@@ -14048,10 +14066,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C72" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A72,": { ""id"": ",A72,", ""name"": """,B72,""", },")</f>
@@ -14060,10 +14078,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C73" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A73,": { ""id"": ",A73,", ""name"": """,B73,""", },")</f>
@@ -14072,10 +14090,10 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C74" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A74,": { ""id"": ",A74,", ""name"": """,B74,""", },")</f>
@@ -14084,10 +14102,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C75" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A75,": { ""id"": ",A75,", ""name"": """,B75,""", },")</f>
@@ -14096,10 +14114,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C76" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A76,": { ""id"": ",A76,", ""name"": """,B76,""", },")</f>
@@ -14108,10 +14126,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C77" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A77,": { ""id"": ",A77,", ""name"": """,B77,""", },")</f>
@@ -14120,10 +14138,10 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C78" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A78,": { ""id"": ",A78,", ""name"": """,B78,""", },")</f>
@@ -14132,10 +14150,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C79" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A79,": { ""id"": ",A79,", ""name"": """,B79,""", },")</f>
@@ -14144,10 +14162,10 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C80" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A80,": { ""id"": ",A80,", ""name"": """,B80,""", },")</f>
@@ -14156,10 +14174,10 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C81" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A81,": { ""id"": ",A81,", ""name"": """,B81,""", },")</f>
@@ -14168,10 +14186,10 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C82" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A82,": { ""id"": ",A82,", ""name"": """,B82,""", },")</f>
@@ -14180,10 +14198,10 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C83" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A83,": { ""id"": ",A83,", ""name"": """,B83,""", },")</f>
@@ -14192,10 +14210,10 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C84" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A84,": { ""id"": ",A84,", ""name"": """,B84,""", },")</f>
@@ -14204,10 +14222,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C85" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A85,": { ""id"": ",A85,", ""name"": """,B85,""", },")</f>
@@ -14216,10 +14234,10 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C86" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A86,": { ""id"": ",A86,", ""name"": """,B86,""", },")</f>
@@ -14228,10 +14246,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C87" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A87,": { ""id"": ",A87,", ""name"": """,B87,""", },")</f>
@@ -14240,10 +14258,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C88" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A88,": { ""id"": ",A88,", ""name"": """,B88,""", },")</f>
@@ -14252,10 +14270,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C89" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A89,": { ""id"": ",A89,", ""name"": """,B89,""", },")</f>
@@ -14264,10 +14282,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C90" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A90,": { ""id"": ",A90,", ""name"": """,B90,""", },")</f>
@@ -14276,10 +14294,10 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C91" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A91,": { ""id"": ",A91,", ""name"": """,B91,""", },")</f>
@@ -14288,10 +14306,10 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C92" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A92,": { ""id"": ",A92,", ""name"": """,B92,""", },")</f>
@@ -14300,10 +14318,10 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C93" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A93,": { ""id"": ",A93,", ""name"": """,B93,""", },")</f>
@@ -14312,10 +14330,10 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C94" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A94,": { ""id"": ",A94,", ""name"": """,B94,""", },")</f>
@@ -14324,10 +14342,10 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C95" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A95,": { ""id"": ",A95,", ""name"": """,B95,""", },")</f>
@@ -14356,23 +14374,23 @@
       <selection pane="topLeft" activeCell="I46" activeCellId="0" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>135</v>
@@ -14383,13 +14401,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="E2" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A2,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B2, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C2, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D2, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14401,13 +14419,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>451</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>359</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>449</v>
       </c>
       <c r="E3" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A3,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B3, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C3, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D3, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14419,13 +14437,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>451</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>449</v>
       </c>
       <c r="E4" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A4,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B4, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C4, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D4, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14437,13 +14455,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>451</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>455</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>449</v>
       </c>
       <c r="E5" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A5,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B5, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C5, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D5, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14455,13 +14473,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>451</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>457</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>449</v>
       </c>
       <c r="E6" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A6,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B6, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C6, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D6, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14473,13 +14491,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>453</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>393</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>451</v>
       </c>
       <c r="E7" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A7,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B7, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C7, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D7, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14491,13 +14509,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>453</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>459</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>451</v>
       </c>
       <c r="E8" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A8,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B8, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C8, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D8, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14509,13 +14527,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>453</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>483</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>451</v>
       </c>
       <c r="E9" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A9,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B9, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C9, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D9, Commands!B:B, 0), 1, 1)),", },")</f>

</xml_diff>

<commit_message>
Added the story achievement for Hollow Bastion, Part II, and made tentative changes to another story achievement's title
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1946" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1962" uniqueCount="506">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -907,7 +907,7 @@
     <t xml:space="preserve">HollowBastionGrandHall</t>
   </si>
   <si>
-    <t xml:space="preserve">Grand Hall(?)</t>
+    <t xml:space="preserve">Grand Hall</t>
   </si>
   <si>
     <t xml:space="preserve">HollowBastionKeyholeEntrance</t>
@@ -968,6 +968,27 @@
   </si>
   <si>
     <t xml:space="preserve">Chapel (Dragon’s Lair)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionGrandHall2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionDataTunnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Tunnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HollowBastionCentralCorruption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Corruption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CastleOblivionHall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrance Hall</t>
   </si>
   <si>
     <t xml:space="preserve">0xFF</t>
@@ -1647,7 +1668,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -11207,12 +11228,13 @@
   <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B91" activeCellId="0" sqref="B91"/>
+      <selection pane="topLeft" activeCell="B95" activeCellId="0" sqref="B95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12807,7 +12829,7 @@
       </c>
       <c r="F76" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A76,": { ""worldId"": ",C76,", ""name"": """,D76,""", ""display"": """,E76,""", ""areaId"": ",B76,", },")</f>
-        <v>75: { "worldId": 0x5, "name": "HollowBastionGrandHall", "display": "Grand Hall(?)", "areaId": 0xd, },</v>
+        <v>75: { "worldId": 0x5, "name": "HollowBastionGrandHall", "display": "Grand Hall", "areaId": 0xd, },</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13108,36 +13130,84 @@
       <c r="A91" s="0" t="n">
         <v>90</v>
       </c>
+      <c r="B91" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="E91" s="0" t="s">
+        <v>294</v>
+      </c>
       <c r="F91" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A91,": { ""worldId"": ",C91,", ""name"": """,D91,""", ""display"": """,E91,""", ""areaId"": ",B91,", },")</f>
-        <v>90: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>90: { "worldId": 0x6, "name": "HollowBastionGrandHall2", "display": "Grand Hall", "areaId": 0xe, },</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
         <v>91</v>
       </c>
+      <c r="B92" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>317</v>
+      </c>
       <c r="F92" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A92,": { ""worldId"": ",C92,", ""name"": """,D92,""", ""display"": """,E92,""", ""areaId"": ",B92,", },")</f>
-        <v>91: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>91: { "worldId": 0x6, "name": "HollowBastionDataTunnel", "display": "Data Tunnel", "areaId": 0xd, },</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
         <v>92</v>
       </c>
+      <c r="B93" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>319</v>
+      </c>
       <c r="F93" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A93,": { ""worldId"": ",C93,", ""name"": """,D93,""", ""display"": """,E93,""", ""areaId"": ",B93,", },")</f>
-        <v>92: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>92: { "worldId": 0x6, "name": "HollowBastionCentralCorruption", "display": "Central Corruption", "areaId": 0x1, },</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
         <v>93</v>
       </c>
+      <c r="B94" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="E94" s="0" t="s">
+        <v>321</v>
+      </c>
       <c r="F94" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A94,": { ""worldId"": ",C94,", ""name"": """,D94,""", ""display"": """,E94,""", ""areaId"": ",B94,", },")</f>
-        <v>93: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>93: { "worldId": 0x7, "name": "CastleOblivionHall", "display": "Entrance Hall", "areaId": 0x7, },</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13207,7 +13277,7 @@
       <selection pane="topLeft" activeCell="F63" activeCellId="0" sqref="F63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -13226,10 +13296,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""", },")</f>
@@ -13238,10 +13308,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""", },")</f>
@@ -13250,10 +13320,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""", },")</f>
@@ -13262,10 +13332,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="C5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""", },")</f>
@@ -13274,10 +13344,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="C6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""", },")</f>
@@ -13286,10 +13356,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="C7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""", },")</f>
@@ -13298,10 +13368,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""", },")</f>
@@ -13310,10 +13380,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="C9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""", },")</f>
@@ -13322,10 +13392,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""", },")</f>
@@ -13334,10 +13404,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="C11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""", },")</f>
@@ -13346,10 +13416,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="C12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""", },")</f>
@@ -13358,10 +13428,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="C13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A13,": { ""id"": ",A13,", ""name"": """,B13,""", },")</f>
@@ -13370,10 +13440,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="C14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A14,": { ""id"": ",A14,", ""name"": """,B14,""", },")</f>
@@ -13382,10 +13452,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="C15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A15,": { ""id"": ",A15,", ""name"": """,B15,""", },")</f>
@@ -13394,10 +13464,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="C16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A16,": { ""id"": ",A16,", ""name"": """,B16,""", },")</f>
@@ -13406,10 +13476,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="C17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A17,": { ""id"": ",A17,", ""name"": """,B17,""", },")</f>
@@ -13418,10 +13488,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="C18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A18,": { ""id"": ",A18,", ""name"": """,B18,""", },")</f>
@@ -13433,7 +13503,7 @@
         <v>301</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="C19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A19,": { ""id"": ",A19,", ""name"": """,B19,""", },")</f>
@@ -13445,7 +13515,7 @@
         <v>267</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="C20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A20,": { ""id"": ",A20,", ""name"": """,B20,""", },")</f>
@@ -13457,7 +13527,7 @@
         <v>256</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="C21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A21,": { ""id"": ",A21,", ""name"": """,B21,""", },")</f>
@@ -13466,10 +13536,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="C22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A22,": { ""id"": ",A22,", ""name"": """,B22,""", },")</f>
@@ -13478,10 +13548,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="C23" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A23,": { ""id"": ",A23,", ""name"": """,B23,""", },")</f>
@@ -13490,10 +13560,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="C24" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A24,": { ""id"": ",A24,", ""name"": """,B24,""", },")</f>
@@ -13502,10 +13572,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="C25" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A25,": { ""id"": ",A25,", ""name"": """,B25,""", },")</f>
@@ -13514,10 +13584,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="C26" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A26,": { ""id"": ",A26,", ""name"": """,B26,""", },")</f>
@@ -13526,10 +13596,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="C27" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A27,": { ""id"": ",A27,", ""name"": """,B27,""", },")</f>
@@ -13538,10 +13608,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="C28" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A28,": { ""id"": ",A28,", ""name"": """,B28,""", },")</f>
@@ -13550,10 +13620,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="C29" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A29,": { ""id"": ",A29,", ""name"": """,B29,""", },")</f>
@@ -13562,10 +13632,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="C30" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A30,": { ""id"": ",A30,", ""name"": """,B30,""", },")</f>
@@ -13574,10 +13644,10 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="C31" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A31,": { ""id"": ",A31,", ""name"": """,B31,""", },")</f>
@@ -13589,7 +13659,7 @@
         <v>203</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="C32" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A32,": { ""id"": ",A32,", ""name"": """,B32,""", },")</f>
@@ -13601,7 +13671,7 @@
         <v>206</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="C33" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A33,": { ""id"": ",A33,", ""name"": """,B33,""", },")</f>
@@ -13613,7 +13683,7 @@
         <v>211</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="C34" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A34,": { ""id"": ",A34,", ""name"": """,B34,""", },")</f>
@@ -13622,10 +13692,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C35" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A35,": { ""id"": ",A35,", ""name"": """,B35,""", },")</f>
@@ -13637,7 +13707,7 @@
         <v>241</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="C36" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A36,": { ""id"": ",A36,", ""name"": """,B36,""", },")</f>
@@ -13646,10 +13716,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="C37" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A37,": { ""id"": ",A37,", ""name"": """,B37,""", },")</f>
@@ -13658,10 +13728,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="C38" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A38,": { ""id"": ",A38,", ""name"": """,B38,""", },")</f>
@@ -13670,10 +13740,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="C39" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A39,": { ""id"": ",A39,", ""name"": """,B39,""", },")</f>
@@ -13682,10 +13752,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="C40" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A40,": { ""id"": ",A40,", ""name"": """,B40,""", },")</f>
@@ -13694,10 +13764,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="C41" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A41,": { ""id"": ",A41,", ""name"": """,B41,""", },")</f>
@@ -13706,10 +13776,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="C42" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A42,": { ""id"": ",A42,", ""name"": """,B42,""", },")</f>
@@ -13718,10 +13788,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="C43" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A43,": { ""id"": ",A43,", ""name"": """,B43,""", },")</f>
@@ -13730,10 +13800,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="C44" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A44,": { ""id"": ",A44,", ""name"": """,B44,""", },")</f>
@@ -13742,10 +13812,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C45" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A45,": { ""id"": ",A45,", ""name"": """,B45,""", },")</f>
@@ -13754,10 +13824,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="C46" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A46,": { ""id"": ",A46,", ""name"": """,B46,""", },")</f>
@@ -13766,10 +13836,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="C47" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A47,": { ""id"": ",A47,", ""name"": """,B47,""", },")</f>
@@ -13778,10 +13848,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="C48" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A48,": { ""id"": ",A48,", ""name"": """,B48,""", },")</f>
@@ -13790,10 +13860,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="C49" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A49,": { ""id"": ",A49,", ""name"": """,B49,""", },")</f>
@@ -13802,10 +13872,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="C50" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A50,": { ""id"": ",A50,", ""name"": """,B50,""", },")</f>
@@ -13814,10 +13884,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="C51" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A51,": { ""id"": ",A51,", ""name"": """,B51,""", },")</f>
@@ -13826,10 +13896,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="C52" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A52,": { ""id"": ",A52,", ""name"": """,B52,""", },")</f>
@@ -13838,10 +13908,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="C53" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A53,": { ""id"": ",A53,", ""name"": """,B53,""", },")</f>
@@ -13850,10 +13920,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="C54" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A54,": { ""id"": ",A54,", ""name"": """,B54,""", },")</f>
@@ -13862,10 +13932,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="C55" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A55,": { ""id"": ",A55,", ""name"": """,B55,""", },")</f>
@@ -13874,10 +13944,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="C56" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A56,": { ""id"": ",A56,", ""name"": """,B56,""", },")</f>
@@ -13886,10 +13956,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="C57" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A57,": { ""id"": ",A57,", ""name"": """,B57,""", },")</f>
@@ -13898,10 +13968,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="C58" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A58,": { ""id"": ",A58,", ""name"": """,B58,""", },")</f>
@@ -13910,10 +13980,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="C59" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A59,": { ""id"": ",A59,", ""name"": """,B59,""", },")</f>
@@ -13922,10 +13992,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
       <c r="C60" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A60,": { ""id"": ",A60,", ""name"": """,B60,""", },")</f>
@@ -13934,10 +14004,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>426</v>
+        <v>433</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="C61" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A61,": { ""id"": ",A61,", ""name"": """,B61,""", },")</f>
@@ -13946,10 +14016,10 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
       <c r="C62" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A62,": { ""id"": ",A62,", ""name"": """,B62,""", },")</f>
@@ -13958,10 +14028,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>431</v>
+        <v>438</v>
       </c>
       <c r="C63" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A63,": { ""id"": ",A63,", ""name"": """,B63,""", },")</f>
@@ -13970,10 +14040,10 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="C64" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A64,": { ""id"": ",A64,", ""name"": """,B64,""", },")</f>
@@ -13982,10 +14052,10 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="C65" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A65,": { ""id"": ",A65,", ""name"": """,B65,""", },")</f>
@@ -13994,10 +14064,10 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="C66" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A66,": { ""id"": ",A66,", ""name"": """,B66,""", },")</f>
@@ -14006,10 +14076,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="C67" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A67,": { ""id"": ",A67,", ""name"": """,B67,""", },")</f>
@@ -14018,10 +14088,10 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="C68" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A68,": { ""id"": ",A68,", ""name"": """,B68,""", },")</f>
@@ -14030,10 +14100,10 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="C69" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A69,": { ""id"": ",A69,", ""name"": """,B69,""", },")</f>
@@ -14042,10 +14112,10 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="C70" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A70,": { ""id"": ",A70,", ""name"": """,B70,""", },")</f>
@@ -14054,10 +14124,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="C71" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A71,": { ""id"": ",A71,", ""name"": """,B71,""", },")</f>
@@ -14066,10 +14136,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="C72" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A72,": { ""id"": ",A72,", ""name"": """,B72,""", },")</f>
@@ -14078,10 +14148,10 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="C73" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A73,": { ""id"": ",A73,", ""name"": """,B73,""", },")</f>
@@ -14090,10 +14160,10 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="C74" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A74,": { ""id"": ",A74,", ""name"": """,B74,""", },")</f>
@@ -14102,10 +14172,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="C75" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A75,": { ""id"": ",A75,", ""name"": """,B75,""", },")</f>
@@ -14114,10 +14184,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="C76" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A76,": { ""id"": ",A76,", ""name"": """,B76,""", },")</f>
@@ -14126,10 +14196,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="C77" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A77,": { ""id"": ",A77,", ""name"": """,B77,""", },")</f>
@@ -14138,10 +14208,10 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="C78" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A78,": { ""id"": ",A78,", ""name"": """,B78,""", },")</f>
@@ -14150,10 +14220,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="C79" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A79,": { ""id"": ",A79,", ""name"": """,B79,""", },")</f>
@@ -14162,10 +14232,10 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="C80" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A80,": { ""id"": ",A80,", ""name"": """,B80,""", },")</f>
@@ -14174,10 +14244,10 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="C81" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A81,": { ""id"": ",A81,", ""name"": """,B81,""", },")</f>
@@ -14186,10 +14256,10 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="C82" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A82,": { ""id"": ",A82,", ""name"": """,B82,""", },")</f>
@@ -14198,10 +14268,10 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="C83" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A83,": { ""id"": ",A83,", ""name"": """,B83,""", },")</f>
@@ -14210,10 +14280,10 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="C84" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A84,": { ""id"": ",A84,", ""name"": """,B84,""", },")</f>
@@ -14222,10 +14292,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>475</v>
+        <v>482</v>
       </c>
       <c r="C85" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A85,": { ""id"": ",A85,", ""name"": """,B85,""", },")</f>
@@ -14234,10 +14304,10 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>476</v>
+        <v>483</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="C86" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A86,": { ""id"": ",A86,", ""name"": """,B86,""", },")</f>
@@ -14246,10 +14316,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="C87" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A87,": { ""id"": ",A87,", ""name"": """,B87,""", },")</f>
@@ -14258,10 +14328,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
       <c r="C88" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A88,": { ""id"": ",A88,", ""name"": """,B88,""", },")</f>
@@ -14270,10 +14340,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>482</v>
+        <v>489</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="C89" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A89,": { ""id"": ",A89,", ""name"": """,B89,""", },")</f>
@@ -14282,10 +14352,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="C90" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A90,": { ""id"": ",A90,", ""name"": """,B90,""", },")</f>
@@ -14294,10 +14364,10 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="C91" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A91,": { ""id"": ",A91,", ""name"": """,B91,""", },")</f>
@@ -14306,10 +14376,10 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="C92" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A92,": { ""id"": ",A92,", ""name"": """,B92,""", },")</f>
@@ -14318,10 +14388,10 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="C93" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A93,": { ""id"": ",A93,", ""name"": """,B93,""", },")</f>
@@ -14330,10 +14400,10 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="C94" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A94,": { ""id"": ",A94,", ""name"": """,B94,""", },")</f>
@@ -14342,10 +14412,10 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="C95" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A95,": { ""id"": ",A95,", ""name"": """,B95,""", },")</f>
@@ -14374,23 +14444,23 @@
       <selection pane="topLeft" activeCell="I46" activeCellId="0" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>135</v>
@@ -14401,13 +14471,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="E2" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A2,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B2, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C2, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D2, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14419,13 +14489,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="E3" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A3,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B3, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C3, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D3, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14437,13 +14507,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="E4" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A4,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B4, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C4, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D4, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14455,13 +14525,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="E5" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A5,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B5, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C5, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D5, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14473,13 +14543,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="E6" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A6,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B6, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C6, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D6, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14491,13 +14561,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="E7" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A7,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B7, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C7, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D7, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14509,13 +14579,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="E8" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A8,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B8, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C8, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D8, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14527,13 +14597,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="E9" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A9,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B9, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C9, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D9, Commands!B:B, 0), 1, 1)),", },")</f>

</xml_diff>

<commit_message>
Added command conversion recipes for ranged commands
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,9 @@
     <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Command Conversion Combinations" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$95</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1962" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="510">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -991,6 +994,9 @@
     <t xml:space="preserve">Entrance Hall</t>
   </si>
   <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
     <t xml:space="preserve">0xFF</t>
   </si>
   <si>
@@ -1003,6 +1009,9 @@
     <t xml:space="preserve">Quick Blitz</t>
   </si>
   <si>
+    <t xml:space="preserve">Melee</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x01</t>
   </si>
   <si>
@@ -1021,6 +1030,9 @@
     <t xml:space="preserve">Strike Raid</t>
   </si>
   <si>
+    <t xml:space="preserve">Ranged</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x04</t>
   </si>
   <si>
@@ -1400,6 +1412,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Support</t>
   </si>
   <si>
     <t xml:space="preserve">0x47</t>
@@ -1550,7 +1565,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1584,6 +1599,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1628,7 +1648,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1645,6 +1665,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1655,6 +1679,10 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1668,7 +1696,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -11227,11 +11255,11 @@
   </sheetPr>
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B95" activeCellId="0" sqref="B95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -13268,16 +13296,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F63" activeCellId="0" sqref="F63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C100" activeCellId="0" sqref="C100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -13291,1138 +13319,1430 @@
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="C2" s="0" t="str">
+        <v>324</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""", },")</f>
         <v>0xFF: { "id": 0xFF, "name": "N/A", },</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="C3" s="0" t="str">
+        <v>326</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""", },")</f>
         <v>0x00: { "id": 0x00, "name": "Quick Blitz", },</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="C4" s="0" t="str">
+      <c r="D4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""", },")</f>
         <v>0x01: { "id": 0x01, "name": "Sliding Dash", },</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="C5" s="0" t="str">
+        <v>331</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""", },")</f>
         <v>0x02: { "id": 0x02, "name": "Round Blitz", },</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="C6" s="0" t="str">
+        <v>333</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""", },")</f>
         <v>0x03: { "id": 0x03, "name": "Strike Raid", },</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="C7" s="0" t="str">
+        <v>336</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""", },")</f>
         <v>0x04: { "id": 0x04, "name": "Rising Strike", },</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="C8" s="0" t="str">
+        <v>338</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""", },")</f>
         <v>0x05: { "id": 0x05, "name": "Sliding Rush", },</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="C9" s="0" t="str">
+        <v>340</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""", },")</f>
         <v>0x06: { "id": 0x06, "name": "Aerial Sweep", },</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="C10" s="0" t="str">
+        <v>342</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""", },")</f>
         <v>0x07: { "id": 0x07, "name": "Air Sweep", },</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>341</v>
-      </c>
-      <c r="C11" s="0" t="str">
+        <v>344</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""", },")</f>
         <v>0x08: { "id": 0x08, "name": "Aerial Slam", },</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="C12" s="0" t="str">
+        <v>346</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""", },")</f>
         <v>0x09: { "id": 0x09, "name": "Land Crash", },</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="C13" s="0" t="str">
+        <v>348</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A13,": { ""id"": ",A13,", ""name"": """,B13,""", },")</f>
         <v>0x0a: { "id": 0x0a, "name": "Fire Edge", },</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="C14" s="0" t="str">
+        <v>350</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A14,": { ""id"": ",A14,", ""name"": """,B14,""", },")</f>
         <v>0x0b: { "id": 0x0b, "name": "Blizzard Edge", },</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="C15" s="0" t="str">
+        <v>352</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A15,": { ""id"": ",A15,", ""name"": """,B15,""", },")</f>
         <v>0x0c: { "id": 0x0c, "name": "Thunder Edge", },</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>351</v>
-      </c>
-      <c r="C16" s="0" t="str">
+        <v>354</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A16,": { ""id"": ",A16,", ""name"": """,B16,""", },")</f>
         <v>0x0d: { "id": 0x0d, "name": "Aero Edge", },</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="C17" s="0" t="str">
+        <v>356</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A17,": { ""id"": ",A17,", ""name"": """,B17,""", },")</f>
         <v>0x0e: { "id": 0x0e, "name": "Heat Dash", },</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="C18" s="0" t="str">
+        <v>358</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A18,": { ""id"": ",A18,", ""name"": """,B18,""", },")</f>
         <v>0x0f: { "id": 0x0f, "name": "Ice Dash", },</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>301</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="C19" s="0" t="str">
+        <v>359</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A19,": { ""id"": ",A19,", ""name"": """,B19,""", },")</f>
         <v>0x10: { "id": 0x10, "name": "Spark Dash", },</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>267</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>357</v>
-      </c>
-      <c r="C20" s="0" t="str">
+        <v>360</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A20,": { ""id"": ",A20,", ""name"": """,B20,""", },")</f>
         <v>0x11: { "id": 0x11, "name": "Wind Dash", },</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>256</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>358</v>
-      </c>
-      <c r="C21" s="0" t="str">
+        <v>361</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A21,": { ""id"": ",A21,", ""name"": """,B21,""", },")</f>
         <v>0x12: { "id": 0x12, "name": "Fire Blast", },</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="C22" s="0" t="str">
+        <v>363</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A22,": { ""id"": ",A22,", ""name"": """,B22,""", },")</f>
         <v>0x13: { "id": 0x13, "name": "Blizzard Blast", },</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="C23" s="0" t="str">
+        <v>365</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D23" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A23,": { ""id"": ",A23,", ""name"": """,B23,""", },")</f>
         <v>0x14: { "id": 0x14, "name": "Thunder Blast", },</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>364</v>
-      </c>
-      <c r="C24" s="0" t="str">
+        <v>367</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D24" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A24,": { ""id"": ",A24,", ""name"": """,B24,""", },")</f>
         <v>0x15: { "id": 0x15, "name": "Aero Blast", },</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>366</v>
-      </c>
-      <c r="C25" s="0" t="str">
+        <v>369</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D25" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A25,": { ""id"": ",A25,", ""name"": """,B25,""", },")</f>
         <v>0x16: { "id": 0x16, "name": "Fire Raid", },</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>368</v>
-      </c>
-      <c r="C26" s="0" t="str">
+        <v>371</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D26" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A26,": { ""id"": ",A26,", ""name"": """,B26,""", },")</f>
         <v>0x17: { "id": 0x17, "name": "Blizzard Raid", },</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>370</v>
-      </c>
-      <c r="C27" s="0" t="str">
+        <v>373</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D27" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A27,": { ""id"": ",A27,", ""name"": """,B27,""", },")</f>
         <v>0x18: { "id": 0x18, "name": "Thunder Raid", },</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>372</v>
-      </c>
-      <c r="C28" s="0" t="str">
+        <v>375</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D28" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A28,": { ""id"": ",A28,", ""name"": """,B28,""", },")</f>
         <v>0x19: { "id": 0x19, "name": "Aero Raid", },</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>374</v>
-      </c>
-      <c r="C29" s="0" t="str">
+        <v>377</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D29" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A29,": { ""id"": ",A29,", ""name"": """,B29,""", },")</f>
         <v>0x1a: { "id": 0x1a, "name": "Fire Buster", },</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>376</v>
-      </c>
-      <c r="C30" s="0" t="str">
+        <v>379</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D30" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A30,": { ""id"": ",A30,", ""name"": """,B30,""", },")</f>
         <v>0x1b: { "id": 0x1b, "name": "Blizzard Buster", },</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="C31" s="0" t="str">
+        <v>381</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D31" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A31,": { ""id"": ",A31,", ""name"": """,B31,""", },")</f>
         <v>0x1c: { "id": 0x1c, "name": "Thunder Buster", },</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>203</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>379</v>
-      </c>
-      <c r="C32" s="0" t="str">
+        <v>382</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D32" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A32,": { ""id"": ",A32,", ""name"": """,B32,""", },")</f>
         <v>0x1d: { "id": 0x1d, "name": "Aero Buster", },</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>206</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>380</v>
-      </c>
-      <c r="C33" s="0" t="str">
+        <v>383</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D33" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A33,": { ""id"": ",A33,", ""name"": """,B33,""", },")</f>
         <v>0x1e: { "id": 0x1e, "name": "Heat Sweep", },</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>211</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>381</v>
-      </c>
-      <c r="C34" s="0" t="str">
+        <v>384</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D34" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A34,": { ""id"": ",A34,", ""name"": """,B34,""", },")</f>
         <v>0x1f: { "id": 0x1f, "name": "Ice Sweep", },</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>383</v>
-      </c>
-      <c r="C35" s="0" t="str">
+        <v>386</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D35" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A35,": { ""id"": ",A35,", ""name"": """,B35,""", },")</f>
         <v>0x20: { "id": 0x20, "name": "Spark Sweep", },</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>241</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>384</v>
-      </c>
-      <c r="C36" s="0" t="str">
+        <v>387</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D36" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A36,": { ""id"": ",A36,", ""name"": """,B36,""", },")</f>
         <v>0x21: { "id": 0x21, "name": "Wind Sweep", },</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>386</v>
-      </c>
-      <c r="C37" s="0" t="str">
+        <v>389</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D37" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A37,": { ""id"": ",A37,", ""name"": """,B37,""", },")</f>
         <v>0x22: { "id": 0x22, "name": "Heat Storm", },</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>388</v>
-      </c>
-      <c r="C38" s="0" t="str">
+        <v>391</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D38" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A38,": { ""id"": ",A38,", ""name"": """,B38,""", },")</f>
         <v>0x23: { "id": 0x23, "name": "Ice Storm", },</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>390</v>
-      </c>
-      <c r="C39" s="0" t="str">
+        <v>393</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D39" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A39,": { ""id"": ",A39,", ""name"": """,B39,""", },")</f>
         <v>0x24: { "id": 0x24, "name": "Spark Storm", },</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>392</v>
-      </c>
-      <c r="C40" s="0" t="str">
+        <v>395</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D40" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A40,": { ""id"": ",A40,", ""name"": """,B40,""", },")</f>
         <v>0x25: { "id": 0x25, "name": "Wind Storm", },</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>394</v>
-      </c>
-      <c r="C41" s="0" t="str">
+        <v>397</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D41" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A41,": { ""id"": ",A41,", ""name"": """,B41,""", },")</f>
         <v>0x26: { "id": 0x26, "name": "Fire Slam", },</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="C42" s="0" t="str">
+        <v>399</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D42" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A42,": { ""id"": ",A42,", ""name"": """,B42,""", },")</f>
         <v>0x27: { "id": 0x27, "name": "Blizzard Slam", },</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="C43" s="0" t="str">
+        <v>401</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D43" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A43,": { ""id"": ",A43,", ""name"": """,B43,""", },")</f>
         <v>0x28: { "id": 0x28, "name": "Thunder Slam", },</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="C44" s="0" t="str">
+        <v>403</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D44" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A44,": { ""id"": ",A44,", ""name"": """,B44,""", },")</f>
         <v>0x29: { "id": 0x29, "name": "Aero Slam", },</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>402</v>
-      </c>
-      <c r="C45" s="0" t="str">
+        <v>405</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D45" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A45,": { ""id"": ",A45,", ""name"": """,B45,""", },")</f>
         <v>0x2a: { "id": 0x2a, "name": "Heat Dive", },</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>404</v>
-      </c>
-      <c r="C46" s="0" t="str">
+        <v>407</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D46" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A46,": { ""id"": ",A46,", ""name"": """,B46,""", },")</f>
         <v>0x2b: { "id": 0x2b, "name": "Ice Dive", },</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="C47" s="0" t="str">
+        <v>409</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D47" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A47,": { ""id"": ",A47,", ""name"": """,B47,""", },")</f>
         <v>0x2c: { "id": 0x2c, "name": "Spark Dive", },</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>408</v>
-      </c>
-      <c r="C48" s="0" t="str">
+        <v>411</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D48" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A48,": { ""id"": ",A48,", ""name"": """,B48,""", },")</f>
         <v>0x2d: { "id": 0x2d, "name": "Wind Dive", },</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="C49" s="0" t="str">
+        <v>413</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D49" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A49,": { ""id"": ",A49,", ""name"": """,B49,""", },")</f>
         <v>0x2e: { "id": 0x2e, "name": "Stun Impact", },</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>412</v>
-      </c>
-      <c r="C50" s="0" t="str">
+        <v>415</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D50" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A50,": { ""id"": ",A50,", ""name"": """,B50,""", },")</f>
         <v>0x2f: { "id": 0x2f, "name": "Muscle Strike", },</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>414</v>
-      </c>
-      <c r="C51" s="0" t="str">
+        <v>417</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D51" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A51,": { ""id"": ",A51,", ""name"": """,B51,""", },")</f>
         <v>0x30: { "id": 0x30, "name": "Chain Rave", },</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>416</v>
-      </c>
-      <c r="C52" s="0" t="str">
+        <v>419</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D52" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A52,": { ""id"": ",A52,", ""name"": """,B52,""", },")</f>
         <v>0x31: { "id": 0x31, "name": "Rising Rush", },</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>418</v>
-      </c>
-      <c r="C53" s="0" t="str">
+        <v>421</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D53" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A53,": { ""id"": ",A53,", ""name"": """,B53,""", },")</f>
         <v>0x32: { "id": 0x32, "name": "Zantetsuken", },</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>420</v>
-      </c>
-      <c r="C54" s="0" t="str">
+        <v>423</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D54" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A54,": { ""id"": ",A54,", ""name"": """,B54,""", },")</f>
         <v>0x33: { "id": 0x33, "name": "Eruption", },</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>422</v>
-      </c>
-      <c r="C55" s="0" t="str">
+        <v>425</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D55" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A55,": { ""id"": ",A55,", ""name"": """,B55,""", },")</f>
         <v>0x34: { "id": 0x34, "name": "Gravity Drop", },</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>424</v>
-      </c>
-      <c r="C56" s="0" t="str">
+        <v>427</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D56" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A56,": { ""id"": ",A56,", ""name"": """,B56,""", },")</f>
         <v>0x35: { "id": 0x35, "name": "Shock Fall", },</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>426</v>
-      </c>
-      <c r="C57" s="0" t="str">
+        <v>429</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D57" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A57,": { ""id"": ",A57,", ""name"": """,B57,""", },")</f>
         <v>0x36: { "id": 0x36, "name": "Judgment Triad", },</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>428</v>
-      </c>
-      <c r="C58" s="0" t="str">
+        <v>431</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D58" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A58,": { ""id"": ",A58,", ""name"": """,B58,""", },")</f>
         <v>0x37: { "id": 0x37, "name": "Fire", },</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>430</v>
-      </c>
-      <c r="C59" s="0" t="str">
+        <v>433</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D59" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A59,": { ""id"": ",A59,", ""name"": """,B59,""", },")</f>
         <v>0x38: { "id": 0x38, "name": "Fira", },</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>432</v>
-      </c>
-      <c r="C60" s="0" t="str">
+        <v>435</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D60" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A60,": { ""id"": ",A60,", ""name"": """,B60,""", },")</f>
         <v>0x39: { "id": 0x39, "name": "Firaga", },</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>434</v>
-      </c>
-      <c r="C61" s="0" t="str">
+        <v>437</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D61" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A61,": { ""id"": ",A61,", ""name"": """,B61,""", },")</f>
         <v>0x3a: { "id": 0x3a, "name": "Blizzard", },</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>436</v>
-      </c>
-      <c r="C62" s="0" t="str">
+        <v>439</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D62" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A62,": { ""id"": ",A62,", ""name"": """,B62,""", },")</f>
         <v>0x3b: { "id": 0x3b, "name": "Blizzara", },</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>438</v>
-      </c>
-      <c r="C63" s="0" t="str">
+        <v>441</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D63" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A63,": { ""id"": ",A63,", ""name"": """,B63,""", },")</f>
         <v>0x3c: { "id": 0x3c, "name": "Blizzaga", },</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>440</v>
-      </c>
-      <c r="C64" s="0" t="str">
+        <v>443</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D64" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A64,": { ""id"": ",A64,", ""name"": """,B64,""", },")</f>
         <v>0x3d: { "id": 0x3d, "name": "Thunder", },</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>442</v>
-      </c>
-      <c r="C65" s="0" t="str">
+        <v>445</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D65" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A65,": { ""id"": ",A65,", ""name"": """,B65,""", },")</f>
         <v>0x3e: { "id": 0x3e, "name": "Thundara", },</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>444</v>
-      </c>
-      <c r="C66" s="0" t="str">
+        <v>447</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D66" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A66,": { ""id"": ",A66,", ""name"": """,B66,""", },")</f>
         <v>0x3f: { "id": 0x3f, "name": "Thundaga", },</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>446</v>
-      </c>
-      <c r="C67" s="0" t="str">
+        <v>449</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D67" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A67,": { ""id"": ",A67,", ""name"": """,B67,""", },")</f>
         <v>0x40: { "id": 0x40, "name": "Aero", },</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>448</v>
-      </c>
-      <c r="C68" s="0" t="str">
+        <v>451</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D68" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A68,": { ""id"": ",A68,", ""name"": """,B68,""", },")</f>
         <v>0x41: { "id": 0x41, "name": "Aerora", },</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>450</v>
-      </c>
-      <c r="C69" s="0" t="str">
+        <v>453</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D69" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A69,": { ""id"": ",A69,", ""name"": """,B69,""", },")</f>
         <v>0x42: { "id": 0x42, "name": "Aeroga", },</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>452</v>
-      </c>
-      <c r="C70" s="0" t="str">
+        <v>455</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D70" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A70,": { ""id"": ",A70,", ""name"": """,B70,""", },")</f>
         <v>0x43: { "id": 0x43, "name": "Magnet", },</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>454</v>
-      </c>
-      <c r="C71" s="0" t="str">
+        <v>457</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D71" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A71,": { ""id"": ",A71,", ""name"": """,B71,""", },")</f>
         <v>0x44: { "id": 0x44, "name": "Magnera", },</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>456</v>
-      </c>
-      <c r="C72" s="0" t="str">
+        <v>459</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D72" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A72,": { ""id"": ",A72,", ""name"": """,B72,""", },")</f>
         <v>0x45: { "id": 0x45, "name": "Magnega", },</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>458</v>
-      </c>
-      <c r="C73" s="0" t="str">
+        <v>461</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="D73" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A73,": { ""id"": ",A73,", ""name"": """,B73,""", },")</f>
         <v>0x46: { "id": 0x46, "name": "Cure", },</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>460</v>
-      </c>
-      <c r="C74" s="0" t="str">
+        <v>464</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="D74" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A74,": { ""id"": ",A74,", ""name"": """,B74,""", },")</f>
         <v>0x47: { "id": 0x47, "name": "Cura", },</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B75" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="C75" s="0" t="s">
         <v>462</v>
       </c>
-      <c r="C75" s="0" t="str">
+      <c r="D75" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A75,": { ""id"": ",A75,", ""name"": """,B75,""", },")</f>
         <v>0x48: { "id": 0x48, "name": "Curaga", },</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>464</v>
-      </c>
-      <c r="C76" s="0" t="str">
+        <v>468</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D76" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A76,": { ""id"": ",A76,", ""name"": """,B76,""", },")</f>
         <v>0x49: { "id": 0x49, "name": "Slow", },</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>466</v>
-      </c>
-      <c r="C77" s="0" t="str">
+        <v>470</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D77" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A77,": { ""id"": ",A77,", ""name"": """,B77,""", },")</f>
         <v>0x4a: { "id": 0x4a, "name": "Stop", },</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="C78" s="0" t="str">
+        <v>472</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D78" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A78,": { ""id"": ",A78,", ""name"": """,B78,""", },")</f>
         <v>0x4b: { "id": 0x4b, "name": "Confuse", },</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>470</v>
-      </c>
-      <c r="C79" s="0" t="str">
+        <v>474</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D79" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A79,": { ""id"": ",A79,", ""name"": """,B79,""", },")</f>
         <v>0x4c: { "id": 0x4c, "name": "Firaga Burst", },</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>472</v>
-      </c>
-      <c r="C80" s="0" t="str">
+        <v>476</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D80" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A80,": { ""id"": ",A80,", ""name"": """,B80,""", },")</f>
         <v>0x4d: { "id": 0x4d, "name": "Triple Firaga", },</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>474</v>
-      </c>
-      <c r="C81" s="0" t="str">
+        <v>478</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D81" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A81,": { ""id"": ",A81,", ""name"": """,B81,""", },")</f>
         <v>0x4e: { "id": 0x4e, "name": "Triple Burst", },</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>476</v>
-      </c>
-      <c r="C82" s="0" t="str">
+        <v>480</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D82" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A82,": { ""id"": ",A82,", ""name"": """,B82,""", },")</f>
         <v>0x4f: { "id": 0x4f, "name": "Blizzaga Pursuit", },</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>478</v>
-      </c>
-      <c r="C83" s="0" t="str">
+        <v>482</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D83" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A83,": { ""id"": ",A83,", ""name"": """,B83,""", },")</f>
         <v>0x50: { "id": 0x50, "name": "Triple Blizzaga", },</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>480</v>
-      </c>
-      <c r="C84" s="0" t="str">
+        <v>484</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D84" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A84,": { ""id"": ",A84,", ""name"": """,B84,""", },")</f>
         <v>0x51: { "id": 0x51, "name": "Triple Pursuit", },</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>482</v>
-      </c>
-      <c r="C85" s="0" t="str">
+        <v>486</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D85" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A85,": { ""id"": ",A85,", ""name"": """,B85,""", },")</f>
         <v>0x52: { "id": 0x52, "name": "Thunder Tracer", },</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="C86" s="0" t="str">
+        <v>488</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D86" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A86,": { ""id"": ",A86,", ""name"": """,B86,""", },")</f>
         <v>0x53: { "id": 0x53, "name": "Pulse Tracer", },</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>486</v>
-      </c>
-      <c r="C87" s="0" t="str">
+        <v>490</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D87" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A87,": { ""id"": ",A87,", ""name"": """,B87,""", },")</f>
         <v>0x54: { "id": 0x54, "name": "Tornado Tracer", },</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>488</v>
-      </c>
-      <c r="C88" s="0" t="str">
+        <v>492</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D88" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A88,": { ""id"": ",A88,", ""name"": """,B88,""", },")</f>
         <v>0x55: { "id": 0x55, "name": "Wind Tracer", },</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="C89" s="0" t="str">
+        <v>494</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D89" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A89,": { ""id"": ",A89,", ""name"": """,B89,""", },")</f>
         <v>0x56: { "id": 0x56, "name": "Magnet Grab", },</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>492</v>
-      </c>
-      <c r="C90" s="0" t="str">
+        <v>496</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="D90" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A90,": { ""id"": ",A90,", ""name"": """,B90,""", },")</f>
         <v>0x57: { "id": 0x57, "name": "Esuna", },</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="C91" s="0" t="str">
+        <v>498</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D91" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A91,": { ""id"": ",A91,", ""name"": """,B91,""", },")</f>
         <v>0x58: { "id": 0x58, "name": "Flame Fall", },</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>496</v>
-      </c>
-      <c r="C92" s="0" t="str">
+        <v>500</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D92" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A92,": { ""id"": ",A92,", ""name"": """,B92,""", },")</f>
         <v>0x59: { "id": 0x59, "name": "Icicle Mine", },</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>498</v>
-      </c>
-      <c r="C93" s="0" t="str">
+        <v>502</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D93" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A93,": { ""id"": ",A93,", ""name"": """,B93,""", },")</f>
         <v>0x5a: { "id": 0x5a, "name": "Exo Spark", },</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="C94" s="0" t="str">
+        <v>504</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D94" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A94,": { ""id"": ",A94,", ""name"": """,B94,""", },")</f>
         <v>0x5b: { "id": 0x5b, "name": "Cyclone", },</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>502</v>
-      </c>
-      <c r="C95" s="0" t="str">
+        <v>506</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D95" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A95,": { ""id"": ",A95,", ""name"": """,B95,""", },")</f>
         <v>0x5c: { "id": 0x5c, "name": "Quake", },</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:C95">
+    <filterColumn colId="0">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Ranged"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -14430,6 +14750,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14438,29 +14759,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I46" activeCellId="0" sqref="I46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C137" activeCellId="0" sqref="C137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>135</v>
@@ -14471,13 +14794,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="E2" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A2,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B2, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C2, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D2, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14489,13 +14812,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="E3" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A3,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B3, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C3, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D3, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14507,13 +14830,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="E4" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A4,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B4, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C4, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D4, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14525,13 +14848,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="E5" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A5,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B5, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C5, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D5, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14543,13 +14866,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="E6" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A6,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B6, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C6, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D6, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14561,13 +14884,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="E7" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A7,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B7, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C7, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D7, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14579,13 +14902,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="E8" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A8,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B8, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C8, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D8, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14597,13 +14920,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="E9" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A9,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B9, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C9, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D9, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14614,144 +14937,2286 @@
       <c r="A10" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="E10" s="0" t="e">
+      <c r="B10" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="E10" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A10,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B10, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C10, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D10, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>8: { "targetId": 0x16, "command1Id": 0x03, "command2Id": 0x01, },</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="E11" s="0" t="e">
+      <c r="B11" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="E11" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A11,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B11, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C11, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D11, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>9: { "targetId": 0x16, "command1Id": 0x04, "command2Id": 0x19, },</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="E12" s="0" t="e">
+      <c r="B12" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="E12" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A12,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B12, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C12, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D12, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>10: { "targetId": 0x16, "command1Id": 0x08, "command2Id": 0x0e, },</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="E13" s="0" t="e">
+      <c r="B13" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="E13" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A13,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B13, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C13, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D13, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>11: { "targetId": 0x16, "command1Id": 0x37, "command2Id": 0x03, },</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="E14" s="0" t="e">
+      <c r="B14" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="E14" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A14,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B14, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C14, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D14, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>12: { "targetId": 0x16, "command1Id": 0x38, "command2Id": 0x03, },</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="E15" s="0" t="e">
+      <c r="B15" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="E15" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A15,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B15, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C15, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D15, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>13: { "targetId": 0x17, "command1Id": 0x03, "command2Id": 0x01, },</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="E16" s="0" t="e">
+      <c r="B16" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="E16" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A16,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B16, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C16, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D16, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>14: { "targetId": 0x17, "command1Id": 0x04, "command2Id": 0x16, },</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="E17" s="0" t="e">
+      <c r="B17" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="E17" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A17,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B17, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C17, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D17, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>15: { "targetId": 0x17, "command1Id": 0x08, "command2Id": 0x0f, },</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="E18" s="0" t="e">
+      <c r="B18" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="E18" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A18,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B18, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C18, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D18, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>16: { "targetId": 0x17, "command1Id": 0x3a, "command2Id": 0x03, },</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="E19" s="0" t="e">
+      <c r="B19" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="E19" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A19,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B19, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C19, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D19, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>17: { "targetId": 0x17, "command1Id": 0x3b, "command2Id": 0x03, },</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="E20" s="0" t="e">
+      <c r="B20" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="E20" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A20,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B20, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C20, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D20, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>18: { "targetId": 0x18, "command1Id": 0x03, "command2Id": 0x02, },</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="E21" s="0" t="e">
+      <c r="B21" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="E21" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A21,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B21, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C21, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D21, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>19: { "targetId": 0x18, "command1Id": 0x04, "command2Id": 0x17, },</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="E22" s="0" t="e">
+      <c r="B22" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="E22" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A22,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B22, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C22, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D22, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>20: { "targetId": 0x18, "command1Id": 0x08, "command2Id": 0x10, },</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="E23" s="0" t="e">
+      <c r="B23" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="E23" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A23,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B23, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C23, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D23, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>21: { "targetId": 0x18, "command1Id": 0x3d, "command2Id": 0x03, },</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="E24" s="0" t="e">
+      <c r="B24" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="E24" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A24,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B24, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C24, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D24, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>22: { "targetId": 0x18, "command1Id": 0x3e, "command2Id": 0x03, },</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="E25" s="0" t="e">
+      <c r="B25" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="E25" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A25,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B25, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C25, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D25, Commands!B:B, 0), 1, 1)),", },")</f>
-        <v>#N/A</v>
+        <v>23: { "targetId": 0x19, "command1Id": 0x09, "command2Id": 0x09, },</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="E26" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A26,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B26, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C26, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D26, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>24: { "targetId": 0x19, "command1Id": 0x08, "command2Id": 0x11, },</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="E27" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A27,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B27, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C27, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D27, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>25: { "targetId": 0x19, "command1Id": 0x11, "command2Id": 0x18, },</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="E28" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A28,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B28, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C28, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D28, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>26: { "targetId": 0x19, "command1Id": 0x40, "command2Id": 0x03, },</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="E29" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A29,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B29, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C29, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D29, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>27: { "targetId": 0x19, "command1Id": 0x41, "command2Id": 0x03, },</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="E30" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A30,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B30, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C30, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D30, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>28: { "targetId": 0x36, "command1Id": 0x2f, "command2Id": 0x55, },</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="E31" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A31,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B31, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C31, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D31, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>29: { "targetId": 0x38, "command1Id": 0x0a, "command2Id": 0x02, },</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E32" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A32,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B32, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C32, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D32, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>30: { "targetId": 0x38, "command1Id": 0x37, "command2Id": 0x0a, },</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="E33" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A33,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B33, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C33, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D33, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>31: { "targetId": 0x38, "command1Id": 0x37, "command2Id": 0x46, },</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="E34" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A34,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B34, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C34, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D34, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>32: { "targetId": 0x38, "command1Id": 0x37, "command2Id": 0x49, },</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E35" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A35,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B35, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C35, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D35, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>33: { "targetId": 0x38, "command1Id": 0x46, "command2Id": 0x0a, },</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E36" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A36,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B36, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C36, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D36, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>34: { "targetId": 0x38, "command1Id": 0x49, "command2Id": 0x0a, },</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E37" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A37,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B37, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C37, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D37, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>35: { "targetId": 0x38, "command1Id": 0x4a, "command2Id": 0x0a, },</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="E38" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A38,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B38, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C38, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D38, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>36: { "targetId": 0x39, "command1Id": 0x12, "command2Id": 0x16, },</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="E39" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A39,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B39, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C39, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D39, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>37: { "targetId": 0x39, "command1Id": 0x38, "command2Id": 0x22, },</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="E40" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A40,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B40, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C40, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D40, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>38: { "targetId": 0x39, "command1Id": 0x4b, "command2Id": 0x22, },</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="E41" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A41,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B41, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C41, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D41, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>39: { "targetId": 0x39, "command1Id": 0x57, "command2Id": 0x22, },</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="E42" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A42,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B42, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C42, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D42, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>40: { "targetId": 0x3b, "command1Id": 0x0f, "command2Id": 0x00, },</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="E43" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A43,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B43, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C43, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D43, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>41: { "targetId": 0x3b, "command1Id": 0x3a, "command2Id": 0x0b, },</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="E44" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A44,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B44, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C44, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D44, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>42: { "targetId": 0x3b, "command1Id": 0x3a, "command2Id": 0x37, },</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="E45" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A45,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B45, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C45, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D45, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>43: { "targetId": 0x3b, "command1Id": 0x3a, "command2Id": 0x3d, },</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="E46" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A46,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B46, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C46, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D46, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>44: { "targetId": 0x3b, "command1Id": 0x3a, "command2Id": 0x46, },</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="E47" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A47,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B47, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C47, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D47, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>45: { "targetId": 0x3b, "command1Id": 0x3a, "command2Id": 0x49, },</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="E48" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A48,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B48, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C48, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D48, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>46: { "targetId": 0x3b, "command1Id": 0x46, "command2Id": 0x0b, },</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="E49" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A49,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B49, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C49, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D49, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>47: { "targetId": 0x3b, "command1Id": 0x49, "command2Id": 0x0b, },</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="E50" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A50,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B50, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C50, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D50, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>48: { "targetId": 0x3b, "command1Id": 0x4a, "command2Id": 0x0b, },</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="E51" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A51,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B51, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C51, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D51, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>49: { "targetId": 0x3c, "command1Id": 0x0f, "command2Id": 0x14, },</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="E52" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A52,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B52, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C52, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D52, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>50: { "targetId": 0x3c, "command1Id": 0x1d, "command2Id": 0x23, },</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="E53" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A53,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B53, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C53, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D53, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>51: { "targetId": 0x3c, "command1Id": 0x2b, "command2Id": 0x3b, },</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="E54" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A54,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B54, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C54, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D54, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>52: { "targetId": 0x3c, "command1Id": 0x4b, "command2Id": 0x23, },</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="E55" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A55,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B55, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C55, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D55, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>53: { "targetId": 0x3c, "command1Id": 0x57, "command2Id": 0x23, },</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="E56" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A56,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B56, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C56, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D56, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>54: { "targetId": 0x3e, "command1Id": 0x0c, "command2Id": 0x37, },</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="E57" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A57,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B57, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C57, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D57, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>55: { "targetId": 0x3e, "command1Id": 0x10, "command2Id": 0x02, },</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E58" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A58,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B58, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C58, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D58, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>56: { "targetId": 0x3e, "command1Id": 0x3d, "command2Id": 0x0c, },</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="E59" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A59,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B59, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C59, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D59, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>57: { "targetId": 0x3e, "command1Id": 0x3d, "command2Id": 0x37, },</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="E60" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A60,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B60, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C60, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D60, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>58: { "targetId": 0x3e, "command1Id": 0x3d, "command2Id": 0x46, },</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="E61" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A61,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B61, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C61, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D61, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>59: { "targetId": 0x3e, "command1Id": 0x3d, "command2Id": 0x49, },</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E62" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A62,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B62, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C62, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D62, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>60: { "targetId": 0x3e, "command1Id": 0x46, "command2Id": 0x0c, },</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E63" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A63,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B63, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C63, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D63, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>61: { "targetId": 0x3e, "command1Id": 0x49, "command2Id": 0x0c, },</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E64" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A64,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B64, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C64, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D64, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>62: { "targetId": 0x3e, "command1Id": 0x4a, "command2Id": 0x0c, },</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="E65" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A65,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B65, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C65, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D65, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>63: { "targetId": 0x3f, "command1Id": 0x0c, "command2Id": 0x19, },</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="E66" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A66,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B66, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C66, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D66, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>64: { "targetId": 0x3f, "command1Id": 0x0c, "command2Id": 0x21, },</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="E67" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A67,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B67, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C67, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D67, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>65: { "targetId": 0x3f, "command1Id": 0x3e, "command2Id": 0x24, },</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="E68" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A68,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B68, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C68, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D68, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>66: { "targetId": 0x3f, "command1Id": 0x4b, "command2Id": 0x24, },</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="E69" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A69,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B69, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C69, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D69, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>67: { "targetId": 0x3f, "command1Id": 0x57, "command2Id": 0x24, },</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="E70" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A70,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B70, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C70, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D70, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>68: { "targetId": 0x41, "command1Id": 0x40, "command2Id": 0x0d, },</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="E71" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A71,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B71, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C71, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D71, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>69: { "targetId": 0x41, "command1Id": 0x46, "command2Id": 0x0d, },</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="E72" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A72,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B72, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C72, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D72, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>70: { "targetId": 0x41, "command1Id": 0x49, "command2Id": 0x0d, },</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="E73" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A73,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B73, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C73, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D73, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>71: { "targetId": 0x41, "command1Id": 0x4a, "command2Id": 0x0d, },</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="E74" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A74,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B74, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C74, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D74, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>72: { "targetId": 0x42, "command1Id": 0x21, "command2Id": 0x46, },</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="E75" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A75,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B75, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C75, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D75, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>73: { "targetId": 0x42, "command1Id": 0x21, "command2Id": 0x49, },</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="E76" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A76,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B76, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C76, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D76, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>74: { "targetId": 0x42, "command1Id": 0x41, "command2Id": 0x25, },</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="E77" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A77,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B77, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C77, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D77, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>75: { "targetId": 0x42, "command1Id": 0x4b, "command2Id": 0x25, },</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="E78" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A78,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B78, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C78, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D78, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>76: { "targetId": 0x42, "command1Id": 0x57, "command2Id": 0x25, },</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="E79" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A79,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B79, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C79, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D79, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>77: { "targetId": 0x44, "command1Id": 0x27, "command2Id": 0x43, },</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="E80" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A80,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B80, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C80, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D80, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>78: { "targetId": 0x44, "command1Id": 0x46, "command2Id": 0x43, },</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="E81" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A81,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B81, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C81, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D81, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>79: { "targetId": 0x44, "command1Id": 0x49, "command2Id": 0x43, },</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="E82" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A82,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B82, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C82, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D82, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>80: { "targetId": 0x44, "command1Id": 0x4a, "command2Id": 0x43, },</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="E83" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A83,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B83, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C83, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D83, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>81: { "targetId": 0x45, "command1Id": 0x48, "command2Id": 0x44, },</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="E84" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A84,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B84, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C84, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D84, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>82: { "targetId": 0x45, "command1Id": 0x4b, "command2Id": 0x44, },</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="E85" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A85,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B85, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C85, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D85, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>83: { "targetId": 0x45, "command1Id": 0x57, "command2Id": 0x44, },</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="E86" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A86,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B86, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C86, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D86, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>84: { "targetId": 0x49, "command1Id": 0x01, "command2Id": 0x46, },</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="E87" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A87,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B87, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C87, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D87, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>85: { "targetId": 0x49, "command1Id": 0x04, "command2Id": 0x46, },</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="E88" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A88,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B88, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C88, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D88, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>86: { "targetId": 0x4c, "command1Id": 0x2e, "command2Id": 0x31, },</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="E89" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A89,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B89, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C89, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D89, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>87: { "targetId": 0x4c, "command1Id": 0x38, "command2Id": 0x4e, },</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="E90" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A90,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B90, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C90, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D90, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>88: { "targetId": 0x4c, "command1Id": 0x39, "command2Id": 0x26, },</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="E91" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A91,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B91, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C91, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D91, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>89: { "targetId": 0x4c, "command1Id": 0x39, "command2Id": 0x4e, },</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="E92" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A92,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B92, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C92, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D92, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>90: { "targetId": 0x4d, "command1Id": 0x2a, "command2Id": 0x39, },</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="E93" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A93,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B93, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C93, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D93, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>91: { "targetId": 0x4d, "command1Id": 0x2f, "command2Id": 0x31, },</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="E94" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A94,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B94, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C94, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D94, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>92: { "targetId": 0x4d, "command1Id": 0x39, "command2Id": 0x4c, },</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="E95" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A95,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B95, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C95, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D95, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>93: { "targetId": 0x4d, "command1Id": 0x4e, "command2Id": 0x39, },</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="E96" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A96,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B96, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C96, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D96, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>94: { "targetId": 0x4e, "command1Id": 0x30, "command2Id": 0x31, },</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="E97" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A97,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B97, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C97, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D97, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>95: { "targetId": 0x4e, "command1Id": 0x38, "command2Id": 0x16, },</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="E98" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A98,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B98, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C98, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D98, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>96: { "targetId": 0x4e, "command1Id": 0x38, "command2Id": 0x4d, },</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="E99" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A99,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B99, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C99, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D99, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>97: { "targetId": 0x4e, "command1Id": 0x39, "command2Id": 0x4d, },</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="E100" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A100,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B100, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C100, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D100, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>98: { "targetId": 0x4f, "command1Id": 0x17, "command2Id": 0x3c, },</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="E101" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A101,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B101, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C101, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D101, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>99: { "targetId": 0x4f, "command1Id": 0x2f, "command2Id": 0x2e, },</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="E102" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A102,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B102, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C102, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D102, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>100: { "targetId": 0x4f, "command1Id": 0x3c, "command2Id": 0x50, },</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="E103" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A103,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B103, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C103, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D103, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>101: { "targetId": 0x4f, "command1Id": 0x51, "command2Id": 0x3c, },</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="E104" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A104,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B104, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C104, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D104, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>102: { "targetId": 0x50, "command1Id": 0x30, "command2Id": 0x2e, },</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="E105" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A105,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B105, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C105, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D105, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>103: { "targetId": 0x50, "command1Id": 0x3c, "command2Id": 0x51, },</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="E106" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A106,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B106, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C106, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D106, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>104: { "targetId": 0x50, "command1Id": 0x53, "command2Id": 0x3c, },</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="E107" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A107,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B107, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C107, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D107, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>105: { "targetId": 0x50, "command1Id": 0x54, "command2Id": 0x3c, },</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="D108" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="E108" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A108,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B108, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C108, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D108, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>106: { "targetId": 0x51, "command1Id": 0x30, "command2Id": 0x2f, },</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="D109" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="E109" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A109,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B109, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C109, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D109, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>107: { "targetId": 0x51, "command1Id": 0x3b, "command2Id": 0x2f, },</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="D110" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="E110" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A110,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B110, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C110, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D110, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>108: { "targetId": 0x51, "command1Id": 0x3c, "command2Id": 0x30, },</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="D111" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="E111" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A111,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B111, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C111, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D111, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>109: { "targetId": 0x51, "command1Id": 0x4f, "command2Id": 0x50, },</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="D112" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="E112" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A112,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B112, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C112, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D112, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>110: { "targetId": 0x52, "command1Id": 0x3e, "command2Id": 0x53, },</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="D113" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="E113" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A113,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B113, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C113, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D113, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>111: { "targetId": 0x52, "command1Id": 0x3f, "command2Id": 0x14, },</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="E114" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A114,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B114, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C114, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D114, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>112: { "targetId": 0x52, "command1Id": 0x3f, "command2Id": 0x39, },</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="D115" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="E115" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A115,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B115, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C115, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D115, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>113: { "targetId": 0x52, "command1Id": 0x3f, "command2Id": 0x53, },</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="D116" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="E116" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A116,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B116, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C116, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D116, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>114: { "targetId": 0x53, "command1Id": 0x20, "command2Id": 0x3f, },</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="D117" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="E117" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A117,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B117, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C117, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D117, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>115: { "targetId": 0x53, "command1Id": 0x3e, "command2Id": 0x3f, },</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E118" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A118,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B118, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C118, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D118, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>116: { "targetId": 0x53, "command1Id": 0x3f, "command2Id": 0x42, },</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="E119" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A119,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B119, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C119, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D119, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>117: { "targetId": 0x53, "command1Id": 0x3f, "command2Id": 0x52, },</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="E120" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A120,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B120, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C120, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D120, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>118: { "targetId": 0x54, "command1Id": 0x39, "command2Id": 0x48, },</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="E121" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A121,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B121, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C121, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D121, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>119: { "targetId": 0x54, "command1Id": 0x41, "command2Id": 0x11, },</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="E122" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A122,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B122, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C122, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D122, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>120: { "targetId": 0x54, "command1Id": 0x41, "command2Id": 0x55, },</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="E123" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A123,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B123, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C123, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D123, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>121: { "targetId": 0x54, "command1Id": 0x42, "command2Id": 0x55, },</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="E124" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A124,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B124, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C124, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D124, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>122: { "targetId": 0x54, "command1Id": 0x45, "command2Id": 0x39, },</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="D125" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="E125" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A125,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B125, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C125, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D125, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>123: { "targetId": 0x55, "command1Id": 0x42, "command2Id": 0x39, },</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="D126" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E126" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A126,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B126, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C126, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D126, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>124: { "targetId": 0x55, "command1Id": 0x54, "command2Id": 0x42, },</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="D127" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="E127" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A127,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B127, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C127, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D127, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>125: { "targetId": 0x55, "command1Id": 0x57, "command2Id": 0x42, },</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="D128" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="E128" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A128,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B128, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C128, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D128, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>126: { "targetId": 0x56, "command1Id": 0x44, "command2Id": 0x45, },</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="D129" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="E129" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A129,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B129, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C129, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D129, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>127: { "targetId": 0x56, "command1Id": 0x45, "command2Id": 0x3c, },</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="D130" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="E130" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A130,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B130, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C130, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D130, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>128: { "targetId": 0x56, "command1Id": 0x4a, "command2Id": 0x45, },</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="D131" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="E131" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A131,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B131, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C131, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D131, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>129: { "targetId": 0x56, "command1Id": 0x55, "command2Id": 0x45, },</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="C132" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="D132" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="E132" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A132,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B132, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C132, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D132, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>130: { "targetId": 0x58, "command1Id": 0x4f, "command2Id": 0x3f, },</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="D133" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="E133" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A133,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B133, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C133, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D133, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>131: { "targetId": 0x59, "command1Id": 0x4f, "command2Id": 0x56, },</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="C134" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="D134" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="E134" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A134,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B134, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C134, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D134, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>132: { "targetId": 0x5a, "command1Id": 0x50, "command2Id": 0x3f, },</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="D135" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="E135" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A135,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B135, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C135, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D135, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>133: { "targetId": 0x5b, "command1Id": 0x55, "command2Id": 0x53, },</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="C136" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="D136" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="E136" s="0" t="str">
+        <f aca="true">_xlfn.CONCAT(A136,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B136, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C136, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D136, Commands!B:B, 0), 1, 1)),", },")</f>
+        <v>134: { "targetId": 0x5c, "command1Id": 0x32, "command2Id": 0x5b, },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added property to commands and added two new unfinished cheevos for Hollow Bastion, Part II.
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" state="visible" r:id="rId2"/>
@@ -1414,7 +1414,7 @@
     <t xml:space="preserve">Cure</t>
   </si>
   <si>
-    <t xml:space="preserve">Support</t>
+    <t xml:space="preserve">Curative</t>
   </si>
   <si>
     <t xml:space="preserve">0x47</t>
@@ -1565,7 +1565,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1599,11 +1599,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1648,7 +1643,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1662,10 +1657,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1693,10 +1684,10 @@
   <dimension ref="A1:D681"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
+      <selection pane="topLeft" activeCell="A677" activeCellId="1" sqref="D2:D95 A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -11256,10 +11247,10 @@
   <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B95" activeCellId="0" sqref="B95"/>
+      <selection pane="topLeft" activeCell="B95" activeCellId="1" sqref="D2:D95 B95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -13296,16 +13287,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C100" activeCellId="0" sqref="C100"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A84" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -13325,7 +13316,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>323</v>
       </c>
@@ -13336,11 +13327,11 @@
         <v>324</v>
       </c>
       <c r="D2" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""", },")</f>
-        <v>0xFF: { "id": 0xFF, "name": "N/A", },</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""", ""category"": """,C2,""" },")</f>
+        <v>0xFF: { "id": 0xFF, "name": "N/A", "category": "N/A" },</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>325</v>
       </c>
@@ -13351,11 +13342,11 @@
         <v>327</v>
       </c>
       <c r="D3" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""", },")</f>
-        <v>0x00: { "id": 0x00, "name": "Quick Blitz", },</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""", ""category"": """,C3,""" },")</f>
+        <v>0x00: { "id": 0x00, "name": "Quick Blitz", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>328</v>
       </c>
@@ -13366,11 +13357,11 @@
         <v>327</v>
       </c>
       <c r="D4" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""", },")</f>
-        <v>0x01: { "id": 0x01, "name": "Sliding Dash", },</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""", ""category"": """,C4,""" },")</f>
+        <v>0x01: { "id": 0x01, "name": "Sliding Dash", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>330</v>
       </c>
@@ -13381,8 +13372,8 @@
         <v>327</v>
       </c>
       <c r="D5" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""", },")</f>
-        <v>0x02: { "id": 0x02, "name": "Round Blitz", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""", ""category"": """,C5,""" },")</f>
+        <v>0x02: { "id": 0x02, "name": "Round Blitz", "category": "Melee" },</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13396,11 +13387,11 @@
         <v>334</v>
       </c>
       <c r="D6" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""", },")</f>
-        <v>0x03: { "id": 0x03, "name": "Strike Raid", },</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""", ""category"": """,C6,""" },")</f>
+        <v>0x03: { "id": 0x03, "name": "Strike Raid", "category": "Ranged" },</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>335</v>
       </c>
@@ -13411,11 +13402,11 @@
         <v>327</v>
       </c>
       <c r="D7" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""", },")</f>
-        <v>0x04: { "id": 0x04, "name": "Rising Strike", },</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""", ""category"": """,C7,""" },")</f>
+        <v>0x04: { "id": 0x04, "name": "Rising Strike", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>337</v>
       </c>
@@ -13426,11 +13417,11 @@
         <v>327</v>
       </c>
       <c r="D8" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""", },")</f>
-        <v>0x05: { "id": 0x05, "name": "Sliding Rush", },</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""", ""category"": """,C8,""" },")</f>
+        <v>0x05: { "id": 0x05, "name": "Sliding Rush", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>339</v>
       </c>
@@ -13441,11 +13432,11 @@
         <v>327</v>
       </c>
       <c r="D9" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""", },")</f>
-        <v>0x06: { "id": 0x06, "name": "Aerial Sweep", },</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""", ""category"": """,C9,""" },")</f>
+        <v>0x06: { "id": 0x06, "name": "Aerial Sweep", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>341</v>
       </c>
@@ -13456,11 +13447,11 @@
         <v>327</v>
       </c>
       <c r="D10" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""", },")</f>
-        <v>0x07: { "id": 0x07, "name": "Air Sweep", },</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""", ""category"": """,C10,""" },")</f>
+        <v>0x07: { "id": 0x07, "name": "Air Sweep", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>343</v>
       </c>
@@ -13471,11 +13462,11 @@
         <v>327</v>
       </c>
       <c r="D11" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""", },")</f>
-        <v>0x08: { "id": 0x08, "name": "Aerial Slam", },</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""", ""category"": """,C11,""" },")</f>
+        <v>0x08: { "id": 0x08, "name": "Aerial Slam", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>345</v>
       </c>
@@ -13486,11 +13477,11 @@
         <v>327</v>
       </c>
       <c r="D12" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""", },")</f>
-        <v>0x09: { "id": 0x09, "name": "Land Crash", },</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""", ""category"": """,C12,""" },")</f>
+        <v>0x09: { "id": 0x09, "name": "Land Crash", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>347</v>
       </c>
@@ -13501,11 +13492,11 @@
         <v>327</v>
       </c>
       <c r="D13" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A13,": { ""id"": ",A13,", ""name"": """,B13,""", },")</f>
-        <v>0x0a: { "id": 0x0a, "name": "Fire Edge", },</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A13,": { ""id"": ",A13,", ""name"": """,B13,""", ""category"": """,C13,""" },")</f>
+        <v>0x0a: { "id": 0x0a, "name": "Fire Edge", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>349</v>
       </c>
@@ -13516,11 +13507,11 @@
         <v>327</v>
       </c>
       <c r="D14" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A14,": { ""id"": ",A14,", ""name"": """,B14,""", },")</f>
-        <v>0x0b: { "id": 0x0b, "name": "Blizzard Edge", },</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A14,": { ""id"": ",A14,", ""name"": """,B14,""", ""category"": """,C14,""" },")</f>
+        <v>0x0b: { "id": 0x0b, "name": "Blizzard Edge", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>351</v>
       </c>
@@ -13531,11 +13522,11 @@
         <v>327</v>
       </c>
       <c r="D15" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A15,": { ""id"": ",A15,", ""name"": """,B15,""", },")</f>
-        <v>0x0c: { "id": 0x0c, "name": "Thunder Edge", },</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A15,": { ""id"": ",A15,", ""name"": """,B15,""", ""category"": """,C15,""" },")</f>
+        <v>0x0c: { "id": 0x0c, "name": "Thunder Edge", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>353</v>
       </c>
@@ -13546,11 +13537,11 @@
         <v>327</v>
       </c>
       <c r="D16" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A16,": { ""id"": ",A16,", ""name"": """,B16,""", },")</f>
-        <v>0x0d: { "id": 0x0d, "name": "Aero Edge", },</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A16,": { ""id"": ",A16,", ""name"": """,B16,""", ""category"": """,C16,""" },")</f>
+        <v>0x0d: { "id": 0x0d, "name": "Aero Edge", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>355</v>
       </c>
@@ -13561,11 +13552,11 @@
         <v>327</v>
       </c>
       <c r="D17" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A17,": { ""id"": ",A17,", ""name"": """,B17,""", },")</f>
-        <v>0x0e: { "id": 0x0e, "name": "Heat Dash", },</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A17,": { ""id"": ",A17,", ""name"": """,B17,""", ""category"": """,C17,""" },")</f>
+        <v>0x0e: { "id": 0x0e, "name": "Heat Dash", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>357</v>
       </c>
@@ -13576,11 +13567,11 @@
         <v>327</v>
       </c>
       <c r="D18" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A18,": { ""id"": ",A18,", ""name"": """,B18,""", },")</f>
-        <v>0x0f: { "id": 0x0f, "name": "Ice Dash", },</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A18,": { ""id"": ",A18,", ""name"": """,B18,""", ""category"": """,C18,""" },")</f>
+        <v>0x0f: { "id": 0x0f, "name": "Ice Dash", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>301</v>
       </c>
@@ -13591,11 +13582,11 @@
         <v>327</v>
       </c>
       <c r="D19" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A19,": { ""id"": ",A19,", ""name"": """,B19,""", },")</f>
-        <v>0x10: { "id": 0x10, "name": "Spark Dash", },</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A19,": { ""id"": ",A19,", ""name"": """,B19,""", ""category"": """,C19,""" },")</f>
+        <v>0x10: { "id": 0x10, "name": "Spark Dash", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>267</v>
       </c>
@@ -13606,11 +13597,11 @@
         <v>327</v>
       </c>
       <c r="D20" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A20,": { ""id"": ",A20,", ""name"": """,B20,""", },")</f>
-        <v>0x11: { "id": 0x11, "name": "Wind Dash", },</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A20,": { ""id"": ",A20,", ""name"": """,B20,""", ""category"": """,C20,""" },")</f>
+        <v>0x11: { "id": 0x11, "name": "Wind Dash", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>256</v>
       </c>
@@ -13621,11 +13612,11 @@
         <v>327</v>
       </c>
       <c r="D21" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A21,": { ""id"": ",A21,", ""name"": """,B21,""", },")</f>
-        <v>0x12: { "id": 0x12, "name": "Fire Blast", },</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A21,": { ""id"": ",A21,", ""name"": """,B21,""", ""category"": """,C21,""" },")</f>
+        <v>0x12: { "id": 0x12, "name": "Fire Blast", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>362</v>
       </c>
@@ -13636,11 +13627,11 @@
         <v>327</v>
       </c>
       <c r="D22" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A22,": { ""id"": ",A22,", ""name"": """,B22,""", },")</f>
-        <v>0x13: { "id": 0x13, "name": "Blizzard Blast", },</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A22,": { ""id"": ",A22,", ""name"": """,B22,""", ""category"": """,C22,""" },")</f>
+        <v>0x13: { "id": 0x13, "name": "Blizzard Blast", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>364</v>
       </c>
@@ -13651,11 +13642,11 @@
         <v>327</v>
       </c>
       <c r="D23" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A23,": { ""id"": ",A23,", ""name"": """,B23,""", },")</f>
-        <v>0x14: { "id": 0x14, "name": "Thunder Blast", },</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A23,": { ""id"": ",A23,", ""name"": """,B23,""", ""category"": """,C23,""" },")</f>
+        <v>0x14: { "id": 0x14, "name": "Thunder Blast", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>366</v>
       </c>
@@ -13666,8 +13657,8 @@
         <v>327</v>
       </c>
       <c r="D24" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A24,": { ""id"": ",A24,", ""name"": """,B24,""", },")</f>
-        <v>0x15: { "id": 0x15, "name": "Aero Blast", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A24,": { ""id"": ",A24,", ""name"": """,B24,""", ""category"": """,C24,""" },")</f>
+        <v>0x15: { "id": 0x15, "name": "Aero Blast", "category": "Melee" },</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13681,8 +13672,8 @@
         <v>334</v>
       </c>
       <c r="D25" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A25,": { ""id"": ",A25,", ""name"": """,B25,""", },")</f>
-        <v>0x16: { "id": 0x16, "name": "Fire Raid", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A25,": { ""id"": ",A25,", ""name"": """,B25,""", ""category"": """,C25,""" },")</f>
+        <v>0x16: { "id": 0x16, "name": "Fire Raid", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13696,8 +13687,8 @@
         <v>334</v>
       </c>
       <c r="D26" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A26,": { ""id"": ",A26,", ""name"": """,B26,""", },")</f>
-        <v>0x17: { "id": 0x17, "name": "Blizzard Raid", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A26,": { ""id"": ",A26,", ""name"": """,B26,""", ""category"": """,C26,""" },")</f>
+        <v>0x17: { "id": 0x17, "name": "Blizzard Raid", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13711,8 +13702,8 @@
         <v>334</v>
       </c>
       <c r="D27" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A27,": { ""id"": ",A27,", ""name"": """,B27,""", },")</f>
-        <v>0x18: { "id": 0x18, "name": "Thunder Raid", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A27,": { ""id"": ",A27,", ""name"": """,B27,""", ""category"": """,C27,""" },")</f>
+        <v>0x18: { "id": 0x18, "name": "Thunder Raid", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13726,11 +13717,11 @@
         <v>334</v>
       </c>
       <c r="D28" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A28,": { ""id"": ",A28,", ""name"": """,B28,""", },")</f>
-        <v>0x19: { "id": 0x19, "name": "Aero Raid", },</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A28,": { ""id"": ",A28,", ""name"": """,B28,""", ""category"": """,C28,""" },")</f>
+        <v>0x19: { "id": 0x19, "name": "Aero Raid", "category": "Ranged" },</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>376</v>
       </c>
@@ -13741,11 +13732,11 @@
         <v>327</v>
       </c>
       <c r="D29" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A29,": { ""id"": ",A29,", ""name"": """,B29,""", },")</f>
-        <v>0x1a: { "id": 0x1a, "name": "Fire Buster", },</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A29,": { ""id"": ",A29,", ""name"": """,B29,""", ""category"": """,C29,""" },")</f>
+        <v>0x1a: { "id": 0x1a, "name": "Fire Buster", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>378</v>
       </c>
@@ -13756,11 +13747,11 @@
         <v>327</v>
       </c>
       <c r="D30" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A30,": { ""id"": ",A30,", ""name"": """,B30,""", },")</f>
-        <v>0x1b: { "id": 0x1b, "name": "Blizzard Buster", },</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A30,": { ""id"": ",A30,", ""name"": """,B30,""", ""category"": """,C30,""" },")</f>
+        <v>0x1b: { "id": 0x1b, "name": "Blizzard Buster", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>380</v>
       </c>
@@ -13771,11 +13762,11 @@
         <v>327</v>
       </c>
       <c r="D31" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A31,": { ""id"": ",A31,", ""name"": """,B31,""", },")</f>
-        <v>0x1c: { "id": 0x1c, "name": "Thunder Buster", },</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A31,": { ""id"": ",A31,", ""name"": """,B31,""", ""category"": """,C31,""" },")</f>
+        <v>0x1c: { "id": 0x1c, "name": "Thunder Buster", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>203</v>
       </c>
@@ -13786,11 +13777,11 @@
         <v>327</v>
       </c>
       <c r="D32" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A32,": { ""id"": ",A32,", ""name"": """,B32,""", },")</f>
-        <v>0x1d: { "id": 0x1d, "name": "Aero Buster", },</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A32,": { ""id"": ",A32,", ""name"": """,B32,""", ""category"": """,C32,""" },")</f>
+        <v>0x1d: { "id": 0x1d, "name": "Aero Buster", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>206</v>
       </c>
@@ -13801,11 +13792,11 @@
         <v>327</v>
       </c>
       <c r="D33" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A33,": { ""id"": ",A33,", ""name"": """,B33,""", },")</f>
-        <v>0x1e: { "id": 0x1e, "name": "Heat Sweep", },</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A33,": { ""id"": ",A33,", ""name"": """,B33,""", ""category"": """,C33,""" },")</f>
+        <v>0x1e: { "id": 0x1e, "name": "Heat Sweep", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>211</v>
       </c>
@@ -13816,11 +13807,11 @@
         <v>327</v>
       </c>
       <c r="D34" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A34,": { ""id"": ",A34,", ""name"": """,B34,""", },")</f>
-        <v>0x1f: { "id": 0x1f, "name": "Ice Sweep", },</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A34,": { ""id"": ",A34,", ""name"": """,B34,""", ""category"": """,C34,""" },")</f>
+        <v>0x1f: { "id": 0x1f, "name": "Ice Sweep", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>385</v>
       </c>
@@ -13831,11 +13822,11 @@
         <v>327</v>
       </c>
       <c r="D35" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A35,": { ""id"": ",A35,", ""name"": """,B35,""", },")</f>
-        <v>0x20: { "id": 0x20, "name": "Spark Sweep", },</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A35,": { ""id"": ",A35,", ""name"": """,B35,""", ""category"": """,C35,""" },")</f>
+        <v>0x20: { "id": 0x20, "name": "Spark Sweep", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>241</v>
       </c>
@@ -13846,11 +13837,11 @@
         <v>327</v>
       </c>
       <c r="D36" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A36,": { ""id"": ",A36,", ""name"": """,B36,""", },")</f>
-        <v>0x21: { "id": 0x21, "name": "Wind Sweep", },</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A36,": { ""id"": ",A36,", ""name"": """,B36,""", ""category"": """,C36,""" },")</f>
+        <v>0x21: { "id": 0x21, "name": "Wind Sweep", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>388</v>
       </c>
@@ -13861,11 +13852,11 @@
         <v>327</v>
       </c>
       <c r="D37" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A37,": { ""id"": ",A37,", ""name"": """,B37,""", },")</f>
-        <v>0x22: { "id": 0x22, "name": "Heat Storm", },</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A37,": { ""id"": ",A37,", ""name"": """,B37,""", ""category"": """,C37,""" },")</f>
+        <v>0x22: { "id": 0x22, "name": "Heat Storm", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>390</v>
       </c>
@@ -13876,11 +13867,11 @@
         <v>327</v>
       </c>
       <c r="D38" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A38,": { ""id"": ",A38,", ""name"": """,B38,""", },")</f>
-        <v>0x23: { "id": 0x23, "name": "Ice Storm", },</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A38,": { ""id"": ",A38,", ""name"": """,B38,""", ""category"": """,C38,""" },")</f>
+        <v>0x23: { "id": 0x23, "name": "Ice Storm", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>392</v>
       </c>
@@ -13891,11 +13882,11 @@
         <v>327</v>
       </c>
       <c r="D39" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A39,": { ""id"": ",A39,", ""name"": """,B39,""", },")</f>
-        <v>0x24: { "id": 0x24, "name": "Spark Storm", },</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A39,": { ""id"": ",A39,", ""name"": """,B39,""", ""category"": """,C39,""" },")</f>
+        <v>0x24: { "id": 0x24, "name": "Spark Storm", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>394</v>
       </c>
@@ -13906,11 +13897,11 @@
         <v>327</v>
       </c>
       <c r="D40" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A40,": { ""id"": ",A40,", ""name"": """,B40,""", },")</f>
-        <v>0x25: { "id": 0x25, "name": "Wind Storm", },</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A40,": { ""id"": ",A40,", ""name"": """,B40,""", ""category"": """,C40,""" },")</f>
+        <v>0x25: { "id": 0x25, "name": "Wind Storm", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>396</v>
       </c>
@@ -13921,11 +13912,11 @@
         <v>327</v>
       </c>
       <c r="D41" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A41,": { ""id"": ",A41,", ""name"": """,B41,""", },")</f>
-        <v>0x26: { "id": 0x26, "name": "Fire Slam", },</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A41,": { ""id"": ",A41,", ""name"": """,B41,""", ""category"": """,C41,""" },")</f>
+        <v>0x26: { "id": 0x26, "name": "Fire Slam", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>398</v>
       </c>
@@ -13936,11 +13927,11 @@
         <v>327</v>
       </c>
       <c r="D42" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A42,": { ""id"": ",A42,", ""name"": """,B42,""", },")</f>
-        <v>0x27: { "id": 0x27, "name": "Blizzard Slam", },</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A42,": { ""id"": ",A42,", ""name"": """,B42,""", ""category"": """,C42,""" },")</f>
+        <v>0x27: { "id": 0x27, "name": "Blizzard Slam", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>400</v>
       </c>
@@ -13951,11 +13942,11 @@
         <v>327</v>
       </c>
       <c r="D43" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A43,": { ""id"": ",A43,", ""name"": """,B43,""", },")</f>
-        <v>0x28: { "id": 0x28, "name": "Thunder Slam", },</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A43,": { ""id"": ",A43,", ""name"": """,B43,""", ""category"": """,C43,""" },")</f>
+        <v>0x28: { "id": 0x28, "name": "Thunder Slam", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>402</v>
       </c>
@@ -13966,11 +13957,11 @@
         <v>327</v>
       </c>
       <c r="D44" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A44,": { ""id"": ",A44,", ""name"": """,B44,""", },")</f>
-        <v>0x29: { "id": 0x29, "name": "Aero Slam", },</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A44,": { ""id"": ",A44,", ""name"": """,B44,""", ""category"": """,C44,""" },")</f>
+        <v>0x29: { "id": 0x29, "name": "Aero Slam", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>404</v>
       </c>
@@ -13981,11 +13972,11 @@
         <v>327</v>
       </c>
       <c r="D45" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A45,": { ""id"": ",A45,", ""name"": """,B45,""", },")</f>
-        <v>0x2a: { "id": 0x2a, "name": "Heat Dive", },</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A45,": { ""id"": ",A45,", ""name"": """,B45,""", ""category"": """,C45,""" },")</f>
+        <v>0x2a: { "id": 0x2a, "name": "Heat Dive", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>406</v>
       </c>
@@ -13996,11 +13987,11 @@
         <v>327</v>
       </c>
       <c r="D46" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A46,": { ""id"": ",A46,", ""name"": """,B46,""", },")</f>
-        <v>0x2b: { "id": 0x2b, "name": "Ice Dive", },</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A46,": { ""id"": ",A46,", ""name"": """,B46,""", ""category"": """,C46,""" },")</f>
+        <v>0x2b: { "id": 0x2b, "name": "Ice Dive", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>408</v>
       </c>
@@ -14011,11 +14002,11 @@
         <v>327</v>
       </c>
       <c r="D47" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A47,": { ""id"": ",A47,", ""name"": """,B47,""", },")</f>
-        <v>0x2c: { "id": 0x2c, "name": "Spark Dive", },</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A47,": { ""id"": ",A47,", ""name"": """,B47,""", ""category"": """,C47,""" },")</f>
+        <v>0x2c: { "id": 0x2c, "name": "Spark Dive", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>410</v>
       </c>
@@ -14026,11 +14017,11 @@
         <v>327</v>
       </c>
       <c r="D48" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A48,": { ""id"": ",A48,", ""name"": """,B48,""", },")</f>
-        <v>0x2d: { "id": 0x2d, "name": "Wind Dive", },</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A48,": { ""id"": ",A48,", ""name"": """,B48,""", ""category"": """,C48,""" },")</f>
+        <v>0x2d: { "id": 0x2d, "name": "Wind Dive", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>412</v>
       </c>
@@ -14041,11 +14032,11 @@
         <v>327</v>
       </c>
       <c r="D49" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A49,": { ""id"": ",A49,", ""name"": """,B49,""", },")</f>
-        <v>0x2e: { "id": 0x2e, "name": "Stun Impact", },</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A49,": { ""id"": ",A49,", ""name"": """,B49,""", ""category"": """,C49,""" },")</f>
+        <v>0x2e: { "id": 0x2e, "name": "Stun Impact", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>414</v>
       </c>
@@ -14056,11 +14047,11 @@
         <v>327</v>
       </c>
       <c r="D50" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A50,": { ""id"": ",A50,", ""name"": """,B50,""", },")</f>
-        <v>0x2f: { "id": 0x2f, "name": "Muscle Strike", },</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A50,": { ""id"": ",A50,", ""name"": """,B50,""", ""category"": """,C50,""" },")</f>
+        <v>0x2f: { "id": 0x2f, "name": "Muscle Strike", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>416</v>
       </c>
@@ -14071,11 +14062,11 @@
         <v>327</v>
       </c>
       <c r="D51" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A51,": { ""id"": ",A51,", ""name"": """,B51,""", },")</f>
-        <v>0x30: { "id": 0x30, "name": "Chain Rave", },</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A51,": { ""id"": ",A51,", ""name"": """,B51,""", ""category"": """,C51,""" },")</f>
+        <v>0x30: { "id": 0x30, "name": "Chain Rave", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>418</v>
       </c>
@@ -14086,11 +14077,11 @@
         <v>327</v>
       </c>
       <c r="D52" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A52,": { ""id"": ",A52,", ""name"": """,B52,""", },")</f>
-        <v>0x31: { "id": 0x31, "name": "Rising Rush", },</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A52,": { ""id"": ",A52,", ""name"": """,B52,""", ""category"": """,C52,""" },")</f>
+        <v>0x31: { "id": 0x31, "name": "Rising Rush", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>420</v>
       </c>
@@ -14101,11 +14092,11 @@
         <v>327</v>
       </c>
       <c r="D53" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A53,": { ""id"": ",A53,", ""name"": """,B53,""", },")</f>
-        <v>0x32: { "id": 0x32, "name": "Zantetsuken", },</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A53,": { ""id"": ",A53,", ""name"": """,B53,""", ""category"": """,C53,""" },")</f>
+        <v>0x32: { "id": 0x32, "name": "Zantetsuken", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>422</v>
       </c>
@@ -14116,11 +14107,11 @@
         <v>327</v>
       </c>
       <c r="D54" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A54,": { ""id"": ",A54,", ""name"": """,B54,""", },")</f>
-        <v>0x33: { "id": 0x33, "name": "Eruption", },</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A54,": { ""id"": ",A54,", ""name"": """,B54,""", ""category"": """,C54,""" },")</f>
+        <v>0x33: { "id": 0x33, "name": "Eruption", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>424</v>
       </c>
@@ -14131,11 +14122,11 @@
         <v>327</v>
       </c>
       <c r="D55" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A55,": { ""id"": ",A55,", ""name"": """,B55,""", },")</f>
-        <v>0x34: { "id": 0x34, "name": "Gravity Drop", },</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A55,": { ""id"": ",A55,", ""name"": """,B55,""", ""category"": """,C55,""" },")</f>
+        <v>0x34: { "id": 0x34, "name": "Gravity Drop", "category": "Melee" },</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>426</v>
       </c>
@@ -14146,8 +14137,8 @@
         <v>327</v>
       </c>
       <c r="D56" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A56,": { ""id"": ",A56,", ""name"": """,B56,""", },")</f>
-        <v>0x35: { "id": 0x35, "name": "Shock Fall", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A56,": { ""id"": ",A56,", ""name"": """,B56,""", ""category"": """,C56,""" },")</f>
+        <v>0x35: { "id": 0x35, "name": "Shock Fall", "category": "Melee" },</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14161,8 +14152,8 @@
         <v>334</v>
       </c>
       <c r="D57" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A57,": { ""id"": ",A57,", ""name"": """,B57,""", },")</f>
-        <v>0x36: { "id": 0x36, "name": "Judgment Triad", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A57,": { ""id"": ",A57,", ""name"": """,B57,""", ""category"": """,C57,""" },")</f>
+        <v>0x36: { "id": 0x36, "name": "Judgment Triad", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14176,8 +14167,8 @@
         <v>334</v>
       </c>
       <c r="D58" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A58,": { ""id"": ",A58,", ""name"": """,B58,""", },")</f>
-        <v>0x37: { "id": 0x37, "name": "Fire", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A58,": { ""id"": ",A58,", ""name"": """,B58,""", ""category"": """,C58,""" },")</f>
+        <v>0x37: { "id": 0x37, "name": "Fire", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14191,8 +14182,8 @@
         <v>334</v>
       </c>
       <c r="D59" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A59,": { ""id"": ",A59,", ""name"": """,B59,""", },")</f>
-        <v>0x38: { "id": 0x38, "name": "Fira", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A59,": { ""id"": ",A59,", ""name"": """,B59,""", ""category"": """,C59,""" },")</f>
+        <v>0x38: { "id": 0x38, "name": "Fira", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14206,8 +14197,8 @@
         <v>334</v>
       </c>
       <c r="D60" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A60,": { ""id"": ",A60,", ""name"": """,B60,""", },")</f>
-        <v>0x39: { "id": 0x39, "name": "Firaga", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A60,": { ""id"": ",A60,", ""name"": """,B60,""", ""category"": """,C60,""" },")</f>
+        <v>0x39: { "id": 0x39, "name": "Firaga", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14221,8 +14212,8 @@
         <v>334</v>
       </c>
       <c r="D61" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A61,": { ""id"": ",A61,", ""name"": """,B61,""", },")</f>
-        <v>0x3a: { "id": 0x3a, "name": "Blizzard", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A61,": { ""id"": ",A61,", ""name"": """,B61,""", ""category"": """,C61,""" },")</f>
+        <v>0x3a: { "id": 0x3a, "name": "Blizzard", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14236,8 +14227,8 @@
         <v>334</v>
       </c>
       <c r="D62" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A62,": { ""id"": ",A62,", ""name"": """,B62,""", },")</f>
-        <v>0x3b: { "id": 0x3b, "name": "Blizzara", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A62,": { ""id"": ",A62,", ""name"": """,B62,""", ""category"": """,C62,""" },")</f>
+        <v>0x3b: { "id": 0x3b, "name": "Blizzara", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14251,8 +14242,8 @@
         <v>334</v>
       </c>
       <c r="D63" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A63,": { ""id"": ",A63,", ""name"": """,B63,""", },")</f>
-        <v>0x3c: { "id": 0x3c, "name": "Blizzaga", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A63,": { ""id"": ",A63,", ""name"": """,B63,""", ""category"": """,C63,""" },")</f>
+        <v>0x3c: { "id": 0x3c, "name": "Blizzaga", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14266,8 +14257,8 @@
         <v>334</v>
       </c>
       <c r="D64" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A64,": { ""id"": ",A64,", ""name"": """,B64,""", },")</f>
-        <v>0x3d: { "id": 0x3d, "name": "Thunder", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A64,": { ""id"": ",A64,", ""name"": """,B64,""", ""category"": """,C64,""" },")</f>
+        <v>0x3d: { "id": 0x3d, "name": "Thunder", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14281,8 +14272,8 @@
         <v>334</v>
       </c>
       <c r="D65" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A65,": { ""id"": ",A65,", ""name"": """,B65,""", },")</f>
-        <v>0x3e: { "id": 0x3e, "name": "Thundara", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A65,": { ""id"": ",A65,", ""name"": """,B65,""", ""category"": """,C65,""" },")</f>
+        <v>0x3e: { "id": 0x3e, "name": "Thundara", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14296,8 +14287,8 @@
         <v>334</v>
       </c>
       <c r="D66" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A66,": { ""id"": ",A66,", ""name"": """,B66,""", },")</f>
-        <v>0x3f: { "id": 0x3f, "name": "Thundaga", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A66,": { ""id"": ",A66,", ""name"": """,B66,""", ""category"": """,C66,""" },")</f>
+        <v>0x3f: { "id": 0x3f, "name": "Thundaga", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14311,8 +14302,8 @@
         <v>334</v>
       </c>
       <c r="D67" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A67,": { ""id"": ",A67,", ""name"": """,B67,""", },")</f>
-        <v>0x40: { "id": 0x40, "name": "Aero", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A67,": { ""id"": ",A67,", ""name"": """,B67,""", ""category"": """,C67,""" },")</f>
+        <v>0x40: { "id": 0x40, "name": "Aero", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14326,8 +14317,8 @@
         <v>334</v>
       </c>
       <c r="D68" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A68,": { ""id"": ",A68,", ""name"": """,B68,""", },")</f>
-        <v>0x41: { "id": 0x41, "name": "Aerora", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A68,": { ""id"": ",A68,", ""name"": """,B68,""", ""category"": """,C68,""" },")</f>
+        <v>0x41: { "id": 0x41, "name": "Aerora", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14341,8 +14332,8 @@
         <v>334</v>
       </c>
       <c r="D69" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A69,": { ""id"": ",A69,", ""name"": """,B69,""", },")</f>
-        <v>0x42: { "id": 0x42, "name": "Aeroga", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A69,": { ""id"": ",A69,", ""name"": """,B69,""", ""category"": """,C69,""" },")</f>
+        <v>0x42: { "id": 0x42, "name": "Aeroga", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14356,8 +14347,8 @@
         <v>334</v>
       </c>
       <c r="D70" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A70,": { ""id"": ",A70,", ""name"": """,B70,""", },")</f>
-        <v>0x43: { "id": 0x43, "name": "Magnet", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A70,": { ""id"": ",A70,", ""name"": """,B70,""", ""category"": """,C70,""" },")</f>
+        <v>0x43: { "id": 0x43, "name": "Magnet", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14371,8 +14362,8 @@
         <v>334</v>
       </c>
       <c r="D71" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A71,": { ""id"": ",A71,", ""name"": """,B71,""", },")</f>
-        <v>0x44: { "id": 0x44, "name": "Magnera", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A71,": { ""id"": ",A71,", ""name"": """,B71,""", ""category"": """,C71,""" },")</f>
+        <v>0x44: { "id": 0x44, "name": "Magnera", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14386,11 +14377,11 @@
         <v>334</v>
       </c>
       <c r="D72" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A72,": { ""id"": ",A72,", ""name"": """,B72,""", },")</f>
-        <v>0x45: { "id": 0x45, "name": "Magnega", },</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A72,": { ""id"": ",A72,", ""name"": """,B72,""", ""category"": """,C72,""" },")</f>
+        <v>0x45: { "id": 0x45, "name": "Magnega", "category": "Ranged" },</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>460</v>
       </c>
@@ -14401,11 +14392,11 @@
         <v>462</v>
       </c>
       <c r="D73" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A73,": { ""id"": ",A73,", ""name"": """,B73,""", },")</f>
-        <v>0x46: { "id": 0x46, "name": "Cure", },</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A73,": { ""id"": ",A73,", ""name"": """,B73,""", ""category"": """,C73,""" },")</f>
+        <v>0x46: { "id": 0x46, "name": "Cure", "category": "Curative" },</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>463</v>
       </c>
@@ -14416,11 +14407,11 @@
         <v>462</v>
       </c>
       <c r="D74" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A74,": { ""id"": ",A74,", ""name"": """,B74,""", },")</f>
-        <v>0x47: { "id": 0x47, "name": "Cura", },</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A74,": { ""id"": ",A74,", ""name"": """,B74,""", ""category"": """,C74,""" },")</f>
+        <v>0x47: { "id": 0x47, "name": "Cura", "category": "Curative" },</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>465</v>
       </c>
@@ -14431,8 +14422,8 @@
         <v>462</v>
       </c>
       <c r="D75" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A75,": { ""id"": ",A75,", ""name"": """,B75,""", },")</f>
-        <v>0x48: { "id": 0x48, "name": "Curaga", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A75,": { ""id"": ",A75,", ""name"": """,B75,""", ""category"": """,C75,""" },")</f>
+        <v>0x48: { "id": 0x48, "name": "Curaga", "category": "Curative" },</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14446,8 +14437,8 @@
         <v>334</v>
       </c>
       <c r="D76" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A76,": { ""id"": ",A76,", ""name"": """,B76,""", },")</f>
-        <v>0x49: { "id": 0x49, "name": "Slow", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A76,": { ""id"": ",A76,", ""name"": """,B76,""", ""category"": """,C76,""" },")</f>
+        <v>0x49: { "id": 0x49, "name": "Slow", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14461,8 +14452,8 @@
         <v>334</v>
       </c>
       <c r="D77" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A77,": { ""id"": ",A77,", ""name"": """,B77,""", },")</f>
-        <v>0x4a: { "id": 0x4a, "name": "Stop", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A77,": { ""id"": ",A77,", ""name"": """,B77,""", ""category"": """,C77,""" },")</f>
+        <v>0x4a: { "id": 0x4a, "name": "Stop", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14476,8 +14467,8 @@
         <v>334</v>
       </c>
       <c r="D78" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A78,": { ""id"": ",A78,", ""name"": """,B78,""", },")</f>
-        <v>0x4b: { "id": 0x4b, "name": "Confuse", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A78,": { ""id"": ",A78,", ""name"": """,B78,""", ""category"": """,C78,""" },")</f>
+        <v>0x4b: { "id": 0x4b, "name": "Confuse", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14491,8 +14482,8 @@
         <v>334</v>
       </c>
       <c r="D79" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A79,": { ""id"": ",A79,", ""name"": """,B79,""", },")</f>
-        <v>0x4c: { "id": 0x4c, "name": "Firaga Burst", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A79,": { ""id"": ",A79,", ""name"": """,B79,""", ""category"": """,C79,""" },")</f>
+        <v>0x4c: { "id": 0x4c, "name": "Firaga Burst", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14506,8 +14497,8 @@
         <v>334</v>
       </c>
       <c r="D80" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A80,": { ""id"": ",A80,", ""name"": """,B80,""", },")</f>
-        <v>0x4d: { "id": 0x4d, "name": "Triple Firaga", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A80,": { ""id"": ",A80,", ""name"": """,B80,""", ""category"": """,C80,""" },")</f>
+        <v>0x4d: { "id": 0x4d, "name": "Triple Firaga", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14521,8 +14512,8 @@
         <v>334</v>
       </c>
       <c r="D81" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A81,": { ""id"": ",A81,", ""name"": """,B81,""", },")</f>
-        <v>0x4e: { "id": 0x4e, "name": "Triple Burst", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A81,": { ""id"": ",A81,", ""name"": """,B81,""", ""category"": """,C81,""" },")</f>
+        <v>0x4e: { "id": 0x4e, "name": "Triple Burst", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14536,8 +14527,8 @@
         <v>334</v>
       </c>
       <c r="D82" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A82,": { ""id"": ",A82,", ""name"": """,B82,""", },")</f>
-        <v>0x4f: { "id": 0x4f, "name": "Blizzaga Pursuit", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A82,": { ""id"": ",A82,", ""name"": """,B82,""", ""category"": """,C82,""" },")</f>
+        <v>0x4f: { "id": 0x4f, "name": "Blizzaga Pursuit", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14551,8 +14542,8 @@
         <v>334</v>
       </c>
       <c r="D83" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A83,": { ""id"": ",A83,", ""name"": """,B83,""", },")</f>
-        <v>0x50: { "id": 0x50, "name": "Triple Blizzaga", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A83,": { ""id"": ",A83,", ""name"": """,B83,""", ""category"": """,C83,""" },")</f>
+        <v>0x50: { "id": 0x50, "name": "Triple Blizzaga", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14566,8 +14557,8 @@
         <v>334</v>
       </c>
       <c r="D84" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A84,": { ""id"": ",A84,", ""name"": """,B84,""", },")</f>
-        <v>0x51: { "id": 0x51, "name": "Triple Pursuit", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A84,": { ""id"": ",A84,", ""name"": """,B84,""", ""category"": """,C84,""" },")</f>
+        <v>0x51: { "id": 0x51, "name": "Triple Pursuit", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14581,8 +14572,8 @@
         <v>334</v>
       </c>
       <c r="D85" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A85,": { ""id"": ",A85,", ""name"": """,B85,""", },")</f>
-        <v>0x52: { "id": 0x52, "name": "Thunder Tracer", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A85,": { ""id"": ",A85,", ""name"": """,B85,""", ""category"": """,C85,""" },")</f>
+        <v>0x52: { "id": 0x52, "name": "Thunder Tracer", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14596,8 +14587,8 @@
         <v>334</v>
       </c>
       <c r="D86" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A86,": { ""id"": ",A86,", ""name"": """,B86,""", },")</f>
-        <v>0x53: { "id": 0x53, "name": "Pulse Tracer", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A86,": { ""id"": ",A86,", ""name"": """,B86,""", ""category"": """,C86,""" },")</f>
+        <v>0x53: { "id": 0x53, "name": "Pulse Tracer", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14611,8 +14602,8 @@
         <v>334</v>
       </c>
       <c r="D87" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A87,": { ""id"": ",A87,", ""name"": """,B87,""", },")</f>
-        <v>0x54: { "id": 0x54, "name": "Tornado Tracer", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A87,": { ""id"": ",A87,", ""name"": """,B87,""", ""category"": """,C87,""" },")</f>
+        <v>0x54: { "id": 0x54, "name": "Tornado Tracer", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14626,8 +14617,8 @@
         <v>334</v>
       </c>
       <c r="D88" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A88,": { ""id"": ",A88,", ""name"": """,B88,""", },")</f>
-        <v>0x55: { "id": 0x55, "name": "Wind Tracer", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A88,": { ""id"": ",A88,", ""name"": """,B88,""", ""category"": """,C88,""" },")</f>
+        <v>0x55: { "id": 0x55, "name": "Wind Tracer", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14641,11 +14632,11 @@
         <v>334</v>
       </c>
       <c r="D89" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A89,": { ""id"": ",A89,", ""name"": """,B89,""", },")</f>
-        <v>0x56: { "id": 0x56, "name": "Magnet Grab", },</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A89,": { ""id"": ",A89,", ""name"": """,B89,""", ""category"": """,C89,""" },")</f>
+        <v>0x56: { "id": 0x56, "name": "Magnet Grab", "category": "Ranged" },</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>495</v>
       </c>
@@ -14656,8 +14647,8 @@
         <v>462</v>
       </c>
       <c r="D90" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A90,": { ""id"": ",A90,", ""name"": """,B90,""", },")</f>
-        <v>0x57: { "id": 0x57, "name": "Esuna", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A90,": { ""id"": ",A90,", ""name"": """,B90,""", ""category"": """,C90,""" },")</f>
+        <v>0x57: { "id": 0x57, "name": "Esuna", "category": "Curative" },</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14671,8 +14662,8 @@
         <v>334</v>
       </c>
       <c r="D91" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A91,": { ""id"": ",A91,", ""name"": """,B91,""", },")</f>
-        <v>0x58: { "id": 0x58, "name": "Flame Fall", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A91,": { ""id"": ",A91,", ""name"": """,B91,""", ""category"": """,C91,""" },")</f>
+        <v>0x58: { "id": 0x58, "name": "Flame Fall", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14686,8 +14677,8 @@
         <v>334</v>
       </c>
       <c r="D92" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A92,": { ""id"": ",A92,", ""name"": """,B92,""", },")</f>
-        <v>0x59: { "id": 0x59, "name": "Icicle Mine", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A92,": { ""id"": ",A92,", ""name"": """,B92,""", ""category"": """,C92,""" },")</f>
+        <v>0x59: { "id": 0x59, "name": "Icicle Mine", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14701,8 +14692,8 @@
         <v>334</v>
       </c>
       <c r="D93" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A93,": { ""id"": ",A93,", ""name"": """,B93,""", },")</f>
-        <v>0x5a: { "id": 0x5a, "name": "Exo Spark", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A93,": { ""id"": ",A93,", ""name"": """,B93,""", ""category"": """,C93,""" },")</f>
+        <v>0x5a: { "id": 0x5a, "name": "Exo Spark", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14716,8 +14707,8 @@
         <v>334</v>
       </c>
       <c r="D94" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A94,": { ""id"": ",A94,", ""name"": """,B94,""", },")</f>
-        <v>0x5b: { "id": 0x5b, "name": "Cyclone", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A94,": { ""id"": ",A94,", ""name"": """,B94,""", ""category"": """,C94,""" },")</f>
+        <v>0x5b: { "id": 0x5b, "name": "Cyclone", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14731,18 +14722,12 @@
         <v>334</v>
       </c>
       <c r="D95" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A95,": { ""id"": ",A95,", ""name"": """,B95,""", },")</f>
-        <v>0x5c: { "id": 0x5c, "name": "Quake", },</v>
+        <f aca="false">_xlfn.CONCAT( ,A95,": { ""id"": ",A95,", ""name"": """,B95,""", ""category"": """,C95,""" },")</f>
+        <v>0x5c: { "id": 0x5c, "name": "Quake", "category": "Ranged" },</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C95">
-    <filterColumn colId="0">
-      <customFilters and="true">
-        <customFilter operator="equal" val="Ranged"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="C1:C95"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -14761,15 +14746,15 @@
   </sheetPr>
   <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C137" activeCellId="0" sqref="C137"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="D2:D95 E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16689,7 +16674,7 @@
       <c r="C107" s="0" t="s">
         <v>490</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="D107" s="2" t="s">
         <v>441</v>
       </c>
       <c r="E107" s="0" t="str">

</xml_diff>

<commit_message>
Began process of updating "Dark Embrace"'s conditions
The new requirements will hopefully be much simpler, so that RATools won't crash when it attempts to generate them.
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2438" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2439" uniqueCount="511">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -995,6 +995,9 @@
   </si>
   <si>
     <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is basic?</t>
   </si>
   <si>
     <t xml:space="preserve">0xFF</t>
@@ -1677,17 +1680,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D681"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A677" activeCellId="1" sqref="D2:D95 A677"/>
+      <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -11231,7 +11234,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -11240,17 +11243,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B95" activeCellId="1" sqref="D2:D95 B95"/>
+      <selection pane="topLeft" activeCell="B95" activeCellId="0" sqref="B95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -13277,7 +13280,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -13286,17 +13289,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A84" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -13313,260 +13316,314 @@
         <v>322</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="D2" s="0" t="str">
+        <v>325</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""", ""category"": """,C2,""" },")</f>
         <v>0xFF: { "id": 0xFF, "name": "N/A", "category": "N/A" },</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D3" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""", ""category"": """,C3,""" },")</f>
         <v>0x00: { "id": 0x00, "name": "Quick Blitz", "category": "Melee" },</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D4" s="0" t="str">
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""", ""category"": """,C4,""" },")</f>
         <v>0x01: { "id": 0x01, "name": "Sliding Dash", "category": "Melee" },</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D5" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""", ""category"": """,C5,""" },")</f>
         <v>0x02: { "id": 0x02, "name": "Round Blitz", "category": "Melee" },</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D6" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""", ""category"": """,C6,""" },")</f>
         <v>0x03: { "id": 0x03, "name": "Strike Raid", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D7" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""", ""category"": """,C7,""" },")</f>
         <v>0x04: { "id": 0x04, "name": "Rising Strike", "category": "Melee" },</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D8" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""", ""category"": """,C8,""" },")</f>
         <v>0x05: { "id": 0x05, "name": "Sliding Rush", "category": "Melee" },</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D9" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""", ""category"": """,C9,""" },")</f>
         <v>0x06: { "id": 0x06, "name": "Aerial Sweep", "category": "Melee" },</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D10" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""", ""category"": """,C10,""" },")</f>
         <v>0x07: { "id": 0x07, "name": "Air Sweep", "category": "Melee" },</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D11" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""", ""category"": """,C11,""" },")</f>
         <v>0x08: { "id": 0x08, "name": "Aerial Slam", "category": "Melee" },</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D12" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""", ""category"": """,C12,""" },")</f>
         <v>0x09: { "id": 0x09, "name": "Land Crash", "category": "Melee" },</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D13" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A13,": { ""id"": ",A13,", ""name"": """,B13,""", ""category"": """,C13,""" },")</f>
         <v>0x0a: { "id": 0x0a, "name": "Fire Edge", "category": "Melee" },</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D14" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A14,": { ""id"": ",A14,", ""name"": """,B14,""", ""category"": """,C14,""" },")</f>
         <v>0x0b: { "id": 0x0b, "name": "Blizzard Edge", "category": "Melee" },</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D15" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A15,": { ""id"": ",A15,", ""name"": """,B15,""", ""category"": """,C15,""" },")</f>
         <v>0x0c: { "id": 0x0c, "name": "Thunder Edge", "category": "Melee" },</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D16" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A16,": { ""id"": ",A16,", ""name"": """,B16,""", ""category"": """,C16,""" },")</f>
         <v>0x0d: { "id": 0x0d, "name": "Aero Edge", "category": "Melee" },</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D17" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A17,": { ""id"": ",A17,", ""name"": """,B17,""", ""category"": """,C17,""" },")</f>
         <v>0x0e: { "id": 0x0e, "name": "Heat Dash", "category": "Melee" },</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D18" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A18,": { ""id"": ",A18,", ""name"": """,B18,""", ""category"": """,C18,""" },")</f>
         <v>0x0f: { "id": 0x0f, "name": "Ice Dash", "category": "Melee" },</v>
       </c>
@@ -13576,12 +13633,15 @@
         <v>301</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D19" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A19,": { ""id"": ",A19,", ""name"": """,B19,""", ""category"": """,C19,""" },")</f>
         <v>0x10: { "id": 0x10, "name": "Spark Dash", "category": "Melee" },</v>
       </c>
@@ -13591,12 +13651,15 @@
         <v>267</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D20" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A20,": { ""id"": ",A20,", ""name"": """,B20,""", ""category"": """,C20,""" },")</f>
         <v>0x11: { "id": 0x11, "name": "Wind Dash", "category": "Melee" },</v>
       </c>
@@ -13606,162 +13669,195 @@
         <v>256</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D21" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A21,": { ""id"": ",A21,", ""name"": """,B21,""", ""category"": """,C21,""" },")</f>
         <v>0x12: { "id": 0x12, "name": "Fire Blast", "category": "Melee" },</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D22" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A22,": { ""id"": ",A22,", ""name"": """,B22,""", ""category"": """,C22,""" },")</f>
         <v>0x13: { "id": 0x13, "name": "Blizzard Blast", "category": "Melee" },</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D23" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A23,": { ""id"": ",A23,", ""name"": """,B23,""", ""category"": """,C23,""" },")</f>
         <v>0x14: { "id": 0x14, "name": "Thunder Blast", "category": "Melee" },</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D24" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A24,": { ""id"": ",A24,", ""name"": """,B24,""", ""category"": """,C24,""" },")</f>
         <v>0x15: { "id": 0x15, "name": "Aero Blast", "category": "Melee" },</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D25" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A25,": { ""id"": ",A25,", ""name"": """,B25,""", ""category"": """,C25,""" },")</f>
         <v>0x16: { "id": 0x16, "name": "Fire Raid", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D26" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A26,": { ""id"": ",A26,", ""name"": """,B26,""", ""category"": """,C26,""" },")</f>
         <v>0x17: { "id": 0x17, "name": "Blizzard Raid", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D27" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A27,": { ""id"": ",A27,", ""name"": """,B27,""", ""category"": """,C27,""" },")</f>
         <v>0x18: { "id": 0x18, "name": "Thunder Raid", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D28" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A28,": { ""id"": ",A28,", ""name"": """,B28,""", ""category"": """,C28,""" },")</f>
         <v>0x19: { "id": 0x19, "name": "Aero Raid", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D29" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A29,": { ""id"": ",A29,", ""name"": """,B29,""", ""category"": """,C29,""" },")</f>
         <v>0x1a: { "id": 0x1a, "name": "Fire Buster", "category": "Melee" },</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D30" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A30,": { ""id"": ",A30,", ""name"": """,B30,""", ""category"": """,C30,""" },")</f>
         <v>0x1b: { "id": 0x1b, "name": "Blizzard Buster", "category": "Melee" },</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D31" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A31,": { ""id"": ",A31,", ""name"": """,B31,""", ""category"": """,C31,""" },")</f>
         <v>0x1c: { "id": 0x1c, "name": "Thunder Buster", "category": "Melee" },</v>
       </c>
@@ -13771,12 +13867,15 @@
         <v>203</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D32" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A32,": { ""id"": ",A32,", ""name"": """,B32,""", ""category"": """,C32,""" },")</f>
         <v>0x1d: { "id": 0x1d, "name": "Aero Buster", "category": "Melee" },</v>
       </c>
@@ -13786,12 +13885,15 @@
         <v>206</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D33" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A33,": { ""id"": ",A33,", ""name"": """,B33,""", ""category"": """,C33,""" },")</f>
         <v>0x1e: { "id": 0x1e, "name": "Heat Sweep", "category": "Melee" },</v>
       </c>
@@ -13801,27 +13903,33 @@
         <v>211</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D34" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A34,": { ""id"": ",A34,", ""name"": """,B34,""", ""category"": """,C34,""" },")</f>
         <v>0x1f: { "id": 0x1f, "name": "Ice Sweep", "category": "Melee" },</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D35" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A35,": { ""id"": ",A35,", ""name"": """,B35,""", ""category"": """,C35,""" },")</f>
         <v>0x20: { "id": 0x20, "name": "Spark Sweep", "category": "Melee" },</v>
       </c>
@@ -13831,897 +13939,1077 @@
         <v>241</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D36" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A36,": { ""id"": ",A36,", ""name"": """,B36,""", ""category"": """,C36,""" },")</f>
         <v>0x21: { "id": 0x21, "name": "Wind Sweep", "category": "Melee" },</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D37" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A37,": { ""id"": ",A37,", ""name"": """,B37,""", ""category"": """,C37,""" },")</f>
         <v>0x22: { "id": 0x22, "name": "Heat Storm", "category": "Melee" },</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D38" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A38,": { ""id"": ",A38,", ""name"": """,B38,""", ""category"": """,C38,""" },")</f>
         <v>0x23: { "id": 0x23, "name": "Ice Storm", "category": "Melee" },</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D39" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A39,": { ""id"": ",A39,", ""name"": """,B39,""", ""category"": """,C39,""" },")</f>
         <v>0x24: { "id": 0x24, "name": "Spark Storm", "category": "Melee" },</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D40" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A40,": { ""id"": ",A40,", ""name"": """,B40,""", ""category"": """,C40,""" },")</f>
         <v>0x25: { "id": 0x25, "name": "Wind Storm", "category": "Melee" },</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D41" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A41,": { ""id"": ",A41,", ""name"": """,B41,""", ""category"": """,C41,""" },")</f>
         <v>0x26: { "id": 0x26, "name": "Fire Slam", "category": "Melee" },</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D42" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A42,": { ""id"": ",A42,", ""name"": """,B42,""", ""category"": """,C42,""" },")</f>
         <v>0x27: { "id": 0x27, "name": "Blizzard Slam", "category": "Melee" },</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D43" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A43,": { ""id"": ",A43,", ""name"": """,B43,""", ""category"": """,C43,""" },")</f>
         <v>0x28: { "id": 0x28, "name": "Thunder Slam", "category": "Melee" },</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D44" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A44,": { ""id"": ",A44,", ""name"": """,B44,""", ""category"": """,C44,""" },")</f>
         <v>0x29: { "id": 0x29, "name": "Aero Slam", "category": "Melee" },</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D45" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A45,": { ""id"": ",A45,", ""name"": """,B45,""", ""category"": """,C45,""" },")</f>
         <v>0x2a: { "id": 0x2a, "name": "Heat Dive", "category": "Melee" },</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D46" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A46,": { ""id"": ",A46,", ""name"": """,B46,""", ""category"": """,C46,""" },")</f>
         <v>0x2b: { "id": 0x2b, "name": "Ice Dive", "category": "Melee" },</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D47" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A47,": { ""id"": ",A47,", ""name"": """,B47,""", ""category"": """,C47,""" },")</f>
         <v>0x2c: { "id": 0x2c, "name": "Spark Dive", "category": "Melee" },</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D48" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A48,": { ""id"": ",A48,", ""name"": """,B48,""", ""category"": """,C48,""" },")</f>
         <v>0x2d: { "id": 0x2d, "name": "Wind Dive", "category": "Melee" },</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D49" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A49,": { ""id"": ",A49,", ""name"": """,B49,""", ""category"": """,C49,""" },")</f>
         <v>0x2e: { "id": 0x2e, "name": "Stun Impact", "category": "Melee" },</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D50" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A50,": { ""id"": ",A50,", ""name"": """,B50,""", ""category"": """,C50,""" },")</f>
         <v>0x2f: { "id": 0x2f, "name": "Muscle Strike", "category": "Melee" },</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D51" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A51,": { ""id"": ",A51,", ""name"": """,B51,""", ""category"": """,C51,""" },")</f>
         <v>0x30: { "id": 0x30, "name": "Chain Rave", "category": "Melee" },</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D52" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A52,": { ""id"": ",A52,", ""name"": """,B52,""", ""category"": """,C52,""" },")</f>
         <v>0x31: { "id": 0x31, "name": "Rising Rush", "category": "Melee" },</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D53" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A53,": { ""id"": ",A53,", ""name"": """,B53,""", ""category"": """,C53,""" },")</f>
         <v>0x32: { "id": 0x32, "name": "Zantetsuken", "category": "Melee" },</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D54" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A54,": { ""id"": ",A54,", ""name"": """,B54,""", ""category"": """,C54,""" },")</f>
         <v>0x33: { "id": 0x33, "name": "Eruption", "category": "Melee" },</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D55" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A55,": { ""id"": ",A55,", ""name"": """,B55,""", ""category"": """,C55,""" },")</f>
         <v>0x34: { "id": 0x34, "name": "Gravity Drop", "category": "Melee" },</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="D56" s="0" t="str">
+        <v>328</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A56,": { ""id"": ",A56,", ""name"": """,B56,""", ""category"": """,C56,""" },")</f>
         <v>0x35: { "id": 0x35, "name": "Shock Fall", "category": "Melee" },</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D57" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A57,": { ""id"": ",A57,", ""name"": """,B57,""", ""category"": """,C57,""" },")</f>
         <v>0x36: { "id": 0x36, "name": "Judgment Triad", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D58" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A58,": { ""id"": ",A58,", ""name"": """,B58,""", ""category"": """,C58,""" },")</f>
         <v>0x37: { "id": 0x37, "name": "Fire", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D59" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A59,": { ""id"": ",A59,", ""name"": """,B59,""", ""category"": """,C59,""" },")</f>
         <v>0x38: { "id": 0x38, "name": "Fira", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D60" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A60,": { ""id"": ",A60,", ""name"": """,B60,""", ""category"": """,C60,""" },")</f>
         <v>0x39: { "id": 0x39, "name": "Firaga", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D61" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E61" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A61,": { ""id"": ",A61,", ""name"": """,B61,""", ""category"": """,C61,""" },")</f>
         <v>0x3a: { "id": 0x3a, "name": "Blizzard", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D62" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A62,": { ""id"": ",A62,", ""name"": """,B62,""", ""category"": """,C62,""" },")</f>
         <v>0x3b: { "id": 0x3b, "name": "Blizzara", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D63" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A63,": { ""id"": ",A63,", ""name"": """,B63,""", ""category"": """,C63,""" },")</f>
         <v>0x3c: { "id": 0x3c, "name": "Blizzaga", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D64" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A64,": { ""id"": ",A64,", ""name"": """,B64,""", ""category"": """,C64,""" },")</f>
         <v>0x3d: { "id": 0x3d, "name": "Thunder", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D65" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A65,": { ""id"": ",A65,", ""name"": """,B65,""", ""category"": """,C65,""" },")</f>
         <v>0x3e: { "id": 0x3e, "name": "Thundara", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D66" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A66,": { ""id"": ",A66,", ""name"": """,B66,""", ""category"": """,C66,""" },")</f>
         <v>0x3f: { "id": 0x3f, "name": "Thundaga", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D67" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A67,": { ""id"": ",A67,", ""name"": """,B67,""", ""category"": """,C67,""" },")</f>
         <v>0x40: { "id": 0x40, "name": "Aero", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D68" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A68,": { ""id"": ",A68,", ""name"": """,B68,""", ""category"": """,C68,""" },")</f>
         <v>0x41: { "id": 0x41, "name": "Aerora", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D69" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A69,": { ""id"": ",A69,", ""name"": """,B69,""", ""category"": """,C69,""" },")</f>
         <v>0x42: { "id": 0x42, "name": "Aeroga", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D70" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A70,": { ""id"": ",A70,", ""name"": """,B70,""", ""category"": """,C70,""" },")</f>
         <v>0x43: { "id": 0x43, "name": "Magnet", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D71" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A71,": { ""id"": ",A71,", ""name"": """,B71,""", ""category"": """,C71,""" },")</f>
         <v>0x44: { "id": 0x44, "name": "Magnera", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D72" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A72,": { ""id"": ",A72,", ""name"": """,B72,""", ""category"": """,C72,""" },")</f>
         <v>0x45: { "id": 0x45, "name": "Magnega", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>462</v>
-      </c>
-      <c r="D73" s="0" t="str">
+        <v>463</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A73,": { ""id"": ",A73,", ""name"": """,B73,""", ""category"": """,C73,""" },")</f>
         <v>0x46: { "id": 0x46, "name": "Cure", "category": "Curative" },</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="C74" s="0" t="s">
         <v>463</v>
       </c>
-      <c r="B74" s="0" t="s">
-        <v>464</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>462</v>
-      </c>
-      <c r="D74" s="0" t="str">
+      <c r="D74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A74,": { ""id"": ",A74,", ""name"": """,B74,""", ""category"": """,C74,""" },")</f>
         <v>0x47: { "id": 0x47, "name": "Cura", "category": "Curative" },</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>462</v>
-      </c>
-      <c r="D75" s="0" t="str">
+        <v>463</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A75,": { ""id"": ",A75,", ""name"": """,B75,""", ""category"": """,C75,""" },")</f>
         <v>0x48: { "id": 0x48, "name": "Curaga", "category": "Curative" },</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D76" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E76" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A76,": { ""id"": ",A76,", ""name"": """,B76,""", ""category"": """,C76,""" },")</f>
         <v>0x49: { "id": 0x49, "name": "Slow", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D77" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E77" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A77,": { ""id"": ",A77,", ""name"": """,B77,""", ""category"": """,C77,""" },")</f>
         <v>0x4a: { "id": 0x4a, "name": "Stop", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D78" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E78" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A78,": { ""id"": ",A78,", ""name"": """,B78,""", ""category"": """,C78,""" },")</f>
         <v>0x4b: { "id": 0x4b, "name": "Confuse", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D79" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A79,": { ""id"": ",A79,", ""name"": """,B79,""", ""category"": """,C79,""" },")</f>
         <v>0x4c: { "id": 0x4c, "name": "Firaga Burst", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D80" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A80,": { ""id"": ",A80,", ""name"": """,B80,""", ""category"": """,C80,""" },")</f>
         <v>0x4d: { "id": 0x4d, "name": "Triple Firaga", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D81" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A81,": { ""id"": ",A81,", ""name"": """,B81,""", ""category"": """,C81,""" },")</f>
         <v>0x4e: { "id": 0x4e, "name": "Triple Burst", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D82" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A82,": { ""id"": ",A82,", ""name"": """,B82,""", ""category"": """,C82,""" },")</f>
         <v>0x4f: { "id": 0x4f, "name": "Blizzaga Pursuit", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D83" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A83,": { ""id"": ",A83,", ""name"": """,B83,""", ""category"": """,C83,""" },")</f>
         <v>0x50: { "id": 0x50, "name": "Triple Blizzaga", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D84" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A84,": { ""id"": ",A84,", ""name"": """,B84,""", ""category"": """,C84,""" },")</f>
         <v>0x51: { "id": 0x51, "name": "Triple Pursuit", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D85" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A85,": { ""id"": ",A85,", ""name"": """,B85,""", ""category"": """,C85,""" },")</f>
         <v>0x52: { "id": 0x52, "name": "Thunder Tracer", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D86" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A86,": { ""id"": ",A86,", ""name"": """,B86,""", ""category"": """,C86,""" },")</f>
         <v>0x53: { "id": 0x53, "name": "Pulse Tracer", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D87" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A87,": { ""id"": ",A87,", ""name"": """,B87,""", ""category"": """,C87,""" },")</f>
         <v>0x54: { "id": 0x54, "name": "Tornado Tracer", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D88" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E88" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A88,": { ""id"": ",A88,", ""name"": """,B88,""", ""category"": """,C88,""" },")</f>
         <v>0x55: { "id": 0x55, "name": "Wind Tracer", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D89" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A89,": { ""id"": ",A89,", ""name"": """,B89,""", ""category"": """,C89,""" },")</f>
         <v>0x56: { "id": 0x56, "name": "Magnet Grab", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>462</v>
-      </c>
-      <c r="D90" s="0" t="str">
+        <v>463</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E90" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A90,": { ""id"": ",A90,", ""name"": """,B90,""", ""category"": """,C90,""" },")</f>
         <v>0x57: { "id": 0x57, "name": "Esuna", "category": "Curative" },</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D91" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A91,": { ""id"": ",A91,", ""name"": """,B91,""", ""category"": """,C91,""" },")</f>
         <v>0x58: { "id": 0x58, "name": "Flame Fall", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D92" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A92,": { ""id"": ",A92,", ""name"": """,B92,""", ""category"": """,C92,""" },")</f>
         <v>0x59: { "id": 0x59, "name": "Icicle Mine", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D93" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E93" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A93,": { ""id"": ",A93,", ""name"": """,B93,""", ""category"": """,C93,""" },")</f>
         <v>0x5a: { "id": 0x5a, "name": "Exo Spark", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D94" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E94" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A94,": { ""id"": ",A94,", ""name"": """,B94,""", ""category"": """,C94,""" },")</f>
         <v>0x5b: { "id": 0x5b, "name": "Cyclone", "category": "Ranged" },</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D95" s="0" t="str">
+        <v>335</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E95" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A95,": { ""id"": ",A95,", ""name"": """,B95,""", ""category"": """,C95,""" },")</f>
         <v>0x5c: { "id": 0x5c, "name": "Quake", "category": "Ranged" },</v>
       </c>
@@ -14730,7 +15018,7 @@
   <autoFilter ref="C1:C95"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -14740,17 +15028,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="D2:D95 E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="14.77"/>
@@ -14759,16 +15047,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>135</v>
@@ -14779,13 +15067,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E2" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A2,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B2, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C2, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D2, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14797,13 +15085,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E3" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A3,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B3, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C3, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D3, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14815,13 +15103,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E4" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A4,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B4, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C4, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D4, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14833,13 +15121,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E5" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A5,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B5, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C5, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D5, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14851,13 +15139,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E6" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A6,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B6, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C6, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D6, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14869,13 +15157,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E7" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A7,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B7, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C7, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D7, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14887,13 +15175,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E8" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A8,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B8, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C8, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D8, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14905,13 +15193,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E9" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A9,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B9, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C9, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D9, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14923,13 +15211,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E10" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A10,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B10, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C10, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D10, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14941,13 +15229,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E11" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A11,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B11, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C11, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D11, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14959,13 +15247,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E12" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A12,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B12, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C12, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D12, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14977,13 +15265,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E13" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A13,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B13, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C13, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D13, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -14995,13 +15283,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E14" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A14,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B14, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C14, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D14, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15013,13 +15301,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E15" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A15,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B15, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C15, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D15, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15031,13 +15319,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E16" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A16,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B16, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C16, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D16, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15049,13 +15337,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E17" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A17,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B17, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C17, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D17, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15067,13 +15355,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E18" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A18,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B18, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C18, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D18, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15085,13 +15373,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E19" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A19,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B19, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C19, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D19, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15103,13 +15391,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E20" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A20,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B20, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C20, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D20, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15121,13 +15409,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E21" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A21,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B21, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C21, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D21, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15139,13 +15427,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E22" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A22,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B22, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C22, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D22, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15157,13 +15445,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E23" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A23,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B23, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C23, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D23, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15175,13 +15463,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E24" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A24,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B24, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C24, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D24, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15193,13 +15481,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E25" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A25,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B25, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C25, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D25, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15211,13 +15499,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E26" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A26,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B26, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C26, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D26, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15229,13 +15517,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E27" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A27,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B27, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C27, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D27, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15247,13 +15535,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E28" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A28,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B28, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C28, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D28, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15265,13 +15553,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E29" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A29,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B29, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C29, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D29, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15283,13 +15571,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E30" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A30,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B30, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C30, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D30, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15301,13 +15589,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E31" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A31,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B31, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C31, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D31, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15319,13 +15607,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E32" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A32,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B32, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C32, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D32, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15337,13 +15625,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E33" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A33,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B33, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C33, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D33, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15355,13 +15643,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E34" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A34,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B34, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C34, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D34, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15373,13 +15661,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E35" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A35,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B35, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C35, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D35, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15391,13 +15679,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E36" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A36,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B36, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C36, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D36, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15409,13 +15697,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E37" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A37,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B37, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C37, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D37, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15427,13 +15715,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E38" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A38,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B38, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C38, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D38, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15445,13 +15733,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E39" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A39,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B39, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C39, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D39, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15463,13 +15751,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E40" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A40,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B40, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C40, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D40, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15481,13 +15769,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E41" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A41,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B41, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C41, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D41, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15499,13 +15787,13 @@
         <v>40</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E42" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A42,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B42, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C42, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D42, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15517,13 +15805,13 @@
         <v>41</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E43" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A43,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B43, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C43, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D43, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15535,13 +15823,13 @@
         <v>42</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E44" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A44,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B44, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C44, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D44, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15553,13 +15841,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A45,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B45, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C45, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D45, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15571,13 +15859,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E46" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A46,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B46, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C46, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D46, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15589,13 +15877,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E47" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A47,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B47, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C47, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D47, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15607,13 +15895,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E48" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A48,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B48, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C48, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D48, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15625,13 +15913,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E49" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A49,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B49, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C49, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D49, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15643,13 +15931,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E50" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A50,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B50, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C50, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D50, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15661,13 +15949,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E51" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A51,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B51, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C51, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D51, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15679,13 +15967,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E52" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A52,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B52, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C52, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D52, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15697,13 +15985,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E53" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A53,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B53, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C53, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D53, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15715,13 +16003,13 @@
         <v>52</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E54" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A54,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B54, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C54, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D54, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15733,13 +16021,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E55" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A55,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B55, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C55, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D55, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15751,13 +16039,13 @@
         <v>54</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E56" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A56,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B56, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C56, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D56, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15769,13 +16057,13 @@
         <v>55</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E57" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A57,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B57, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C57, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D57, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15787,13 +16075,13 @@
         <v>56</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E58" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A58,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B58, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C58, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D58, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15805,13 +16093,13 @@
         <v>57</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E59" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A59,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B59, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C59, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D59, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15823,13 +16111,13 @@
         <v>58</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E60" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A60,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B60, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C60, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D60, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15841,13 +16129,13 @@
         <v>59</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E61" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A61,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B61, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C61, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D61, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15859,13 +16147,13 @@
         <v>60</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E62" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A62,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B62, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C62, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D62, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15877,13 +16165,13 @@
         <v>61</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E63" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A63,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B63, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C63, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D63, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15895,13 +16183,13 @@
         <v>62</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E64" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A64,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B64, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C64, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D64, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15913,13 +16201,13 @@
         <v>63</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E65" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A65,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B65, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C65, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D65, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15931,13 +16219,13 @@
         <v>64</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="E66" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A66,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B66, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C66, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D66, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15949,13 +16237,13 @@
         <v>65</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E67" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A67,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B67, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C67, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D67, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15967,13 +16255,13 @@
         <v>66</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E68" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A68,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B68, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C68, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D68, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15985,13 +16273,13 @@
         <v>67</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E69" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A69,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B69, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C69, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D69, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16003,13 +16291,13 @@
         <v>68</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E70" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A70,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B70, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C70, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D70, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16021,13 +16309,13 @@
         <v>69</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E71" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A71,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B71, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C71, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D71, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16039,13 +16327,13 @@
         <v>70</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E72" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A72,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B72, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C72, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D72, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16057,13 +16345,13 @@
         <v>71</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E73" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A73,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B73, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C73, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D73, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16075,13 +16363,13 @@
         <v>72</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E74" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A74,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B74, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C74, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D74, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16093,13 +16381,13 @@
         <v>73</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E75" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A75,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B75, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C75, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D75, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16111,13 +16399,13 @@
         <v>74</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E76" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A76,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B76, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C76, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D76, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16129,13 +16417,13 @@
         <v>75</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E77" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A77,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B77, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C77, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D77, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16147,13 +16435,13 @@
         <v>76</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E78" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A78,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B78, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C78, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D78, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16165,13 +16453,13 @@
         <v>77</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E79" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A79,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B79, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C79, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D79, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16183,13 +16471,13 @@
         <v>78</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E80" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A80,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B80, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C80, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D80, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16201,13 +16489,13 @@
         <v>79</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E81" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A81,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B81, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C81, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D81, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16219,13 +16507,13 @@
         <v>80</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E82" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A82,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B82, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C82, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D82, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16237,13 +16525,13 @@
         <v>81</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E83" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A83,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B83, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C83, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D83, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16255,13 +16543,13 @@
         <v>82</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E84" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A84,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B84, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C84, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D84, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16273,13 +16561,13 @@
         <v>83</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E85" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A85,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B85, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C85, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D85, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16291,13 +16579,13 @@
         <v>84</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E86" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A86,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B86, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C86, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D86, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16309,13 +16597,13 @@
         <v>85</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E87" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A87,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B87, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C87, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D87, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16327,13 +16615,13 @@
         <v>86</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E88" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A88,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B88, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C88, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D88, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16345,13 +16633,13 @@
         <v>87</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E89" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A89,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B89, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C89, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D89, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16363,13 +16651,13 @@
         <v>88</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E90" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A90,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B90, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C90, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D90, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16381,13 +16669,13 @@
         <v>89</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E91" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A91,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B91, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C91, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D91, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16399,13 +16687,13 @@
         <v>90</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E92" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A92,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B92, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C92, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D92, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16417,13 +16705,13 @@
         <v>91</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E93" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A93,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B93, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C93, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D93, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16435,13 +16723,13 @@
         <v>92</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="E94" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A94,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B94, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C94, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D94, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16453,13 +16741,13 @@
         <v>93</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E95" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A95,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B95, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C95, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D95, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16471,13 +16759,13 @@
         <v>94</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E96" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A96,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B96, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C96, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D96, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16489,13 +16777,13 @@
         <v>95</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E97" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A97,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B97, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C97, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D97, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16507,13 +16795,13 @@
         <v>96</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E98" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A98,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B98, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C98, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D98, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16525,13 +16813,13 @@
         <v>97</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E99" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A99,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B99, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C99, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D99, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16543,13 +16831,13 @@
         <v>98</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E100" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A100,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B100, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C100, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D100, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16561,13 +16849,13 @@
         <v>99</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E101" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A101,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B101, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C101, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D101, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16579,13 +16867,13 @@
         <v>100</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="E102" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A102,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B102, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C102, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D102, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16597,13 +16885,13 @@
         <v>101</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E103" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A103,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B103, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C103, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D103, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16615,13 +16903,13 @@
         <v>102</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E104" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A104,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B104, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C104, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D104, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16633,13 +16921,13 @@
         <v>103</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E105" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A105,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B105, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C105, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D105, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16651,13 +16939,13 @@
         <v>104</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E106" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A106,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B106, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C106, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D106, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16669,13 +16957,13 @@
         <v>105</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E107" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A107,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B107, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C107, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D107, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16687,13 +16975,13 @@
         <v>106</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E108" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A108,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B108, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C108, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D108, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16705,13 +16993,13 @@
         <v>107</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E109" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A109,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B109, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C109, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D109, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16723,13 +17011,13 @@
         <v>108</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E110" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A110,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B110, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C110, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D110, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16741,13 +17029,13 @@
         <v>109</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="E111" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A111,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B111, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C111, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D111, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16759,13 +17047,13 @@
         <v>110</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E112" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A112,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B112, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C112, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D112, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16777,13 +17065,13 @@
         <v>111</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E113" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A113,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B113, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C113, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D113, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16795,13 +17083,13 @@
         <v>112</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E114" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A114,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B114, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C114, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D114, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16813,13 +17101,13 @@
         <v>113</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E115" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A115,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B115, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C115, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D115, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16831,13 +17119,13 @@
         <v>114</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E116" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A116,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B116, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C116, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D116, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16849,13 +17137,13 @@
         <v>115</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E117" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A117,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B117, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C117, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D117, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16867,13 +17155,13 @@
         <v>116</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E118" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A118,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B118, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C118, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D118, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16885,13 +17173,13 @@
         <v>117</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="E119" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A119,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B119, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C119, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D119, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16903,13 +17191,13 @@
         <v>118</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E120" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A120,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B120, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C120, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D120, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16921,13 +17209,13 @@
         <v>119</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E121" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A121,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B121, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C121, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D121, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16939,13 +17227,13 @@
         <v>120</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E122" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A122,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B122, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C122, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D122, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16957,13 +17245,13 @@
         <v>121</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E123" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A123,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B123, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C123, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D123, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16975,13 +17263,13 @@
         <v>122</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E124" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A124,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B124, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C124, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D124, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16993,13 +17281,13 @@
         <v>123</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E125" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A125,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B125, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C125, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D125, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17011,13 +17299,13 @@
         <v>124</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E126" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A126,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B126, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C126, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D126, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17029,13 +17317,13 @@
         <v>125</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E127" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A127,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B127, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C127, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D127, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17047,13 +17335,13 @@
         <v>126</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="E128" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A128,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B128, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C128, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D128, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17065,13 +17353,13 @@
         <v>127</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E129" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A129,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B129, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C129, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D129, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17083,13 +17371,13 @@
         <v>128</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="E130" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A130,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B130, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C130, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D130, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17101,13 +17389,13 @@
         <v>129</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="E131" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A131,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B131, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C131, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D131, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17119,13 +17407,13 @@
         <v>130</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E132" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A132,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B132, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C132, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D132, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17137,13 +17425,13 @@
         <v>131</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="E133" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A133,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B133, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C133, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D133, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17155,13 +17443,13 @@
         <v>132</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E134" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A134,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B134, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C134, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D134, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17173,13 +17461,13 @@
         <v>133</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E135" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A135,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B135, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C135, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D135, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17191,13 +17479,13 @@
         <v>134</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="E136" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A136,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B136, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C136, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D136, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17207,7 +17495,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added final cheevos and leaderboards up to the end of Hollow Bastion, Part II.
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,8 @@
     <sheet name="Command Conversion Combinations" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$95</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$D$95</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$95</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2439" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2447" uniqueCount="513">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -992,6 +993,12 @@
   </si>
   <si>
     <t xml:space="preserve">Entrance Hall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CastleOblivionSomewhere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CastleOblivionSomewhere2</t>
   </si>
   <si>
     <t xml:space="preserve">Category</t>
@@ -1690,7 +1697,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -11249,11 +11256,11 @@
   </sheetPr>
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B95" activeCellId="0" sqref="B95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B97" activeCellId="0" sqref="B97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -13236,18 +13243,42 @@
       <c r="A95" s="0" t="n">
         <v>94</v>
       </c>
+      <c r="B95" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="E95" s="0" t="s">
+        <v>296</v>
+      </c>
       <c r="F95" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A95,": { ""worldId"": ",C95,", ""name"": """,D95,""", ""display"": """,E95,""", ""areaId"": ",B95,", },")</f>
-        <v>94: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>94: { "worldId": 0x7, "name": "CastleOblivionSomewhere", "display": "Somewhere in the datascape…", "areaId": 0x1, },</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
         <v>95</v>
       </c>
+      <c r="B96" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>296</v>
+      </c>
       <c r="F96" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A96,": { ""worldId"": ",C96,", ""name"": """,D96,""", ""display"": """,E96,""", ""areaId"": ",B96,", },")</f>
-        <v>95: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>95: { "worldId": 0x7, "name": "CastleOblivionSomewhere2", "display": "Somewhere in the datascape…", "areaId": 0xa, },</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13290,19 +13321,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C96" activeCellId="0" sqref="C96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13313,1709 +13345,1715 @@
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""", ""category"": """,C2,""" },")</f>
-        <v>0xFF: { "id": 0xFF, "name": "N/A", "category": "N/A" },</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A2,": { ""id"": ",A2,", ""name"": """,B2,""", ""category"": """,C2,""", ""isBasic"": ",D2," },")</f>
+        <v>0xFF: { "id": 0xFF, "name": "N/A", "category": "N/A", "isBasic": 1 },</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""", ""category"": """,C3,""" },")</f>
-        <v>0x00: { "id": 0x00, "name": "Quick Blitz", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A3,": { ""id"": ",A3,", ""name"": """,B3,""", ""category"": """,C3,""", ""isBasic"": ",D3," },")</f>
+        <v>0x00: { "id": 0x00, "name": "Quick Blitz", "category": "Melee", "isBasic": 1 },</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>330</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>328</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""", ""category"": """,C4,""" },")</f>
-        <v>0x01: { "id": 0x01, "name": "Sliding Dash", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A4,": { ""id"": ",A4,", ""name"": """,B4,""", ""category"": """,C4,""", ""isBasic"": ",D4," },")</f>
+        <v>0x01: { "id": 0x01, "name": "Sliding Dash", "category": "Melee", "isBasic": 1 },</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""", ""category"": """,C5,""" },")</f>
-        <v>0x02: { "id": 0x02, "name": "Round Blitz", "category": "Melee" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A5,": { ""id"": ",A5,", ""name"": """,B5,""", ""category"": """,C5,""", ""isBasic"": ",D5," },")</f>
+        <v>0x02: { "id": 0x02, "name": "Round Blitz", "category": "Melee", "isBasic": 1 },</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""", ""category"": """,C6,""" },")</f>
-        <v>0x03: { "id": 0x03, "name": "Strike Raid", "category": "Ranged" },</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A6,": { ""id"": ",A6,", ""name"": """,B6,""", ""category"": """,C6,""", ""isBasic"": ",D6," },")</f>
+        <v>0x03: { "id": 0x03, "name": "Strike Raid", "category": "Ranged", "isBasic": 1 },</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""", ""category"": """,C7,""" },")</f>
-        <v>0x04: { "id": 0x04, "name": "Rising Strike", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A7,": { ""id"": ",A7,", ""name"": """,B7,""", ""category"": """,C7,""", ""isBasic"": ",D7," },")</f>
+        <v>0x04: { "id": 0x04, "name": "Rising Strike", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""", ""category"": """,C8,""" },")</f>
-        <v>0x05: { "id": 0x05, "name": "Sliding Rush", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A8,": { ""id"": ",A8,", ""name"": """,B8,""", ""category"": """,C8,""", ""isBasic"": ",D8," },")</f>
+        <v>0x05: { "id": 0x05, "name": "Sliding Rush", "category": "Melee", "isBasic": 1 },</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E9" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""", ""category"": """,C9,""" },")</f>
-        <v>0x06: { "id": 0x06, "name": "Aerial Sweep", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A9,": { ""id"": ",A9,", ""name"": """,B9,""", ""category"": """,C9,""", ""isBasic"": ",D9," },")</f>
+        <v>0x06: { "id": 0x06, "name": "Aerial Sweep", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""", ""category"": """,C10,""" },")</f>
-        <v>0x07: { "id": 0x07, "name": "Air Sweep", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A10,": { ""id"": ",A10,", ""name"": """,B10,""", ""category"": """,C10,""", ""isBasic"": ",D10," },")</f>
+        <v>0x07: { "id": 0x07, "name": "Air Sweep", "category": "Melee", "isBasic": 1 },</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""", ""category"": """,C11,""" },")</f>
-        <v>0x08: { "id": 0x08, "name": "Aerial Slam", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A11,": { ""id"": ",A11,", ""name"": """,B11,""", ""category"": """,C11,""", ""isBasic"": ",D11," },")</f>
+        <v>0x08: { "id": 0x08, "name": "Aerial Slam", "category": "Melee", "isBasic": 1 },</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E12" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""", ""category"": """,C12,""" },")</f>
-        <v>0x09: { "id": 0x09, "name": "Land Crash", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A12,": { ""id"": ",A12,", ""name"": """,B12,""", ""category"": """,C12,""", ""isBasic"": ",D12," },")</f>
+        <v>0x09: { "id": 0x09, "name": "Land Crash", "category": "Melee", "isBasic": 1 },</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A13,": { ""id"": ",A13,", ""name"": """,B13,""", ""category"": """,C13,""" },")</f>
-        <v>0x0a: { "id": 0x0a, "name": "Fire Edge", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A13,": { ""id"": ",A13,", ""name"": """,B13,""", ""category"": """,C13,""", ""isBasic"": ",D13," },")</f>
+        <v>0x0a: { "id": 0x0a, "name": "Fire Edge", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A14,": { ""id"": ",A14,", ""name"": """,B14,""", ""category"": """,C14,""" },")</f>
-        <v>0x0b: { "id": 0x0b, "name": "Blizzard Edge", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A14,": { ""id"": ",A14,", ""name"": """,B14,""", ""category"": """,C14,""", ""isBasic"": ",D14," },")</f>
+        <v>0x0b: { "id": 0x0b, "name": "Blizzard Edge", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A15,": { ""id"": ",A15,", ""name"": """,B15,""", ""category"": """,C15,""" },")</f>
-        <v>0x0c: { "id": 0x0c, "name": "Thunder Edge", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A15,": { ""id"": ",A15,", ""name"": """,B15,""", ""category"": """,C15,""", ""isBasic"": ",D15," },")</f>
+        <v>0x0c: { "id": 0x0c, "name": "Thunder Edge", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A16,": { ""id"": ",A16,", ""name"": """,B16,""", ""category"": """,C16,""" },")</f>
-        <v>0x0d: { "id": 0x0d, "name": "Aero Edge", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A16,": { ""id"": ",A16,", ""name"": """,B16,""", ""category"": """,C16,""", ""isBasic"": ",D16," },")</f>
+        <v>0x0d: { "id": 0x0d, "name": "Aero Edge", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A17,": { ""id"": ",A17,", ""name"": """,B17,""", ""category"": """,C17,""" },")</f>
-        <v>0x0e: { "id": 0x0e, "name": "Heat Dash", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A17,": { ""id"": ",A17,", ""name"": """,B17,""", ""category"": """,C17,""", ""isBasic"": ",D17," },")</f>
+        <v>0x0e: { "id": 0x0e, "name": "Heat Dash", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E18" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A18,": { ""id"": ",A18,", ""name"": """,B18,""", ""category"": """,C18,""" },")</f>
-        <v>0x0f: { "id": 0x0f, "name": "Ice Dash", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A18,": { ""id"": ",A18,", ""name"": """,B18,""", ""category"": """,C18,""", ""isBasic"": ",D18," },")</f>
+        <v>0x0f: { "id": 0x0f, "name": "Ice Dash", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>301</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E19" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A19,": { ""id"": ",A19,", ""name"": """,B19,""", ""category"": """,C19,""" },")</f>
-        <v>0x10: { "id": 0x10, "name": "Spark Dash", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A19,": { ""id"": ",A19,", ""name"": """,B19,""", ""category"": """,C19,""", ""isBasic"": ",D19," },")</f>
+        <v>0x10: { "id": 0x10, "name": "Spark Dash", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>267</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E20" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A20,": { ""id"": ",A20,", ""name"": """,B20,""", ""category"": """,C20,""" },")</f>
-        <v>0x11: { "id": 0x11, "name": "Wind Dash", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A20,": { ""id"": ",A20,", ""name"": """,B20,""", ""category"": """,C20,""", ""isBasic"": ",D20," },")</f>
+        <v>0x11: { "id": 0x11, "name": "Wind Dash", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>256</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E21" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A21,": { ""id"": ",A21,", ""name"": """,B21,""", ""category"": """,C21,""" },")</f>
-        <v>0x12: { "id": 0x12, "name": "Fire Blast", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A21,": { ""id"": ",A21,", ""name"": """,B21,""", ""category"": """,C21,""", ""isBasic"": ",D21," },")</f>
+        <v>0x12: { "id": 0x12, "name": "Fire Blast", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E22" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A22,": { ""id"": ",A22,", ""name"": """,B22,""", ""category"": """,C22,""" },")</f>
-        <v>0x13: { "id": 0x13, "name": "Blizzard Blast", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A22,": { ""id"": ",A22,", ""name"": """,B22,""", ""category"": """,C22,""", ""isBasic"": ",D22," },")</f>
+        <v>0x13: { "id": 0x13, "name": "Blizzard Blast", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E23" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A23,": { ""id"": ",A23,", ""name"": """,B23,""", ""category"": """,C23,""" },")</f>
-        <v>0x14: { "id": 0x14, "name": "Thunder Blast", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A23,": { ""id"": ",A23,", ""name"": """,B23,""", ""category"": """,C23,""", ""isBasic"": ",D23," },")</f>
+        <v>0x14: { "id": 0x14, "name": "Thunder Blast", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E24" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A24,": { ""id"": ",A24,", ""name"": """,B24,""", ""category"": """,C24,""" },")</f>
-        <v>0x15: { "id": 0x15, "name": "Aero Blast", "category": "Melee" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A24,": { ""id"": ",A24,", ""name"": """,B24,""", ""category"": """,C24,""", ""isBasic"": ",D24," },")</f>
+        <v>0x15: { "id": 0x15, "name": "Aero Blast", "category": "Melee", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E25" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A25,": { ""id"": ",A25,", ""name"": """,B25,""", ""category"": """,C25,""" },")</f>
-        <v>0x16: { "id": 0x16, "name": "Fire Raid", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A25,": { ""id"": ",A25,", ""name"": """,B25,""", ""category"": """,C25,""", ""isBasic"": ",D25," },")</f>
+        <v>0x16: { "id": 0x16, "name": "Fire Raid", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E26" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A26,": { ""id"": ",A26,", ""name"": """,B26,""", ""category"": """,C26,""" },")</f>
-        <v>0x17: { "id": 0x17, "name": "Blizzard Raid", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A26,": { ""id"": ",A26,", ""name"": """,B26,""", ""category"": """,C26,""", ""isBasic"": ",D26," },")</f>
+        <v>0x17: { "id": 0x17, "name": "Blizzard Raid", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E27" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A27,": { ""id"": ",A27,", ""name"": """,B27,""", ""category"": """,C27,""" },")</f>
-        <v>0x18: { "id": 0x18, "name": "Thunder Raid", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A27,": { ""id"": ",A27,", ""name"": """,B27,""", ""category"": """,C27,""", ""isBasic"": ",D27," },")</f>
+        <v>0x18: { "id": 0x18, "name": "Thunder Raid", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E28" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A28,": { ""id"": ",A28,", ""name"": """,B28,""", ""category"": """,C28,""" },")</f>
-        <v>0x19: { "id": 0x19, "name": "Aero Raid", "category": "Ranged" },</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A28,": { ""id"": ",A28,", ""name"": """,B28,""", ""category"": """,C28,""", ""isBasic"": ",D28," },")</f>
+        <v>0x19: { "id": 0x19, "name": "Aero Raid", "category": "Ranged", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E29" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A29,": { ""id"": ",A29,", ""name"": """,B29,""", ""category"": """,C29,""" },")</f>
-        <v>0x1a: { "id": 0x1a, "name": "Fire Buster", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A29,": { ""id"": ",A29,", ""name"": """,B29,""", ""category"": """,C29,""", ""isBasic"": ",D29," },")</f>
+        <v>0x1a: { "id": 0x1a, "name": "Fire Buster", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E30" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A30,": { ""id"": ",A30,", ""name"": """,B30,""", ""category"": """,C30,""" },")</f>
-        <v>0x1b: { "id": 0x1b, "name": "Blizzard Buster", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A30,": { ""id"": ",A30,", ""name"": """,B30,""", ""category"": """,C30,""", ""isBasic"": ",D30," },")</f>
+        <v>0x1b: { "id": 0x1b, "name": "Blizzard Buster", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E31" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A31,": { ""id"": ",A31,", ""name"": """,B31,""", ""category"": """,C31,""" },")</f>
-        <v>0x1c: { "id": 0x1c, "name": "Thunder Buster", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A31,": { ""id"": ",A31,", ""name"": """,B31,""", ""category"": """,C31,""", ""isBasic"": ",D31," },")</f>
+        <v>0x1c: { "id": 0x1c, "name": "Thunder Buster", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>203</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E32" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A32,": { ""id"": ",A32,", ""name"": """,B32,""", ""category"": """,C32,""" },")</f>
-        <v>0x1d: { "id": 0x1d, "name": "Aero Buster", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A32,": { ""id"": ",A32,", ""name"": """,B32,""", ""category"": """,C32,""", ""isBasic"": ",D32," },")</f>
+        <v>0x1d: { "id": 0x1d, "name": "Aero Buster", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>206</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E33" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A33,": { ""id"": ",A33,", ""name"": """,B33,""", ""category"": """,C33,""" },")</f>
-        <v>0x1e: { "id": 0x1e, "name": "Heat Sweep", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A33,": { ""id"": ",A33,", ""name"": """,B33,""", ""category"": """,C33,""", ""isBasic"": ",D33," },")</f>
+        <v>0x1e: { "id": 0x1e, "name": "Heat Sweep", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>211</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E34" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A34,": { ""id"": ",A34,", ""name"": """,B34,""", ""category"": """,C34,""" },")</f>
-        <v>0x1f: { "id": 0x1f, "name": "Ice Sweep", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A34,": { ""id"": ",A34,", ""name"": """,B34,""", ""category"": """,C34,""", ""isBasic"": ",D34," },")</f>
+        <v>0x1f: { "id": 0x1f, "name": "Ice Sweep", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E35" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A35,": { ""id"": ",A35,", ""name"": """,B35,""", ""category"": """,C35,""" },")</f>
-        <v>0x20: { "id": 0x20, "name": "Spark Sweep", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A35,": { ""id"": ",A35,", ""name"": """,B35,""", ""category"": """,C35,""", ""isBasic"": ",D35," },")</f>
+        <v>0x20: { "id": 0x20, "name": "Spark Sweep", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>241</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E36" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A36,": { ""id"": ",A36,", ""name"": """,B36,""", ""category"": """,C36,""" },")</f>
-        <v>0x21: { "id": 0x21, "name": "Wind Sweep", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A36,": { ""id"": ",A36,", ""name"": """,B36,""", ""category"": """,C36,""", ""isBasic"": ",D36," },")</f>
+        <v>0x21: { "id": 0x21, "name": "Wind Sweep", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E37" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A37,": { ""id"": ",A37,", ""name"": """,B37,""", ""category"": """,C37,""" },")</f>
-        <v>0x22: { "id": 0x22, "name": "Heat Storm", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A37,": { ""id"": ",A37,", ""name"": """,B37,""", ""category"": """,C37,""", ""isBasic"": ",D37," },")</f>
+        <v>0x22: { "id": 0x22, "name": "Heat Storm", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E38" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A38,": { ""id"": ",A38,", ""name"": """,B38,""", ""category"": """,C38,""" },")</f>
-        <v>0x23: { "id": 0x23, "name": "Ice Storm", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A38,": { ""id"": ",A38,", ""name"": """,B38,""", ""category"": """,C38,""", ""isBasic"": ",D38," },")</f>
+        <v>0x23: { "id": 0x23, "name": "Ice Storm", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E39" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A39,": { ""id"": ",A39,", ""name"": """,B39,""", ""category"": """,C39,""" },")</f>
-        <v>0x24: { "id": 0x24, "name": "Spark Storm", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A39,": { ""id"": ",A39,", ""name"": """,B39,""", ""category"": """,C39,""", ""isBasic"": ",D39," },")</f>
+        <v>0x24: { "id": 0x24, "name": "Spark Storm", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E40" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A40,": { ""id"": ",A40,", ""name"": """,B40,""", ""category"": """,C40,""" },")</f>
-        <v>0x25: { "id": 0x25, "name": "Wind Storm", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A40,": { ""id"": ",A40,", ""name"": """,B40,""", ""category"": """,C40,""", ""isBasic"": ",D40," },")</f>
+        <v>0x25: { "id": 0x25, "name": "Wind Storm", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E41" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A41,": { ""id"": ",A41,", ""name"": """,B41,""", ""category"": """,C41,""" },")</f>
-        <v>0x26: { "id": 0x26, "name": "Fire Slam", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A41,": { ""id"": ",A41,", ""name"": """,B41,""", ""category"": """,C41,""", ""isBasic"": ",D41," },")</f>
+        <v>0x26: { "id": 0x26, "name": "Fire Slam", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E42" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A42,": { ""id"": ",A42,", ""name"": """,B42,""", ""category"": """,C42,""" },")</f>
-        <v>0x27: { "id": 0x27, "name": "Blizzard Slam", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A42,": { ""id"": ",A42,", ""name"": """,B42,""", ""category"": """,C42,""", ""isBasic"": ",D42," },")</f>
+        <v>0x27: { "id": 0x27, "name": "Blizzard Slam", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E43" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A43,": { ""id"": ",A43,", ""name"": """,B43,""", ""category"": """,C43,""" },")</f>
-        <v>0x28: { "id": 0x28, "name": "Thunder Slam", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A43,": { ""id"": ",A43,", ""name"": """,B43,""", ""category"": """,C43,""", ""isBasic"": ",D43," },")</f>
+        <v>0x28: { "id": 0x28, "name": "Thunder Slam", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E44" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A44,": { ""id"": ",A44,", ""name"": """,B44,""", ""category"": """,C44,""" },")</f>
-        <v>0x29: { "id": 0x29, "name": "Aero Slam", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A44,": { ""id"": ",A44,", ""name"": """,B44,""", ""category"": """,C44,""", ""isBasic"": ",D44," },")</f>
+        <v>0x29: { "id": 0x29, "name": "Aero Slam", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E45" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A45,": { ""id"": ",A45,", ""name"": """,B45,""", ""category"": """,C45,""" },")</f>
-        <v>0x2a: { "id": 0x2a, "name": "Heat Dive", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A45,": { ""id"": ",A45,", ""name"": """,B45,""", ""category"": """,C45,""", ""isBasic"": ",D45," },")</f>
+        <v>0x2a: { "id": 0x2a, "name": "Heat Dive", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E46" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A46,": { ""id"": ",A46,", ""name"": """,B46,""", ""category"": """,C46,""" },")</f>
-        <v>0x2b: { "id": 0x2b, "name": "Ice Dive", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A46,": { ""id"": ",A46,", ""name"": """,B46,""", ""category"": """,C46,""", ""isBasic"": ",D46," },")</f>
+        <v>0x2b: { "id": 0x2b, "name": "Ice Dive", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E47" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A47,": { ""id"": ",A47,", ""name"": """,B47,""", ""category"": """,C47,""" },")</f>
-        <v>0x2c: { "id": 0x2c, "name": "Spark Dive", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A47,": { ""id"": ",A47,", ""name"": """,B47,""", ""category"": """,C47,""", ""isBasic"": ",D47," },")</f>
+        <v>0x2c: { "id": 0x2c, "name": "Spark Dive", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E48" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A48,": { ""id"": ",A48,", ""name"": """,B48,""", ""category"": """,C48,""" },")</f>
-        <v>0x2d: { "id": 0x2d, "name": "Wind Dive", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A48,": { ""id"": ",A48,", ""name"": """,B48,""", ""category"": """,C48,""", ""isBasic"": ",D48," },")</f>
+        <v>0x2d: { "id": 0x2d, "name": "Wind Dive", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E49" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A49,": { ""id"": ",A49,", ""name"": """,B49,""", ""category"": """,C49,""" },")</f>
-        <v>0x2e: { "id": 0x2e, "name": "Stun Impact", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A49,": { ""id"": ",A49,", ""name"": """,B49,""", ""category"": """,C49,""", ""isBasic"": ",D49," },")</f>
+        <v>0x2e: { "id": 0x2e, "name": "Stun Impact", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E50" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A50,": { ""id"": ",A50,", ""name"": """,B50,""", ""category"": """,C50,""" },")</f>
-        <v>0x2f: { "id": 0x2f, "name": "Muscle Strike", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A50,": { ""id"": ",A50,", ""name"": """,B50,""", ""category"": """,C50,""", ""isBasic"": ",D50," },")</f>
+        <v>0x2f: { "id": 0x2f, "name": "Muscle Strike", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E51" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A51,": { ""id"": ",A51,", ""name"": """,B51,""", ""category"": """,C51,""" },")</f>
-        <v>0x30: { "id": 0x30, "name": "Chain Rave", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A51,": { ""id"": ",A51,", ""name"": """,B51,""", ""category"": """,C51,""", ""isBasic"": ",D51," },")</f>
+        <v>0x30: { "id": 0x30, "name": "Chain Rave", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E52" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A52,": { ""id"": ",A52,", ""name"": """,B52,""", ""category"": """,C52,""" },")</f>
-        <v>0x31: { "id": 0x31, "name": "Rising Rush", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A52,": { ""id"": ",A52,", ""name"": """,B52,""", ""category"": """,C52,""", ""isBasic"": ",D52," },")</f>
+        <v>0x31: { "id": 0x31, "name": "Rising Rush", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E53" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A53,": { ""id"": ",A53,", ""name"": """,B53,""", ""category"": """,C53,""" },")</f>
-        <v>0x32: { "id": 0x32, "name": "Zantetsuken", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A53,": { ""id"": ",A53,", ""name"": """,B53,""", ""category"": """,C53,""", ""isBasic"": ",D53," },")</f>
+        <v>0x32: { "id": 0x32, "name": "Zantetsuken", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E54" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A54,": { ""id"": ",A54,", ""name"": """,B54,""", ""category"": """,C54,""" },")</f>
-        <v>0x33: { "id": 0x33, "name": "Eruption", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A54,": { ""id"": ",A54,", ""name"": """,B54,""", ""category"": """,C54,""", ""isBasic"": ",D54," },")</f>
+        <v>0x33: { "id": 0x33, "name": "Eruption", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E55" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A55,": { ""id"": ",A55,", ""name"": """,B55,""", ""category"": """,C55,""" },")</f>
-        <v>0x34: { "id": 0x34, "name": "Gravity Drop", "category": "Melee" },</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A55,": { ""id"": ",A55,", ""name"": """,B55,""", ""category"": """,C55,""", ""isBasic"": ",D55," },")</f>
+        <v>0x34: { "id": 0x34, "name": "Gravity Drop", "category": "Melee", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E56" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A56,": { ""id"": ",A56,", ""name"": """,B56,""", ""category"": """,C56,""" },")</f>
-        <v>0x35: { "id": 0x35, "name": "Shock Fall", "category": "Melee" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A56,": { ""id"": ",A56,", ""name"": """,B56,""", ""category"": """,C56,""", ""isBasic"": ",D56," },")</f>
+        <v>0x35: { "id": 0x35, "name": "Shock Fall", "category": "Melee", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E57" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A57,": { ""id"": ",A57,", ""name"": """,B57,""", ""category"": """,C57,""" },")</f>
-        <v>0x36: { "id": 0x36, "name": "Judgment Triad", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A57,": { ""id"": ",A57,", ""name"": """,B57,""", ""category"": """,C57,""", ""isBasic"": ",D57," },")</f>
+        <v>0x36: { "id": 0x36, "name": "Judgment Triad", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E58" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A58,": { ""id"": ",A58,", ""name"": """,B58,""", ""category"": """,C58,""" },")</f>
-        <v>0x37: { "id": 0x37, "name": "Fire", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A58,": { ""id"": ",A58,", ""name"": """,B58,""", ""category"": """,C58,""", ""isBasic"": ",D58," },")</f>
+        <v>0x37: { "id": 0x37, "name": "Fire", "category": "Ranged", "isBasic": 1 },</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E59" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A59,": { ""id"": ",A59,", ""name"": """,B59,""", ""category"": """,C59,""" },")</f>
-        <v>0x38: { "id": 0x38, "name": "Fira", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A59,": { ""id"": ",A59,", ""name"": """,B59,""", ""category"": """,C59,""", ""isBasic"": ",D59," },")</f>
+        <v>0x38: { "id": 0x38, "name": "Fira", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E60" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A60,": { ""id"": ",A60,", ""name"": """,B60,""", ""category"": """,C60,""" },")</f>
-        <v>0x39: { "id": 0x39, "name": "Firaga", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A60,": { ""id"": ",A60,", ""name"": """,B60,""", ""category"": """,C60,""", ""isBasic"": ",D60," },")</f>
+        <v>0x39: { "id": 0x39, "name": "Firaga", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E61" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A61,": { ""id"": ",A61,", ""name"": """,B61,""", ""category"": """,C61,""" },")</f>
-        <v>0x3a: { "id": 0x3a, "name": "Blizzard", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A61,": { ""id"": ",A61,", ""name"": """,B61,""", ""category"": """,C61,""", ""isBasic"": ",D61," },")</f>
+        <v>0x3a: { "id": 0x3a, "name": "Blizzard", "category": "Ranged", "isBasic": 1 },</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E62" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A62,": { ""id"": ",A62,", ""name"": """,B62,""", ""category"": """,C62,""" },")</f>
-        <v>0x3b: { "id": 0x3b, "name": "Blizzara", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A62,": { ""id"": ",A62,", ""name"": """,B62,""", ""category"": """,C62,""", ""isBasic"": ",D62," },")</f>
+        <v>0x3b: { "id": 0x3b, "name": "Blizzara", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E63" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A63,": { ""id"": ",A63,", ""name"": """,B63,""", ""category"": """,C63,""" },")</f>
-        <v>0x3c: { "id": 0x3c, "name": "Blizzaga", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A63,": { ""id"": ",A63,", ""name"": """,B63,""", ""category"": """,C63,""", ""isBasic"": ",D63," },")</f>
+        <v>0x3c: { "id": 0x3c, "name": "Blizzaga", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E64" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A64,": { ""id"": ",A64,", ""name"": """,B64,""", ""category"": """,C64,""" },")</f>
-        <v>0x3d: { "id": 0x3d, "name": "Thunder", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A64,": { ""id"": ",A64,", ""name"": """,B64,""", ""category"": """,C64,""", ""isBasic"": ",D64," },")</f>
+        <v>0x3d: { "id": 0x3d, "name": "Thunder", "category": "Ranged", "isBasic": 1 },</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E65" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A65,": { ""id"": ",A65,", ""name"": """,B65,""", ""category"": """,C65,""" },")</f>
-        <v>0x3e: { "id": 0x3e, "name": "Thundara", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A65,": { ""id"": ",A65,", ""name"": """,B65,""", ""category"": """,C65,""", ""isBasic"": ",D65," },")</f>
+        <v>0x3e: { "id": 0x3e, "name": "Thundara", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E66" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A66,": { ""id"": ",A66,", ""name"": """,B66,""", ""category"": """,C66,""" },")</f>
-        <v>0x3f: { "id": 0x3f, "name": "Thundaga", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A66,": { ""id"": ",A66,", ""name"": """,B66,""", ""category"": """,C66,""", ""isBasic"": ",D66," },")</f>
+        <v>0x3f: { "id": 0x3f, "name": "Thundaga", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E67" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A67,": { ""id"": ",A67,", ""name"": """,B67,""", ""category"": """,C67,""" },")</f>
-        <v>0x40: { "id": 0x40, "name": "Aero", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A67,": { ""id"": ",A67,", ""name"": """,B67,""", ""category"": """,C67,""", ""isBasic"": ",D67," },")</f>
+        <v>0x40: { "id": 0x40, "name": "Aero", "category": "Ranged", "isBasic": 1 },</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E68" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A68,": { ""id"": ",A68,", ""name"": """,B68,""", ""category"": """,C68,""" },")</f>
-        <v>0x41: { "id": 0x41, "name": "Aerora", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A68,": { ""id"": ",A68,", ""name"": """,B68,""", ""category"": """,C68,""", ""isBasic"": ",D68," },")</f>
+        <v>0x41: { "id": 0x41, "name": "Aerora", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E69" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A69,": { ""id"": ",A69,", ""name"": """,B69,""", ""category"": """,C69,""" },")</f>
-        <v>0x42: { "id": 0x42, "name": "Aeroga", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A69,": { ""id"": ",A69,", ""name"": """,B69,""", ""category"": """,C69,""", ""isBasic"": ",D69," },")</f>
+        <v>0x42: { "id": 0x42, "name": "Aeroga", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E70" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A70,": { ""id"": ",A70,", ""name"": """,B70,""", ""category"": """,C70,""" },")</f>
-        <v>0x43: { "id": 0x43, "name": "Magnet", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A70,": { ""id"": ",A70,", ""name"": """,B70,""", ""category"": """,C70,""", ""isBasic"": ",D70," },")</f>
+        <v>0x43: { "id": 0x43, "name": "Magnet", "category": "Ranged", "isBasic": 1 },</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E71" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A71,": { ""id"": ",A71,", ""name"": """,B71,""", ""category"": """,C71,""" },")</f>
-        <v>0x44: { "id": 0x44, "name": "Magnera", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A71,": { ""id"": ",A71,", ""name"": """,B71,""", ""category"": """,C71,""", ""isBasic"": ",D71," },")</f>
+        <v>0x44: { "id": 0x44, "name": "Magnera", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E72" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A72,": { ""id"": ",A72,", ""name"": """,B72,""", ""category"": """,C72,""" },")</f>
-        <v>0x45: { "id": 0x45, "name": "Magnega", "category": "Ranged" },</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A72,": { ""id"": ",A72,", ""name"": """,B72,""", ""category"": """,C72,""", ""isBasic"": ",D72," },")</f>
+        <v>0x45: { "id": 0x45, "name": "Magnega", "category": "Ranged", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E73" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A73,": { ""id"": ",A73,", ""name"": """,B73,""", ""category"": """,C73,""" },")</f>
-        <v>0x46: { "id": 0x46, "name": "Cure", "category": "Curative" },</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A73,": { ""id"": ",A73,", ""name"": """,B73,""", ""category"": """,C73,""", ""isBasic"": ",D73," },")</f>
+        <v>0x46: { "id": 0x46, "name": "Cure", "category": "Curative", "isBasic": 1 },</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B74" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="C74" s="0" t="s">
         <v>465</v>
       </c>
-      <c r="C74" s="0" t="s">
-        <v>463</v>
-      </c>
       <c r="D74" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E74" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A74,": { ""id"": ",A74,", ""name"": """,B74,""", ""category"": """,C74,""" },")</f>
-        <v>0x47: { "id": 0x47, "name": "Cura", "category": "Curative" },</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A74,": { ""id"": ",A74,", ""name"": """,B74,""", ""category"": """,C74,""", ""isBasic"": ",D74," },")</f>
+        <v>0x47: { "id": 0x47, "name": "Cura", "category": "Curative", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E75" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A75,": { ""id"": ",A75,", ""name"": """,B75,""", ""category"": """,C75,""" },")</f>
-        <v>0x48: { "id": 0x48, "name": "Curaga", "category": "Curative" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A75,": { ""id"": ",A75,", ""name"": """,B75,""", ""category"": """,C75,""", ""isBasic"": ",D75," },")</f>
+        <v>0x48: { "id": 0x48, "name": "Curaga", "category": "Curative", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E76" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A76,": { ""id"": ",A76,", ""name"": """,B76,""", ""category"": """,C76,""" },")</f>
-        <v>0x49: { "id": 0x49, "name": "Slow", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A76,": { ""id"": ",A76,", ""name"": """,B76,""", ""category"": """,C76,""", ""isBasic"": ",D76," },")</f>
+        <v>0x49: { "id": 0x49, "name": "Slow", "category": "Ranged", "isBasic": 1 },</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E77" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A77,": { ""id"": ",A77,", ""name"": """,B77,""", ""category"": """,C77,""" },")</f>
-        <v>0x4a: { "id": 0x4a, "name": "Stop", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A77,": { ""id"": ",A77,", ""name"": """,B77,""", ""category"": """,C77,""", ""isBasic"": ",D77," },")</f>
+        <v>0x4a: { "id": 0x4a, "name": "Stop", "category": "Ranged", "isBasic": 1 },</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E78" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A78,": { ""id"": ",A78,", ""name"": """,B78,""", ""category"": """,C78,""" },")</f>
-        <v>0x4b: { "id": 0x4b, "name": "Confuse", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A78,": { ""id"": ",A78,", ""name"": """,B78,""", ""category"": """,C78,""", ""isBasic"": ",D78," },")</f>
+        <v>0x4b: { "id": 0x4b, "name": "Confuse", "category": "Ranged", "isBasic": 1 },</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D79" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E79" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A79,": { ""id"": ",A79,", ""name"": """,B79,""", ""category"": """,C79,""" },")</f>
-        <v>0x4c: { "id": 0x4c, "name": "Firaga Burst", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A79,": { ""id"": ",A79,", ""name"": """,B79,""", ""category"": """,C79,""", ""isBasic"": ",D79," },")</f>
+        <v>0x4c: { "id": 0x4c, "name": "Firaga Burst", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D80" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E80" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A80,": { ""id"": ",A80,", ""name"": """,B80,""", ""category"": """,C80,""" },")</f>
-        <v>0x4d: { "id": 0x4d, "name": "Triple Firaga", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A80,": { ""id"": ",A80,", ""name"": """,B80,""", ""category"": """,C80,""", ""isBasic"": ",D80," },")</f>
+        <v>0x4d: { "id": 0x4d, "name": "Triple Firaga", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E81" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A81,": { ""id"": ",A81,", ""name"": """,B81,""", ""category"": """,C81,""" },")</f>
-        <v>0x4e: { "id": 0x4e, "name": "Triple Burst", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A81,": { ""id"": ",A81,", ""name"": """,B81,""", ""category"": """,C81,""", ""isBasic"": ",D81," },")</f>
+        <v>0x4e: { "id": 0x4e, "name": "Triple Burst", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E82" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A82,": { ""id"": ",A82,", ""name"": """,B82,""", ""category"": """,C82,""" },")</f>
-        <v>0x4f: { "id": 0x4f, "name": "Blizzaga Pursuit", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A82,": { ""id"": ",A82,", ""name"": """,B82,""", ""category"": """,C82,""", ""isBasic"": ",D82," },")</f>
+        <v>0x4f: { "id": 0x4f, "name": "Blizzaga Pursuit", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E83" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A83,": { ""id"": ",A83,", ""name"": """,B83,""", ""category"": """,C83,""" },")</f>
-        <v>0x50: { "id": 0x50, "name": "Triple Blizzaga", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A83,": { ""id"": ",A83,", ""name"": """,B83,""", ""category"": """,C83,""", ""isBasic"": ",D83," },")</f>
+        <v>0x50: { "id": 0x50, "name": "Triple Blizzaga", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E84" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A84,": { ""id"": ",A84,", ""name"": """,B84,""", ""category"": """,C84,""" },")</f>
-        <v>0x51: { "id": 0x51, "name": "Triple Pursuit", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A84,": { ""id"": ",A84,", ""name"": """,B84,""", ""category"": """,C84,""", ""isBasic"": ",D84," },")</f>
+        <v>0x51: { "id": 0x51, "name": "Triple Pursuit", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E85" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A85,": { ""id"": ",A85,", ""name"": """,B85,""", ""category"": """,C85,""" },")</f>
-        <v>0x52: { "id": 0x52, "name": "Thunder Tracer", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A85,": { ""id"": ",A85,", ""name"": """,B85,""", ""category"": """,C85,""", ""isBasic"": ",D85," },")</f>
+        <v>0x52: { "id": 0x52, "name": "Thunder Tracer", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D86" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E86" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A86,": { ""id"": ",A86,", ""name"": """,B86,""", ""category"": """,C86,""" },")</f>
-        <v>0x53: { "id": 0x53, "name": "Pulse Tracer", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A86,": { ""id"": ",A86,", ""name"": """,B86,""", ""category"": """,C86,""", ""isBasic"": ",D86," },")</f>
+        <v>0x53: { "id": 0x53, "name": "Pulse Tracer", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D87" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E87" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A87,": { ""id"": ",A87,", ""name"": """,B87,""", ""category"": """,C87,""" },")</f>
-        <v>0x54: { "id": 0x54, "name": "Tornado Tracer", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A87,": { ""id"": ",A87,", ""name"": """,B87,""", ""category"": """,C87,""", ""isBasic"": ",D87," },")</f>
+        <v>0x54: { "id": 0x54, "name": "Tornado Tracer", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D88" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E88" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A88,": { ""id"": ",A88,", ""name"": """,B88,""", ""category"": """,C88,""" },")</f>
-        <v>0x55: { "id": 0x55, "name": "Wind Tracer", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A88,": { ""id"": ",A88,", ""name"": """,B88,""", ""category"": """,C88,""", ""isBasic"": ",D88," },")</f>
+        <v>0x55: { "id": 0x55, "name": "Wind Tracer", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E89" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A89,": { ""id"": ",A89,", ""name"": """,B89,""", ""category"": """,C89,""" },")</f>
-        <v>0x56: { "id": 0x56, "name": "Magnet Grab", "category": "Ranged" },</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">_xlfn.CONCAT( ,A89,": { ""id"": ",A89,", ""name"": """,B89,""", ""category"": """,C89,""", ""isBasic"": ",D89," },")</f>
+        <v>0x56: { "id": 0x56, "name": "Magnet Grab", "category": "Ranged", "isBasic": 0 },</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E90" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A90,": { ""id"": ",A90,", ""name"": """,B90,""", ""category"": """,C90,""" },")</f>
-        <v>0x57: { "id": 0x57, "name": "Esuna", "category": "Curative" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A90,": { ""id"": ",A90,", ""name"": """,B90,""", ""category"": """,C90,""", ""isBasic"": ",D90," },")</f>
+        <v>0x57: { "id": 0x57, "name": "Esuna", "category": "Curative", "isBasic": 1 },</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D91" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E91" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A91,": { ""id"": ",A91,", ""name"": """,B91,""", ""category"": """,C91,""" },")</f>
-        <v>0x58: { "id": 0x58, "name": "Flame Fall", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A91,": { ""id"": ",A91,", ""name"": """,B91,""", ""category"": """,C91,""", ""isBasic"": ",D91," },")</f>
+        <v>0x58: { "id": 0x58, "name": "Flame Fall", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D92" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E92" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A92,": { ""id"": ",A92,", ""name"": """,B92,""", ""category"": """,C92,""" },")</f>
-        <v>0x59: { "id": 0x59, "name": "Icicle Mine", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A92,": { ""id"": ",A92,", ""name"": """,B92,""", ""category"": """,C92,""", ""isBasic"": ",D92," },")</f>
+        <v>0x59: { "id": 0x59, "name": "Icicle Mine", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D93" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E93" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A93,": { ""id"": ",A93,", ""name"": """,B93,""", ""category"": """,C93,""" },")</f>
-        <v>0x5a: { "id": 0x5a, "name": "Exo Spark", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A93,": { ""id"": ",A93,", ""name"": """,B93,""", ""category"": """,C93,""", ""isBasic"": ",D93," },")</f>
+        <v>0x5a: { "id": 0x5a, "name": "Exo Spark", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D94" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E94" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A94,": { ""id"": ",A94,", ""name"": """,B94,""", ""category"": """,C94,""" },")</f>
-        <v>0x5b: { "id": 0x5b, "name": "Cyclone", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A94,": { ""id"": ",A94,", ""name"": """,B94,""", ""category"": """,C94,""", ""isBasic"": ",D94," },")</f>
+        <v>0x5b: { "id": 0x5b, "name": "Cyclone", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D95" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E95" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT( ,A95,": { ""id"": ",A95,", ""name"": """,B95,""", ""category"": """,C95,""" },")</f>
-        <v>0x5c: { "id": 0x5c, "name": "Quake", "category": "Ranged" },</v>
+        <f aca="false">_xlfn.CONCAT( ,A95,": { ""id"": ",A95,", ""name"": """,B95,""", ""category"": """,C95,""", ""isBasic"": ",D95," },")</f>
+        <v>0x5c: { "id": 0x5c, "name": "Quake", "category": "Ranged", "isBasic": 0 },</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C95"/>
+  <autoFilter ref="A1:D95">
+    <filterColumn colId="2">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Ranged"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -15034,11 +15072,11 @@
   </sheetPr>
   <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="14.77"/>
@@ -15047,16 +15085,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>135</v>
@@ -15067,13 +15105,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="E2" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A2,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B2, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C2, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D2, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15085,13 +15123,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E3" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A3,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B3, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C3, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D3, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15103,13 +15141,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E4" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A4,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B4, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C4, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D4, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15121,13 +15159,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E5" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A5,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B5, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C5, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D5, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15139,13 +15177,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E6" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A6,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B6, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C6, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D6, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15157,13 +15195,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>467</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>465</v>
       </c>
       <c r="E7" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A7,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B7, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C7, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D7, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15175,13 +15213,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>467</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>473</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>465</v>
       </c>
       <c r="E8" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A8,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B8, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C8, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D8, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15193,13 +15231,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>467</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>497</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>465</v>
       </c>
       <c r="E9" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A9,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B9, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C9, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D9, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15211,13 +15249,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E10" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A10,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B10, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C10, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D10, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15229,13 +15267,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="E11" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A11,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B11, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C11, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D11, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15247,13 +15285,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E12" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A12,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B12, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C12, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D12, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15265,13 +15303,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E13" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A13,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B13, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C13, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D13, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15283,13 +15321,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E14" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A14,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B14, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C14, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D14, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15301,13 +15339,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E15" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A15,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B15, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C15, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D15, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15319,13 +15357,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>372</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>370</v>
       </c>
       <c r="E16" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A16,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B16, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C16, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D16, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15337,13 +15375,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E17" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A17,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B17, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C17, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D17, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15355,13 +15393,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E18" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A18,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B18, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C18, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D18, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15373,13 +15411,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E19" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A19,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B19, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C19, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D19, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15391,13 +15429,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>334</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>332</v>
       </c>
       <c r="E20" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A20,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B20, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C20, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D20, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15409,13 +15447,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>374</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>372</v>
       </c>
       <c r="E21" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A21,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B21, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C21, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D21, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15427,13 +15465,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E22" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A22,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B22, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C22, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D22, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15445,13 +15483,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E23" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A23,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B23, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C23, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D23, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15463,13 +15501,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E24" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A24,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B24, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C24, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D24, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15481,13 +15519,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E25" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A25,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B25, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C25, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D25, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15499,13 +15537,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E26" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A26,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B26, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C26, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D26, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15517,13 +15555,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>376</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>361</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>374</v>
       </c>
       <c r="E27" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A27,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B27, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C27, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D27, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15535,13 +15573,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E28" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A28,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B28, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C28, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D28, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15553,13 +15591,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E29" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A29,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B29, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C29, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D29, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15571,13 +15609,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="E30" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A30,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B30, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C30, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D30, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15589,13 +15627,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E31" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A31,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B31, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C31, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D31, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15607,13 +15645,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>434</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>432</v>
-      </c>
       <c r="D32" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E32" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A32,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B32, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C32, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D32, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15625,13 +15663,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>434</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>432</v>
-      </c>
       <c r="D33" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E33" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A33,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B33, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C33, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D33, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15643,13 +15681,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="C34" s="0" t="s">
         <v>434</v>
       </c>
-      <c r="C34" s="0" t="s">
-        <v>432</v>
-      </c>
       <c r="D34" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="E34" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A34,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B34, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C34, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D34, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15661,13 +15699,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E35" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A35,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B35, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C35, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D35, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15679,13 +15717,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E36" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A36,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B36, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C36, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D36, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15697,13 +15735,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E37" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A37,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B37, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C37, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D37, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15715,13 +15753,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="E38" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A38,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B38, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C38, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D38, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15733,13 +15771,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="C39" s="0" t="s">
         <v>436</v>
       </c>
-      <c r="C39" s="0" t="s">
-        <v>434</v>
-      </c>
       <c r="D39" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="E39" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A39,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B39, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C39, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D39, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15751,13 +15789,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="E40" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A40,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B40, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C40, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D40, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15769,13 +15807,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="E41" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A41,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B41, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C41, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D41, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15787,13 +15825,13 @@
         <v>40</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E42" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A42,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B42, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C42, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D42, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15805,13 +15843,13 @@
         <v>41</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>440</v>
       </c>
-      <c r="C43" s="0" t="s">
-        <v>438</v>
-      </c>
       <c r="D43" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E43" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A43,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B43, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C43, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D43, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15823,13 +15861,13 @@
         <v>42</v>
       </c>
       <c r="B44" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="C44" s="0" t="s">
         <v>440</v>
       </c>
-      <c r="C44" s="0" t="s">
-        <v>438</v>
-      </c>
       <c r="D44" s="0" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="E44" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A44,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B44, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C44, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D44, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15841,13 +15879,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="C45" s="0" t="s">
         <v>440</v>
       </c>
-      <c r="C45" s="0" t="s">
-        <v>438</v>
-      </c>
       <c r="D45" s="0" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A45,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B45, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C45, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D45, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15859,13 +15897,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>440</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>438</v>
-      </c>
       <c r="D46" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E46" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A46,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B46, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C46, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D46, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15877,13 +15915,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="C47" s="0" t="s">
         <v>440</v>
       </c>
-      <c r="C47" s="0" t="s">
-        <v>438</v>
-      </c>
       <c r="D47" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="E47" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A47,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B47, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C47, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D47, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15895,13 +15933,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E48" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A48,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B48, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C48, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D48, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15913,13 +15951,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E49" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A49,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B49, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C49, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D49, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15931,13 +15969,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E50" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A50,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B50, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C50, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D50, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15949,13 +15987,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E51" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A51,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B51, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C51, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D51, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15967,13 +16005,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E52" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A52,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B52, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C52, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D52, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15985,13 +16023,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D53" s="0" t="s">
         <v>442</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>408</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>440</v>
       </c>
       <c r="E53" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A53,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B53, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C53, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D53, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16003,13 +16041,13 @@
         <v>52</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E54" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A54,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B54, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C54, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D54, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16021,13 +16059,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E55" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A55,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B55, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C55, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D55, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16039,13 +16077,13 @@
         <v>54</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="E56" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A56,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B56, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C56, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D56, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16057,13 +16095,13 @@
         <v>55</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E57" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A57,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B57, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C57, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D57, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16075,13 +16113,13 @@
         <v>56</v>
       </c>
       <c r="B58" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="C58" s="0" t="s">
         <v>446</v>
       </c>
-      <c r="C58" s="0" t="s">
-        <v>444</v>
-      </c>
       <c r="D58" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E58" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A58,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B58, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C58, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D58, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16093,13 +16131,13 @@
         <v>57</v>
       </c>
       <c r="B59" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="C59" s="0" t="s">
         <v>446</v>
       </c>
-      <c r="C59" s="0" t="s">
-        <v>444</v>
-      </c>
       <c r="D59" s="0" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="E59" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A59,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B59, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C59, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D59, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16111,13 +16149,13 @@
         <v>58</v>
       </c>
       <c r="B60" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="C60" s="0" t="s">
         <v>446</v>
       </c>
-      <c r="C60" s="0" t="s">
-        <v>444</v>
-      </c>
       <c r="D60" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E60" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A60,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B60, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C60, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D60, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16129,13 +16167,13 @@
         <v>59</v>
       </c>
       <c r="B61" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="C61" s="0" t="s">
         <v>446</v>
       </c>
-      <c r="C61" s="0" t="s">
-        <v>444</v>
-      </c>
       <c r="D61" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="E61" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A61,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B61, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C61, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D61, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16147,13 +16185,13 @@
         <v>60</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E62" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A62,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B62, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C62, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D62, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16165,13 +16203,13 @@
         <v>61</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E63" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A63,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B63, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C63, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D63, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16183,13 +16221,13 @@
         <v>62</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E64" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A64,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B64, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C64, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D64, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16201,13 +16239,13 @@
         <v>63</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="E65" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A65,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B65, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C65, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D65, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16219,13 +16257,13 @@
         <v>64</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="E66" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A66,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B66, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C66, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D66, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16237,13 +16275,13 @@
         <v>65</v>
       </c>
       <c r="B67" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="C67" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="C67" s="0" t="s">
-        <v>446</v>
-      </c>
       <c r="D67" s="0" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E67" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A67,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B67, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C67, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D67, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16255,13 +16293,13 @@
         <v>66</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E68" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A68,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B68, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C68, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D68, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16273,13 +16311,13 @@
         <v>67</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E69" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A69,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B69, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C69, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D69, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16291,13 +16329,13 @@
         <v>68</v>
       </c>
       <c r="B70" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="C70" s="0" t="s">
         <v>452</v>
       </c>
-      <c r="C70" s="0" t="s">
-        <v>450</v>
-      </c>
       <c r="D70" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E70" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A70,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B70, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C70, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D70, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16309,13 +16347,13 @@
         <v>69</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E71" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A71,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B71, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C71, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D71, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16327,13 +16365,13 @@
         <v>70</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E72" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A72,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B72, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C72, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D72, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16345,13 +16383,13 @@
         <v>71</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E73" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A73,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B73, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C73, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D73, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16363,13 +16401,13 @@
         <v>72</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E74" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A74,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B74, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C74, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D74, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16381,13 +16419,13 @@
         <v>73</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="E75" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A75,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B75, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C75, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D75, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16399,13 +16437,13 @@
         <v>74</v>
       </c>
       <c r="B76" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="C76" s="0" t="s">
         <v>454</v>
       </c>
-      <c r="C76" s="0" t="s">
-        <v>452</v>
-      </c>
       <c r="D76" s="0" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="E76" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A76,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B76, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C76, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D76, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16417,13 +16455,13 @@
         <v>75</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="E77" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A77,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B77, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C77, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D77, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16435,13 +16473,13 @@
         <v>76</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="E78" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A78,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B78, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C78, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D78, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16453,13 +16491,13 @@
         <v>77</v>
       </c>
       <c r="B79" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="D79" s="0" t="s">
         <v>458</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="D79" s="0" t="s">
-        <v>456</v>
       </c>
       <c r="E79" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A79,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B79, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C79, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D79, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16471,13 +16509,13 @@
         <v>78</v>
       </c>
       <c r="B80" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="D80" s="0" t="s">
         <v>458</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>462</v>
-      </c>
-      <c r="D80" s="0" t="s">
-        <v>456</v>
       </c>
       <c r="E80" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A80,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B80, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C80, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D80, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16489,13 +16527,13 @@
         <v>79</v>
       </c>
       <c r="B81" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="D81" s="0" t="s">
         <v>458</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>469</v>
-      </c>
-      <c r="D81" s="0" t="s">
-        <v>456</v>
       </c>
       <c r="E81" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A81,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B81, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C81, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D81, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16507,13 +16545,13 @@
         <v>80</v>
       </c>
       <c r="B82" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="D82" s="0" t="s">
         <v>458</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>471</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>456</v>
       </c>
       <c r="E82" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A82,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B82, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C82, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D82, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16525,13 +16563,13 @@
         <v>81</v>
       </c>
       <c r="B83" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="D83" s="0" t="s">
         <v>460</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>458</v>
       </c>
       <c r="E83" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A83,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B83, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C83, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D83, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16543,13 +16581,13 @@
         <v>82</v>
       </c>
       <c r="B84" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D84" s="0" t="s">
         <v>460</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>473</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>458</v>
       </c>
       <c r="E84" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A84,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B84, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C84, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D84, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16561,13 +16599,13 @@
         <v>83</v>
       </c>
       <c r="B85" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="D85" s="0" t="s">
         <v>460</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>497</v>
-      </c>
-      <c r="D85" s="0" t="s">
-        <v>458</v>
       </c>
       <c r="E85" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A85,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B85, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C85, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D85, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16579,13 +16617,13 @@
         <v>84</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E86" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A86,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B86, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C86, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D86, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16597,13 +16635,13 @@
         <v>85</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E87" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A87,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B87, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C87, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D87, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16615,13 +16653,13 @@
         <v>86</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="E88" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A88,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B88, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C88, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D88, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16633,13 +16671,13 @@
         <v>87</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="E89" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A89,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B89, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C89, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D89, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16651,13 +16689,13 @@
         <v>88</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="E90" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A90,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B90, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C90, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D90, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16669,13 +16707,13 @@
         <v>89</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="E91" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A91,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B91, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C91, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D91, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16687,13 +16725,13 @@
         <v>90</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E92" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A92,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B92, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C92, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D92, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16705,13 +16743,13 @@
         <v>91</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="E93" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A93,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B93, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C93, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D93, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16723,13 +16761,13 @@
         <v>92</v>
       </c>
       <c r="B94" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="D94" s="0" t="s">
         <v>477</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>436</v>
-      </c>
-      <c r="D94" s="0" t="s">
-        <v>475</v>
       </c>
       <c r="E94" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A94,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B94, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C94, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D94, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16741,13 +16779,13 @@
         <v>93</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E95" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A95,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B95, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C95, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D95, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16759,13 +16797,13 @@
         <v>94</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="E96" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A96,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B96, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C96, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D96, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16777,13 +16815,13 @@
         <v>95</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="E97" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A97,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B97, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C97, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D97, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16795,13 +16833,13 @@
         <v>96</v>
       </c>
       <c r="B98" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="D98" s="0" t="s">
         <v>479</v>
-      </c>
-      <c r="C98" s="0" t="s">
-        <v>434</v>
-      </c>
-      <c r="D98" s="0" t="s">
-        <v>477</v>
       </c>
       <c r="E98" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A98,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B98, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C98, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D98, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16813,13 +16851,13 @@
         <v>97</v>
       </c>
       <c r="B99" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="D99" s="0" t="s">
         <v>479</v>
-      </c>
-      <c r="C99" s="0" t="s">
-        <v>436</v>
-      </c>
-      <c r="D99" s="0" t="s">
-        <v>477</v>
       </c>
       <c r="E99" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A99,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B99, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C99, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D99, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16831,13 +16869,13 @@
         <v>98</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E100" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A100,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B100, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C100, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D100, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16849,13 +16887,13 @@
         <v>99</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C101" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="D101" s="0" t="s">
         <v>416</v>
-      </c>
-      <c r="D101" s="0" t="s">
-        <v>414</v>
       </c>
       <c r="E101" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A101,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B101, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C101, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D101, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16867,13 +16905,13 @@
         <v>100</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E102" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A102,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B102, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C102, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D102, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16885,13 +16923,13 @@
         <v>101</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E103" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A103,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B103, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C103, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D103, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16903,13 +16941,13 @@
         <v>102</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="E104" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A104,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B104, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C104, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D104, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16921,13 +16959,13 @@
         <v>103</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="E105" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A105,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B105, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C105, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D105, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16939,13 +16977,13 @@
         <v>104</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E106" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A106,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B106, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C106, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D106, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16957,13 +16995,13 @@
         <v>105</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E107" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A107,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B107, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C107, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D107, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16975,13 +17013,13 @@
         <v>106</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C108" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="D108" s="0" t="s">
         <v>418</v>
-      </c>
-      <c r="D108" s="0" t="s">
-        <v>416</v>
       </c>
       <c r="E108" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A108,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B108, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C108, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D108, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16993,13 +17031,13 @@
         <v>107</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="E109" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A109,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B109, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C109, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D109, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17011,13 +17049,13 @@
         <v>108</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="E110" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A110,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B110, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C110, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D110, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17029,13 +17067,13 @@
         <v>109</v>
       </c>
       <c r="B111" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="D111" s="0" t="s">
         <v>485</v>
-      </c>
-      <c r="C111" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="D111" s="0" t="s">
-        <v>483</v>
       </c>
       <c r="E111" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A111,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B111, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C111, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D111, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17047,13 +17085,13 @@
         <v>110</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="E112" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A112,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B112, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C112, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D112, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17065,13 +17103,13 @@
         <v>111</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E113" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A113,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B113, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C113, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D113, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17083,13 +17121,13 @@
         <v>112</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E114" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A114,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B114, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C114, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D114, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17101,13 +17139,13 @@
         <v>113</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="E115" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A115,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B115, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C115, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D115, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17119,13 +17157,13 @@
         <v>114</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="E116" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A116,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B116, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C116, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D116, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17137,13 +17175,13 @@
         <v>115</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="E117" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A117,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B117, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C117, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D117, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17155,13 +17193,13 @@
         <v>116</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="E118" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A118,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B118, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C118, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D118, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17173,13 +17211,13 @@
         <v>117</v>
       </c>
       <c r="B119" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="D119" s="0" t="s">
         <v>489</v>
-      </c>
-      <c r="C119" s="0" t="s">
-        <v>448</v>
-      </c>
-      <c r="D119" s="0" t="s">
-        <v>487</v>
       </c>
       <c r="E119" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A119,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B119, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C119, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D119, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17191,13 +17229,13 @@
         <v>118</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="E120" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A120,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B120, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C120, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D120, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17209,13 +17247,13 @@
         <v>119</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E121" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A121,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B121, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C121, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D121, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17227,13 +17265,13 @@
         <v>120</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="E122" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A122,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B122, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C122, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D122, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17245,13 +17283,13 @@
         <v>121</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="E123" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A123,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B123, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C123, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D123, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17263,13 +17301,13 @@
         <v>122</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E124" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A124,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B124, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C124, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D124, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17281,13 +17319,13 @@
         <v>123</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E125" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A125,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B125, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C125, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D125, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17299,13 +17337,13 @@
         <v>124</v>
       </c>
       <c r="B126" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C126" s="0" t="s">
         <v>493</v>
       </c>
-      <c r="C126" s="0" t="s">
-        <v>491</v>
-      </c>
       <c r="D126" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="E126" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A126,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B126, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C126, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D126, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17317,13 +17355,13 @@
         <v>125</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="E127" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A127,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B127, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C127, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D127, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17335,13 +17373,13 @@
         <v>126</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="E128" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A128,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B128, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C128, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D128, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17353,13 +17391,13 @@
         <v>127</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E129" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A129,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B129, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C129, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D129, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17371,13 +17409,13 @@
         <v>128</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="E130" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A130,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B130, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C130, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D130, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17389,13 +17427,13 @@
         <v>129</v>
       </c>
       <c r="B131" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="C131" s="0" t="s">
         <v>495</v>
       </c>
-      <c r="C131" s="0" t="s">
-        <v>493</v>
-      </c>
       <c r="D131" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="E131" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A131,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B131, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C131, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D131, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17407,13 +17445,13 @@
         <v>130</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="E132" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A132,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B132, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C132, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D132, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17425,13 +17463,13 @@
         <v>131</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="E133" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A133,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B133, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C133, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D133, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17443,13 +17481,13 @@
         <v>132</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="E134" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A134,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B134, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C134, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D134, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17461,13 +17499,13 @@
         <v>133</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="E135" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A135,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B135, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C135, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D135, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17479,13 +17517,13 @@
         <v>134</v>
       </c>
       <c r="B136" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="C136" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="D136" s="0" t="s">
         <v>507</v>
-      </c>
-      <c r="C136" s="0" t="s">
-        <v>422</v>
-      </c>
-      <c r="D136" s="0" t="s">
-        <v>505</v>
       </c>
       <c r="E136" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A136,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B136, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C136, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D136, Commands!B:B, 0), 1, 1)),", },")</f>

</xml_diff>

<commit_message>
Added achievements up to the end of the final boss, and removed "Twilight Triumph" due to spam
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -14,8 +14,8 @@
     <sheet name="Command Conversion Combinations" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$D$95</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$95</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$95</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$D$95</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2447" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2479" uniqueCount="527">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -999,6 +999,48 @@
   </si>
   <si>
     <t xml:space="preserve">CastleOblivionSomewhere2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CastleOblivionDestinyIslands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CastleOblivionTraverseTown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traverse Town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CastleOblivionWonderland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wonderland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CastleOblivionOlympusColiseum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olympus Coliseum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CastleOblivionAgrabah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agrabah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CastleOblivionHollowBastionObstacleCourse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hollow Bastion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CastleOblivionSorrow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Station of Sorrow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CastleOblivionHollowBastion</t>
   </si>
   <si>
     <t xml:space="preserve">Category</t>
@@ -1697,7 +1739,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -11254,16 +11296,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B97" activeCellId="0" sqref="B97"/>
+      <selection pane="topLeft" activeCell="B105" activeCellId="0" sqref="B105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13285,27 +13328,177 @@
       <c r="A97" s="0" t="n">
         <v>96</v>
       </c>
+      <c r="B97" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>146</v>
+      </c>
       <c r="F97" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A97,": { ""worldId"": ",C97,", ""name"": """,D97,""", ""display"": """,E97,""", ""areaId"": ",B97,", },")</f>
-        <v>96: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>96: { "worldId": 0x7, "name": "CastleOblivionDestinyIslands", "display": "Destiny Islands", "areaId": 0x9, },</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
         <v>97</v>
       </c>
+      <c r="B98" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>326</v>
+      </c>
       <c r="F98" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A98,": { ""worldId"": ",C98,", ""name"": """,D98,""", ""display"": """,E98,""", ""areaId"": ",B98,", },")</f>
-        <v>97: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>97: { "worldId": 0x7, "name": "CastleOblivionTraverseTown", "display": "Traverse Town", "areaId": 0x1, },</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
         <v>98</v>
       </c>
+      <c r="B99" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>328</v>
+      </c>
       <c r="F99" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A99,": { ""worldId"": ",C99,", ""name"": """,D99,""", ""display"": """,E99,""", ""areaId"": ",B99,", },")</f>
-        <v>98: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>98: { "worldId": 0x7, "name": "CastleOblivionWonderland", "display": "Wonderland", "areaId": 0x2, },</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="E100" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="F100" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A100,": { ""worldId"": ",C100,", ""name"": """,D100,""", ""display"": """,E100,""", ""areaId"": ",B100,", },")</f>
+        <v>99: { "worldId": 0x7, "name": "CastleOblivionOlympusColiseum", "display": "Olympus Coliseum", "areaId": 0x3, },</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="E101" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="F101" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A101,": { ""worldId"": ",C101,", ""name"": """,D101,""", ""display"": """,E101,""", ""areaId"": ",B101,", },")</f>
+        <v>100: { "worldId": 0x7, "name": "CastleOblivionAgrabah", "display": "Agrabah", "areaId": 0x4, },</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="E102" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="F102" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A102,": { ""worldId"": ",C102,", ""name"": """,D102,""", ""display"": """,E102,""", ""areaId"": ",B102,", },")</f>
+        <v>101: { "worldId": 0x7, "name": "CastleOblivionHollowBastionObstacleCourse", "display": "Hollow Bastion", "areaId": 0x6, },</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="E103" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="F103" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A103,": { ""worldId"": ",C103,", ""name"": """,D103,""", ""display"": """,E103,""", ""areaId"": ",B103,", },")</f>
+        <v>102: { "worldId": 0x7, "name": "CastleOblivionSorrow", "display": "Station of Sorrow", "areaId": 0x8, },</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="F104" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A104,": { ""worldId"": ",C104,", ""name"": """,D104,""", ""display"": """,E104,""", ""areaId"": ",B104,", },")</f>
+        <v>103: { "worldId": 0x7, "name": "CastleOblivionHollowBastion", "display": "Hollow Bastion", "areaId": 0x5, },</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="F105" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A105,": { ""worldId"": ",C105,", ""name"": """,D105,""", ""display"": """,E105,""", ""areaId"": ",B105,", },")</f>
+        <v>104: { "worldId": , "name": "", "display": "", "areaId": , },</v>
       </c>
     </row>
   </sheetData>
@@ -13330,7 +13523,7 @@
       <selection pane="topLeft" activeCell="C96" activeCellId="0" sqref="C96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -13345,10 +13538,10 @@
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>325</v>
+        <v>339</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>135</v>
@@ -13356,13 +13549,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>327</v>
+        <v>341</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>327</v>
+        <v>341</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -13374,13 +13567,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>328</v>
+        <v>342</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -13392,13 +13585,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>331</v>
+        <v>345</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -13410,13 +13603,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>333</v>
+        <v>347</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>334</v>
+        <v>348</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -13428,13 +13621,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>335</v>
+        <v>349</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -13446,13 +13639,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0</v>
@@ -13464,13 +13657,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>340</v>
+        <v>354</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>341</v>
+        <v>355</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -13482,13 +13675,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>342</v>
+        <v>356</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0</v>
@@ -13500,13 +13693,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>344</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>330</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -13518,13 +13711,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>346</v>
+        <v>360</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
@@ -13536,13 +13729,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>1</v>
@@ -13554,13 +13747,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>351</v>
+        <v>365</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>0</v>
@@ -13572,13 +13765,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>352</v>
+        <v>366</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>353</v>
+        <v>367</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0</v>
@@ -13590,13 +13783,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>354</v>
+        <v>368</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0</v>
@@ -13608,13 +13801,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>356</v>
+        <v>370</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0</v>
@@ -13626,13 +13819,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>358</v>
+        <v>372</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0</v>
@@ -13644,13 +13837,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>360</v>
+        <v>374</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>0</v>
@@ -13665,10 +13858,10 @@
         <v>301</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>362</v>
+        <v>376</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>0</v>
@@ -13683,10 +13876,10 @@
         <v>267</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0</v>
@@ -13701,10 +13894,10 @@
         <v>256</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0</v>
@@ -13716,13 +13909,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0</v>
@@ -13734,13 +13927,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0</v>
@@ -13752,13 +13945,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>0</v>
@@ -13770,13 +13963,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>0</v>
@@ -13788,13 +13981,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>0</v>
@@ -13806,13 +13999,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>0</v>
@@ -13824,13 +14017,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>0</v>
@@ -13842,13 +14035,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>379</v>
+        <v>393</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>380</v>
+        <v>394</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>0</v>
@@ -13860,13 +14053,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>381</v>
+        <v>395</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>382</v>
+        <v>396</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>0</v>
@@ -13878,13 +14071,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>383</v>
+        <v>397</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>384</v>
+        <v>398</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>0</v>
@@ -13899,10 +14092,10 @@
         <v>203</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>385</v>
+        <v>399</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>0</v>
@@ -13917,10 +14110,10 @@
         <v>206</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>386</v>
+        <v>400</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>0</v>
@@ -13935,10 +14128,10 @@
         <v>211</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>387</v>
+        <v>401</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>0</v>
@@ -13950,13 +14143,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>389</v>
+        <v>403</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>0</v>
@@ -13971,10 +14164,10 @@
         <v>241</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>0</v>
@@ -13986,13 +14179,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>0</v>
@@ -14004,13 +14197,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>0</v>
@@ -14022,13 +14215,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>396</v>
+        <v>410</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>0</v>
@@ -14040,13 +14233,13 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>397</v>
+        <v>411</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>398</v>
+        <v>412</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>0</v>
@@ -14058,13 +14251,13 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>399</v>
+        <v>413</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>400</v>
+        <v>414</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>0</v>
@@ -14076,13 +14269,13 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>402</v>
+        <v>416</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>0</v>
@@ -14094,13 +14287,13 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>403</v>
+        <v>417</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>404</v>
+        <v>418</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>0</v>
@@ -14112,13 +14305,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>0</v>
@@ -14130,13 +14323,13 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>407</v>
+        <v>421</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>0</v>
@@ -14148,13 +14341,13 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>409</v>
+        <v>423</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>0</v>
@@ -14166,13 +14359,13 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>411</v>
+        <v>425</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>412</v>
+        <v>426</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>0</v>
@@ -14184,13 +14377,13 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>413</v>
+        <v>427</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>414</v>
+        <v>428</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>0</v>
@@ -14202,13 +14395,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>415</v>
+        <v>429</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>416</v>
+        <v>430</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>0</v>
@@ -14220,13 +14413,13 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>417</v>
+        <v>431</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>0</v>
@@ -14238,13 +14431,13 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>419</v>
+        <v>433</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>0</v>
@@ -14256,13 +14449,13 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>421</v>
+        <v>435</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>422</v>
+        <v>436</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>0</v>
@@ -14274,13 +14467,13 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>423</v>
+        <v>437</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>424</v>
+        <v>438</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>0</v>
@@ -14292,13 +14485,13 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>425</v>
+        <v>439</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>426</v>
+        <v>440</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>0</v>
@@ -14310,13 +14503,13 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>427</v>
+        <v>441</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>428</v>
+        <v>442</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>0</v>
@@ -14328,13 +14521,13 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>429</v>
+        <v>443</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>430</v>
+        <v>444</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>0</v>
@@ -14346,13 +14539,13 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>431</v>
+        <v>445</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>432</v>
+        <v>446</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>0</v>
@@ -14364,13 +14557,13 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>433</v>
+        <v>447</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>434</v>
+        <v>448</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>1</v>
@@ -14382,13 +14575,13 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>435</v>
+        <v>449</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>0</v>
@@ -14400,13 +14593,13 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>437</v>
+        <v>451</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>0</v>
@@ -14418,13 +14611,13 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>439</v>
+        <v>453</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>1</v>
@@ -14436,13 +14629,13 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>441</v>
+        <v>455</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>0</v>
@@ -14454,13 +14647,13 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>443</v>
+        <v>457</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>0</v>
@@ -14472,13 +14665,13 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>445</v>
+        <v>459</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>1</v>
@@ -14490,13 +14683,13 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>447</v>
+        <v>461</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>0</v>
@@ -14508,13 +14701,13 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>449</v>
+        <v>463</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>0</v>
@@ -14526,13 +14719,13 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>451</v>
+        <v>465</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>452</v>
+        <v>466</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>1</v>
@@ -14544,13 +14737,13 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>453</v>
+        <v>467</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>0</v>
@@ -14562,13 +14755,13 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>455</v>
+        <v>469</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>0</v>
@@ -14580,13 +14773,13 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>457</v>
+        <v>471</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>1</v>
@@ -14598,13 +14791,13 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>459</v>
+        <v>473</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>0</v>
@@ -14616,13 +14809,13 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>461</v>
+        <v>475</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>0</v>
@@ -14634,13 +14827,13 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>463</v>
+        <v>477</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>465</v>
+        <v>479</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>1</v>
@@ -14652,13 +14845,13 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>466</v>
+        <v>480</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>467</v>
+        <v>481</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>465</v>
+        <v>479</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>0</v>
@@ -14670,13 +14863,13 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>468</v>
+        <v>482</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>469</v>
+        <v>483</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>465</v>
+        <v>479</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>0</v>
@@ -14688,13 +14881,13 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>470</v>
+        <v>484</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>1</v>
@@ -14706,13 +14899,13 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>472</v>
+        <v>486</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>473</v>
+        <v>487</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>1</v>
@@ -14724,13 +14917,13 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>474</v>
+        <v>488</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>475</v>
+        <v>489</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>1</v>
@@ -14742,13 +14935,13 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>476</v>
+        <v>490</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D79" s="0" t="n">
         <v>0</v>
@@ -14760,13 +14953,13 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>478</v>
+        <v>492</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D80" s="0" t="n">
         <v>0</v>
@@ -14778,13 +14971,13 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>480</v>
+        <v>494</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>0</v>
@@ -14796,13 +14989,13 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>482</v>
+        <v>496</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>0</v>
@@ -14814,13 +15007,13 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>484</v>
+        <v>498</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>0</v>
@@ -14832,13 +15025,13 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>486</v>
+        <v>500</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>0</v>
@@ -14850,13 +15043,13 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>488</v>
+        <v>502</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>489</v>
+        <v>503</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>0</v>
@@ -14868,13 +15061,13 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>490</v>
+        <v>504</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D86" s="0" t="n">
         <v>0</v>
@@ -14886,13 +15079,13 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>492</v>
+        <v>506</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D87" s="0" t="n">
         <v>0</v>
@@ -14904,13 +15097,13 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>494</v>
+        <v>508</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D88" s="0" t="n">
         <v>0</v>
@@ -14922,13 +15115,13 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>496</v>
+        <v>510</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>497</v>
+        <v>511</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>0</v>
@@ -14940,13 +15133,13 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>498</v>
+        <v>512</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>499</v>
+        <v>513</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>465</v>
+        <v>479</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>1</v>
@@ -14958,13 +15151,13 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>500</v>
+        <v>514</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>501</v>
+        <v>515</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D91" s="0" t="n">
         <v>0</v>
@@ -14976,13 +15169,13 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>502</v>
+        <v>516</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>503</v>
+        <v>517</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D92" s="0" t="n">
         <v>0</v>
@@ -14994,13 +15187,13 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>504</v>
+        <v>518</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D93" s="0" t="n">
         <v>0</v>
@@ -15012,13 +15205,13 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>506</v>
+        <v>520</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>507</v>
+        <v>521</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D94" s="0" t="n">
         <v>0</v>
@@ -15030,13 +15223,13 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>508</v>
+        <v>522</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>509</v>
+        <v>523</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D95" s="0" t="n">
         <v>0</v>
@@ -15047,7 +15240,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D95">
+  <autoFilter ref="C1:C95">
     <filterColumn colId="2">
       <customFilters and="true">
         <customFilter operator="equal" val="Ranged"/>
@@ -15076,7 +15269,7 @@
       <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="14.77"/>
@@ -15085,16 +15278,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>510</v>
+        <v>524</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>511</v>
+        <v>525</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>512</v>
+        <v>526</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>135</v>
@@ -15105,13 +15298,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>334</v>
+        <v>348</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="E2" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A2,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B2, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C2, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D2, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15123,13 +15316,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>467</v>
+        <v>481</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="E3" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A3,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B3, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C3, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D3, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15141,13 +15334,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>467</v>
+        <v>481</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="E4" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A4,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B4, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C4, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D4, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15159,13 +15352,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>467</v>
+        <v>481</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="E5" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A5,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B5, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C5, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D5, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15177,13 +15370,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>467</v>
+        <v>481</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>473</v>
+        <v>487</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="E6" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A6,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B6, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C6, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D6, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15195,13 +15388,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>469</v>
+        <v>483</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>467</v>
+        <v>481</v>
       </c>
       <c r="E7" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A7,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B7, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C7, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D7, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15213,13 +15406,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>469</v>
+        <v>483</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>475</v>
+        <v>489</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>467</v>
+        <v>481</v>
       </c>
       <c r="E8" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A8,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B8, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C8, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D8, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15231,13 +15424,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>469</v>
+        <v>483</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>499</v>
+        <v>513</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>467</v>
+        <v>481</v>
       </c>
       <c r="E9" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A9,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B9, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C9, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D9, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15249,13 +15442,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
       <c r="E10" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A10,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B10, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C10, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D10, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15267,13 +15460,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="E11" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A11,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B11, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C11, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D11, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15285,13 +15478,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="E12" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A12,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B12, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C12, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D12, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15303,13 +15496,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>434</v>
+        <v>448</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="E13" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A13,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B13, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C13, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D13, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15321,13 +15514,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="E14" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A14,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B14, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C14, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D14, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15339,13 +15532,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
       <c r="E15" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A15,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B15, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C15, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D15, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15357,13 +15550,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="E16" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A16,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B16, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C16, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D16, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15375,13 +15568,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="E17" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A17,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B17, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C17, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D17, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15393,13 +15586,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="E18" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A18,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B18, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C18, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D18, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15411,13 +15604,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="E19" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A19,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B19, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C19, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D19, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15429,13 +15622,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>334</v>
+        <v>348</v>
       </c>
       <c r="E20" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A20,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B20, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C20, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D20, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15447,13 +15640,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="E21" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A21,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B21, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C21, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D21, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15465,13 +15658,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>376</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>362</v>
       </c>
       <c r="E22" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A22,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B22, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C22, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D22, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15483,13 +15676,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="E23" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A23,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B23, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C23, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D23, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15501,13 +15694,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="E24" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A24,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B24, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C24, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D24, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15519,13 +15712,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
       <c r="E25" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A25,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B25, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C25, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D25, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15537,13 +15730,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="E26" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A26,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B26, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C26, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D26, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15555,13 +15748,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
       <c r="E27" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A27,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B27, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C27, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D27, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15573,13 +15766,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>452</v>
+        <v>466</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="E28" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A28,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B28, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C28, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D28, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15591,13 +15784,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="E29" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A29,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B29, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C29, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D29, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15609,13 +15802,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>432</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>418</v>
-      </c>
       <c r="D30" s="0" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="E30" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A30,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B30, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C30, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D30, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15627,13 +15820,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>351</v>
+        <v>365</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>334</v>
+        <v>348</v>
       </c>
       <c r="E31" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A31,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B31, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C31, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D31, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15645,13 +15838,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>434</v>
+        <v>448</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>351</v>
+        <v>365</v>
       </c>
       <c r="E32" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A32,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B32, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C32, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D32, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15663,13 +15856,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>434</v>
+        <v>448</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="E33" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A33,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B33, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C33, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D33, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15681,13 +15874,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>434</v>
+        <v>448</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="E34" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A34,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B34, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C34, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D34, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15699,13 +15892,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>351</v>
+        <v>365</v>
       </c>
       <c r="E35" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A35,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B35, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C35, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D35, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15717,13 +15910,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>351</v>
+        <v>365</v>
       </c>
       <c r="E36" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A36,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B36, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C36, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D36, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15735,13 +15928,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>473</v>
+        <v>487</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>351</v>
+        <v>365</v>
       </c>
       <c r="E37" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A37,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B37, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C37, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D37, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15753,13 +15946,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="E38" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A38,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B38, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C38, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D38, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15771,13 +15964,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="E39" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A39,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B39, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C39, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D39, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15789,13 +15982,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>475</v>
+        <v>489</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="E40" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A40,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B40, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C40, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D40, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15807,13 +16000,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>499</v>
+        <v>513</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="E41" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A41,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B41, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C41, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D41, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15825,13 +16018,13 @@
         <v>40</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="E42" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A42,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B42, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C42, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D42, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15843,13 +16036,13 @@
         <v>41</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>353</v>
+        <v>367</v>
       </c>
       <c r="E43" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A43,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B43, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C43, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D43, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15861,13 +16054,13 @@
         <v>42</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>434</v>
+        <v>448</v>
       </c>
       <c r="E44" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A44,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B44, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C44, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D44, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15879,13 +16072,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A45,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B45, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C45, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D45, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15897,13 +16090,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="E46" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A46,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B46, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C46, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D46, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15915,13 +16108,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="E47" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A47,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B47, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C47, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D47, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15933,13 +16126,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>353</v>
+        <v>367</v>
       </c>
       <c r="E48" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A48,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B48, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C48, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D48, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15951,13 +16144,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>353</v>
+        <v>367</v>
       </c>
       <c r="E49" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A49,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B49, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C49, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D49, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15969,13 +16162,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>473</v>
+        <v>487</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>353</v>
+        <v>367</v>
       </c>
       <c r="E50" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A50,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B50, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C50, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D50, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15987,13 +16180,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="E51" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A51,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B51, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C51, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D51, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16005,13 +16198,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>385</v>
+        <v>399</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="E52" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A52,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B52, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C52, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D52, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16023,13 +16216,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="E53" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A53,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B53, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C53, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D53, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16041,13 +16234,13 @@
         <v>52</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>475</v>
+        <v>489</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="E54" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A54,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B54, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C54, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D54, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16059,13 +16252,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>499</v>
+        <v>513</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
       <c r="E55" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A55,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B55, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C55, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D55, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16077,13 +16270,13 @@
         <v>54</v>
       </c>
       <c r="B56" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="D56" s="0" t="s">
         <v>448</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>434</v>
       </c>
       <c r="E56" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A56,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B56, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C56, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D56, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16095,13 +16288,13 @@
         <v>55</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>362</v>
+        <v>376</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>334</v>
+        <v>348</v>
       </c>
       <c r="E57" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A57,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B57, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C57, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D57, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16113,13 +16306,13 @@
         <v>56</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="E58" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A58,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B58, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C58, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D58, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16131,13 +16324,13 @@
         <v>57</v>
       </c>
       <c r="B59" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="D59" s="0" t="s">
         <v>448</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>446</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>434</v>
       </c>
       <c r="E59" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A59,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B59, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C59, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D59, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16149,13 +16342,13 @@
         <v>58</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="E60" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A60,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B60, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C60, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D60, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16167,13 +16360,13 @@
         <v>59</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="E61" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A61,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B61, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C61, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D61, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16185,13 +16378,13 @@
         <v>60</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="E62" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A62,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B62, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C62, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D62, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16203,13 +16396,13 @@
         <v>61</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="E63" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A63,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B63, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C63, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D63, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16221,13 +16414,13 @@
         <v>62</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>473</v>
+        <v>487</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="E64" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A64,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B64, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C64, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D64, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16239,13 +16432,13 @@
         <v>63</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
       <c r="E65" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A65,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B65, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C65, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D65, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16257,13 +16450,13 @@
         <v>64</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="E66" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A66,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B66, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C66, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D66, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16275,13 +16468,13 @@
         <v>65</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>396</v>
+        <v>410</v>
       </c>
       <c r="E67" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A67,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B67, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C67, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D67, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16293,13 +16486,13 @@
         <v>66</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>475</v>
+        <v>489</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>396</v>
+        <v>410</v>
       </c>
       <c r="E68" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A68,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B68, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C68, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D68, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16311,13 +16504,13 @@
         <v>67</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>499</v>
+        <v>513</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>396</v>
+        <v>410</v>
       </c>
       <c r="E69" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A69,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B69, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C69, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D69, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16329,13 +16522,13 @@
         <v>68</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>452</v>
+        <v>466</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="E70" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A70,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B70, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C70, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D70, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16347,13 +16540,13 @@
         <v>69</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="E71" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A71,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B71, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C71, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D71, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16365,13 +16558,13 @@
         <v>70</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="E72" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A72,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B72, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C72, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D72, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16383,13 +16576,13 @@
         <v>71</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>473</v>
+        <v>487</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="E73" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A73,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B73, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C73, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D73, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16401,13 +16594,13 @@
         <v>72</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="E74" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A74,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B74, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C74, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D74, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16419,13 +16612,13 @@
         <v>73</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="E75" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A75,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B75, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C75, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D75, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16437,13 +16630,13 @@
         <v>74</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>398</v>
+        <v>412</v>
       </c>
       <c r="E76" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A76,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B76, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C76, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D76, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16455,13 +16648,13 @@
         <v>75</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>475</v>
+        <v>489</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>398</v>
+        <v>412</v>
       </c>
       <c r="E77" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A77,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B77, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C77, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D77, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16473,13 +16666,13 @@
         <v>76</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>499</v>
+        <v>513</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>398</v>
+        <v>412</v>
       </c>
       <c r="E78" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A78,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B78, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C78, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D78, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16491,13 +16684,13 @@
         <v>77</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>402</v>
+        <v>416</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="E79" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A79,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B79, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C79, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D79, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16509,13 +16702,13 @@
         <v>78</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="E80" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A80,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B80, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C80, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D80, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16527,13 +16720,13 @@
         <v>79</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="E81" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A81,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B81, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C81, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D81, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16545,13 +16738,13 @@
         <v>80</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>473</v>
+        <v>487</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="E82" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A82,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B82, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C82, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D82, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16563,13 +16756,13 @@
         <v>81</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>469</v>
+        <v>483</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="E83" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A83,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B83, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C83, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D83, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16581,13 +16774,13 @@
         <v>82</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>475</v>
+        <v>489</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="E84" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A84,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B84, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C84, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D84, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16599,13 +16792,13 @@
         <v>83</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>499</v>
+        <v>513</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="E85" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A85,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B85, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C85, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D85, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16617,13 +16810,13 @@
         <v>84</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="E86" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A86,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B86, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C86, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D86, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16635,13 +16828,13 @@
         <v>85</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>464</v>
+        <v>478</v>
       </c>
       <c r="E87" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A87,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B87, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C87, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D87, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16653,13 +16846,13 @@
         <v>86</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>416</v>
+        <v>430</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>422</v>
+        <v>436</v>
       </c>
       <c r="E88" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A88,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B88, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C88, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D88, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16671,13 +16864,13 @@
         <v>87</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="E89" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A89,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B89, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C89, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D89, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16689,13 +16882,13 @@
         <v>88</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>400</v>
+        <v>414</v>
       </c>
       <c r="E90" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A90,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B90, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C90, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D90, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16707,13 +16900,13 @@
         <v>89</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="E91" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A91,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B91, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C91, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D91, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16725,13 +16918,13 @@
         <v>90</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="E92" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A92,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B92, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C92, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D92, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16743,13 +16936,13 @@
         <v>91</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>422</v>
+        <v>436</v>
       </c>
       <c r="E93" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A93,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B93, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C93, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D93, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16761,13 +16954,13 @@
         <v>92</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="E94" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A94,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B94, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C94, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D94, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16779,13 +16972,13 @@
         <v>93</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="E95" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A95,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B95, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C95, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D95, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16797,13 +16990,13 @@
         <v>94</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>422</v>
+        <v>436</v>
       </c>
       <c r="E96" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A96,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B96, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C96, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D96, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16815,13 +17008,13 @@
         <v>95</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="E97" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A97,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B97, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C97, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D97, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16833,13 +17026,13 @@
         <v>96</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="E98" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A98,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B98, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C98, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D98, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16851,13 +17044,13 @@
         <v>97</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="E99" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A99,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B99, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C99, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D99, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16869,13 +17062,13 @@
         <v>98</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="E100" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A100,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B100, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C100, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D100, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16887,13 +17080,13 @@
         <v>99</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>416</v>
+        <v>430</v>
       </c>
       <c r="E101" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A101,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B101, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C101, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D101, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16905,13 +17098,13 @@
         <v>100</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="E102" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A102,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B102, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C102, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D102, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16923,13 +17116,13 @@
         <v>101</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="E103" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A103,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B103, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C103, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D103, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16941,13 +17134,13 @@
         <v>102</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>416</v>
+        <v>430</v>
       </c>
       <c r="E104" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A104,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B104, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C104, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D104, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16959,13 +17152,13 @@
         <v>103</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="E105" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A105,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B105, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C105, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D105, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16977,13 +17170,13 @@
         <v>104</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="E106" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A106,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B106, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C106, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D106, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16995,13 +17188,13 @@
         <v>105</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="E107" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A107,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B107, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C107, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D107, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17013,13 +17206,13 @@
         <v>106</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="E108" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A108,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B108, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C108, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D108, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17031,13 +17224,13 @@
         <v>107</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>442</v>
+        <v>456</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="E109" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A109,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B109, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C109, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D109, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17049,13 +17242,13 @@
         <v>108</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="E110" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A110,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B110, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C110, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D110, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17067,13 +17260,13 @@
         <v>109</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="E111" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A111,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B111, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C111, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D111, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17085,13 +17278,13 @@
         <v>110</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>489</v>
+        <v>503</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="E112" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A112,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B112, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C112, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D112, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17103,13 +17296,13 @@
         <v>111</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>489</v>
+        <v>503</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="E113" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A113,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B113, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C113, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D113, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17121,13 +17314,13 @@
         <v>112</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>489</v>
+        <v>503</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="E114" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A114,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B114, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C114, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D114, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17139,13 +17332,13 @@
         <v>113</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>489</v>
+        <v>503</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="E115" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A115,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B115, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C115, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D115, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17157,13 +17350,13 @@
         <v>114</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>389</v>
+        <v>403</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="E116" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A116,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B116, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C116, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D116, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17175,13 +17368,13 @@
         <v>115</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>448</v>
+        <v>462</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="E117" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A117,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B117, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C117, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D117, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17193,13 +17386,13 @@
         <v>116</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="E118" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A118,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B118, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C118, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D118, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17211,13 +17404,13 @@
         <v>117</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>489</v>
+        <v>503</v>
       </c>
       <c r="E119" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A119,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B119, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C119, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D119, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17229,13 +17422,13 @@
         <v>118</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>469</v>
+        <v>483</v>
       </c>
       <c r="E120" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A120,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B120, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C120, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D120, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17247,13 +17440,13 @@
         <v>119</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="E121" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A121,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B121, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C121, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D121, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17265,13 +17458,13 @@
         <v>120</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>454</v>
+        <v>468</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="E122" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A122,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B122, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C122, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D122, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17283,13 +17476,13 @@
         <v>121</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="E123" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A123,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B123, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C123, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D123, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17301,13 +17494,13 @@
         <v>122</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="E124" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A124,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B124, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C124, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D124, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17319,13 +17512,13 @@
         <v>123</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="E125" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A125,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B125, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C125, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D125, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17337,13 +17530,13 @@
         <v>124</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="E126" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A126,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B126, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C126, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D126, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17355,13 +17548,13 @@
         <v>125</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>499</v>
+        <v>513</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="E127" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A127,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B127, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C127, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D127, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17373,13 +17566,13 @@
         <v>126</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>497</v>
+        <v>511</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="E128" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A128,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B128, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C128, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D128, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17391,13 +17584,13 @@
         <v>127</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>497</v>
+        <v>511</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>444</v>
+        <v>458</v>
       </c>
       <c r="E129" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A129,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B129, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C129, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D129, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17409,13 +17602,13 @@
         <v>128</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>497</v>
+        <v>511</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>473</v>
+        <v>487</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="E130" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A130,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B130, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C130, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D130, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17427,13 +17620,13 @@
         <v>129</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>497</v>
+        <v>511</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>462</v>
+        <v>476</v>
       </c>
       <c r="E131" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A131,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B131, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C131, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D131, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17445,13 +17638,13 @@
         <v>130</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>501</v>
+        <v>515</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="E132" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A132,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B132, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C132, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D132, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17463,13 +17656,13 @@
         <v>131</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>503</v>
+        <v>517</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>497</v>
+        <v>511</v>
       </c>
       <c r="E133" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A133,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B133, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C133, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D133, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17481,13 +17674,13 @@
         <v>132</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>450</v>
+        <v>464</v>
       </c>
       <c r="E134" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A134,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B134, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C134, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D134, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17499,13 +17692,13 @@
         <v>133</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>507</v>
+        <v>521</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="E135" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A135,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B135, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C135, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D135, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17517,13 +17710,13 @@
         <v>134</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>509</v>
+        <v>523</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>424</v>
+        <v>438</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>507</v>
+        <v>521</v>
       </c>
       <c r="E136" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A136,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B136, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C136, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D136, Commands!B:B, 0), 1, 1)),", },")</f>

</xml_diff>

<commit_message>
Touched up remaining achievements (unless I add one for the High Crest gauntlet)
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
+++ b/Kingdom Hearts Recoded/Kingdom Hearts Recoded.xlsx
@@ -14,8 +14,8 @@
     <sheet name="Command Conversion Combinations" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$95</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$D$95</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$D$95</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$95</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2479" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2543" uniqueCount="558">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -1043,6 +1043,135 @@
     <t xml:space="preserve">CastleOblivionHollowBastion</t>
   </si>
   <si>
+    <t xml:space="preserve">OlympusLayer16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusSave2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OlympusLayer30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer 30</t>
+  </si>
+  <si>
     <t xml:space="preserve">Category</t>
   </si>
   <si>
@@ -1166,63 +1295,33 @@
     <t xml:space="preserve">Fire Blast</t>
   </si>
   <si>
-    <t xml:space="preserve">0x13</t>
-  </si>
-  <si>
     <t xml:space="preserve">Blizzard Blast</t>
   </si>
   <si>
-    <t xml:space="preserve">0x14</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thunder Blast</t>
   </si>
   <si>
-    <t xml:space="preserve">0x15</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aero Blast</t>
   </si>
   <si>
-    <t xml:space="preserve">0x16</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fire Raid</t>
   </si>
   <si>
-    <t xml:space="preserve">0x17</t>
-  </si>
-  <si>
     <t xml:space="preserve">Blizzard Raid</t>
   </si>
   <si>
-    <t xml:space="preserve">0x18</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thunder Raid</t>
   </si>
   <si>
-    <t xml:space="preserve">0x19</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aero Raid</t>
   </si>
   <si>
-    <t xml:space="preserve">0x1a</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fire Buster</t>
   </si>
   <si>
-    <t xml:space="preserve">0x1b</t>
-  </si>
-  <si>
     <t xml:space="preserve">Blizzard Buster</t>
   </si>
   <si>
-    <t xml:space="preserve">0x1c</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thunder Buster</t>
   </si>
   <si>
@@ -1235,16 +1334,10 @@
     <t xml:space="preserve">Ice Sweep</t>
   </si>
   <si>
-    <t xml:space="preserve">0x20</t>
-  </si>
-  <si>
     <t xml:space="preserve">Spark Sweep</t>
   </si>
   <si>
     <t xml:space="preserve">Wind Sweep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x22</t>
   </si>
   <si>
     <t xml:space="preserve">Heat Storm</t>
@@ -1739,7 +1832,7 @@
       <selection pane="topLeft" activeCell="A677" activeCellId="0" sqref="A677"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.35"/>
@@ -11296,13 +11389,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B105" activeCellId="0" sqref="B105"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D121" activeCellId="0" sqref="D121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -13496,9 +13589,336 @@
       <c r="A105" s="0" t="n">
         <v>104</v>
       </c>
+      <c r="B105" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="E105" s="0" t="s">
+        <v>339</v>
+      </c>
       <c r="F105" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A105,": { ""worldId"": ",C105,", ""name"": """,D105,""", ""display"": """,E105,""", ""areaId"": ",B105,", },")</f>
-        <v>104: { "worldId": , "name": "", "display": "", "areaId": , },</v>
+        <v>104: { "worldId": 0x3, "name": "OlympusLayer16", "display": "Layer 16", "areaId": 0xf, },</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="E106" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="F106" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A106,": { ""worldId"": ",C106,", ""name"": """,D106,""", ""display"": """,E106,""", ""areaId"": ",B106,", },")</f>
+        <v>105: { "worldId": 0x3, "name": "OlympusLayer17", "display": "Layer 17", "areaId": 0x10, },</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="F107" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A107,": { ""worldId"": ",C107,", ""name"": """,D107,""", ""display"": """,E107,""", ""areaId"": ",B107,", },")</f>
+        <v>106: { "worldId": 0x3, "name": "OlympusLayer18", "display": "Layer 18", "areaId": 0x11, },</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D108" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="E108" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="F108" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A108,": { ""worldId"": ",C108,", ""name"": """,D108,""", ""display"": """,E108,""", ""areaId"": ",B108,", },")</f>
+        <v>107: { "worldId": 0x3, "name": "OlympusSave2", "display": "Save Room", "areaId": 0x20, },</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D109" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="E109" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="F109" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A109,": { ""worldId"": ",C109,", ""name"": """,D109,""", ""display"": """,E109,""", ""areaId"": ",B109,", },")</f>
+        <v>108: { "worldId": 0x3, "name": "OlympusLayer19", "display": "Layer 19", "areaId": 0x12, },</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D110" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="E110" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="F110" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A110,": { ""worldId"": ",C110,", ""name"": """,D110,""", ""display"": """,E110,""", ""areaId"": ",B110,", },")</f>
+        <v>109: { "worldId": 0x3, "name": "OlympusLayer20", "display": "Layer 20", "areaId": 0x13, },</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D111" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E111" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="F111" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A111,": { ""worldId"": ",C111,", ""name"": """,D111,""", ""display"": """,E111,""", ""areaId"": ",B111,", },")</f>
+        <v>110: { "worldId": 0x3, "name": "OlympusLayer21", "display": "Layer 21", "areaId": 0x14, },</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D112" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="E112" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="F112" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A112,": { ""worldId"": ",C112,", ""name"": """,D112,""", ""display"": """,E112,""", ""areaId"": ",B112,", },")</f>
+        <v>111: { "worldId": 0x3, "name": "OlympusLayer22", "display": "Layer 22", "areaId": 0x15, },</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D113" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="E113" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="F113" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A113,": { ""worldId"": ",C113,", ""name"": """,D113,""", ""display"": """,E113,""", ""areaId"": ",B113,", },")</f>
+        <v>112: { "worldId": 0x3, "name": "OlympusLayer23", "display": "Layer 23", "areaId": 0x16, },</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="E114" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="F114" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A114,": { ""worldId"": ",C114,", ""name"": """,D114,""", ""display"": """,E114,""", ""areaId"": ",B114,", },")</f>
+        <v>113: { "worldId": 0x3, "name": "OlympusLayer24", "display": "Layer 24", "areaId": 0x17, },</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D115" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="E115" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="F115" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A115,": { ""worldId"": ",C115,", ""name"": """,D115,""", ""display"": """,E115,""", ""areaId"": ",B115,", },")</f>
+        <v>114: { "worldId": 0x3, "name": "OlympusLayer25", "display": "Layer 25", "areaId": 0x18, },</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D116" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="E116" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="F116" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A116,": { ""worldId"": ",C116,", ""name"": """,D116,""", ""display"": """,E116,""", ""areaId"": ",B116,", },")</f>
+        <v>115: { "worldId": 0x3, "name": "OlympusLayer26", "display": "Layer 26", "areaId": 0x19, },</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D117" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="E117" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="F117" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A117,": { ""worldId"": ",C117,", ""name"": """,D117,""", ""display"": """,E117,""", ""areaId"": ",B117,", },")</f>
+        <v>116: { "worldId": 0x3, "name": "OlympusLayer27", "display": "Layer 27", "areaId": 0x1a, },</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="F118" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A118,": { ""worldId"": ",C118,", ""name"": """,D118,""", ""display"": """,E118,""", ""areaId"": ",B118,", },")</f>
+        <v>117: { "worldId": 0x3, "name": "OlympusLayer28", "display": "Layer 28", "areaId": 0x1b, },</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="F119" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A119,": { ""worldId"": ",C119,", ""name"": """,D119,""", ""display"": """,E119,""", ""areaId"": ",B119,", },")</f>
+        <v>118: { "worldId": 0x3, "name": "OlympusLayer29", "display": "Layer 29", "areaId": 0x1c, },</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="E120" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="F120" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A120,": { ""worldId"": ",C120,", ""name"": """,D120,""", ""display"": """,E120,""", ""areaId"": ",B120,", },")</f>
+        <v>119: { "worldId": 0x3, "name": "OlympusLayer30", "display": "Layer 30", "areaId": 0x22, },</v>
       </c>
     </row>
   </sheetData>
@@ -13523,7 +13943,7 @@
       <selection pane="topLeft" activeCell="C96" activeCellId="0" sqref="C96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -13538,10 +13958,10 @@
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>338</v>
+        <v>381</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>339</v>
+        <v>382</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>135</v>
@@ -13549,13 +13969,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>340</v>
+        <v>383</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>341</v>
+        <v>384</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>341</v>
+        <v>384</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -13567,13 +13987,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>342</v>
+        <v>385</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>343</v>
+        <v>386</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -13585,13 +14005,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>345</v>
+        <v>388</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>346</v>
+        <v>389</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -13603,13 +14023,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>347</v>
+        <v>390</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>348</v>
+        <v>391</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -13621,13 +14041,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>349</v>
+        <v>392</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -13639,13 +14059,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>352</v>
+        <v>395</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>353</v>
+        <v>396</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0</v>
@@ -13657,13 +14077,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>354</v>
+        <v>397</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>355</v>
+        <v>398</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -13675,13 +14095,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>356</v>
+        <v>399</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>357</v>
+        <v>400</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0</v>
@@ -13693,13 +14113,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>358</v>
+        <v>401</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>359</v>
+        <v>402</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -13711,13 +14131,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>360</v>
+        <v>403</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>361</v>
+        <v>404</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
@@ -13729,13 +14149,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>362</v>
+        <v>405</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>363</v>
+        <v>406</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>1</v>
@@ -13747,13 +14167,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>364</v>
+        <v>407</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>365</v>
+        <v>408</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>0</v>
@@ -13765,13 +14185,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>366</v>
+        <v>409</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>367</v>
+        <v>410</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0</v>
@@ -13783,13 +14203,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>368</v>
+        <v>411</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>369</v>
+        <v>412</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0</v>
@@ -13801,13 +14221,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>370</v>
+        <v>413</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>371</v>
+        <v>414</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0</v>
@@ -13819,13 +14239,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>372</v>
+        <v>415</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>373</v>
+        <v>416</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0</v>
@@ -13837,13 +14257,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>374</v>
+        <v>417</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>375</v>
+        <v>418</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>0</v>
@@ -13858,10 +14278,10 @@
         <v>301</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>376</v>
+        <v>419</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>0</v>
@@ -13876,10 +14296,10 @@
         <v>267</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>377</v>
+        <v>420</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0</v>
@@ -13894,10 +14314,10 @@
         <v>256</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>378</v>
+        <v>421</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0</v>
@@ -13909,13 +14329,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>379</v>
+        <v>348</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>380</v>
+        <v>422</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0</v>
@@ -13927,13 +14347,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>381</v>
+        <v>351</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>382</v>
+        <v>423</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0</v>
@@ -13945,13 +14365,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>383</v>
+        <v>354</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>384</v>
+        <v>424</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>0</v>
@@ -13963,13 +14383,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>385</v>
+        <v>357</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>386</v>
+        <v>425</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>0</v>
@@ -13981,13 +14401,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>387</v>
+        <v>360</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>388</v>
+        <v>426</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>0</v>
@@ -13999,13 +14419,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>389</v>
+        <v>363</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>0</v>
@@ -14017,13 +14437,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>391</v>
+        <v>366</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>392</v>
+        <v>428</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>0</v>
@@ -14035,13 +14455,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>394</v>
+        <v>429</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>0</v>
@@ -14053,13 +14473,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>395</v>
+        <v>372</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>396</v>
+        <v>430</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>0</v>
@@ -14071,13 +14491,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>397</v>
+        <v>375</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>398</v>
+        <v>431</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>0</v>
@@ -14092,10 +14512,10 @@
         <v>203</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>399</v>
+        <v>432</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>0</v>
@@ -14110,10 +14530,10 @@
         <v>206</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>400</v>
+        <v>433</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>0</v>
@@ -14128,10 +14548,10 @@
         <v>211</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>401</v>
+        <v>434</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>0</v>
@@ -14143,13 +14563,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>402</v>
+        <v>344</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>403</v>
+        <v>435</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>0</v>
@@ -14164,10 +14584,10 @@
         <v>241</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>404</v>
+        <v>436</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>0</v>
@@ -14179,13 +14599,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>405</v>
+        <v>378</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>406</v>
+        <v>437</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>0</v>
@@ -14197,13 +14617,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>407</v>
+        <v>438</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>408</v>
+        <v>439</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>0</v>
@@ -14215,13 +14635,13 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>409</v>
+        <v>440</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>410</v>
+        <v>441</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>0</v>
@@ -14233,13 +14653,13 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>411</v>
+        <v>442</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>412</v>
+        <v>443</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>0</v>
@@ -14251,13 +14671,13 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>413</v>
+        <v>444</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>414</v>
+        <v>445</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>0</v>
@@ -14269,13 +14689,13 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>415</v>
+        <v>446</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>416</v>
+        <v>447</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>0</v>
@@ -14287,13 +14707,13 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>417</v>
+        <v>448</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>418</v>
+        <v>449</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>0</v>
@@ -14305,13 +14725,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>0</v>
@@ -14323,13 +14743,13 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>421</v>
+        <v>452</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>422</v>
+        <v>453</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>0</v>
@@ -14341,13 +14761,13 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>423</v>
+        <v>454</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>424</v>
+        <v>455</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>0</v>
@@ -14359,13 +14779,13 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>425</v>
+        <v>456</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>426</v>
+        <v>457</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>0</v>
@@ -14377,13 +14797,13 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>427</v>
+        <v>458</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>428</v>
+        <v>459</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>0</v>
@@ -14395,13 +14815,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>429</v>
+        <v>460</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>430</v>
+        <v>461</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>0</v>
@@ -14413,13 +14833,13 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>431</v>
+        <v>462</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>432</v>
+        <v>463</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>0</v>
@@ -14431,13 +14851,13 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>433</v>
+        <v>464</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>434</v>
+        <v>465</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>0</v>
@@ -14449,13 +14869,13 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>435</v>
+        <v>466</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>436</v>
+        <v>467</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>0</v>
@@ -14467,13 +14887,13 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>437</v>
+        <v>468</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>438</v>
+        <v>469</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>0</v>
@@ -14485,13 +14905,13 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>439</v>
+        <v>470</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>440</v>
+        <v>471</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>0</v>
@@ -14503,13 +14923,13 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>441</v>
+        <v>472</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>442</v>
+        <v>473</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>0</v>
@@ -14521,13 +14941,13 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>443</v>
+        <v>474</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>444</v>
+        <v>475</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>344</v>
+        <v>387</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>0</v>
@@ -14539,13 +14959,13 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>445</v>
+        <v>476</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>446</v>
+        <v>477</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>0</v>
@@ -14557,13 +14977,13 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>447</v>
+        <v>478</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>448</v>
+        <v>479</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>1</v>
@@ -14575,13 +14995,13 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>449</v>
+        <v>480</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>0</v>
@@ -14593,13 +15013,13 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>451</v>
+        <v>482</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>0</v>
@@ -14611,13 +15031,13 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>453</v>
+        <v>484</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>454</v>
+        <v>485</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>1</v>
@@ -14629,13 +15049,13 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>455</v>
+        <v>486</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>0</v>
@@ -14647,13 +15067,13 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>457</v>
+        <v>488</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>0</v>
@@ -14665,13 +15085,13 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>459</v>
+        <v>490</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>460</v>
+        <v>491</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>1</v>
@@ -14683,13 +15103,13 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>461</v>
+        <v>492</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>0</v>
@@ -14701,13 +15121,13 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>463</v>
+        <v>494</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>0</v>
@@ -14719,13 +15139,13 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>465</v>
+        <v>496</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>466</v>
+        <v>497</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>1</v>
@@ -14737,13 +15157,13 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>467</v>
+        <v>498</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>468</v>
+        <v>499</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>0</v>
@@ -14755,13 +15175,13 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>469</v>
+        <v>500</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>470</v>
+        <v>501</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>0</v>
@@ -14773,13 +15193,13 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>471</v>
+        <v>502</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>472</v>
+        <v>503</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>1</v>
@@ -14791,13 +15211,13 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>473</v>
+        <v>504</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>474</v>
+        <v>505</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>0</v>
@@ -14809,13 +15229,13 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>475</v>
+        <v>506</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>476</v>
+        <v>507</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>0</v>
@@ -14827,13 +15247,13 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>477</v>
+        <v>508</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>479</v>
+        <v>510</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>1</v>
@@ -14845,13 +15265,13 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>480</v>
+        <v>511</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>481</v>
+        <v>512</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>479</v>
+        <v>510</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>0</v>
@@ -14863,13 +15283,13 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>482</v>
+        <v>513</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>483</v>
+        <v>514</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>479</v>
+        <v>510</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>0</v>
@@ -14881,13 +15301,13 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>484</v>
+        <v>515</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>1</v>
@@ -14899,13 +15319,13 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>486</v>
+        <v>517</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>487</v>
+        <v>518</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>1</v>
@@ -14917,13 +15337,13 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>488</v>
+        <v>519</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>489</v>
+        <v>520</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>1</v>
@@ -14935,13 +15355,13 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>490</v>
+        <v>521</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>491</v>
+        <v>522</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D79" s="0" t="n">
         <v>0</v>
@@ -14953,13 +15373,13 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>492</v>
+        <v>523</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>493</v>
+        <v>524</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D80" s="0" t="n">
         <v>0</v>
@@ -14971,13 +15391,13 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>494</v>
+        <v>525</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>495</v>
+        <v>526</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>0</v>
@@ -14989,13 +15409,13 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>496</v>
+        <v>527</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>497</v>
+        <v>528</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>0</v>
@@ -15007,13 +15427,13 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>498</v>
+        <v>529</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>499</v>
+        <v>530</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>0</v>
@@ -15025,13 +15445,13 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>500</v>
+        <v>531</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>501</v>
+        <v>532</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>0</v>
@@ -15043,13 +15463,13 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>502</v>
+        <v>533</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>503</v>
+        <v>534</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>0</v>
@@ -15061,13 +15481,13 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>504</v>
+        <v>535</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>505</v>
+        <v>536</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D86" s="0" t="n">
         <v>0</v>
@@ -15079,13 +15499,13 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>506</v>
+        <v>537</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>507</v>
+        <v>538</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D87" s="0" t="n">
         <v>0</v>
@@ -15097,13 +15517,13 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>508</v>
+        <v>539</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D88" s="0" t="n">
         <v>0</v>
@@ -15115,13 +15535,13 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>510</v>
+        <v>541</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>511</v>
+        <v>542</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>0</v>
@@ -15133,13 +15553,13 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>512</v>
+        <v>543</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>513</v>
+        <v>544</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>479</v>
+        <v>510</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>1</v>
@@ -15151,13 +15571,13 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>514</v>
+        <v>545</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>515</v>
+        <v>546</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D91" s="0" t="n">
         <v>0</v>
@@ -15169,13 +15589,13 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>516</v>
+        <v>547</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>517</v>
+        <v>548</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D92" s="0" t="n">
         <v>0</v>
@@ -15187,13 +15607,13 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>518</v>
+        <v>549</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>519</v>
+        <v>550</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D93" s="0" t="n">
         <v>0</v>
@@ -15205,13 +15625,13 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>520</v>
+        <v>551</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>521</v>
+        <v>552</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D94" s="0" t="n">
         <v>0</v>
@@ -15223,13 +15643,13 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>522</v>
+        <v>553</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>523</v>
+        <v>554</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>351</v>
+        <v>394</v>
       </c>
       <c r="D95" s="0" t="n">
         <v>0</v>
@@ -15240,7 +15660,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C95">
+  <autoFilter ref="A1:D95">
     <filterColumn colId="2">
       <customFilters and="true">
         <customFilter operator="equal" val="Ranged"/>
@@ -15269,7 +15689,7 @@
       <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="14.77"/>
@@ -15278,16 +15698,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>524</v>
+        <v>555</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>525</v>
+        <v>556</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>526</v>
+        <v>557</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>135</v>
@@ -15298,13 +15718,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>348</v>
+        <v>391</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="E2" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A2,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B2, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C2, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D2, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15316,13 +15736,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>481</v>
+        <v>512</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>388</v>
+        <v>426</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="E3" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A3,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B3, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C3, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D3, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15334,13 +15754,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>481</v>
+        <v>512</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>474</v>
+        <v>505</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="E4" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A4,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B4, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C4, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D4, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15352,13 +15772,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>481</v>
+        <v>512</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="E5" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A5,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B5, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C5, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D5, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15370,13 +15790,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>481</v>
+        <v>512</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>487</v>
+        <v>518</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="E6" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A6,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B6, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C6, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D6, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15388,13 +15808,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>483</v>
+        <v>514</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>422</v>
+        <v>453</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>481</v>
+        <v>512</v>
       </c>
       <c r="E7" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A7,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B7, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C7, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D7, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15406,13 +15826,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>483</v>
+        <v>514</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>489</v>
+        <v>520</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>481</v>
+        <v>512</v>
       </c>
       <c r="E8" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A8,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B8, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C8, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D8, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15424,13 +15844,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>483</v>
+        <v>514</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>513</v>
+        <v>544</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>481</v>
+        <v>512</v>
       </c>
       <c r="E9" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A9,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B9, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C9, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D9, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15442,13 +15862,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>386</v>
+        <v>425</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>346</v>
+        <v>389</v>
       </c>
       <c r="E10" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A10,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B10, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C10, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D10, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15460,13 +15880,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>386</v>
+        <v>425</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>353</v>
+        <v>396</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>392</v>
+        <v>428</v>
       </c>
       <c r="E11" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A11,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B11, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C11, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D11, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15478,13 +15898,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>386</v>
+        <v>425</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>361</v>
+        <v>404</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>373</v>
+        <v>416</v>
       </c>
       <c r="E12" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A12,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B12, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C12, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D12, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15496,13 +15916,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>386</v>
+        <v>425</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>448</v>
+        <v>479</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="E13" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A13,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B13, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C13, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D13, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15514,13 +15934,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>386</v>
+        <v>425</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="E14" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A14,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B14, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C14, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D14, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15532,13 +15952,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>388</v>
+        <v>426</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>346</v>
+        <v>389</v>
       </c>
       <c r="E15" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A15,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B15, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C15, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D15, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15550,13 +15970,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>388</v>
+        <v>426</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>353</v>
+        <v>396</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>386</v>
+        <v>425</v>
       </c>
       <c r="E16" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A16,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B16, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C16, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D16, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15568,13 +15988,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>388</v>
+        <v>426</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>361</v>
+        <v>404</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>375</v>
+        <v>418</v>
       </c>
       <c r="E17" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A17,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B17, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C17, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D17, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15586,13 +16006,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>388</v>
+        <v>426</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>454</v>
+        <v>485</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="E18" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A18,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B18, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C18, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D18, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15604,13 +16024,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>388</v>
+        <v>426</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="E19" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A19,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B19, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C19, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D19, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15622,13 +16042,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>348</v>
+        <v>391</v>
       </c>
       <c r="E20" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A20,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B20, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C20, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D20, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15640,13 +16060,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>353</v>
+        <v>396</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>388</v>
+        <v>426</v>
       </c>
       <c r="E21" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A21,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B21, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C21, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D21, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15658,13 +16078,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>361</v>
+        <v>404</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>376</v>
+        <v>419</v>
       </c>
       <c r="E22" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A22,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B22, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C22, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D22, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15676,13 +16096,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>460</v>
+        <v>491</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="E23" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A23,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B23, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C23, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D23, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15694,13 +16114,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="E24" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A24,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B24, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C24, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D24, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15712,13 +16132,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>392</v>
+        <v>428</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>363</v>
+        <v>406</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>363</v>
+        <v>406</v>
       </c>
       <c r="E25" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A25,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B25, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C25, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D25, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15730,13 +16150,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>392</v>
+        <v>428</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>361</v>
+        <v>404</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>377</v>
+        <v>420</v>
       </c>
       <c r="E26" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A26,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B26, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C26, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D26, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15748,13 +16168,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>392</v>
+        <v>428</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>377</v>
+        <v>420</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="E27" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A27,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B27, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C27, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D27, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15766,13 +16186,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>392</v>
+        <v>428</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>466</v>
+        <v>497</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="E28" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A28,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B28, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C28, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D28, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15784,13 +16204,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>392</v>
+        <v>428</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>468</v>
+        <v>499</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="E29" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A29,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B29, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C29, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D29, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15802,13 +16222,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>446</v>
+        <v>477</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>432</v>
+        <v>463</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
       <c r="E30" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A30,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B30, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C30, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D30, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15820,13 +16240,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>365</v>
+        <v>408</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>348</v>
+        <v>391</v>
       </c>
       <c r="E31" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A31,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B31, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C31, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D31, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15838,13 +16258,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>448</v>
+        <v>479</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>365</v>
+        <v>408</v>
       </c>
       <c r="E32" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A32,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B32, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C32, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D32, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15856,13 +16276,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>448</v>
+        <v>479</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="E33" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A33,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B33, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C33, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D33, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15874,13 +16294,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>448</v>
+        <v>479</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="E34" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A34,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B34, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C34, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D34, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15892,13 +16312,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>365</v>
+        <v>408</v>
       </c>
       <c r="E35" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A35,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B35, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C35, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D35, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15910,13 +16330,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>365</v>
+        <v>408</v>
       </c>
       <c r="E36" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A36,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B36, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C36, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D36, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15928,13 +16348,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>487</v>
+        <v>518</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>365</v>
+        <v>408</v>
       </c>
       <c r="E37" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A37,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B37, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C37, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D37, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15946,13 +16366,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>378</v>
+        <v>421</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>386</v>
+        <v>425</v>
       </c>
       <c r="E38" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A38,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B38, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C38, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D38, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15964,13 +16384,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>406</v>
+        <v>437</v>
       </c>
       <c r="E39" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A39,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B39, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C39, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D39, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -15982,13 +16402,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>489</v>
+        <v>520</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>406</v>
+        <v>437</v>
       </c>
       <c r="E40" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A40,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B40, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C40, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D40, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16000,13 +16420,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>513</v>
+        <v>544</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>406</v>
+        <v>437</v>
       </c>
       <c r="E41" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A41,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B41, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C41, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D41, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16018,13 +16438,13 @@
         <v>40</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>375</v>
+        <v>418</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>343</v>
+        <v>386</v>
       </c>
       <c r="E42" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A42,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B42, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C42, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D42, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16036,13 +16456,13 @@
         <v>41</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>454</v>
+        <v>485</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>367</v>
+        <v>410</v>
       </c>
       <c r="E43" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A43,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B43, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C43, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D43, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16054,13 +16474,13 @@
         <v>42</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>454</v>
+        <v>485</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>448</v>
+        <v>479</v>
       </c>
       <c r="E44" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A44,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B44, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C44, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D44, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16072,13 +16492,13 @@
         <v>43</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>454</v>
+        <v>485</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>460</v>
+        <v>491</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A45,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B45, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C45, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D45, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16090,13 +16510,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>454</v>
+        <v>485</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="E46" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A46,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B46, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C46, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D46, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16108,13 +16528,13 @@
         <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>454</v>
+        <v>485</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="E47" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A47,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B47, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C47, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D47, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16126,13 +16546,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>367</v>
+        <v>410</v>
       </c>
       <c r="E48" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A48,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B48, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C48, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D48, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16144,13 +16564,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>367</v>
+        <v>410</v>
       </c>
       <c r="E49" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A49,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B49, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C49, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D49, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16162,13 +16582,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>487</v>
+        <v>518</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>367</v>
+        <v>410</v>
       </c>
       <c r="E50" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A50,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B50, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C50, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D50, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16180,13 +16600,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>375</v>
+        <v>418</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>382</v>
+        <v>423</v>
       </c>
       <c r="E51" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A51,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B51, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C51, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D51, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16198,13 +16618,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>399</v>
+        <v>432</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>408</v>
+        <v>439</v>
       </c>
       <c r="E52" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A52,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B52, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C52, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D52, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16216,13 +16636,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>424</v>
+        <v>455</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="E53" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A53,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B53, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C53, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D53, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16234,13 +16654,13 @@
         <v>52</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>489</v>
+        <v>520</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>408</v>
+        <v>439</v>
       </c>
       <c r="E54" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A54,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B54, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C54, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D54, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16252,13 +16672,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>513</v>
+        <v>544</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>408</v>
+        <v>439</v>
       </c>
       <c r="E55" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A55,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B55, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C55, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D55, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16270,13 +16690,13 @@
         <v>54</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>369</v>
+        <v>412</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>448</v>
+        <v>479</v>
       </c>
       <c r="E56" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A56,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B56, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C56, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D56, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16288,13 +16708,13 @@
         <v>55</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>376</v>
+        <v>419</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>348</v>
+        <v>391</v>
       </c>
       <c r="E57" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A57,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B57, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C57, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D57, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16306,13 +16726,13 @@
         <v>56</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>460</v>
+        <v>491</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>369</v>
+        <v>412</v>
       </c>
       <c r="E58" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A58,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B58, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C58, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D58, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16324,13 +16744,13 @@
         <v>57</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>460</v>
+        <v>491</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>448</v>
+        <v>479</v>
       </c>
       <c r="E59" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A59,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B59, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C59, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D59, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16342,13 +16762,13 @@
         <v>58</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>460</v>
+        <v>491</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="E60" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A60,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B60, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C60, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D60, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16360,13 +16780,13 @@
         <v>59</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>460</v>
+        <v>491</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="E61" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A61,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B61, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C61, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D61, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16378,13 +16798,13 @@
         <v>60</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>369</v>
+        <v>412</v>
       </c>
       <c r="E62" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A62,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B62, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C62, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D62, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16396,13 +16816,13 @@
         <v>61</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>369</v>
+        <v>412</v>
       </c>
       <c r="E63" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A63,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B63, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C63, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D63, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16414,13 +16834,13 @@
         <v>62</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>487</v>
+        <v>518</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>369</v>
+        <v>412</v>
       </c>
       <c r="E64" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A64,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B64, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C64, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D64, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16432,13 +16852,13 @@
         <v>63</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>369</v>
+        <v>412</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>392</v>
+        <v>428</v>
       </c>
       <c r="E65" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A65,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B65, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C65, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D65, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16450,13 +16870,13 @@
         <v>64</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>369</v>
+        <v>412</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>404</v>
+        <v>436</v>
       </c>
       <c r="E66" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A66,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B66, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C66, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D66, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16468,13 +16888,13 @@
         <v>65</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>410</v>
+        <v>441</v>
       </c>
       <c r="E67" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A67,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B67, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C67, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D67, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16486,13 +16906,13 @@
         <v>66</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>489</v>
+        <v>520</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>410</v>
+        <v>441</v>
       </c>
       <c r="E68" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A68,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B68, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C68, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D68, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16504,13 +16924,13 @@
         <v>67</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>513</v>
+        <v>544</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>410</v>
+        <v>441</v>
       </c>
       <c r="E69" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A69,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B69, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C69, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D69, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16522,13 +16942,13 @@
         <v>68</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>468</v>
+        <v>499</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>466</v>
+        <v>497</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>371</v>
+        <v>414</v>
       </c>
       <c r="E70" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A70,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B70, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C70, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D70, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16540,13 +16960,13 @@
         <v>69</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>468</v>
+        <v>499</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>371</v>
+        <v>414</v>
       </c>
       <c r="E71" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A71,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B71, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C71, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D71, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16558,13 +16978,13 @@
         <v>70</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>468</v>
+        <v>499</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>371</v>
+        <v>414</v>
       </c>
       <c r="E72" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A72,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B72, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C72, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D72, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16576,13 +16996,13 @@
         <v>71</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>468</v>
+        <v>499</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>487</v>
+        <v>518</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>371</v>
+        <v>414</v>
       </c>
       <c r="E73" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A73,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B73, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C73, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D73, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16594,13 +17014,13 @@
         <v>72</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>470</v>
+        <v>501</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>404</v>
+        <v>436</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="E74" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A74,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B74, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C74, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D74, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16612,13 +17032,13 @@
         <v>73</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>470</v>
+        <v>501</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>404</v>
+        <v>436</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="E75" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A75,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B75, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C75, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D75, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16630,13 +17050,13 @@
         <v>74</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>470</v>
+        <v>501</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>468</v>
+        <v>499</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>412</v>
+        <v>443</v>
       </c>
       <c r="E76" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A76,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B76, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C76, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D76, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16648,13 +17068,13 @@
         <v>75</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>470</v>
+        <v>501</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>489</v>
+        <v>520</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>412</v>
+        <v>443</v>
       </c>
       <c r="E77" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A77,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B77, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C77, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D77, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16666,13 +17086,13 @@
         <v>76</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>470</v>
+        <v>501</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>513</v>
+        <v>544</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>412</v>
+        <v>443</v>
       </c>
       <c r="E78" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A78,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B78, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C78, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D78, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16684,13 +17104,13 @@
         <v>77</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>474</v>
+        <v>505</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>416</v>
+        <v>447</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>472</v>
+        <v>503</v>
       </c>
       <c r="E79" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A79,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B79, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C79, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D79, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16702,13 +17122,13 @@
         <v>78</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>474</v>
+        <v>505</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>472</v>
+        <v>503</v>
       </c>
       <c r="E80" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A80,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B80, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C80, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D80, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16720,13 +17140,13 @@
         <v>79</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>474</v>
+        <v>505</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>472</v>
+        <v>503</v>
       </c>
       <c r="E81" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A81,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B81, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C81, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D81, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16738,13 +17158,13 @@
         <v>80</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>474</v>
+        <v>505</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>487</v>
+        <v>518</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>472</v>
+        <v>503</v>
       </c>
       <c r="E82" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A82,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B82, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C82, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D82, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16756,13 +17176,13 @@
         <v>81</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>476</v>
+        <v>507</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>483</v>
+        <v>514</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>474</v>
+        <v>505</v>
       </c>
       <c r="E83" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A83,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B83, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C83, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D83, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16774,13 +17194,13 @@
         <v>82</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>476</v>
+        <v>507</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>489</v>
+        <v>520</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>474</v>
+        <v>505</v>
       </c>
       <c r="E84" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A84,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B84, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C84, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D84, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16792,13 +17212,13 @@
         <v>83</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>476</v>
+        <v>507</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>513</v>
+        <v>544</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>474</v>
+        <v>505</v>
       </c>
       <c r="E85" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A85,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B85, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C85, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D85, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16810,13 +17230,13 @@
         <v>84</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>346</v>
+        <v>389</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="E86" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A86,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B86, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C86, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D86, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16828,13 +17248,13 @@
         <v>85</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>353</v>
+        <v>396</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>478</v>
+        <v>509</v>
       </c>
       <c r="E87" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A87,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B87, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C87, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D87, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16846,13 +17266,13 @@
         <v>86</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>491</v>
+        <v>522</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>430</v>
+        <v>461</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>436</v>
+        <v>467</v>
       </c>
       <c r="E88" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A88,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B88, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C88, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D88, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16864,13 +17284,13 @@
         <v>87</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>491</v>
+        <v>522</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>495</v>
+        <v>526</v>
       </c>
       <c r="E89" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A89,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B89, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C89, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D89, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16882,13 +17302,13 @@
         <v>88</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>491</v>
+        <v>522</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>414</v>
+        <v>445</v>
       </c>
       <c r="E90" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A90,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B90, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C90, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D90, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16900,13 +17320,13 @@
         <v>89</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>491</v>
+        <v>522</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>495</v>
+        <v>526</v>
       </c>
       <c r="E91" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A91,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B91, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C91, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D91, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16918,13 +17338,13 @@
         <v>90</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>493</v>
+        <v>524</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>422</v>
+        <v>453</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="E92" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A92,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B92, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C92, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D92, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16936,13 +17356,13 @@
         <v>91</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>493</v>
+        <v>524</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>432</v>
+        <v>463</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>436</v>
+        <v>467</v>
       </c>
       <c r="E93" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A93,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B93, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C93, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D93, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16954,13 +17374,13 @@
         <v>92</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>493</v>
+        <v>524</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>491</v>
+        <v>522</v>
       </c>
       <c r="E94" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A94,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B94, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C94, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D94, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16972,13 +17392,13 @@
         <v>93</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>493</v>
+        <v>524</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>495</v>
+        <v>526</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="E95" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A95,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B95, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C95, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D95, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -16990,13 +17410,13 @@
         <v>94</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>495</v>
+        <v>526</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>434</v>
+        <v>465</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>436</v>
+        <v>467</v>
       </c>
       <c r="E96" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A96,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B96, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C96, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D96, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17008,13 +17428,13 @@
         <v>95</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>495</v>
+        <v>526</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>386</v>
+        <v>425</v>
       </c>
       <c r="E97" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A97,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B97, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C97, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D97, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17026,13 +17446,13 @@
         <v>96</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>495</v>
+        <v>526</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>450</v>
+        <v>481</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>493</v>
+        <v>524</v>
       </c>
       <c r="E98" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A98,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B98, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C98, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D98, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17044,13 +17464,13 @@
         <v>97</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>495</v>
+        <v>526</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>493</v>
+        <v>524</v>
       </c>
       <c r="E99" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A99,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B99, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C99, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D99, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17062,13 +17482,13 @@
         <v>98</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>497</v>
+        <v>528</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>388</v>
+        <v>426</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="E100" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A100,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B100, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C100, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D100, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17080,13 +17500,13 @@
         <v>99</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>497</v>
+        <v>528</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>432</v>
+        <v>463</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>430</v>
+        <v>461</v>
       </c>
       <c r="E101" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A101,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B101, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C101, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D101, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17098,13 +17518,13 @@
         <v>100</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>497</v>
+        <v>528</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>499</v>
+        <v>530</v>
       </c>
       <c r="E102" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A102,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B102, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C102, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D102, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17116,13 +17536,13 @@
         <v>101</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>497</v>
+        <v>528</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>501</v>
+        <v>532</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="E103" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A103,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B103, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C103, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D103, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17134,13 +17554,13 @@
         <v>102</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>499</v>
+        <v>530</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>434</v>
+        <v>465</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>430</v>
+        <v>461</v>
       </c>
       <c r="E104" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A104,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B104, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C104, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D104, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17152,13 +17572,13 @@
         <v>103</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>499</v>
+        <v>530</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>501</v>
+        <v>532</v>
       </c>
       <c r="E105" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A105,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B105, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C105, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D105, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17170,13 +17590,13 @@
         <v>104</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>499</v>
+        <v>530</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>505</v>
+        <v>536</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="E106" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A106,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B106, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C106, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D106, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17188,13 +17608,13 @@
         <v>105</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>499</v>
+        <v>530</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>507</v>
+        <v>538</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="E107" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A107,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B107, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C107, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D107, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17206,13 +17626,13 @@
         <v>106</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>501</v>
+        <v>532</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>434</v>
+        <v>465</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>432</v>
+        <v>463</v>
       </c>
       <c r="E108" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A108,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B108, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C108, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D108, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17224,13 +17644,13 @@
         <v>107</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>501</v>
+        <v>532</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>456</v>
+        <v>487</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>432</v>
+        <v>463</v>
       </c>
       <c r="E109" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A109,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B109, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C109, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D109, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17242,13 +17662,13 @@
         <v>108</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>501</v>
+        <v>532</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>434</v>
+        <v>465</v>
       </c>
       <c r="E110" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A110,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B110, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C110, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D110, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17260,13 +17680,13 @@
         <v>109</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>501</v>
+        <v>532</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>497</v>
+        <v>528</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>499</v>
+        <v>530</v>
       </c>
       <c r="E111" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A111,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B111, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C111, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D111, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17278,13 +17698,13 @@
         <v>110</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>503</v>
+        <v>534</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>505</v>
+        <v>536</v>
       </c>
       <c r="E112" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A112,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B112, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C112, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D112, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17296,13 +17716,13 @@
         <v>111</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>503</v>
+        <v>534</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>382</v>
+        <v>423</v>
       </c>
       <c r="E113" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A113,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B113, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C113, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D113, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17314,13 +17734,13 @@
         <v>112</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>503</v>
+        <v>534</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="E114" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A114,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B114, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C114, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D114, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17332,13 +17752,13 @@
         <v>113</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>503</v>
+        <v>534</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>505</v>
+        <v>536</v>
       </c>
       <c r="E115" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A115,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B115, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C115, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D115, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17350,13 +17770,13 @@
         <v>114</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>505</v>
+        <v>536</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>403</v>
+        <v>435</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="E116" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A116,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B116, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C116, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D116, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17368,13 +17788,13 @@
         <v>115</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>505</v>
+        <v>536</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>462</v>
+        <v>493</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="E117" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A117,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B117, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C117, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D117, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17386,13 +17806,13 @@
         <v>116</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>505</v>
+        <v>536</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>470</v>
+        <v>501</v>
       </c>
       <c r="E118" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A118,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B118, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C118, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D118, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17404,13 +17824,13 @@
         <v>117</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>505</v>
+        <v>536</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>503</v>
+        <v>534</v>
       </c>
       <c r="E119" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A119,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B119, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C119, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D119, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17422,13 +17842,13 @@
         <v>118</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>507</v>
+        <v>538</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>483</v>
+        <v>514</v>
       </c>
       <c r="E120" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A120,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B120, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C120, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D120, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17440,13 +17860,13 @@
         <v>119</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>507</v>
+        <v>538</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>468</v>
+        <v>499</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>377</v>
+        <v>420</v>
       </c>
       <c r="E121" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A121,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B121, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C121, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D121, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17458,13 +17878,13 @@
         <v>120</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>507</v>
+        <v>538</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>468</v>
+        <v>499</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
       <c r="E122" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A122,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B122, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C122, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D122, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17476,13 +17896,13 @@
         <v>121</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>507</v>
+        <v>538</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>470</v>
+        <v>501</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
       <c r="E123" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A123,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B123, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C123, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D123, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17494,13 +17914,13 @@
         <v>122</v>
       </c>
       <c r="B124" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="C124" s="0" t="s">
         <v>507</v>
       </c>
-      <c r="C124" s="0" t="s">
-        <v>476</v>
-      </c>
       <c r="D124" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="E124" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A124,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B124, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C124, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D124, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17512,13 +17932,13 @@
         <v>123</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>470</v>
+        <v>501</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>452</v>
+        <v>483</v>
       </c>
       <c r="E125" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A125,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B125, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C125, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D125, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17530,13 +17950,13 @@
         <v>124</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>507</v>
+        <v>538</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>470</v>
+        <v>501</v>
       </c>
       <c r="E126" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A126,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B126, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C126, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D126, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17548,13 +17968,13 @@
         <v>125</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>513</v>
+        <v>544</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>470</v>
+        <v>501</v>
       </c>
       <c r="E127" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A127,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B127, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C127, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D127, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17566,13 +17986,13 @@
         <v>126</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>511</v>
+        <v>542</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>474</v>
+        <v>505</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>476</v>
+        <v>507</v>
       </c>
       <c r="E128" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A128,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B128, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C128, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D128, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17584,13 +18004,13 @@
         <v>127</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>511</v>
+        <v>542</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>476</v>
+        <v>507</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="E129" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A129,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B129, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C129, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D129, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17602,13 +18022,13 @@
         <v>128</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>511</v>
+        <v>542</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>487</v>
+        <v>518</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>476</v>
+        <v>507</v>
       </c>
       <c r="E130" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A130,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B130, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C130, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D130, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17620,13 +18040,13 @@
         <v>129</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>511</v>
+        <v>542</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>476</v>
+        <v>507</v>
       </c>
       <c r="E131" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A131,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B131, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C131, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D131, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17638,13 +18058,13 @@
         <v>130</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>515</v>
+        <v>546</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>497</v>
+        <v>528</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="E132" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A132,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B132, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C132, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D132, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17656,13 +18076,13 @@
         <v>131</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>517</v>
+        <v>548</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>497</v>
+        <v>528</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>511</v>
+        <v>542</v>
       </c>
       <c r="E133" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A133,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B133, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C133, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D133, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17674,13 +18094,13 @@
         <v>132</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>519</v>
+        <v>550</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>499</v>
+        <v>530</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="E134" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A134,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B134, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C134, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D134, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17692,13 +18112,13 @@
         <v>133</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>521</v>
+        <v>552</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>505</v>
+        <v>536</v>
       </c>
       <c r="E135" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A135,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B135, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C135, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D135, Commands!B:B, 0), 1, 1)),", },")</f>
@@ -17710,13 +18130,13 @@
         <v>134</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>523</v>
+        <v>554</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>438</v>
+        <v>469</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>521</v>
+        <v>552</v>
       </c>
       <c r="E136" s="0" t="str">
         <f aca="true">_xlfn.CONCAT(A136,": { ""targetId"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(B136, Commands!B:B, 0), 1, 1)),", ""command1Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(C136, Commands!B:B, 0), 1, 1)),", ""command2Id"": ",INDIRECT("Commands." &amp; ADDRESS(MATCH(D136, Commands!B:B, 0), 1, 1)),", },")</f>

</xml_diff>